<commit_message>
🔄 Actualización automática del mapa (2025-07-18 15:15:41)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P89"/>
+  <dimension ref="A1:P88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6274,7 +6274,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6308</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6284,17 +6284,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>Guayaquil 637</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>807896343</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6309,7 +6309,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Columna con base corroida oxidada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6331,10 +6331,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.459566</v>
+        <v>-58.437378</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.634615</v>
+        <v>-34.62116</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6350,27 +6350,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6308</t>
+          <t>6330</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Guayaquil 637</t>
+          <t>REPUBLICA DE LA INDIA 3106</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>807896343</t>
+          <t>807965776</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6385,7 +6385,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada e inclinada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6407,14 +6407,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.437378</v>
+        <v>-58.413941</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.62116</v>
+        <v>-34.57698</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6426,7 +6426,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6330</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6436,7 +6436,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>REPUBLICA DE LA INDIA 3106</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -6446,7 +6446,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>807965776</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6461,15 +6461,15 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada e inclinada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -6479,18 +6479,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.413941</v>
+        <v>-58.405749</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.57698</v>
+        <v>-34.58224</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6502,27 +6502,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6537,15 +6537,15 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -6559,26 +6559,26 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.405749</v>
+        <v>-58.473179</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.58224</v>
+        <v>-34.629138</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>-502</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6588,17 +6588,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>Tagle 2562</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>808036198</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6613,7 +6613,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Colocar columna para pedir traspaso nodo teco</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6621,60 +6621,60 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.473179</v>
+        <v>-58.400188</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.629138</v>
+        <v>-34.583882</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-502</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Tagle 2562</t>
+          <t>GUARDIA VIEJA 4377</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808036198</t>
+          <t>808099347</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso nodo teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6702,7 +6702,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -6711,14 +6711,14 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.400188</v>
+        <v>-58.426322</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.583882</v>
+        <v>-34.600097</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6730,7 +6730,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>6383</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6740,17 +6740,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>GUARDIA VIEJA 4377</t>
+          <t>FALCON, RAMON L.,CNEL. 1411</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808099347</t>
+          <t>808099320</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6787,14 +6787,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.426322</v>
+        <v>-58.448523</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.600097</v>
+        <v>-34.62452</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -6806,17 +6806,17 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>6383</t>
+          <t>-506</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1411</t>
+          <t>Espinosa 591</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -6826,7 +6826,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808099320</t>
+          <t>808150511</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6854,7 +6854,7 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L85" t="inlineStr">
@@ -6863,10 +6863,10 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.448523</v>
+        <v>-58.449</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.62452</v>
+        <v>-34.616077</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -6882,27 +6882,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>-506</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Espinosa 591</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>808150511</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6930,23 +6930,23 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.449</v>
+        <v>-58.363292</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.616077</v>
+        <v>-34.642869</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -6958,17 +6958,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>-513</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>Montes de Oca 1809</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -6978,7 +6978,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>808240768</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6993,7 +6993,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7011,14 +7011,14 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.363292</v>
+        <v>-58.372941</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.642869</v>
+        <v>-34.648341</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -7034,27 +7034,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>-513</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Montes de Oca 1809</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>808240768</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7069,7 +7069,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7091,93 +7091,17 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.372941</v>
+        <v>-58.432805</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.648341</v>
+        <v>-34.574345</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>-517</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>7/16/2025</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Av Dorrego 2721</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>808373635</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
-        </is>
-      </c>
-      <c r="I89" t="n">
-        <v>1</v>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M89" t="n">
-        <v>-58.432805</v>
-      </c>
-      <c r="N89" t="n">
-        <v>-34.574345</v>
-      </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P89" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-21 15:09:05)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -1017,7 +1017,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>No corresponde</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1025,7 +1025,11 @@
           <t>Fuente Teco</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M8" t="n">
         <v>-58.412544</v>
       </c>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-24 06:58:13)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P88"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7111,6 +7111,78 @@
         </is>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>-529</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>7/23/2025</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Libertad 820</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>-58.384097</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.598913</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Recoleta</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-24 10:12:07)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -7132,7 +7132,11 @@
           <t>1</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr"/>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>ICD30189941</t>
+        </is>
+      </c>
       <c r="F89" t="inlineStr">
         <is>
           <t>Optical Power</t>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-07 07:22:44)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P93"/>
+  <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7495,6 +7495,82 @@
         </is>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>-548</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>8/6/2025</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Sucre 1533</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Traspasar red a columna de TLC y Retirar columna quebrada</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
+        <v>1</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M94" t="n">
+        <v>-58.44649</v>
+      </c>
+      <c r="N94" t="n">
+        <v>-34.558808</v>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P94" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-11 07:12:48)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P95"/>
+  <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7571,82 +7571,6 @@
         </is>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>5894</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>5/27/2025</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>ALBARELLOS AV. 3100</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>Pendiente ADM</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>Reparacion de rienda</t>
-        </is>
-      </c>
-      <c r="I95" t="n">
-        <v>0</v>
-      </c>
-      <c r="J95" t="inlineStr">
-        <is>
-          <t>Tensor</t>
-        </is>
-      </c>
-      <c r="K95" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M95" t="n">
-        <v>-58.512533</v>
-      </c>
-      <c r="N95" t="n">
-        <v>-34.579243</v>
-      </c>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P95" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-13 08:41:25)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P94"/>
+  <dimension ref="A1:P95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,17 +518,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1497</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4/4/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SANCHEZ DE BUSTAMANTE 2064</t>
+          <t>José Andrés Pacheco de Melo 2084</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>784804268</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -548,16 +548,16 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
+          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -566,19 +566,15 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>-58.406882</v>
+        <v>-58.395656</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.588287</v>
+        <v>-34.590364</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -594,27 +590,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2463</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>7/15/2024</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>795698153</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -624,12 +620,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -642,7 +638,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -651,36 +647,36 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.40589</v>
+        <v>-58.496935</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.584156</v>
+        <v>-34.599084</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MCAL SOLANO LOPEZ 3110</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -690,7 +686,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>792101640</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -700,12 +696,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Retirar columna. TLC ya traspaso nodo</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -718,7 +714,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -727,46 +723,46 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.498448</v>
+        <v>-58.441405</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.595287</v>
+        <v>-34.594348</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3154</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8/27/2024</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BRAVO, MARIO 853</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>795498456</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -776,41 +772,37 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Sacar la rienda de la plantera</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
         <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.41606</v>
+        <v>-58.483821</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.599935</v>
+        <v>-34.677698</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -822,27 +814,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1871</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9/5/2024</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bulnes 1810</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>796016024</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -852,16 +844,16 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -870,7 +862,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -879,14 +871,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.413803</v>
+        <v>-58.406585</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.590308</v>
+        <v>-34.592933</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -898,27 +890,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3291</t>
+          <t>1497</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>9/13/2024</t>
+          <t>4/4/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>GUISE 1933</t>
+          <t>SANCHEZ DE BUSTAMANTE 2064</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>796325224</t>
+          <t>784804268</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -933,20 +925,20 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Retirar columna ya traspasaron fuente propia</t>
+          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -955,14 +947,14 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.412544</v>
+        <v>-58.406882</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.590435</v>
+        <v>-34.588287</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -974,27 +966,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3887</t>
+          <t>2463</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>7/15/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4819</t>
+          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>798894281</t>
+          <t>795698153</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1009,7 +1001,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1017,28 +1009,28 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.432085</v>
+        <v>-58.40589</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.60178</v>
+        <v>-34.584156</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1050,27 +1042,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3893</t>
+          <t>2805</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>8/6/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>HERRERA 402</t>
+          <t>MCAL SOLANO LOPEZ 3110</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>798894295</t>
+          <t>792101640</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1085,7 +1077,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Inclinado En el form cargaron foto de otro caso</t>
+          <t>Retirar columna. TLC ya traspaso nodo</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1093,60 +1085,60 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.378613</v>
+        <v>-58.498448</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.6349</v>
+        <v>-34.595287</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>3154</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>8/27/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>José Andrés Pacheco de Melo 2084</t>
+          <t>BRAVO, MARIO 853</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>795498456</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1156,12 +1148,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
+          <t>Sacar la rienda de la plantera</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1169,24 +1161,28 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
       <c r="M10" t="n">
-        <v>-58.395656</v>
+        <v>-58.41606</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.590364</v>
+        <v>-34.599935</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1198,27 +1194,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>798897458</t>
+          <t>1871</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10/15/2024</t>
+          <t>9/5/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Rojas 1091</t>
+          <t>Bulnes 1810</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>798897458</t>
+          <t>796016024</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1233,7 +1229,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Columna fuera de plomo (inclinada)</t>
+          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1241,24 +1237,28 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr"/>
+          <t>Nodo TLC</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M11" t="n">
-        <v>-58.446458</v>
+        <v>-58.413803</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.608741</v>
+        <v>-34.590308</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1270,17 +1270,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3938</t>
+          <t>3291</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>11/5/2024</t>
+          <t>9/13/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2604</t>
+          <t>GUISE 1933</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>799246642</t>
+          <t>796325224</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Realizar traspasos y retiro de columna vieja</t>
+          <t>Retirar columna ya traspasaron fuente propia</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1313,24 +1313,24 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.426169</v>
+        <v>-58.412544</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.579697</v>
+        <v>-34.590435</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1346,17 +1346,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4025</t>
+          <t>3887</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MEXICO 4249</t>
+          <t>ESTADO DE ISRAEL AV. 4819</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>799981143</t>
+          <t>798894281</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Ver foto, colocar columna para traspasar</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1389,28 +1389,28 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.425997</v>
+        <v>-58.432085</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.620454</v>
+        <v>-34.60178</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1422,27 +1422,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4222</t>
+          <t>3893</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HUMAHUACA 4500</t>
+          <t>HERRERA 402</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>800810078</t>
+          <t>798894295</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Columna con base corroída/oxidada</t>
+          <t>Inclinado En el form cargaron foto de otro caso</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1475,18 +1475,18 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.428283</v>
+        <v>-58.378613</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.601207</v>
+        <v>-34.6349</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1498,17 +1498,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>4426</t>
+          <t>798897458</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>12/19/2024</t>
+          <t>10/15/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LORA, FELIX 27</t>
+          <t>Rojas 1091</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1518,7 +1518,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>801768138</t>
+          <t>798897458</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
+          <t>Columna fuera de plomo (inclinada)</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1541,24 +1541,20 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
-        <v>-58.443626</v>
+        <v>-58.446458</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.621032</v>
+        <v>-34.608741</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1574,27 +1570,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>6243</t>
+          <t>3938</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1/30/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>GARCIA, TEODORO 3252</t>
+          <t>GODOY CRUZ 2604</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>779373118</t>
+          <t>799246642</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1605,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Colocar R400 para posterior traspaso</t>
+          <t>Realizar traspasos y retiro de columna vieja</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1617,60 +1613,60 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.450789</v>
+        <v>-58.426169</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.577949</v>
+        <v>-34.579697</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>-51</t>
+          <t>4025</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/5/2024</t>
+          <t>11/12/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CHARCAS /ALT/ 4176</t>
+          <t>MEXICO 4249</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>782773317</t>
+          <t>799981143</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,11 +1681,11 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">columna de 114mm de nuestra propiedad que esta quebrada y en mal estado, para remplazar ubicada en CHARCAS 4176 </t>
+          <t>Ver foto, colocar columna para traspasar</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1707,14 +1703,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.421741</v>
+        <v>-58.425997</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.584789</v>
+        <v>-34.620454</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1726,27 +1722,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>-212</t>
+          <t>4222</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>11/28/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>FIGUEROA CNEL APOLINARIO /ALT/ 863</t>
+          <t>HUMAHUACA 4500</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>799485362</t>
+          <t>800810078</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,11 +1757,11 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir el traspaso</t>
+          <t>Columna con base corroída/oxidada</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1774,7 +1770,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1783,46 +1779,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.450579</v>
+        <v>-58.428283</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.607673</v>
+        <v>-34.601207</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5884</t>
+          <t>4426</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>12/19/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>OLLEROS 2952</t>
+          <t>LORA, FELIX 27</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>799450967</t>
+          <t>801768138</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,11 +1833,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso</t>
+          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1850,7 +1846,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1859,14 +1855,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.447022</v>
+        <v>-58.443626</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.575873</v>
+        <v>-34.621032</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1878,27 +1874,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4528</t>
+          <t>6243</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1/16/2025</t>
+          <t>1/30/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>BARCO CENTENERA DEL 545</t>
+          <t>GARCIA, TEODORO 3252</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>802774521</t>
+          <t>779373118</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,7 +1909,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para posterior traspaso</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1926,7 +1922,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1935,46 +1931,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.440625</v>
+        <v>-58.450789</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.625499</v>
+        <v>-34.577949</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>-51</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>4/5/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>CHARCAS /ALT/ 4176</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>782773317</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1984,16 +1980,16 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">columna de 114mm de nuestra propiedad que esta quebrada y en mal estado, para remplazar ubicada en CHARCAS 4176 </t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2011,46 +2007,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.496935</v>
+        <v>-58.421741</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.599084</v>
+        <v>-34.584789</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>-212</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>FIGUEROA CNEL APOLINARIO /ALT/ 863</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>799485362</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2065,11 +2061,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Colocar columna para pedir el traspaso</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2078,7 +2074,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2087,46 +2083,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.400156</v>
+        <v>-58.450579</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.631369</v>
+        <v>-34.607673</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>5884</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>OLLEROS 2952</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>799450967</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,11 +2137,11 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Solo retirar columna ya se realizo traspaso</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2163,14 +2159,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.402062</v>
+        <v>-58.447022</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.635143</v>
+        <v>-34.575873</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2182,27 +2178,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4768</t>
+          <t>4528</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>1/16/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 684</t>
+          <t>BARCO CENTENERA DEL 545</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>802988221</t>
+          <t>802774521</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2239,14 +2235,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.443039</v>
+        <v>-58.440625</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.612262</v>
+        <v>-34.625499</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2258,27 +2254,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4831</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2/4/2025</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MERCEDES 3054</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>803086856</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2289,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Sacar rienda a pique ver con inspector</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2306,55 +2302,55 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.506348</v>
+        <v>-58.400156</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.607461</v>
+        <v>-34.631369</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>6066</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ALBARIÑO 1331</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>803651213</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2365,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Podrida en la base</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2382,7 +2378,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2391,46 +2387,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.496255</v>
+        <v>-58.402062</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.650599</v>
+        <v>-34.635143</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>4768</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>VALLESE, FELIPE 684</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>802988221</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,11 +2441,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Picada info para cierre tambien entro como caso 6909</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2467,14 +2463,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.371855</v>
+        <v>-58.443039</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.646958</v>
+        <v>-34.612262</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2486,27 +2482,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>4831</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>2/4/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>MERCEDES 3054</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>803086856</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,11 +2517,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Sacar rienda a pique ver con inspector</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2539,50 +2535,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.403583</v>
+        <v>-58.506348</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.591604</v>
+        <v>-34.607461</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>6066</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>2/26/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>ALBARIÑO 1331</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>803651213</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2592,12 +2588,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+          <t>Podrida en la base</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2610,7 +2606,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2619,46 +2615,46 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.441405</v>
+        <v>-58.496255</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.594348</v>
+        <v>-34.650599</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4572</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 5263</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804309785</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,11 +2669,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2695,14 +2691,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.439791</v>
+        <v>-58.371855</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.61969</v>
+        <v>-34.646958</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2714,27 +2710,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2744,12 +2740,16 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Base picada</t>
+        </is>
+      </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2758,7 +2758,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2767,14 +2767,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.483821</v>
+        <v>-58.403583</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.677698</v>
+        <v>-34.591604</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2786,27 +2786,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5521</t>
+          <t>4572</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>EL PEREGRINO 3115</t>
+          <t>RIVADAVIA AV. 5263</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804569000</t>
+          <t>804309785</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Volvio a ingresar se inclino el poste - caso 6316</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2829,7 +2829,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2839,50 +2839,50 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.485232</v>
+        <v>-58.439791</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.611573</v>
+        <v>-34.61969</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>5521</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>EL PEREGRINO 3115</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>804569000</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2897,7 +2897,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Volvio a ingresar se inclino el poste - caso 6316</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2905,60 +2905,60 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.445131</v>
+        <v>-58.485232</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.572117</v>
+        <v>-34.611573</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Columna corroída en su base</t>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2986,7 +2986,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2995,14 +2995,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.425764</v>
+        <v>-58.445131</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.604359</v>
+        <v>-34.572117</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3014,27 +3014,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Columna corroída en su base</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3071,10 +3071,10 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.439751</v>
+        <v>-58.425764</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.609908</v>
+        <v>-34.604359</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3090,7 +3090,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5632</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 93</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804876047</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3147,14 +3147,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.43607</v>
+        <v>-58.439751</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.61926</v>
+        <v>-34.609908</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3166,7 +3166,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5632</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3176,17 +3176,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>MORENO, JOSE MARIA AV. 93</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>804876047</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3223,14 +3223,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.375515</v>
+        <v>-58.43607</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.634393</v>
+        <v>-34.61926</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3242,27 +3242,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5887</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4/25/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>PALPA 3162</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>805010113</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3277,7 +3277,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Cambiar columna podrida en base.</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3299,46 +3299,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.451203</v>
+        <v>-58.375515</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.576561</v>
+        <v>-34.634393</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>5887</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/25/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>PALPA 3162</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>805010113</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3353,7 +3353,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna podrida en base.</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3375,46 +3375,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.415839</v>
+        <v>-58.451203</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.599291</v>
+        <v>-34.576561</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Migueletes 1326</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3451,46 +3451,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.440177</v>
+        <v>-58.415839</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.56291</v>
+        <v>-34.599291</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>Migueletes 1326</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3505,7 +3505,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3527,46 +3527,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.469148</v>
+        <v>-58.440177</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.687883</v>
+        <v>-34.56291</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3603,14 +3603,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.395063</v>
+        <v>-58.469148</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.606257</v>
+        <v>-34.687883</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3622,7 +3622,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3632,17 +3632,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3665,12 +3665,12 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3679,14 +3679,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.429977</v>
+        <v>-58.395063</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.615514</v>
+        <v>-34.606257</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3708,17 +3708,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3755,14 +3755,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.421623</v>
+        <v>-58.429977</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.614541</v>
+        <v>-34.615514</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3774,27 +3774,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-416</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Paraguay 3765</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>806926557</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3809,7 +3809,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3817,12 +3817,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3831,14 +3831,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.416562</v>
+        <v>-58.421623</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.590589</v>
+        <v>-34.614541</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3850,7 +3850,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-416</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3860,17 +3860,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>Paraguay 3765</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>806926557</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3885,7 +3885,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3907,14 +3907,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.429972</v>
+        <v>-58.416562</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.632042</v>
+        <v>-34.590589</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3926,7 +3926,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3936,17 +3936,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3983,26 +3983,26 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.47888</v>
+        <v>-58.429972</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.571108</v>
+        <v>-34.632042</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4012,17 +4012,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4037,7 +4037,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4059,26 +4059,26 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.443196</v>
+        <v>-58.47888</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.618534</v>
+        <v>-34.571108</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-437</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4088,17 +4088,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Cochabamba 4090</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806926861</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4126,7 +4126,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4135,14 +4135,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.422268</v>
+        <v>-58.443196</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.627754</v>
+        <v>-34.618534</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4154,7 +4154,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-438</t>
+          <t>-437</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4164,17 +4164,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Juncal 4565</t>
+          <t>Cochabamba 4090</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806926927</t>
+          <t>806926861</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4189,7 +4189,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4202,7 +4202,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -4211,14 +4211,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.423148</v>
+        <v>-58.422268</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.576964</v>
+        <v>-34.627754</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4230,7 +4230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>-438</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4240,17 +4240,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>Juncal 4565</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>806926927</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4260,16 +4260,16 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -4287,14 +4287,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.406585</v>
+        <v>-58.423148</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.592933</v>
+        <v>-34.576964</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -7568,6 +7568,82 @@
       <c r="P94" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>6917</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>8/12/2025</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>BRIN, MINISTRO 1375</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>808918700</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
+        </is>
+      </c>
+      <c r="I95" t="n">
+        <v>1</v>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M95" t="n">
+        <v>-58.355342</v>
+      </c>
+      <c r="N95" t="n">
+        <v>-34.63565</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P95" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-13 13:48:06)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -518,17 +518,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>1497</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>4/4/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>José Andrés Pacheco de Melo 2084</t>
+          <t>SANCHEZ DE BUSTAMANTE 2064</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>784804268</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -548,16 +548,16 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
+          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -566,15 +566,19 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr"/>
+          <t>Nodo TLC</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M2" t="n">
-        <v>-58.395656</v>
+        <v>-58.406882</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.590364</v>
+        <v>-34.588287</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -590,27 +594,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>2463</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>7/15/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>795698153</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -620,12 +624,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -638,7 +642,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -647,36 +651,36 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.496935</v>
+        <v>-58.40589</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.599084</v>
+        <v>-34.584156</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>2805</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>8/6/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>MCAL SOLANO LOPEZ 3110</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -686,7 +690,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>792101640</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -696,12 +700,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+          <t>Retirar columna. TLC ya traspaso nodo</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -714,7 +718,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -723,46 +727,46 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.441405</v>
+        <v>-58.498448</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.594348</v>
+        <v>-34.595287</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>3154</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>8/27/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>BRAVO, MARIO 853</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>795498456</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -772,37 +776,41 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Sacar la rienda de la plantera</t>
+        </is>
+      </c>
       <c r="I5" t="n">
         <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.483821</v>
+        <v>-58.41606</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.677698</v>
+        <v>-34.599935</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -814,27 +822,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>1871</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>9/5/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>Bulnes 1810</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>796016024</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -844,16 +852,16 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -862,7 +870,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -871,14 +879,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.406585</v>
+        <v>-58.413803</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.592933</v>
+        <v>-34.590308</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -890,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1497</t>
+          <t>3291</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4/4/2024</t>
+          <t>9/13/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SANCHEZ DE BUSTAMANTE 2064</t>
+          <t>GUISE 1933</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>784804268</t>
+          <t>796325224</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -925,20 +933,20 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
+          <t>Retirar columna ya traspasaron fuente propia</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -947,14 +955,14 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.406882</v>
+        <v>-58.412544</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.588287</v>
+        <v>-34.590435</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -966,27 +974,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2463</t>
+          <t>3887</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7/15/2024</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
+          <t>ESTADO DE ISRAEL AV. 4819</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>795698153</t>
+          <t>798894281</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1001,7 +1009,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1009,28 +1017,28 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.40589</v>
+        <v>-58.432085</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.584156</v>
+        <v>-34.60178</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1042,27 +1050,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>3893</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MCAL SOLANO LOPEZ 3110</t>
+          <t>HERRERA 402</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>792101640</t>
+          <t>798894295</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1077,7 +1085,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Retirar columna. TLC ya traspaso nodo</t>
+          <t>Inclinado En el form cargaron foto de otro caso</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1085,60 +1093,60 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.498448</v>
+        <v>-58.378613</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.595287</v>
+        <v>-34.6349</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3154</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>8/27/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>BRAVO, MARIO 853</t>
+          <t>José Andrés Pacheco de Melo 2084</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>795498456</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1148,12 +1156,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Sacar la rienda de la plantera</t>
+          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1161,28 +1169,24 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>Poste</t>
-        </is>
-      </c>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="n">
-        <v>-58.41606</v>
+        <v>-58.395656</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.599935</v>
+        <v>-34.590364</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1194,27 +1198,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1871</t>
+          <t>798897458</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>9/5/2024</t>
+          <t>10/15/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Bulnes 1810</t>
+          <t>Rojas 1091</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>796016024</t>
+          <t>798897458</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1229,7 +1233,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
+          <t>Columna fuera de plomo (inclinada)</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1237,28 +1241,24 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr"/>
       <c r="M11" t="n">
-        <v>-58.413803</v>
+        <v>-58.446458</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.590308</v>
+        <v>-34.608741</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1270,17 +1270,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3291</t>
+          <t>3938</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>9/13/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>GUISE 1933</t>
+          <t>GODOY CRUZ 2604</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>796325224</t>
+          <t>799246642</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Retirar columna ya traspasaron fuente propia</t>
+          <t>Realizar traspasos y retiro de columna vieja</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1313,24 +1313,24 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.412544</v>
+        <v>-58.426169</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.590435</v>
+        <v>-34.579697</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1346,17 +1346,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3887</t>
+          <t>4025</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>11/12/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4819</t>
+          <t>MEXICO 4249</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>798894281</t>
+          <t>799981143</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Ver foto, colocar columna para traspasar</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1389,28 +1389,28 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.432085</v>
+        <v>-58.425997</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.60178</v>
+        <v>-34.620454</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1422,27 +1422,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3893</t>
+          <t>4222</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>11/28/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HERRERA 402</t>
+          <t>HUMAHUACA 4500</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>798894295</t>
+          <t>800810078</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Inclinado En el form cargaron foto de otro caso</t>
+          <t>Columna con base corroída/oxidada</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1475,18 +1475,18 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.378613</v>
+        <v>-58.428283</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.6349</v>
+        <v>-34.601207</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1498,17 +1498,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>798897458</t>
+          <t>4426</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10/15/2024</t>
+          <t>12/19/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Rojas 1091</t>
+          <t>LORA, FELIX 27</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1518,7 +1518,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>798897458</t>
+          <t>801768138</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Columna fuera de plomo (inclinada)</t>
+          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1541,20 +1541,24 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr"/>
+          <t>Nodo TLC</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M15" t="n">
-        <v>-58.446458</v>
+        <v>-58.443626</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.608741</v>
+        <v>-34.621032</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1570,27 +1574,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3938</t>
+          <t>6243</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>11/5/2024</t>
+          <t>1/30/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2604</t>
+          <t>GARCIA, TEODORO 3252</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>799246642</t>
+          <t>779373118</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1605,7 +1609,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Realizar traspasos y retiro de columna vieja</t>
+          <t>Colocar R400 para posterior traspaso</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1613,60 +1617,60 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.426169</v>
+        <v>-58.450789</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.579697</v>
+        <v>-34.577949</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>4025</t>
+          <t>-51</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>4/5/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>MEXICO 4249</t>
+          <t>CHARCAS /ALT/ 4176</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>799981143</t>
+          <t>782773317</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1681,11 +1685,11 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Ver foto, colocar columna para traspasar</t>
+          <t xml:space="preserve">columna de 114mm de nuestra propiedad que esta quebrada y en mal estado, para remplazar ubicada en CHARCAS 4176 </t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1703,14 +1707,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.425997</v>
+        <v>-58.421741</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.620454</v>
+        <v>-34.584789</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1722,27 +1726,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>4222</t>
+          <t>-212</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>HUMAHUACA 4500</t>
+          <t>FIGUEROA CNEL APOLINARIO /ALT/ 863</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>800810078</t>
+          <t>799485362</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1757,11 +1761,11 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Columna con base corroída/oxidada</t>
+          <t>Colocar columna para pedir el traspaso</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1770,7 +1774,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1779,46 +1783,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.428283</v>
+        <v>-58.450579</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.601207</v>
+        <v>-34.607673</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4426</t>
+          <t>5884</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>12/19/2024</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>LORA, FELIX 27</t>
+          <t>OLLEROS 2952</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>801768138</t>
+          <t>799450967</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1833,11 +1837,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
+          <t>Solo retirar columna ya se realizo traspaso</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1846,7 +1850,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1855,14 +1859,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.443626</v>
+        <v>-58.447022</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.621032</v>
+        <v>-34.575873</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1874,27 +1878,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>6243</t>
+          <t>4528</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1/30/2024</t>
+          <t>1/16/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>GARCIA, TEODORO 3252</t>
+          <t>BARCO CENTENERA DEL 545</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>779373118</t>
+          <t>802774521</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1909,7 +1913,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Colocar R400 para posterior traspaso</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1922,7 +1926,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1931,46 +1935,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.450789</v>
+        <v>-58.440625</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.577949</v>
+        <v>-34.625499</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-51</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/5/2024</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CHARCAS /ALT/ 4176</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>782773317</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1980,16 +1984,16 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t xml:space="preserve">columna de 114mm de nuestra propiedad que esta quebrada y en mal estado, para remplazar ubicada en CHARCAS 4176 </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2007,46 +2011,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.421741</v>
+        <v>-58.496935</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.584789</v>
+        <v>-34.599084</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-212</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>FIGUEROA CNEL APOLINARIO /ALT/ 863</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>799485362</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2061,11 +2065,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir el traspaso</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2074,7 +2078,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2083,46 +2087,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.450579</v>
+        <v>-58.400156</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.607673</v>
+        <v>-34.631369</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5884</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OLLEROS 2952</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>799450967</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2137,11 +2141,11 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2159,14 +2163,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.447022</v>
+        <v>-58.402062</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.575873</v>
+        <v>-34.635143</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2178,27 +2182,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4528</t>
+          <t>4768</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1/16/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>BARCO CENTENERA DEL 545</t>
+          <t>VALLESE, FELIPE 684</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>802774521</t>
+          <t>802988221</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2213,7 +2217,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada info para cierre tambien entro como caso 6909</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2235,14 +2239,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.440625</v>
+        <v>-58.443039</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.625499</v>
+        <v>-34.612262</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2254,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>4831</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>2/4/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>MERCEDES 3054</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>803086856</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2289,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Sacar rienda a pique ver con inspector</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2302,55 +2306,55 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.400156</v>
+        <v>-58.506348</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.631369</v>
+        <v>-34.607461</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>6066</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>2/26/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>ALBARIÑO 1331</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>803651213</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2365,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Podrida en la base</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2378,7 +2382,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2387,46 +2391,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.402062</v>
+        <v>-58.496255</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.635143</v>
+        <v>-34.650599</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4768</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 684</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>802988221</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2441,11 +2445,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada info para cierre tambien entro como caso 6909</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2463,14 +2467,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.443039</v>
+        <v>-58.371855</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.612262</v>
+        <v>-34.646958</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2482,27 +2486,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4831</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2/4/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>MERCEDES 3054</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>803086856</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2517,11 +2521,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Sacar rienda a pique ver con inspector</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2535,50 +2539,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.506348</v>
+        <v>-58.403583</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.607461</v>
+        <v>-34.591604</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6066</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ALBARIÑO 1331</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>803651213</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2588,12 +2592,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Podrida en la base</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2606,7 +2610,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2615,46 +2619,46 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.496255</v>
+        <v>-58.441405</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.650599</v>
+        <v>-34.594348</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>4572</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>RIVADAVIA AV. 5263</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>804309785</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2669,11 +2673,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2691,14 +2695,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.371855</v>
+        <v>-58.439791</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.646958</v>
+        <v>-34.61969</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2710,27 +2714,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2740,16 +2744,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Base picada</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr"/>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2758,7 +2758,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2767,14 +2767,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.403583</v>
+        <v>-58.483821</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.591604</v>
+        <v>-34.677698</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2786,27 +2786,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4572</t>
+          <t>5521</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 5263</t>
+          <t>EL PEREGRINO 3115</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804309785</t>
+          <t>804569000</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Volvio a ingresar se inclino el poste - caso 6316</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2829,7 +2829,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2839,50 +2839,50 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.439791</v>
+        <v>-58.485232</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.61969</v>
+        <v>-34.611573</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5521</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>EL PEREGRINO 3115</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804569000</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2897,7 +2897,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Volvio a ingresar se inclino el poste - caso 6316</t>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2905,60 +2905,60 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.485232</v>
+        <v>-58.445131</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.611573</v>
+        <v>-34.572117</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Columna corroída en su base</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2986,7 +2986,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2995,14 +2995,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.445131</v>
+        <v>-58.425764</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.572117</v>
+        <v>-34.604359</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3014,27 +3014,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Columna corroída en su base</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3071,10 +3071,10 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.425764</v>
+        <v>-58.439751</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.604359</v>
+        <v>-34.609908</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3090,7 +3090,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>5632</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>MORENO, JOSE MARIA AV. 93</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>804876047</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3147,14 +3147,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.439751</v>
+        <v>-58.43607</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.609908</v>
+        <v>-34.61926</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3166,7 +3166,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5632</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3176,17 +3176,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 93</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804876047</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3223,14 +3223,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.43607</v>
+        <v>-58.375515</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.61926</v>
+        <v>-34.634393</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3242,27 +3242,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5887</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/25/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>PALPA 3162</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>805010113</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3277,7 +3277,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Cambiar columna podrida en base.</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3299,46 +3299,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.375515</v>
+        <v>-58.451203</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.634393</v>
+        <v>-34.576561</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5887</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4/25/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>PALPA 3162</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>805010113</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3353,7 +3353,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Cambiar columna podrida en base.</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3375,46 +3375,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.451203</v>
+        <v>-58.415839</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.576561</v>
+        <v>-34.599291</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>Migueletes 1326</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3451,46 +3451,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.415839</v>
+        <v>-58.440177</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.599291</v>
+        <v>-34.56291</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Migueletes 1326</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3505,7 +3505,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3527,46 +3527,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.440177</v>
+        <v>-58.469148</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.56291</v>
+        <v>-34.687883</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3603,14 +3603,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.469148</v>
+        <v>-58.395063</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.687883</v>
+        <v>-34.606257</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3622,7 +3622,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3632,17 +3632,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3665,12 +3665,12 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3679,14 +3679,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.395063</v>
+        <v>-58.429977</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.606257</v>
+        <v>-34.615514</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3708,17 +3708,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3755,14 +3755,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.429977</v>
+        <v>-58.421623</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.615514</v>
+        <v>-34.614541</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3774,27 +3774,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>-416</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>Paraguay 3765</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>806926557</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3809,7 +3809,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3817,12 +3817,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3831,14 +3831,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.421623</v>
+        <v>-58.416562</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.614541</v>
+        <v>-34.590589</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3850,7 +3850,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-416</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3860,17 +3860,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Paraguay 3765</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806926557</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3885,7 +3885,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3907,14 +3907,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.416562</v>
+        <v>-58.429972</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.590589</v>
+        <v>-34.632042</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3926,7 +3926,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3936,17 +3936,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3983,26 +3983,26 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.429972</v>
+        <v>-58.47888</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.632042</v>
+        <v>-34.571108</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4012,17 +4012,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4037,7 +4037,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4059,26 +4059,26 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.47888</v>
+        <v>-58.443196</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.571108</v>
+        <v>-34.618534</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>-437</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4088,17 +4088,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>Cochabamba 4090</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>806926861</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4126,7 +4126,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4135,14 +4135,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.443196</v>
+        <v>-58.422268</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.618534</v>
+        <v>-34.627754</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4154,7 +4154,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-437</t>
+          <t>-438</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4164,17 +4164,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Cochabamba 4090</t>
+          <t>Juncal 4565</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806926861</t>
+          <t>806926927</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4189,7 +4189,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4202,7 +4202,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -4211,14 +4211,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.422268</v>
+        <v>-58.423148</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.627754</v>
+        <v>-34.576964</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4230,7 +4230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-438</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4240,17 +4240,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Juncal 4565</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>806926927</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4260,16 +4260,16 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -4287,14 +4287,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.423148</v>
+        <v>-58.406585</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.576964</v>
+        <v>-34.592933</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-21 08:07:01)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -518,17 +518,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1497</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4/4/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SANCHEZ DE BUSTAMANTE 2064</t>
+          <t>José Andrés Pacheco de Melo 2084</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>784804268</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -548,16 +548,16 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
+          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -566,19 +566,15 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>-58.406882</v>
+        <v>-58.395656</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.588287</v>
+        <v>-34.590364</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -594,27 +590,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2463</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>7/15/2024</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>795698153</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -624,12 +620,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -642,7 +638,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -651,36 +647,36 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.40589</v>
+        <v>-58.496935</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.584156</v>
+        <v>-34.599084</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>MCAL SOLANO LOPEZ 3110</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -690,7 +686,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>792101640</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -700,12 +696,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Retirar columna. TLC ya traspaso nodo</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -718,7 +714,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -727,46 +723,46 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.498448</v>
+        <v>-58.441405</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.595287</v>
+        <v>-34.594348</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3154</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8/27/2024</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BRAVO, MARIO 853</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>795498456</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -776,41 +772,37 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Sacar la rienda de la plantera</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
         <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.41606</v>
+        <v>-58.483821</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.599935</v>
+        <v>-34.677698</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -822,27 +814,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1871</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>9/5/2024</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bulnes 1810</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>796016024</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -852,16 +844,16 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -870,7 +862,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -879,14 +871,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.413803</v>
+        <v>-58.406585</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.590308</v>
+        <v>-34.592933</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -898,27 +890,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3291</t>
+          <t>1497</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>9/13/2024</t>
+          <t>4/4/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>GUISE 1933</t>
+          <t>SANCHEZ DE BUSTAMANTE 2064</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>796325224</t>
+          <t>784804268</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -933,20 +925,20 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Retirar columna ya traspasaron fuente propia</t>
+          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -955,14 +947,14 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.412544</v>
+        <v>-58.406882</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.590435</v>
+        <v>-34.588287</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -974,27 +966,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3887</t>
+          <t>2463</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>7/15/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4819</t>
+          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>798894281</t>
+          <t>795698153</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1009,7 +1001,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1017,28 +1009,28 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.432085</v>
+        <v>-58.40589</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.60178</v>
+        <v>-34.584156</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1050,27 +1042,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3893</t>
+          <t>2805</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>8/6/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>HERRERA 402</t>
+          <t>MCAL SOLANO LOPEZ 3110</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>798894295</t>
+          <t>792101640</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1085,7 +1077,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Inclinado En el form cargaron foto de otro caso</t>
+          <t>Retirar columna. TLC ya traspaso nodo</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1093,60 +1085,60 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.378613</v>
+        <v>-58.498448</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.6349</v>
+        <v>-34.595287</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>3154</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>8/27/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>José Andrés Pacheco de Melo 2084</t>
+          <t>BRAVO, MARIO 853</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>795498456</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1156,12 +1148,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
+          <t>Sacar la rienda de la plantera</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1169,24 +1161,28 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
       <c r="M10" t="n">
-        <v>-58.395656</v>
+        <v>-58.41606</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.590364</v>
+        <v>-34.599935</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1198,27 +1194,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>798897458</t>
+          <t>1871</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10/15/2024</t>
+          <t>9/5/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Rojas 1091</t>
+          <t>Bulnes 1810</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>798897458</t>
+          <t>796016024</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1233,7 +1229,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Columna fuera de plomo (inclinada)</t>
+          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1241,24 +1237,28 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr"/>
+          <t>Nodo TLC</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M11" t="n">
-        <v>-58.446458</v>
+        <v>-58.413803</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.608741</v>
+        <v>-34.590308</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1270,17 +1270,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3938</t>
+          <t>3291</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>11/5/2024</t>
+          <t>9/13/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2604</t>
+          <t>GUISE 1933</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>799246642</t>
+          <t>796325224</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1305,7 +1305,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Realizar traspasos y retiro de columna vieja</t>
+          <t>Retirar columna ya traspasaron fuente propia</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1313,24 +1313,24 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.426169</v>
+        <v>-58.412544</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.579697</v>
+        <v>-34.590435</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1346,17 +1346,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4025</t>
+          <t>3887</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MEXICO 4249</t>
+          <t>ESTADO DE ISRAEL AV. 4819</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>799981143</t>
+          <t>798894281</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Ver foto, colocar columna para traspasar</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1389,28 +1389,28 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.425997</v>
+        <v>-58.432085</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.620454</v>
+        <v>-34.60178</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1422,27 +1422,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4222</t>
+          <t>3893</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HUMAHUACA 4500</t>
+          <t>HERRERA 402</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>800810078</t>
+          <t>798894295</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1457,7 +1457,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Columna con base corroída/oxidada</t>
+          <t>Inclinado En el form cargaron foto de otro caso</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1475,18 +1475,18 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.428283</v>
+        <v>-58.378613</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.601207</v>
+        <v>-34.6349</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1498,17 +1498,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>4426</t>
+          <t>798897458</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>12/19/2024</t>
+          <t>10/15/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>LORA, FELIX 27</t>
+          <t>Rojas 1091</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1518,7 +1518,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>801768138</t>
+          <t>798897458</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
+          <t>Columna fuera de plomo (inclinada)</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1541,24 +1541,20 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
-        <v>-58.443626</v>
+        <v>-58.446458</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.621032</v>
+        <v>-34.608741</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1574,27 +1570,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>6243</t>
+          <t>3938</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1/30/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>GARCIA, TEODORO 3252</t>
+          <t>GODOY CRUZ 2604</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>779373118</t>
+          <t>799246642</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1609,7 +1605,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Colocar R400 para posterior traspaso</t>
+          <t>Realizar traspasos y retiro de columna vieja</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1617,60 +1613,60 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.450789</v>
+        <v>-58.426169</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.577949</v>
+        <v>-34.579697</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>-51</t>
+          <t>4025</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/5/2024</t>
+          <t>11/12/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CHARCAS /ALT/ 4176</t>
+          <t>MEXICO 4249</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>782773317</t>
+          <t>799981143</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1685,11 +1681,11 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t xml:space="preserve">columna de 114mm de nuestra propiedad que esta quebrada y en mal estado, para remplazar ubicada en CHARCAS 4176 </t>
+          <t>Ver foto, colocar columna para traspasar</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1707,14 +1703,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.421741</v>
+        <v>-58.425997</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.584789</v>
+        <v>-34.620454</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1726,27 +1722,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>-212</t>
+          <t>4222</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>11/28/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>FIGUEROA CNEL APOLINARIO /ALT/ 863</t>
+          <t>HUMAHUACA 4500</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>799485362</t>
+          <t>800810078</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1761,11 +1757,11 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir el traspaso</t>
+          <t>Columna con base corroída/oxidada</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1774,7 +1770,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1783,46 +1779,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.450579</v>
+        <v>-58.428283</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.607673</v>
+        <v>-34.601207</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5884</t>
+          <t>4426</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>12/19/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>OLLEROS 2952</t>
+          <t>LORA, FELIX 27</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>799450967</t>
+          <t>801768138</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1837,11 +1833,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso</t>
+          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1850,7 +1846,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1859,14 +1855,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.447022</v>
+        <v>-58.443626</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.575873</v>
+        <v>-34.621032</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1878,27 +1874,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4528</t>
+          <t>6243</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1/16/2025</t>
+          <t>1/30/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>BARCO CENTENERA DEL 545</t>
+          <t>GARCIA, TEODORO 3252</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>802774521</t>
+          <t>779373118</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1913,7 +1909,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para posterior traspaso</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1926,7 +1922,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1935,46 +1931,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.440625</v>
+        <v>-58.450789</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.625499</v>
+        <v>-34.577949</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>-51</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>4/5/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>CHARCAS /ALT/ 4176</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>782773317</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1984,16 +1980,16 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">columna de 114mm de nuestra propiedad que esta quebrada y en mal estado, para remplazar ubicada en CHARCAS 4176 </t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2011,46 +2007,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.496935</v>
+        <v>-58.421741</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.599084</v>
+        <v>-34.584789</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>-212</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>FIGUEROA CNEL APOLINARIO /ALT/ 863</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>799485362</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2065,11 +2061,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Colocar columna para pedir el traspaso</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2078,7 +2074,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2087,46 +2083,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.400156</v>
+        <v>-58.450579</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.631369</v>
+        <v>-34.607673</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>5884</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>OLLEROS 2952</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>799450967</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,11 +2137,11 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Solo retirar columna ya se realizo traspaso</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2163,14 +2159,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.402062</v>
+        <v>-58.447022</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.635143</v>
+        <v>-34.575873</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2182,27 +2178,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4768</t>
+          <t>4528</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>1/16/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 684</t>
+          <t>BARCO CENTENERA DEL 545</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>802988221</t>
+          <t>802774521</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,7 +2213,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada info para cierre tambien entro como caso 6909</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2239,14 +2235,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.443039</v>
+        <v>-58.440625</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.612262</v>
+        <v>-34.625499</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2258,27 +2254,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4831</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2/4/2025</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MERCEDES 3054</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>803086856</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2289,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Sacar rienda a pique ver con inspector</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2306,55 +2302,55 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.506348</v>
+        <v>-58.400156</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.607461</v>
+        <v>-34.631369</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>6066</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ALBARIÑO 1331</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>803651213</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2365,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Podrida en la base</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2382,7 +2378,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2391,46 +2387,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.496255</v>
+        <v>-58.402062</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.650599</v>
+        <v>-34.635143</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>4768</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>VALLESE, FELIPE 684</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>802988221</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,11 +2441,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Picada info para cierre tambien entro como caso 6909</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2467,14 +2463,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.371855</v>
+        <v>-58.443039</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.646958</v>
+        <v>-34.612262</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2486,27 +2482,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>4831</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>2/4/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>MERCEDES 3054</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>803086856</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,11 +2517,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Sacar rienda a pique ver con inspector</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2539,50 +2535,50 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.403583</v>
+        <v>-58.506348</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.591604</v>
+        <v>-34.607461</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>6066</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>2/26/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>ALBARIÑO 1331</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>803651213</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2592,12 +2588,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+          <t>Podrida en la base</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2610,7 +2606,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2619,46 +2615,46 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.441405</v>
+        <v>-58.496255</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.594348</v>
+        <v>-34.650599</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4572</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 5263</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804309785</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,11 +2669,11 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -2695,14 +2691,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.439791</v>
+        <v>-58.371855</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.61969</v>
+        <v>-34.646958</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2714,27 +2710,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2744,12 +2740,16 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Base picada</t>
+        </is>
+      </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2758,7 +2758,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2767,14 +2767,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.483821</v>
+        <v>-58.403583</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.677698</v>
+        <v>-34.591604</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2786,27 +2786,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5521</t>
+          <t>4572</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>EL PEREGRINO 3115</t>
+          <t>RIVADAVIA AV. 5263</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804569000</t>
+          <t>804309785</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Volvio a ingresar se inclino el poste - caso 6316</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2829,7 +2829,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2839,50 +2839,50 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.485232</v>
+        <v>-58.439791</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.611573</v>
+        <v>-34.61969</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>5521</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>EL PEREGRINO 3115</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>804569000</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2897,7 +2897,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Volvio a ingresar se inclino el poste - caso 6316</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2905,60 +2905,60 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.445131</v>
+        <v>-58.485232</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.572117</v>
+        <v>-34.611573</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Columna corroída en su base</t>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2986,7 +2986,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2995,14 +2995,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.425764</v>
+        <v>-58.445131</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.604359</v>
+        <v>-34.572117</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3014,27 +3014,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Columna corroída en su base</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3071,10 +3071,10 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.439751</v>
+        <v>-58.425764</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.609908</v>
+        <v>-34.604359</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3090,7 +3090,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5632</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 93</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804876047</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3147,14 +3147,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.43607</v>
+        <v>-58.439751</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.61926</v>
+        <v>-34.609908</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3166,7 +3166,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5632</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3176,17 +3176,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>MORENO, JOSE MARIA AV. 93</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>804876047</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3223,14 +3223,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.375515</v>
+        <v>-58.43607</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.634393</v>
+        <v>-34.61926</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3242,27 +3242,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5887</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4/25/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>PALPA 3162</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>805010113</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3277,7 +3277,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Cambiar columna podrida en base.</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3299,46 +3299,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.451203</v>
+        <v>-58.375515</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.576561</v>
+        <v>-34.634393</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>5887</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/25/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>PALPA 3162</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>805010113</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3353,7 +3353,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna podrida en base.</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3375,46 +3375,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.415839</v>
+        <v>-58.451203</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.599291</v>
+        <v>-34.576561</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Migueletes 1326</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3451,46 +3451,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.440177</v>
+        <v>-58.415839</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.56291</v>
+        <v>-34.599291</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>Migueletes 1326</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3505,7 +3505,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3527,46 +3527,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.469148</v>
+        <v>-58.440177</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.687883</v>
+        <v>-34.56291</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3603,14 +3603,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.395063</v>
+        <v>-58.469148</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.606257</v>
+        <v>-34.687883</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3622,7 +3622,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3632,17 +3632,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3665,12 +3665,12 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3679,14 +3679,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.429977</v>
+        <v>-58.395063</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.615514</v>
+        <v>-34.606257</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3708,17 +3708,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3755,14 +3755,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.421623</v>
+        <v>-58.429977</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.614541</v>
+        <v>-34.615514</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3774,27 +3774,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-416</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Paraguay 3765</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>806926557</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3809,7 +3809,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3817,12 +3817,12 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3831,14 +3831,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.416562</v>
+        <v>-58.421623</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.590589</v>
+        <v>-34.614541</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3850,7 +3850,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-416</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3860,17 +3860,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>Paraguay 3765</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>806926557</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3885,7 +3885,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3907,14 +3907,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.429972</v>
+        <v>-58.416562</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.632042</v>
+        <v>-34.590589</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3926,7 +3926,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3936,17 +3936,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3983,26 +3983,26 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.47888</v>
+        <v>-58.429972</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.571108</v>
+        <v>-34.632042</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4012,17 +4012,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4037,7 +4037,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4059,26 +4059,26 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.443196</v>
+        <v>-58.47888</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.618534</v>
+        <v>-34.571108</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-437</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4088,17 +4088,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Cochabamba 4090</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806926861</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4126,7 +4126,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4135,14 +4135,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.422268</v>
+        <v>-58.443196</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.627754</v>
+        <v>-34.618534</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4154,7 +4154,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-438</t>
+          <t>-437</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4164,17 +4164,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Juncal 4565</t>
+          <t>Cochabamba 4090</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806926927</t>
+          <t>806926861</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4189,7 +4189,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4202,7 +4202,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -4211,14 +4211,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.423148</v>
+        <v>-58.422268</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.576964</v>
+        <v>-34.627754</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4230,7 +4230,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>-438</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4240,17 +4240,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>Juncal 4565</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>806926927</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4260,16 +4260,16 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -4287,14 +4287,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.406585</v>
+        <v>-58.423148</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.592933</v>
+        <v>-34.576964</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-25 10:39:06)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P96"/>
+  <dimension ref="A1:P95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7574,27 +7574,27 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>-548</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Sucre 1533</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30326446 </t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -7609,7 +7609,7 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Traspasar red a columna de TLC y Retirar columna quebrada</t>
+          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
         </is>
       </c>
       <c r="I95" t="n">
@@ -7617,7 +7617,7 @@
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
@@ -7631,93 +7631,17 @@
         </is>
       </c>
       <c r="M95" t="n">
-        <v>-58.44649</v>
+        <v>-58.355342</v>
       </c>
       <c r="N95" t="n">
-        <v>-34.558808</v>
+        <v>-34.63565</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P95" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>6917</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>8/12/2025</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>BRIN, MINISTRO 1375</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>808918700</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
-        </is>
-      </c>
-      <c r="I96" t="n">
-        <v>1</v>
-      </c>
-      <c r="J96" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M96" t="n">
-        <v>-58.355342</v>
-      </c>
-      <c r="N96" t="n">
-        <v>-34.63565</v>
-      </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P96" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-26 15:13:42)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -3049,7 +3049,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Columna corroída en su base</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -7194,7 +7194,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>-513</t>
+          <t>7030</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -7204,7 +7204,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Montes de Oca 1809</t>
+          <t>MONTES DE OCA, MANUEL AV. 1809</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -7214,7 +7214,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>808240768</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-29 08:11:54)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -5446,27 +5446,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6168</t>
+          <t>6214</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
+          <t>GONZALEZ, JOAQUIN V. 2308</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807537512</t>
+          <t>807605710</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5489,7 +5489,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5499,50 +5499,50 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.422775</v>
+        <v>-58.497698</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.604135</v>
+        <v>-34.612038</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6214</t>
+          <t>6229</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>GONZALEZ, JOAQUIN V. 2308</t>
+          <t>ALVAREZ THOMAS AV. 309</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807605710</t>
+          <t>807762987</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Reparar rienda </t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5565,7 +5565,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5579,26 +5579,26 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.497698</v>
+        <v>-58.44848</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.612038</v>
+        <v>-34.581338</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6229</t>
+          <t>6228</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5608,7 +5608,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 309</t>
+          <t>NEWBERY, JORGE AV. 3416</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5618,7 +5618,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>807762987</t>
+          <t>807762990</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reparar rienda </t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5655,26 +5655,26 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.44848</v>
+        <v>-58.448496</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.581338</v>
+        <v>-34.58182</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6076</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5684,17 +5684,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE AV. 3416</t>
+          <t>MATHEU 727</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>807762990</t>
+          <t>807763063</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5717,60 +5717,60 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.448496</v>
+        <v>-58.400169</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.58182</v>
+        <v>-34.617784</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6076</t>
+          <t>6249</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/25/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>MATHEU 727</t>
+          <t>GODOY CRUZ 2696</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>807763063</t>
+          <t>807789682</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5785,7 +5785,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
+          <t>Inclinada posible cambio</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5798,7 +5798,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -5807,14 +5807,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.400169</v>
+        <v>-58.425296</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.617784</v>
+        <v>-34.578706</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5826,27 +5826,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6249</t>
+          <t>6271</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>6/25/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2696</t>
+          <t>ARGERICH 740</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>807789682</t>
+          <t>807789686</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Inclinada posible cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5883,46 +5883,46 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.425296</v>
+        <v>-58.474467</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.578706</v>
+        <v>-34.624161</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6271</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>ARGERICH 740</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>807789686</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5945,7 +5945,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5959,46 +5959,46 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.474467</v>
+        <v>-58.432644</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.624161</v>
+        <v>-34.595434</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Colocar columna para pedir traspaso</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6021,12 +6021,12 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -6035,14 +6035,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.432644</v>
+        <v>-58.401827</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.595434</v>
+        <v>-34.617667</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6054,27 +6054,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6284</t>
+          <t>6298</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>CHILE 2561</t>
+          <t>RIVERA INDARTE AV. 1406</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>807851584</t>
+          <t>807877127</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6089,7 +6089,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso</t>
+          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6102,7 +6102,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -6111,14 +6111,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.401827</v>
+        <v>-58.450359</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.617667</v>
+        <v>-34.643582</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6130,7 +6130,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6298</t>
+          <t>6308</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6140,17 +6140,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>RIVERA INDARTE AV. 1406</t>
+          <t>Guayaquil 637</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>807877127</t>
+          <t>807896343</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6165,7 +6165,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6187,10 +6187,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.450359</v>
+        <v>-58.437378</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.643582</v>
+        <v>-34.62116</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6206,27 +6206,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6308</t>
+          <t>6330</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Guayaquil 637</t>
+          <t>REPUBLICA DE LA INDIA 3106</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>807896343</t>
+          <t>807965776</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6241,7 +6241,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada e inclinada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6263,14 +6263,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.437378</v>
+        <v>-58.413941</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.62116</v>
+        <v>-34.57698</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6282,7 +6282,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6330</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6292,7 +6292,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>REPUBLICA DE LA INDIA 3106</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -6302,7 +6302,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>807965776</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6317,15 +6317,15 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada e inclinada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -6335,18 +6335,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.413941</v>
+        <v>-58.405749</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.57698</v>
+        <v>-34.58224</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6358,27 +6358,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6393,15 +6393,15 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -6415,26 +6415,26 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.405749</v>
+        <v>-58.473179</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.58224</v>
+        <v>-34.629138</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>-502</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6444,17 +6444,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>Tagle 2562</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>808036198</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6469,7 +6469,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Colocar columna para pedir traspaso nodo teco</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6477,60 +6477,60 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.473179</v>
+        <v>-58.400188</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.629138</v>
+        <v>-34.583882</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-502</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Tagle 2562</t>
+          <t>GUARDIA VIEJA 4377</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808036198</t>
+          <t>808099347</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6545,7 +6545,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso nodo teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6558,7 +6558,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
@@ -6567,14 +6567,14 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.400188</v>
+        <v>-58.426322</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.583882</v>
+        <v>-34.600097</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6586,7 +6586,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>6383</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6596,17 +6596,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>GUARDIA VIEJA 4377</t>
+          <t>FALCON, RAMON L.,CNEL. 1411</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808099347</t>
+          <t>808099320</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6643,14 +6643,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.426322</v>
+        <v>-58.448523</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.600097</v>
+        <v>-34.62452</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6662,17 +6662,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6383</t>
+          <t>-506</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1411</t>
+          <t>Espinosa 591</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -6682,7 +6682,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808099320</t>
+          <t>808150511</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6710,7 +6710,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -6719,10 +6719,10 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.448523</v>
+        <v>-58.449</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.62452</v>
+        <v>-34.616077</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -6738,27 +6738,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>-506</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Espinosa 591</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808150511</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6786,23 +6786,23 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.449</v>
+        <v>-58.363292</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.616077</v>
+        <v>-34.642869</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -6814,17 +6814,17 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>7030</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>MONTES DE OCA, MANUEL AV. 1809</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -6834,7 +6834,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>ICD30501825</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6849,7 +6849,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6867,14 +6867,14 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.363292</v>
+        <v>-58.372941</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.642869</v>
+        <v>-34.648341</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -6890,27 +6890,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>7030</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 1809</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>ICD30501825</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6925,7 +6925,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6947,14 +6947,14 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.372941</v>
+        <v>-58.432805</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.648341</v>
+        <v>-34.574345</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -6966,27 +6966,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>-517</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Av Dorrego 2721</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>808373635</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -7001,7 +7001,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7023,14 +7023,14 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.432805</v>
+        <v>-58.384097</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.574345</v>
+        <v>-34.598913</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
@@ -7042,27 +7042,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7077,7 +7077,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7099,46 +7099,46 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.384097</v>
+        <v>-58.513643</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.598913</v>
+        <v>-34.594169</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>-531</t>
+          <t>6558</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4632</t>
+          <t>NAZCA 5168</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>808530239</t>
+          <t>808703877</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7153,7 +7153,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
+          <t>Aplomar y corregir caja de empalme colgando</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -7161,7 +7161,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
@@ -7175,10 +7175,10 @@
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.513643</v>
+        <v>-58.505593</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.594169</v>
+        <v>-34.582601</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
@@ -7194,17 +7194,17 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>6558</t>
+          <t>5894</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>NAZCA 5168</t>
+          <t>ALBARELLOS AV. 3100</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -7214,7 +7214,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>808703877</t>
+          <t>ICD30340076</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -7224,20 +7224,20 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Transito</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Aplomar y corregir caja de empalme colgando</t>
+          <t>QAP fotos del gcba tenia las incorrectas</t>
         </is>
       </c>
       <c r="I90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
@@ -7247,14 +7247,14 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.505593</v>
+        <v>-58.512533</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.582601</v>
+        <v>-34.579243</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-30 08:22:29)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P91"/>
+  <dimension ref="A1:P90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7194,27 +7194,27 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>5894</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>ALBARELLOS AV. 3100</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>ICD30340076</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -7224,20 +7224,20 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>Pendiente de Transito</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>QAP fotos del gcba tenia las incorrectas</t>
+          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
         </is>
       </c>
       <c r="I90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
@@ -7247,97 +7247,21 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.512533</v>
+        <v>-58.355342</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.579243</v>
+        <v>-34.63565</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>6917</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>8/12/2025</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>BRIN, MINISTRO 1375</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>808918700</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
-        </is>
-      </c>
-      <c r="I91" t="n">
-        <v>1</v>
-      </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M91" t="n">
-        <v>-58.355342</v>
-      </c>
-      <c r="N91" t="n">
-        <v>-34.63565</v>
-      </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P91" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-02 08:02:10)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P90"/>
+  <dimension ref="A1:P89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2182,17 +2182,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4768</t>
+          <t>4696</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>2/10/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 684</t>
+          <t>YERBAL 489</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>802988221</t>
+          <t>803607520</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada info para cierre tambien entro como caso 6909</t>
+          <t>Desmonte de columna ya traspasaron nodo</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -2239,14 +2239,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.443039</v>
+        <v>-58.438053</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.612262</v>
+        <v>-34.617481</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2258,17 +2258,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4696</t>
+          <t>4938</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2/10/2025</t>
+          <t>2/14/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>YERBAL 489</t>
+          <t>CHACO 195</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2278,7 +2278,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>803607520</t>
+          <t>803607699</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron nodo</t>
+          <t>Desmontar columna personal propio traspaso nodo</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2315,10 +2315,10 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.438053</v>
+        <v>-58.431522</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.617481</v>
+        <v>-34.617523</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2334,27 +2334,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>6066</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2/14/2025</t>
+          <t>2/26/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CHACO 195</t>
+          <t>ALBARIÑO 1331</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>803607699</t>
+          <t>803651213</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Desmontar columna personal propio traspaso nodo</t>
+          <t>Podrida en la base</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2382,7 +2382,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2391,46 +2391,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.431522</v>
+        <v>-58.496255</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.617523</v>
+        <v>-34.650599</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6066</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>ALBARIÑO 1331</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>803651213</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,11 +2445,11 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Podrida en la base</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2467,36 +2467,36 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.496255</v>
+        <v>-58.371855</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.650599</v>
+        <v>-34.646958</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2543,14 +2543,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.371855</v>
+        <v>-58.403583</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.646958</v>
+        <v>-34.591604</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2562,27 +2562,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2592,16 +2592,16 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2610,7 +2610,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2619,14 +2619,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.403583</v>
+        <v>-58.441405</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.591604</v>
+        <v>-34.594348</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2638,7 +2638,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2648,17 +2648,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2671,11 +2671,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
-        </is>
-      </c>
+      <c r="H30" t="inlineStr"/>
       <c r="I30" t="n">
         <v>1</v>
       </c>
@@ -2695,14 +2691,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.441405</v>
+        <v>-58.483821</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.594348</v>
+        <v>-34.677698</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2714,27 +2710,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2744,10 +2740,14 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+        </is>
+      </c>
       <c r="I31" t="n">
         <v>1</v>
       </c>
@@ -2767,14 +2767,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.483821</v>
+        <v>-58.445131</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.677698</v>
+        <v>-34.572117</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2786,27 +2786,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2834,7 +2834,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2843,14 +2843,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.445131</v>
+        <v>-58.425764</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.572117</v>
+        <v>-34.604359</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2862,27 +2862,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2897,7 +2897,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2905,7 +2905,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2919,10 +2919,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.425764</v>
+        <v>-58.439751</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.604359</v>
+        <v>-34.609908</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2938,7 +2938,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>5632</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>MORENO, JOSE MARIA AV. 93</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2958,7 +2958,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>804876047</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2995,14 +2995,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.439751</v>
+        <v>-58.43607</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.609908</v>
+        <v>-34.61926</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3014,7 +3014,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5632</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 93</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804876047</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3071,14 +3071,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.43607</v>
+        <v>-58.375515</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.61926</v>
+        <v>-34.634393</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3090,27 +3090,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3147,14 +3147,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.375515</v>
+        <v>-58.415839</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.634393</v>
+        <v>-34.599291</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3166,27 +3166,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>Migueletes 1326</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3223,46 +3223,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.415839</v>
+        <v>-58.440177</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.599291</v>
+        <v>-34.56291</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Migueletes 1326</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3277,7 +3277,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3299,46 +3299,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.440177</v>
+        <v>-58.469148</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.56291</v>
+        <v>-34.687883</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3353,7 +3353,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3366,7 +3366,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3375,14 +3375,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.469148</v>
+        <v>-58.395063</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.687883</v>
+        <v>-34.606257</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3394,7 +3394,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3404,17 +3404,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3429,7 +3429,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3437,12 +3437,12 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3451,14 +3451,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.395063</v>
+        <v>-58.429977</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.606257</v>
+        <v>-34.615514</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3470,7 +3470,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3480,17 +3480,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3527,14 +3527,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.429977</v>
+        <v>-58.421623</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.615514</v>
+        <v>-34.614541</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3546,27 +3546,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>-416</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>Paraguay 3765</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>806926557</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3589,12 +3589,12 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3603,14 +3603,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.421623</v>
+        <v>-58.416562</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.614541</v>
+        <v>-34.590589</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3622,7 +3622,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-416</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3632,17 +3632,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Paraguay 3765</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>806926557</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3670,7 +3670,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3679,14 +3679,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.416562</v>
+        <v>-58.429972</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.590589</v>
+        <v>-34.632042</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3708,17 +3708,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3733,7 +3733,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3755,26 +3755,26 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.429972</v>
+        <v>-58.47888</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.632042</v>
+        <v>-34.571108</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3784,17 +3784,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3809,7 +3809,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3831,26 +3831,26 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.47888</v>
+        <v>-58.443196</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.571108</v>
+        <v>-34.618534</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>-437</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3860,17 +3860,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>Cochabamba 4090</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>806926861</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3885,7 +3885,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3907,14 +3907,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.443196</v>
+        <v>-58.422268</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.618534</v>
+        <v>-34.627754</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3926,7 +3926,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-437</t>
+          <t>-438</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3936,17 +3936,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Cochabamba 4090</t>
+          <t>Juncal 4565</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806926861</t>
+          <t>806926927</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3974,7 +3974,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3983,14 +3983,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.422268</v>
+        <v>-58.423148</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.627754</v>
+        <v>-34.576964</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -4002,7 +4002,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-438</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4012,17 +4012,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Juncal 4565</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806926927</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4032,16 +4032,16 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4059,14 +4059,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.423148</v>
+        <v>-58.406585</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.576964</v>
+        <v>-34.592933</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4078,7 +4078,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>-445</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4088,17 +4088,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>Joaquin V Gonzalez 4410</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>806945058</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4108,16 +4108,16 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -4126,55 +4126,55 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.406585</v>
+        <v>-58.51232</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.592933</v>
+        <v>-34.595637</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-445</t>
+          <t>5937</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4410</t>
+          <t>MONROE 4833</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806945058</t>
+          <t>807044121</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4189,7 +4189,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4207,18 +4207,18 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.51232</v>
+        <v>-58.483104</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.595637</v>
+        <v>-34.572353</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4230,27 +4230,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5937</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>MONROE 4833</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807044121</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4265,7 +4265,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4273,7 +4273,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4283,14 +4283,14 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.483104</v>
+        <v>-58.483927</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.572353</v>
+        <v>-34.570689</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4306,17 +4306,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4326,7 +4326,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4341,7 +4341,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4349,7 +4349,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4359,18 +4359,18 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.483927</v>
+        <v>-58.492605</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.570689</v>
+        <v>-34.581454</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4382,7 +4382,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4392,17 +4392,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4439,26 +4439,26 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.492605</v>
+        <v>-58.467789</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.581454</v>
+        <v>-34.68463</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>-451</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4468,17 +4468,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>Uriarte 2426</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>807044071</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4493,7 +4493,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4506,7 +4506,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -4515,14 +4515,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.467789</v>
+        <v>-58.423551</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.68463</v>
+        <v>-34.581258</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4534,27 +4534,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-451</t>
+          <t>5947</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Uriarte 2426</t>
+          <t>CAFAYATE 5007</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807044071</t>
+          <t>807129336</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Columna inclinada Columna con base corroída oxidada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4582,7 +4582,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -4591,14 +4591,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.423551</v>
+        <v>-58.468182</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.581258</v>
+        <v>-34.685231</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4610,7 +4610,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5947</t>
+          <t>5948</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4620,7 +4620,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CAFAYATE 5007</t>
+          <t>MURGUIONDO 3990</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4630,7 +4630,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807129336</t>
+          <t>807129347</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4645,7 +4645,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Columna inclinada Columna con base corroída oxidada</t>
+          <t>COLUMNA INCLINADA</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4663,14 +4663,14 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.468182</v>
+        <v>-58.477944</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.685231</v>
+        <v>-34.675149</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4686,7 +4686,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5948</t>
+          <t>5954</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4696,17 +4696,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>MURGUIONDO 3990</t>
+          <t>YAPEYU 938</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807129347</t>
+          <t>807129372</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4721,7 +4721,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>COLUMNA INCLINADA</t>
+          <t>Columna Picada, tambien resolver cables panseados y cortados reclaman ambas cosas</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4739,14 +4739,14 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.477944</v>
+        <v>-58.4212</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.675149</v>
+        <v>-34.623575</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4762,27 +4762,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5954</t>
+          <t>5973</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>YAPEYU 938</t>
+          <t>PALOS 432</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807129372</t>
+          <t>807168105</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4797,7 +4797,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Columna Picada, tambien resolver cables panseados y cortados reclaman ambas cosas</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4819,14 +4819,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.4212</v>
+        <v>-58.362579</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.623575</v>
+        <v>-34.635096</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4838,7 +4838,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>5973</t>
+          <t>3715</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4848,17 +4848,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>PALOS 432</t>
+          <t>EL SERENO 358</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807168105</t>
+          <t>807168098</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4873,7 +4873,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4881,7 +4881,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4891,30 +4891,30 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.362579</v>
+        <v>-58.487371</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.635096</v>
+        <v>-34.640099</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>3715</t>
+          <t>5997</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4924,17 +4924,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>EL SERENO 358</t>
+          <t>MARMOL, JOSE 256</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807168098</t>
+          <t>807187768</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada coincide con reclamo de cables con mismo numero de caso</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4957,7 +4957,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4967,30 +4967,30 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.487371</v>
+        <v>-58.425845</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.640099</v>
+        <v>-34.616562</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>5997</t>
+          <t>807187860</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5000,7 +5000,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 256</t>
+          <t>San Juan 3960</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -5010,7 +5010,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807187768</t>
+          <t>807187860</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables con mismo numero de caso</t>
+          <t>Colocar columna contactar a Matias Tapia 1171744701 por si hay alguna duda o problema que surja en el momento ya que es para posterior tendido de ftth</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5047,14 +5047,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.425845</v>
+        <v>-58.420909</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.616562</v>
+        <v>-34.626221</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5066,17 +5066,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>807187860</t>
+          <t>6004</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>San Juan 3960</t>
+          <t>MAZA 181</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5086,7 +5086,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807187860</t>
+          <t>807215439</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Colocar columna contactar a Matias Tapia 1171744701 por si hay alguna duda o problema que surja en el momento ya que es para posterior tendido de ftth</t>
+          <t>Picada coincide con reclamo de cables</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5123,14 +5123,14 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.420909</v>
+        <v>-58.416477</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.626221</v>
+        <v>-34.61303</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5142,7 +5142,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6004</t>
+          <t>6007</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5152,7 +5152,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MAZA 181</t>
+          <t>HUMAHUACA 4435</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5162,7 +5162,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807215439</t>
+          <t>807215448</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5199,10 +5199,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.416477</v>
+        <v>-58.427424</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.61303</v>
+        <v>-34.601217</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5218,7 +5218,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6007</t>
+          <t>6008</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5228,7 +5228,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>HUMAHUACA 4435</t>
+          <t>ESTADO DE ISRAEL AV. 4306</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807215448</t>
+          <t>807215455</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5253,7 +5253,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5275,10 +5275,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.427424</v>
+        <v>-58.426665</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.601217</v>
+        <v>-34.598019</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5294,7 +5294,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6008</t>
+          <t>6010</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5304,7 +5304,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4306</t>
+          <t>ESTADO DE PALESTINA 771</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5314,7 +5314,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807215455</t>
+          <t>807215458</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5329,7 +5329,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada y mal ubicada coincide con reclamo de cables</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5351,10 +5351,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.426665</v>
+        <v>-58.425478</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.598019</v>
+        <v>-34.601865</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5370,27 +5370,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6010</t>
+          <t>6214</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>ESTADO DE PALESTINA 771</t>
+          <t>GONZALEZ, JOAQUIN V. 2308</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807215458</t>
+          <t>807605710</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada y mal ubicada coincide con reclamo de cables</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5413,7 +5413,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5423,50 +5423,50 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.425478</v>
+        <v>-58.497698</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.601865</v>
+        <v>-34.612038</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6214</t>
+          <t>6229</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>GONZALEZ, JOAQUIN V. 2308</t>
+          <t>ALVAREZ THOMAS AV. 309</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807605710</t>
+          <t>807762987</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Reparar rienda </t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5489,7 +5489,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -5503,26 +5503,26 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.497698</v>
+        <v>-58.44848</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.612038</v>
+        <v>-34.581338</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6229</t>
+          <t>6228</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5532,7 +5532,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 309</t>
+          <t>NEWBERY, JORGE AV. 3416</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5542,7 +5542,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807762987</t>
+          <t>807762990</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reparar rienda </t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5579,26 +5579,26 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.44848</v>
+        <v>-58.448496</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.581338</v>
+        <v>-34.58182</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6076</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5608,17 +5608,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE AV. 3416</t>
+          <t>MATHEU 727</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>807762990</t>
+          <t>807763063</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5641,60 +5641,60 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.448496</v>
+        <v>-58.400169</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.58182</v>
+        <v>-34.617784</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6076</t>
+          <t>6249</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/25/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>MATHEU 727</t>
+          <t>GODOY CRUZ 2696</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>807763063</t>
+          <t>807789682</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
+          <t>Inclinada posible cambio</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5722,7 +5722,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -5731,14 +5731,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.400169</v>
+        <v>-58.425296</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.617784</v>
+        <v>-34.578706</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5750,27 +5750,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6249</t>
+          <t>6271</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>6/25/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2696</t>
+          <t>ARGERICH 740</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>807789682</t>
+          <t>807789686</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5785,7 +5785,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Inclinada posible cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5807,46 +5807,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.425296</v>
+        <v>-58.474467</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.578706</v>
+        <v>-34.624161</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6271</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ARGERICH 740</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>807789686</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5869,7 +5869,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5883,46 +5883,46 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.474467</v>
+        <v>-58.432644</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.624161</v>
+        <v>-34.595434</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Colocar columna para pedir traspaso</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5945,12 +5945,12 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -5959,14 +5959,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.432644</v>
+        <v>-58.401827</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.595434</v>
+        <v>-34.617667</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5978,27 +5978,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6284</t>
+          <t>6298</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>CHILE 2561</t>
+          <t>RIVERA INDARTE AV. 1406</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>807851584</t>
+          <t>807877127</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso</t>
+          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6026,7 +6026,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -6035,14 +6035,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.401827</v>
+        <v>-58.450359</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.617667</v>
+        <v>-34.643582</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6054,7 +6054,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6298</t>
+          <t>6308</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6064,17 +6064,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>RIVERA INDARTE AV. 1406</t>
+          <t>Guayaquil 637</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>807877127</t>
+          <t>807896343</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6089,7 +6089,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6111,10 +6111,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.450359</v>
+        <v>-58.437378</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.643582</v>
+        <v>-34.62116</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6130,27 +6130,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6308</t>
+          <t>6330</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Guayaquil 637</t>
+          <t>REPUBLICA DE LA INDIA 3106</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>807896343</t>
+          <t>807965776</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6165,7 +6165,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada e inclinada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6187,14 +6187,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.437378</v>
+        <v>-58.413941</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.62116</v>
+        <v>-34.57698</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6206,7 +6206,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6330</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6216,7 +6216,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>REPUBLICA DE LA INDIA 3106</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -6226,7 +6226,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>807965776</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6241,15 +6241,15 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada e inclinada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I77" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -6259,18 +6259,18 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.413941</v>
+        <v>-58.405749</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.57698</v>
+        <v>-34.58224</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6282,27 +6282,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6317,15 +6317,15 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -6339,26 +6339,26 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.405749</v>
+        <v>-58.473179</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.58224</v>
+        <v>-34.629138</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>-502</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6368,17 +6368,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>Tagle 2562</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>808036198</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6393,7 +6393,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Colocar columna para pedir traspaso nodo teco</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6401,60 +6401,60 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.473179</v>
+        <v>-58.400188</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.629138</v>
+        <v>-34.583882</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-502</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Tagle 2562</t>
+          <t>GUARDIA VIEJA 4377</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808036198</t>
+          <t>808099347</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6469,7 +6469,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso nodo teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6482,7 +6482,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
@@ -6491,14 +6491,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.400188</v>
+        <v>-58.426322</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.583882</v>
+        <v>-34.600097</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6510,7 +6510,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>6383</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6520,17 +6520,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>GUARDIA VIEJA 4377</t>
+          <t>FALCON, RAMON L.,CNEL. 1411</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808099347</t>
+          <t>808099320</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6567,14 +6567,14 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.426322</v>
+        <v>-58.448523</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.600097</v>
+        <v>-34.62452</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6586,17 +6586,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6383</t>
+          <t>-506</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1411</t>
+          <t>Espinosa 591</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -6606,7 +6606,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808099320</t>
+          <t>808150511</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6634,7 +6634,7 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
@@ -6643,10 +6643,10 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.448523</v>
+        <v>-58.449</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.62452</v>
+        <v>-34.616077</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -6662,27 +6662,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-506</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Espinosa 591</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808150511</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6710,23 +6710,23 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.449</v>
+        <v>-58.363292</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.616077</v>
+        <v>-34.642869</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6738,17 +6738,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>7030</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>MONTES DE OCA, MANUEL AV. 1809</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -6758,7 +6758,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>ICD30501825</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6791,14 +6791,14 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.363292</v>
+        <v>-58.372941</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.642869</v>
+        <v>-34.648341</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -6814,27 +6814,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7030</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 1809</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>ICD30501825</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6849,7 +6849,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6871,14 +6871,14 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.372941</v>
+        <v>-58.432805</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.648341</v>
+        <v>-34.574345</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -6890,27 +6890,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>-517</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Av Dorrego 2721</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>808373635</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6925,7 +6925,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6947,14 +6947,14 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.432805</v>
+        <v>-58.384097</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.574345</v>
+        <v>-34.598913</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -6966,27 +6966,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -7001,7 +7001,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7023,46 +7023,46 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.384097</v>
+        <v>-58.513643</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.598913</v>
+        <v>-34.594169</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>-531</t>
+          <t>6558</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4632</t>
+          <t>NAZCA 5168</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>808530239</t>
+          <t>808703877</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7077,7 +7077,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
+          <t>Aplomar y corregir caja de empalme colgando</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7085,7 +7085,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -7099,10 +7099,10 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.513643</v>
+        <v>-58.505593</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.594169</v>
+        <v>-34.582601</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
@@ -7118,27 +7118,27 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>6558</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>NAZCA 5168</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>808703877</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7153,7 +7153,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Aplomar y corregir caja de empalme colgando</t>
+          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -7161,7 +7161,7 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
@@ -7175,93 +7175,17 @@
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.505593</v>
+        <v>-58.355342</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.582601</v>
+        <v>-34.63565</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>6917</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>8/12/2025</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>BRIN, MINISTRO 1375</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>808918700</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
-        </is>
-      </c>
-      <c r="I90" t="n">
-        <v>1</v>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M90" t="n">
-        <v>-58.355342</v>
-      </c>
-      <c r="N90" t="n">
-        <v>-34.63565</v>
-      </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P90" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-02 08:13:00)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P89"/>
+  <dimension ref="A1:P88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2938,7 +2938,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5632</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2948,17 +2948,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 93</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804876047</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2981,7 +2981,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2995,14 +2995,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.43607</v>
+        <v>-58.375515</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.61926</v>
+        <v>-34.634393</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3014,27 +3014,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3071,14 +3071,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.375515</v>
+        <v>-58.415839</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.634393</v>
+        <v>-34.599291</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3090,27 +3090,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>Migueletes 1326</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3147,46 +3147,46 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.415839</v>
+        <v>-58.440177</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.599291</v>
+        <v>-34.56291</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Migueletes 1326</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3223,46 +3223,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.440177</v>
+        <v>-58.469148</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.56291</v>
+        <v>-34.687883</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3277,7 +3277,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3290,7 +3290,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3299,14 +3299,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.469148</v>
+        <v>-58.395063</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.687883</v>
+        <v>-34.606257</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3318,7 +3318,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3328,17 +3328,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3353,7 +3353,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3361,12 +3361,12 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3375,14 +3375,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.395063</v>
+        <v>-58.429977</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.606257</v>
+        <v>-34.615514</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3394,7 +3394,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3404,17 +3404,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3451,14 +3451,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.429977</v>
+        <v>-58.421623</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.615514</v>
+        <v>-34.614541</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3470,27 +3470,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>-416</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>Paraguay 3765</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>806926557</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3505,7 +3505,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3513,12 +3513,12 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3527,14 +3527,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.421623</v>
+        <v>-58.416562</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.614541</v>
+        <v>-34.590589</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3546,7 +3546,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-416</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3556,17 +3556,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Paraguay 3765</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>806926557</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3603,14 +3603,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.416562</v>
+        <v>-58.429972</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.590589</v>
+        <v>-34.632042</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3622,7 +3622,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3632,17 +3632,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3679,26 +3679,26 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.429972</v>
+        <v>-58.47888</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.632042</v>
+        <v>-34.571108</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3708,17 +3708,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3733,7 +3733,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3755,26 +3755,26 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.47888</v>
+        <v>-58.443196</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.571108</v>
+        <v>-34.618534</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>-437</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3784,17 +3784,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>Cochabamba 4090</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>806926861</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3809,7 +3809,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3822,7 +3822,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3831,14 +3831,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.443196</v>
+        <v>-58.422268</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.618534</v>
+        <v>-34.627754</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3850,7 +3850,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-437</t>
+          <t>-438</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3860,17 +3860,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Cochabamba 4090</t>
+          <t>Juncal 4565</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806926861</t>
+          <t>806926927</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3885,7 +3885,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3907,14 +3907,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.422268</v>
+        <v>-58.423148</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.627754</v>
+        <v>-34.576964</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3926,7 +3926,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-438</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3936,17 +3936,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Juncal 4565</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806926927</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3956,16 +3956,16 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3983,14 +3983,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.423148</v>
+        <v>-58.406585</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.576964</v>
+        <v>-34.592933</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -4002,7 +4002,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>-445</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4012,17 +4012,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>Joaquin V Gonzalez 4410</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>806945058</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4032,16 +4032,16 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4050,55 +4050,55 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.406585</v>
+        <v>-58.51232</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.592933</v>
+        <v>-34.595637</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-445</t>
+          <t>5937</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4410</t>
+          <t>MONROE 4833</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806945058</t>
+          <t>807044121</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4131,18 +4131,18 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.51232</v>
+        <v>-58.483104</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.595637</v>
+        <v>-34.572353</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4154,27 +4154,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5937</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>MONROE 4833</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807044121</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4189,7 +4189,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4197,7 +4197,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -4207,14 +4207,14 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.483104</v>
+        <v>-58.483927</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.572353</v>
+        <v>-34.570689</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4230,17 +4230,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4250,7 +4250,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4265,7 +4265,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4273,7 +4273,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4283,18 +4283,18 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.483927</v>
+        <v>-58.492605</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.570689</v>
+        <v>-34.581454</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4306,7 +4306,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4316,17 +4316,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4363,26 +4363,26 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.492605</v>
+        <v>-58.467789</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.581454</v>
+        <v>-34.68463</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>-451</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4392,17 +4392,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>Uriarte 2426</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>807044071</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4417,7 +4417,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4430,7 +4430,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4439,14 +4439,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.467789</v>
+        <v>-58.423551</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.68463</v>
+        <v>-34.581258</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4458,27 +4458,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-451</t>
+          <t>5947</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Uriarte 2426</t>
+          <t>CAFAYATE 5007</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807044071</t>
+          <t>807129336</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4493,7 +4493,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Columna inclinada Columna con base corroída oxidada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4506,7 +4506,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -4515,14 +4515,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.423551</v>
+        <v>-58.468182</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.581258</v>
+        <v>-34.685231</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4534,7 +4534,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5947</t>
+          <t>5948</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4544,7 +4544,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>CAFAYATE 5007</t>
+          <t>MURGUIONDO 3990</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4554,7 +4554,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807129336</t>
+          <t>807129347</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Columna inclinada Columna con base corroída oxidada</t>
+          <t>COLUMNA INCLINADA</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4587,14 +4587,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.468182</v>
+        <v>-58.477944</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.685231</v>
+        <v>-34.675149</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4610,7 +4610,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5948</t>
+          <t>5954</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4620,17 +4620,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>MURGUIONDO 3990</t>
+          <t>YAPEYU 938</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807129347</t>
+          <t>807129372</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4645,7 +4645,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>COLUMNA INCLINADA</t>
+          <t>Columna Picada, tambien resolver cables panseados y cortados reclaman ambas cosas</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4663,14 +4663,14 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.477944</v>
+        <v>-58.4212</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.675149</v>
+        <v>-34.623575</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4686,27 +4686,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5954</t>
+          <t>5973</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>YAPEYU 938</t>
+          <t>PALOS 432</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807129372</t>
+          <t>807168105</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4721,7 +4721,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Columna Picada, tambien resolver cables panseados y cortados reclaman ambas cosas</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4743,14 +4743,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.4212</v>
+        <v>-58.362579</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.623575</v>
+        <v>-34.635096</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4762,7 +4762,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5973</t>
+          <t>3715</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4772,17 +4772,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>PALOS 432</t>
+          <t>EL SERENO 358</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807168105</t>
+          <t>807168098</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4797,7 +4797,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4805,7 +4805,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4815,30 +4815,30 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.362579</v>
+        <v>-58.487371</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.635096</v>
+        <v>-34.640099</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>3715</t>
+          <t>5997</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4848,17 +4848,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>EL SERENO 358</t>
+          <t>MARMOL, JOSE 256</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807168098</t>
+          <t>807187768</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4873,7 +4873,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada coincide con reclamo de cables con mismo numero de caso</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4881,7 +4881,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4891,30 +4891,30 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.487371</v>
+        <v>-58.425845</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.640099</v>
+        <v>-34.616562</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>5997</t>
+          <t>807187860</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4924,7 +4924,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 256</t>
+          <t>San Juan 3960</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4934,7 +4934,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807187768</t>
+          <t>807187860</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables con mismo numero de caso</t>
+          <t>Colocar columna contactar a Matias Tapia 1171744701 por si hay alguna duda o problema que surja en el momento ya que es para posterior tendido de ftth</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4971,14 +4971,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.425845</v>
+        <v>-58.420909</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.616562</v>
+        <v>-34.626221</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4990,17 +4990,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>807187860</t>
+          <t>6004</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>San Juan 3960</t>
+          <t>MAZA 181</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -5010,7 +5010,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807187860</t>
+          <t>807215439</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Colocar columna contactar a Matias Tapia 1171744701 por si hay alguna duda o problema que surja en el momento ya que es para posterior tendido de ftth</t>
+          <t>Picada coincide con reclamo de cables</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5047,14 +5047,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.420909</v>
+        <v>-58.416477</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.626221</v>
+        <v>-34.61303</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5066,7 +5066,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6004</t>
+          <t>6007</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5076,7 +5076,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>MAZA 181</t>
+          <t>HUMAHUACA 4435</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5086,7 +5086,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807215439</t>
+          <t>807215448</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5123,10 +5123,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.416477</v>
+        <v>-58.427424</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.61303</v>
+        <v>-34.601217</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5142,7 +5142,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6007</t>
+          <t>6008</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5152,7 +5152,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>HUMAHUACA 4435</t>
+          <t>ESTADO DE ISRAEL AV. 4306</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5162,7 +5162,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807215448</t>
+          <t>807215455</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5177,7 +5177,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5199,10 +5199,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.427424</v>
+        <v>-58.426665</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.601217</v>
+        <v>-34.598019</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5218,7 +5218,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6008</t>
+          <t>6010</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5228,7 +5228,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4306</t>
+          <t>ESTADO DE PALESTINA 771</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807215455</t>
+          <t>807215458</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5253,7 +5253,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada y mal ubicada coincide con reclamo de cables</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5275,10 +5275,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.426665</v>
+        <v>-58.425478</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.598019</v>
+        <v>-34.601865</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5294,27 +5294,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6010</t>
+          <t>6214</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>ESTADO DE PALESTINA 771</t>
+          <t>GONZALEZ, JOAQUIN V. 2308</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807215458</t>
+          <t>807605710</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5329,7 +5329,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada y mal ubicada coincide con reclamo de cables</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5337,7 +5337,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5347,50 +5347,50 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.425478</v>
+        <v>-58.497698</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.601865</v>
+        <v>-34.612038</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6214</t>
+          <t>6229</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>GONZALEZ, JOAQUIN V. 2308</t>
+          <t>ALVAREZ THOMAS AV. 309</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807605710</t>
+          <t>807762987</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Reparar rienda </t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5413,7 +5413,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -5427,26 +5427,26 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.497698</v>
+        <v>-58.44848</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.612038</v>
+        <v>-34.581338</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6229</t>
+          <t>6228</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 309</t>
+          <t>NEWBERY, JORGE AV. 3416</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5466,7 +5466,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807762987</t>
+          <t>807762990</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reparar rienda </t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5503,26 +5503,26 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.44848</v>
+        <v>-58.448496</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.581338</v>
+        <v>-34.58182</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6076</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5532,17 +5532,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE AV. 3416</t>
+          <t>MATHEU 727</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807762990</t>
+          <t>807763063</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5565,60 +5565,60 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.448496</v>
+        <v>-58.400169</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.58182</v>
+        <v>-34.617784</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6076</t>
+          <t>6249</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/25/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>MATHEU 727</t>
+          <t>GODOY CRUZ 2696</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>807763063</t>
+          <t>807789682</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
+          <t>Inclinada posible cambio</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5646,7 +5646,7 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -5655,14 +5655,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.400169</v>
+        <v>-58.425296</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.617784</v>
+        <v>-34.578706</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5674,27 +5674,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6249</t>
+          <t>6271</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>6/25/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2696</t>
+          <t>ARGERICH 740</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>807789682</t>
+          <t>807789686</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Inclinada posible cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5731,46 +5731,46 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.425296</v>
+        <v>-58.474467</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.578706</v>
+        <v>-34.624161</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6271</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>ARGERICH 740</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>807789686</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5785,7 +5785,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5793,7 +5793,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -5807,46 +5807,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.474467</v>
+        <v>-58.432644</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.624161</v>
+        <v>-34.595434</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Colocar columna para pedir traspaso</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5869,12 +5869,12 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
@@ -5883,14 +5883,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.432644</v>
+        <v>-58.401827</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.595434</v>
+        <v>-34.617667</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5902,27 +5902,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6284</t>
+          <t>6298</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>CHILE 2561</t>
+          <t>RIVERA INDARTE AV. 1406</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>807851584</t>
+          <t>807877127</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso</t>
+          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5950,7 +5950,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -5959,14 +5959,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.401827</v>
+        <v>-58.450359</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.617667</v>
+        <v>-34.643582</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5978,7 +5978,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6298</t>
+          <t>6308</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5988,17 +5988,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>RIVERA INDARTE AV. 1406</t>
+          <t>Guayaquil 637</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>807877127</t>
+          <t>807896343</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6035,10 +6035,10 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.450359</v>
+        <v>-58.437378</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.643582</v>
+        <v>-34.62116</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -6054,27 +6054,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6308</t>
+          <t>6330</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Guayaquil 637</t>
+          <t>REPUBLICA DE LA INDIA 3106</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>807896343</t>
+          <t>807965776</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6089,7 +6089,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada e inclinada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6111,14 +6111,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.437378</v>
+        <v>-58.413941</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.62116</v>
+        <v>-34.57698</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6130,7 +6130,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6330</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6140,7 +6140,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>REPUBLICA DE LA INDIA 3106</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -6150,7 +6150,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>807965776</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6165,15 +6165,15 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada e inclinada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -6183,18 +6183,18 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.413941</v>
+        <v>-58.405749</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.57698</v>
+        <v>-34.58224</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6206,27 +6206,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6241,15 +6241,15 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -6263,26 +6263,26 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.405749</v>
+        <v>-58.473179</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.58224</v>
+        <v>-34.629138</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>-502</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6292,17 +6292,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>Tagle 2562</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>808036198</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6317,7 +6317,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Colocar columna para pedir traspaso nodo teco</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6325,60 +6325,60 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.473179</v>
+        <v>-58.400188</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.629138</v>
+        <v>-34.583882</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-502</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Tagle 2562</t>
+          <t>GUARDIA VIEJA 4377</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808036198</t>
+          <t>808099347</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6393,7 +6393,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso nodo teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6406,7 +6406,7 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
@@ -6415,14 +6415,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.400188</v>
+        <v>-58.426322</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.583882</v>
+        <v>-34.600097</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6434,7 +6434,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>6383</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6444,17 +6444,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>GUARDIA VIEJA 4377</t>
+          <t>FALCON, RAMON L.,CNEL. 1411</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808099347</t>
+          <t>808099320</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6491,14 +6491,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.426322</v>
+        <v>-58.448523</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.600097</v>
+        <v>-34.62452</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6510,17 +6510,17 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6383</t>
+          <t>-506</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1411</t>
+          <t>Espinosa 591</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -6530,7 +6530,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808099320</t>
+          <t>808150511</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6558,7 +6558,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
@@ -6567,10 +6567,10 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.448523</v>
+        <v>-58.449</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.62452</v>
+        <v>-34.616077</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -6586,27 +6586,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>-506</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Espinosa 591</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808150511</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6634,23 +6634,23 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.449</v>
+        <v>-58.363292</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.616077</v>
+        <v>-34.642869</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6662,17 +6662,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>7030</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>MONTES DE OCA, MANUEL AV. 1809</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -6682,7 +6682,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>ICD30501825</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6697,7 +6697,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6715,14 +6715,14 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.363292</v>
+        <v>-58.372941</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.642869</v>
+        <v>-34.648341</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -6738,27 +6738,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7030</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 1809</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>ICD30501825</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6795,14 +6795,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.372941</v>
+        <v>-58.432805</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.648341</v>
+        <v>-34.574345</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -6814,27 +6814,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>-517</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Av Dorrego 2721</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>808373635</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6849,7 +6849,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6871,14 +6871,14 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.432805</v>
+        <v>-58.384097</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.574345</v>
+        <v>-34.598913</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -6890,27 +6890,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6925,7 +6925,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6947,46 +6947,46 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.384097</v>
+        <v>-58.513643</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.598913</v>
+        <v>-34.594169</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>-531</t>
+          <t>6558</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4632</t>
+          <t>NAZCA 5168</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>808530239</t>
+          <t>808703877</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -7001,7 +7001,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
+          <t>Aplomar y corregir caja de empalme colgando</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7009,7 +7009,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -7023,10 +7023,10 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.513643</v>
+        <v>-58.505593</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.594169</v>
+        <v>-34.582601</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -7042,27 +7042,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>6558</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>NAZCA 5168</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>808703877</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7077,7 +7077,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Aplomar y corregir caja de empalme colgando</t>
+          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7085,7 +7085,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -7099,93 +7099,17 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.505593</v>
+        <v>-58.355342</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.582601</v>
+        <v>-34.63565</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>6917</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>8/12/2025</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>BRIN, MINISTRO 1375</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>808918700</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
-        </is>
-      </c>
-      <c r="I89" t="n">
-        <v>1</v>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M89" t="n">
-        <v>-58.355342</v>
-      </c>
-      <c r="N89" t="n">
-        <v>-34.63565</v>
-      </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P89" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-04 21:00:51)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P87"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1802,27 +1802,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4528</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1/16/2025</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>BARCO CENTENERA DEL 545</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>802774521</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1832,7 +1832,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1850,7 +1850,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1859,46 +1859,46 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.440625</v>
+        <v>-58.496935</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.625499</v>
+        <v>-34.599084</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1908,12 +1908,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1935,36 +1935,36 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.496935</v>
+        <v>-58.400156</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.599084</v>
+        <v>-34.631369</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -2011,10 +2011,10 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.400156</v>
+        <v>-58.402062</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.631369</v>
+        <v>-34.635143</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -2030,27 +2030,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>4696</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>2/10/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>YERBAL 489</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>803607520</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Desmonte de columna ya traspasaron nodo</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2087,14 +2087,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.402062</v>
+        <v>-58.438053</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.635143</v>
+        <v>-34.617481</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2106,17 +2106,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4696</t>
+          <t>4938</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2/10/2025</t>
+          <t>2/14/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>YERBAL 489</t>
+          <t>CHACO 195</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>803607520</t>
+          <t>803607699</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron nodo</t>
+          <t>Desmontar columna personal propio traspaso nodo</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2163,10 +2163,10 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.438053</v>
+        <v>-58.431522</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.617481</v>
+        <v>-34.617523</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2182,27 +2182,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>6066</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2/14/2025</t>
+          <t>2/26/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>CHACO 195</t>
+          <t>ALBARIÑO 1331</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>803607699</t>
+          <t>803651213</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Desmontar columna personal propio traspaso nodo</t>
+          <t>Podrida en la base</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -2239,46 +2239,46 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.431522</v>
+        <v>-58.496255</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.617523</v>
+        <v>-34.650599</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6066</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ALBARIÑO 1331</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>803651213</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,11 +2293,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Podrida en la base</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2315,36 +2315,36 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.496255</v>
+        <v>-58.371855</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.650599</v>
+        <v>-34.646958</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2354,7 +2354,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2391,14 +2391,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.371855</v>
+        <v>-58.403583</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.646958</v>
+        <v>-34.591604</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2410,27 +2410,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2440,16 +2440,16 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2467,14 +2467,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.403583</v>
+        <v>-58.441405</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.591604</v>
+        <v>-34.594348</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2486,7 +2486,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2496,17 +2496,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2519,11 +2519,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
-        </is>
-      </c>
+      <c r="H28" t="inlineStr"/>
       <c r="I28" t="n">
         <v>1</v>
       </c>
@@ -2543,14 +2539,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.441405</v>
+        <v>-58.483821</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.594348</v>
+        <v>-34.677698</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2562,27 +2558,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2592,10 +2588,14 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+        </is>
+      </c>
       <c r="I29" t="n">
         <v>1</v>
       </c>
@@ -2615,14 +2615,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.483821</v>
+        <v>-58.445131</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.677698</v>
+        <v>-34.572117</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2634,27 +2634,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2669,7 +2669,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2691,14 +2691,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.445131</v>
+        <v>-58.425764</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.572117</v>
+        <v>-34.604359</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2710,27 +2710,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2745,7 +2745,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2767,10 +2767,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.425764</v>
+        <v>-58.439751</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.604359</v>
+        <v>-34.609908</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2786,7 +2786,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2796,17 +2796,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2829,7 +2829,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2843,14 +2843,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.439751</v>
+        <v>-58.375515</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.609908</v>
+        <v>-34.634393</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2862,27 +2862,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2897,7 +2897,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2919,14 +2919,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.375515</v>
+        <v>-58.415839</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.634393</v>
+        <v>-34.599291</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2938,27 +2938,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>Migueletes 1326</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2995,46 +2995,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.415839</v>
+        <v>-58.440177</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.599291</v>
+        <v>-34.56291</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Migueletes 1326</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3071,46 +3071,46 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.440177</v>
+        <v>-58.469148</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.56291</v>
+        <v>-34.687883</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3138,7 +3138,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3147,14 +3147,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.469148</v>
+        <v>-58.395063</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.687883</v>
+        <v>-34.606257</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3166,7 +3166,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3176,17 +3176,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3209,12 +3209,12 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3223,14 +3223,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.395063</v>
+        <v>-58.429977</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.606257</v>
+        <v>-34.615514</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3242,7 +3242,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3252,17 +3252,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3299,14 +3299,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.429977</v>
+        <v>-58.421623</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.615514</v>
+        <v>-34.614541</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3318,27 +3318,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>-416</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>Paraguay 3765</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>806926557</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3353,7 +3353,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3361,12 +3361,12 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3375,14 +3375,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.421623</v>
+        <v>-58.416562</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.614541</v>
+        <v>-34.590589</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3394,7 +3394,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-416</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3404,17 +3404,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Paraguay 3765</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>806926557</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3429,7 +3429,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3442,7 +3442,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3451,14 +3451,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.416562</v>
+        <v>-58.429972</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.590589</v>
+        <v>-34.632042</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3470,7 +3470,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3480,17 +3480,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3505,7 +3505,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3527,26 +3527,26 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.429972</v>
+        <v>-58.47888</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.632042</v>
+        <v>-34.571108</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3556,17 +3556,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3603,26 +3603,26 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.47888</v>
+        <v>-58.443196</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.571108</v>
+        <v>-34.618534</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>-437</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3632,17 +3632,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>Cochabamba 4090</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>806926861</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3670,7 +3670,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3679,14 +3679,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.443196</v>
+        <v>-58.422268</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.618534</v>
+        <v>-34.627754</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-437</t>
+          <t>-438</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3708,17 +3708,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Cochabamba 4090</t>
+          <t>Juncal 4565</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>806926861</t>
+          <t>806926927</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3733,7 +3733,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3746,7 +3746,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3755,14 +3755,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.422268</v>
+        <v>-58.423148</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.627754</v>
+        <v>-34.576964</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3774,7 +3774,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-438</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3784,17 +3784,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Juncal 4565</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>806926927</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3804,16 +3804,16 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3831,14 +3831,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.423148</v>
+        <v>-58.406585</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.576964</v>
+        <v>-34.592933</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3850,7 +3850,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>-445</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3860,17 +3860,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>Joaquin V Gonzalez 4410</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>806945058</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3880,16 +3880,16 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -3898,55 +3898,55 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.406585</v>
+        <v>-58.51232</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.592933</v>
+        <v>-34.595637</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-445</t>
+          <t>5937</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4410</t>
+          <t>MONROE 4833</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806945058</t>
+          <t>807044121</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3979,18 +3979,18 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.51232</v>
+        <v>-58.483104</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.595637</v>
+        <v>-34.572353</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -4002,27 +4002,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5937</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MONROE 4833</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807044121</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4037,7 +4037,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4055,14 +4055,14 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.483104</v>
+        <v>-58.483927</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.572353</v>
+        <v>-34.570689</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4078,17 +4078,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4098,7 +4098,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4113,7 +4113,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4121,7 +4121,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4131,18 +4131,18 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.483927</v>
+        <v>-58.492605</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.570689</v>
+        <v>-34.581454</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4154,7 +4154,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4164,17 +4164,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4211,26 +4211,26 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.492605</v>
+        <v>-58.467789</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.581454</v>
+        <v>-34.68463</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>-451</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4240,17 +4240,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>Uriarte 2426</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>807044071</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4265,7 +4265,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4278,7 +4278,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4287,14 +4287,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.467789</v>
+        <v>-58.423551</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.68463</v>
+        <v>-34.581258</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4306,27 +4306,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-451</t>
+          <t>5947</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Uriarte 2426</t>
+          <t>CAFAYATE 5007</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807044071</t>
+          <t>807129336</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4341,7 +4341,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Columna inclinada Columna con base corroída oxidada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4354,7 +4354,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4363,14 +4363,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.423551</v>
+        <v>-58.468182</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.581258</v>
+        <v>-34.685231</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4382,7 +4382,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5947</t>
+          <t>5948</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4392,7 +4392,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>CAFAYATE 5007</t>
+          <t>MURGUIONDO 3990</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4402,7 +4402,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807129336</t>
+          <t>807129347</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4417,7 +4417,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Columna inclinada Columna con base corroída oxidada</t>
+          <t>COLUMNA INCLINADA</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4435,14 +4435,14 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.468182</v>
+        <v>-58.477944</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.685231</v>
+        <v>-34.675149</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4458,7 +4458,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>5948</t>
+          <t>5954</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4468,17 +4468,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MURGUIONDO 3990</t>
+          <t>YAPEYU 938</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807129347</t>
+          <t>807129372</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4493,7 +4493,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>COLUMNA INCLINADA</t>
+          <t>Columna Picada, tambien resolver cables panseados y cortados reclaman ambas cosas</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4511,14 +4511,14 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.477944</v>
+        <v>-58.4212</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.675149</v>
+        <v>-34.623575</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4534,27 +4534,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5954</t>
+          <t>5973</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>YAPEYU 938</t>
+          <t>PALOS 432</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807129372</t>
+          <t>807168105</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Columna Picada, tambien resolver cables panseados y cortados reclaman ambas cosas</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4591,14 +4591,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.4212</v>
+        <v>-58.362579</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.623575</v>
+        <v>-34.635096</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4610,7 +4610,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5973</t>
+          <t>3715</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4620,17 +4620,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>PALOS 432</t>
+          <t>EL SERENO 358</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807168105</t>
+          <t>807168098</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4645,7 +4645,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4653,7 +4653,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4663,30 +4663,30 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.362579</v>
+        <v>-58.487371</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.635096</v>
+        <v>-34.640099</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>3715</t>
+          <t>5997</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4696,17 +4696,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>EL SERENO 358</t>
+          <t>MARMOL, JOSE 256</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807168098</t>
+          <t>807187768</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4721,7 +4721,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada coincide con reclamo de cables con mismo numero de caso</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4729,7 +4729,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4739,30 +4739,30 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.487371</v>
+        <v>-58.425845</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.640099</v>
+        <v>-34.616562</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5997</t>
+          <t>807187860</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4772,7 +4772,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 256</t>
+          <t>San Juan 3960</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -4782,7 +4782,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807187768</t>
+          <t>807187860</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4797,7 +4797,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables con mismo numero de caso</t>
+          <t>Colocar columna contactar a Matias Tapia 1171744701 por si hay alguna duda o problema que surja en el momento ya que es para posterior tendido de ftth</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4819,14 +4819,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.425845</v>
+        <v>-58.420909</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.616562</v>
+        <v>-34.626221</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4838,17 +4838,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>807187860</t>
+          <t>6004</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>San Juan 3960</t>
+          <t>MAZA 181</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -4858,7 +4858,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807187860</t>
+          <t>807215439</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4873,7 +4873,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Colocar columna contactar a Matias Tapia 1171744701 por si hay alguna duda o problema que surja en el momento ya que es para posterior tendido de ftth</t>
+          <t>Picada coincide con reclamo de cables</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4895,14 +4895,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.420909</v>
+        <v>-58.416477</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.626221</v>
+        <v>-34.61303</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4914,7 +4914,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6004</t>
+          <t>6007</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4924,7 +4924,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MAZA 181</t>
+          <t>HUMAHUACA 4435</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4934,7 +4934,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807215439</t>
+          <t>807215448</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4971,10 +4971,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.416477</v>
+        <v>-58.427424</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.61303</v>
+        <v>-34.601217</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4990,7 +4990,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6007</t>
+          <t>6008</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5000,7 +5000,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>HUMAHUACA 4435</t>
+          <t>ESTADO DE ISRAEL AV. 4306</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -5010,7 +5010,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807215448</t>
+          <t>807215455</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5047,10 +5047,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.427424</v>
+        <v>-58.426665</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.601217</v>
+        <v>-34.598019</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5066,7 +5066,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6008</t>
+          <t>6010</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5076,7 +5076,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4306</t>
+          <t>ESTADO DE PALESTINA 771</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5086,7 +5086,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807215455</t>
+          <t>807215458</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada y mal ubicada coincide con reclamo de cables</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5123,10 +5123,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.426665</v>
+        <v>-58.425478</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.598019</v>
+        <v>-34.601865</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5142,27 +5142,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6010</t>
+          <t>6214</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>ESTADO DE PALESTINA 771</t>
+          <t>GONZALEZ, JOAQUIN V. 2308</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807215458</t>
+          <t>807605710</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5177,7 +5177,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada y mal ubicada coincide con reclamo de cables</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5185,7 +5185,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5195,50 +5195,50 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.425478</v>
+        <v>-58.497698</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.601865</v>
+        <v>-34.612038</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6214</t>
+          <t>6229</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>GONZALEZ, JOAQUIN V. 2308</t>
+          <t>ALVAREZ THOMAS AV. 309</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807605710</t>
+          <t>807762987</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5253,7 +5253,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Reparar rienda </t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5275,26 +5275,26 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.497698</v>
+        <v>-58.44848</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.612038</v>
+        <v>-34.581338</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6229</t>
+          <t>6228</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5304,7 +5304,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 309</t>
+          <t>NEWBERY, JORGE AV. 3416</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5314,7 +5314,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807762987</t>
+          <t>807762990</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5329,7 +5329,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reparar rienda </t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5351,26 +5351,26 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.44848</v>
+        <v>-58.448496</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.581338</v>
+        <v>-34.58182</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6076</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5380,17 +5380,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE AV. 3416</t>
+          <t>MATHEU 727</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807762990</t>
+          <t>807763063</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5413,60 +5413,60 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.448496</v>
+        <v>-58.400169</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.58182</v>
+        <v>-34.617784</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6076</t>
+          <t>6249</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/25/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>MATHEU 727</t>
+          <t>GODOY CRUZ 2696</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807763063</t>
+          <t>807789682</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
+          <t>Inclinada posible cambio</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5494,7 +5494,7 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
@@ -5503,14 +5503,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.400169</v>
+        <v>-58.425296</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.617784</v>
+        <v>-34.578706</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5522,27 +5522,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6249</t>
+          <t>6271</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>6/25/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2696</t>
+          <t>ARGERICH 740</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807789682</t>
+          <t>807789686</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Inclinada posible cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5579,46 +5579,46 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.425296</v>
+        <v>-58.474467</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.578706</v>
+        <v>-34.624161</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6271</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ARGERICH 740</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>807789686</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5641,7 +5641,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5655,46 +5655,46 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.474467</v>
+        <v>-58.432644</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.624161</v>
+        <v>-34.595434</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Colocar columna para pedir traspaso</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5717,12 +5717,12 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -5731,14 +5731,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.432644</v>
+        <v>-58.401827</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.595434</v>
+        <v>-34.617667</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5750,27 +5750,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6284</t>
+          <t>6298</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>CHILE 2561</t>
+          <t>RIVERA INDARTE AV. 1406</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>807851584</t>
+          <t>807877127</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5785,7 +5785,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso</t>
+          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5798,7 +5798,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -5807,14 +5807,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.401827</v>
+        <v>-58.450359</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.617667</v>
+        <v>-34.643582</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5826,27 +5826,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6298</t>
+          <t>6330</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>RIVERA INDARTE AV. 1406</t>
+          <t>REPUBLICA DE LA INDIA 3106</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>807877127</t>
+          <t>807965776</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5861,7 +5861,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
+          <t>Picada e inclinada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5883,14 +5883,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.450359</v>
+        <v>-58.413941</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.643582</v>
+        <v>-34.57698</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5902,27 +5902,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6308</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Guayaquil 637</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>807896343</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5937,15 +5937,15 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5955,18 +5955,18 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.437378</v>
+        <v>-58.405749</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.62116</v>
+        <v>-34.58224</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5978,27 +5978,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6330</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>REPUBLICA DE LA INDIA 3106</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>807965776</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada e inclinada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6021,7 +6021,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -6031,40 +6031,40 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.413941</v>
+        <v>-58.473179</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.57698</v>
+        <v>-34.629138</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>-502</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>Tagle 2562</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -6074,7 +6074,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>808036198</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6089,32 +6089,32 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar columna para pedir traspaso nodo teco</t>
         </is>
       </c>
       <c r="I75" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.405749</v>
+        <v>-58.400188</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.58224</v>
+        <v>-34.583882</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6130,27 +6130,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>GUARDIA VIEJA 4377</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>808099347</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6165,7 +6165,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6173,7 +6173,7 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -6183,50 +6183,50 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.473179</v>
+        <v>-58.426322</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.629138</v>
+        <v>-34.600097</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-502</t>
+          <t>-506</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Tagle 2562</t>
+          <t>Espinosa 591</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808036198</t>
+          <t>808150511</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6241,7 +6241,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso nodo teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6263,14 +6263,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.400188</v>
+        <v>-58.449</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.583882</v>
+        <v>-34.616077</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6282,27 +6282,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>GUARDIA VIEJA 4377</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808099347</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6335,18 +6335,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.426322</v>
+        <v>-58.363292</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.600097</v>
+        <v>-34.642869</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6358,27 +6358,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6383</t>
+          <t>7030</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1411</t>
+          <t>MONTES DE OCA, MANUEL AV. 1809</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808099320</t>
+          <t>ICD30501825</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6393,7 +6393,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6415,14 +6415,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.448523</v>
+        <v>-58.372941</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.62452</v>
+        <v>-34.648341</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6434,27 +6434,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-506</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Espinosa 591</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808150511</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6469,7 +6469,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6482,7 +6482,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
@@ -6491,14 +6491,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.449</v>
+        <v>-58.432805</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.616077</v>
+        <v>-34.574345</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6510,27 +6510,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6545,7 +6545,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6563,18 +6563,18 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.363292</v>
+        <v>-58.384097</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.642869</v>
+        <v>-34.598913</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6586,27 +6586,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7030</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 1809</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>ICD30501825</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6621,7 +6621,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6643,46 +6643,46 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.372941</v>
+        <v>-58.513643</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.648341</v>
+        <v>-34.594169</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-517</t>
+          <t>6558</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Av Dorrego 2721</t>
+          <t>NAZCA 5168</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808373635</t>
+          <t>808703877</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6697,7 +6697,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
+          <t>Aplomar y corregir caja de empalme colgando</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6705,7 +6705,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -6719,46 +6719,46 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.432805</v>
+        <v>-58.505593</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.574345</v>
+        <v>-34.582601</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6795,245 +6795,17 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.384097</v>
+        <v>-58.355342</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.598913</v>
+        <v>-34.63565</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>-531</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>7/25/2025</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Joaquin V Gonzalez 4632</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>808530239</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
-        </is>
-      </c>
-      <c r="I85" t="n">
-        <v>1</v>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M85" t="n">
-        <v>-58.513643</v>
-      </c>
-      <c r="N85" t="n">
-        <v>-34.594169</v>
-      </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P85" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>6558</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>8/4/2025</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>NAZCA 5168</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>808703877</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>Aplomar y corregir caja de empalme colgando</t>
-        </is>
-      </c>
-      <c r="I86" t="n">
-        <v>1</v>
-      </c>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M86" t="n">
-        <v>-58.505593</v>
-      </c>
-      <c r="N86" t="n">
-        <v>-34.582601</v>
-      </c>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P86" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>6917</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>8/12/2025</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>BRIN, MINISTRO 1375</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>808918700</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
-        </is>
-      </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M87" t="n">
-        <v>-58.355342</v>
-      </c>
-      <c r="N87" t="n">
-        <v>-34.63565</v>
-      </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P87" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-08 07:30:27)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2182,27 +2182,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>6066</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2/26/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ALBARIÑO 1331</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>803651213</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2217,11 +2217,11 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Podrida en la base</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2239,36 +2239,36 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.496255</v>
+        <v>-58.371855</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.650599</v>
+        <v>-34.646958</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2278,7 +2278,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2315,14 +2315,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.371855</v>
+        <v>-58.403583</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.646958</v>
+        <v>-34.591604</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2334,27 +2334,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2364,16 +2364,16 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -2382,7 +2382,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2391,14 +2391,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.403583</v>
+        <v>-58.441405</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.591604</v>
+        <v>-34.594348</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2410,7 +2410,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2420,17 +2420,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2443,11 +2443,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
-        </is>
-      </c>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="n">
         <v>1</v>
       </c>
@@ -2467,14 +2463,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.441405</v>
+        <v>-58.483821</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.594348</v>
+        <v>-34.677698</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2486,27 +2482,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2516,10 +2512,14 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+        </is>
+      </c>
       <c r="I28" t="n">
         <v>1</v>
       </c>
@@ -2539,14 +2539,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.483821</v>
+        <v>-58.445131</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.677698</v>
+        <v>-34.572117</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2558,27 +2558,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2615,14 +2615,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.445131</v>
+        <v>-58.425764</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.572117</v>
+        <v>-34.604359</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2634,27 +2634,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2669,7 +2669,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2677,7 +2677,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2691,10 +2691,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.425764</v>
+        <v>-58.439751</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.604359</v>
+        <v>-34.609908</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2710,7 +2710,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2720,17 +2720,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2745,7 +2745,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2767,14 +2767,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.439751</v>
+        <v>-58.375515</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.609908</v>
+        <v>-34.634393</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2786,27 +2786,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2843,14 +2843,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.375515</v>
+        <v>-58.415839</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.634393</v>
+        <v>-34.599291</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2862,27 +2862,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/7/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>Migueletes 1326</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>805707264</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2919,46 +2919,46 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.415839</v>
+        <v>-58.440177</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.599291</v>
+        <v>-34.56291</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/7/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Migueletes 1326</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>805707264</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2995,46 +2995,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.440177</v>
+        <v>-58.469148</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.56291</v>
+        <v>-34.687883</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3071,14 +3071,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.469148</v>
+        <v>-58.395063</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.687883</v>
+        <v>-34.606257</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3090,7 +3090,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3100,17 +3100,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3133,12 +3133,12 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3147,14 +3147,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.395063</v>
+        <v>-58.429977</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.606257</v>
+        <v>-34.615514</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3166,7 +3166,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3176,17 +3176,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3223,14 +3223,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.429977</v>
+        <v>-58.421623</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.615514</v>
+        <v>-34.614541</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3242,27 +3242,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>-416</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>Paraguay 3765</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>806926557</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3277,7 +3277,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3285,12 +3285,12 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3299,14 +3299,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.421623</v>
+        <v>-58.416562</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.614541</v>
+        <v>-34.590589</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3318,7 +3318,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-416</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3328,17 +3328,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Paraguay 3765</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>806926557</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3353,7 +3353,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3366,7 +3366,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3375,14 +3375,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.416562</v>
+        <v>-58.429972</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.590589</v>
+        <v>-34.632042</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3394,7 +3394,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3404,17 +3404,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3429,7 +3429,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3451,26 +3451,26 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.429972</v>
+        <v>-58.47888</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.632042</v>
+        <v>-34.571108</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3480,17 +3480,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3505,7 +3505,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3527,26 +3527,26 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.47888</v>
+        <v>-58.443196</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.571108</v>
+        <v>-34.618534</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>-437</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3556,17 +3556,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>Cochabamba 4090</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>806926861</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3603,14 +3603,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.443196</v>
+        <v>-58.422268</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.618534</v>
+        <v>-34.627754</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3622,7 +3622,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-437</t>
+          <t>-438</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3632,17 +3632,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Cochabamba 4090</t>
+          <t>Juncal 4565</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>806926861</t>
+          <t>806926927</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3657,7 +3657,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3670,7 +3670,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3679,14 +3679,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.422268</v>
+        <v>-58.423148</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.627754</v>
+        <v>-34.576964</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3698,7 +3698,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-438</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3708,17 +3708,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Juncal 4565</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>806926927</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3728,16 +3728,16 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -3755,14 +3755,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.423148</v>
+        <v>-58.406585</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.576964</v>
+        <v>-34.592933</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3774,7 +3774,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>-445</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3784,17 +3784,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>Joaquin V Gonzalez 4410</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>806945058</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3804,16 +3804,16 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -3822,55 +3822,55 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.406585</v>
+        <v>-58.51232</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.592933</v>
+        <v>-34.595637</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-445</t>
+          <t>5937</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4410</t>
+          <t>MONROE 4833</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806945058</t>
+          <t>807044121</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3885,7 +3885,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3903,18 +3903,18 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.51232</v>
+        <v>-58.483104</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.595637</v>
+        <v>-34.572353</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3926,27 +3926,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5937</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MONROE 4833</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807044121</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3969,7 +3969,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3979,14 +3979,14 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.483104</v>
+        <v>-58.483927</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.572353</v>
+        <v>-34.570689</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -4002,17 +4002,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4022,7 +4022,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4037,7 +4037,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4045,7 +4045,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4055,18 +4055,18 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.483927</v>
+        <v>-58.492605</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.570689</v>
+        <v>-34.581454</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4078,7 +4078,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4088,17 +4088,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4135,26 +4135,26 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.492605</v>
+        <v>-58.467789</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.581454</v>
+        <v>-34.68463</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>-451</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4164,17 +4164,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>Uriarte 2426</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>807044071</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4189,7 +4189,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4202,7 +4202,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -4211,14 +4211,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.467789</v>
+        <v>-58.423551</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.68463</v>
+        <v>-34.581258</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4230,27 +4230,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-451</t>
+          <t>5947</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Uriarte 2426</t>
+          <t>CAFAYATE 5007</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807044071</t>
+          <t>807129336</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4265,7 +4265,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Columna inclinada Columna con base corroída oxidada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4278,7 +4278,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4287,14 +4287,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.423551</v>
+        <v>-58.468182</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.581258</v>
+        <v>-34.685231</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4306,7 +4306,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5947</t>
+          <t>5948</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4316,7 +4316,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>CAFAYATE 5007</t>
+          <t>MURGUIONDO 3990</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4326,7 +4326,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807129336</t>
+          <t>807129347</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4341,7 +4341,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Columna inclinada Columna con base corroída oxidada</t>
+          <t>COLUMNA INCLINADA</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4359,14 +4359,14 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.468182</v>
+        <v>-58.477944</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.685231</v>
+        <v>-34.675149</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4382,7 +4382,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5948</t>
+          <t>5954</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4392,17 +4392,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MURGUIONDO 3990</t>
+          <t>YAPEYU 938</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807129347</t>
+          <t>807129372</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4417,7 +4417,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>COLUMNA INCLINADA</t>
+          <t>Columna Picada, tambien resolver cables panseados y cortados reclaman ambas cosas</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4435,14 +4435,14 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.477944</v>
+        <v>-58.4212</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.675149</v>
+        <v>-34.623575</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4458,27 +4458,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>5954</t>
+          <t>5973</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>YAPEYU 938</t>
+          <t>PALOS 432</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807129372</t>
+          <t>807168105</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4493,7 +4493,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Columna Picada, tambien resolver cables panseados y cortados reclaman ambas cosas</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4515,14 +4515,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.4212</v>
+        <v>-58.362579</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.623575</v>
+        <v>-34.635096</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4534,7 +4534,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5973</t>
+          <t>3715</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4544,17 +4544,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>PALOS 432</t>
+          <t>EL SERENO 358</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807168105</t>
+          <t>807168098</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4569,7 +4569,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4577,7 +4577,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4587,30 +4587,30 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.362579</v>
+        <v>-58.487371</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.635096</v>
+        <v>-34.640099</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>3715</t>
+          <t>5997</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4620,17 +4620,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>EL SERENO 358</t>
+          <t>MARMOL, JOSE 256</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807168098</t>
+          <t>807187768</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4645,7 +4645,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada coincide con reclamo de cables con mismo numero de caso</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4653,7 +4653,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4663,30 +4663,30 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.487371</v>
+        <v>-58.425845</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.640099</v>
+        <v>-34.616562</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5997</t>
+          <t>807187860</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4696,7 +4696,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 256</t>
+          <t>San Juan 3960</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4706,7 +4706,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807187768</t>
+          <t>807187860</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4721,7 +4721,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables con mismo numero de caso</t>
+          <t>Colocar columna contactar a Matias Tapia 1171744701 por si hay alguna duda o problema que surja en el momento ya que es para posterior tendido de ftth</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4743,14 +4743,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.425845</v>
+        <v>-58.420909</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.616562</v>
+        <v>-34.626221</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4762,17 +4762,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>807187860</t>
+          <t>6004</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>San Juan 3960</t>
+          <t>MAZA 181</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -4782,7 +4782,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807187860</t>
+          <t>807215439</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4797,7 +4797,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Colocar columna contactar a Matias Tapia 1171744701 por si hay alguna duda o problema que surja en el momento ya que es para posterior tendido de ftth</t>
+          <t>Picada coincide con reclamo de cables</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4819,14 +4819,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.420909</v>
+        <v>-58.416477</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.626221</v>
+        <v>-34.61303</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4838,7 +4838,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6004</t>
+          <t>6007</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4848,7 +4848,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>MAZA 181</t>
+          <t>HUMAHUACA 4435</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -4858,7 +4858,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807215439</t>
+          <t>807215448</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4895,10 +4895,10 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.416477</v>
+        <v>-58.427424</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.61303</v>
+        <v>-34.601217</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4914,7 +4914,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6007</t>
+          <t>6008</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4924,7 +4924,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>HUMAHUACA 4435</t>
+          <t>ESTADO DE ISRAEL AV. 4306</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4934,7 +4934,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807215448</t>
+          <t>807215455</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4971,10 +4971,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.427424</v>
+        <v>-58.426665</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.601217</v>
+        <v>-34.598019</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4990,7 +4990,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6008</t>
+          <t>6010</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5000,7 +5000,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4306</t>
+          <t>ESTADO DE PALESTINA 771</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -5010,7 +5010,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807215455</t>
+          <t>807215458</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5025,7 +5025,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada y mal ubicada coincide con reclamo de cables</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5047,10 +5047,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.426665</v>
+        <v>-58.425478</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.598019</v>
+        <v>-34.601865</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5066,27 +5066,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6010</t>
+          <t>6214</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ESTADO DE PALESTINA 771</t>
+          <t>GONZALEZ, JOAQUIN V. 2308</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807215458</t>
+          <t>807605710</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada y mal ubicada coincide con reclamo de cables</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5109,7 +5109,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -5119,50 +5119,50 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.425478</v>
+        <v>-58.497698</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.601865</v>
+        <v>-34.612038</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6214</t>
+          <t>6229</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>GONZALEZ, JOAQUIN V. 2308</t>
+          <t>ALVAREZ THOMAS AV. 309</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807605710</t>
+          <t>807762987</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5177,7 +5177,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Reparar rienda </t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5185,7 +5185,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -5199,26 +5199,26 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.497698</v>
+        <v>-58.44848</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.612038</v>
+        <v>-34.581338</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6229</t>
+          <t>6228</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5228,7 +5228,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 309</t>
+          <t>NEWBERY, JORGE AV. 3416</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5238,7 +5238,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807762987</t>
+          <t>807762990</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5253,7 +5253,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t xml:space="preserve">Reparar rienda </t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5275,26 +5275,26 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.44848</v>
+        <v>-58.448496</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.581338</v>
+        <v>-34.58182</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6228</t>
+          <t>6076</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5304,17 +5304,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE AV. 3416</t>
+          <t>MATHEU 727</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807762990</t>
+          <t>807763063</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5329,7 +5329,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5337,60 +5337,60 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.448496</v>
+        <v>-58.400169</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.58182</v>
+        <v>-34.617784</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6076</t>
+          <t>6249</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/25/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>MATHEU 727</t>
+          <t>GODOY CRUZ 2696</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807763063</t>
+          <t>807789682</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5405,7 +5405,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
+          <t>Inclinada posible cambio</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5418,7 +5418,7 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L66" t="inlineStr">
@@ -5427,14 +5427,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.400169</v>
+        <v>-58.425296</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.617784</v>
+        <v>-34.578706</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5446,27 +5446,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6249</t>
+          <t>6271</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/25/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2696</t>
+          <t>ARGERICH 740</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807789682</t>
+          <t>807789686</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Inclinada posible cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5503,46 +5503,46 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.425296</v>
+        <v>-58.474467</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.578706</v>
+        <v>-34.624161</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6271</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>ARGERICH 740</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807789686</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5557,7 +5557,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5565,7 +5565,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5579,46 +5579,46 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.474467</v>
+        <v>-58.432644</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.624161</v>
+        <v>-34.595434</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Colocar columna para pedir traspaso</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5641,12 +5641,12 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -5655,14 +5655,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.432644</v>
+        <v>-58.401827</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.595434</v>
+        <v>-34.617667</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5674,27 +5674,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6284</t>
+          <t>6298</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>CHILE 2561</t>
+          <t>RIVERA INDARTE AV. 1406</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>807851584</t>
+          <t>807877127</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5709,7 +5709,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso</t>
+          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5722,7 +5722,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -5731,14 +5731,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.401827</v>
+        <v>-58.450359</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.617667</v>
+        <v>-34.643582</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5750,27 +5750,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6298</t>
+          <t>6330</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>RIVERA INDARTE AV. 1406</t>
+          <t>REPUBLICA DE LA INDIA 3106</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>807877127</t>
+          <t>807965776</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5785,7 +5785,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
+          <t>Picada e inclinada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5807,14 +5807,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.450359</v>
+        <v>-58.413941</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.643582</v>
+        <v>-34.57698</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5826,7 +5826,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6330</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5836,7 +5836,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>REPUBLICA DE LA INDIA 3106</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -5846,7 +5846,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>807965776</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5861,15 +5861,15 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada e inclinada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5879,18 +5879,18 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.413941</v>
+        <v>-58.405749</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.57698</v>
+        <v>-34.58224</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5902,27 +5902,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5937,15 +5937,15 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I73" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5959,26 +5959,26 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.405749</v>
+        <v>-58.473179</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.58224</v>
+        <v>-34.629138</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>-502</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5988,17 +5988,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>Tagle 2562</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>808036198</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6013,7 +6013,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Colocar columna para pedir traspaso nodo teco</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6021,60 +6021,60 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.473179</v>
+        <v>-58.400188</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.629138</v>
+        <v>-34.583882</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-502</t>
+          <t>6377</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Tagle 2562</t>
+          <t>GUARDIA VIEJA 4377</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808036198</t>
+          <t>808099347</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6089,7 +6089,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso nodo teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6102,7 +6102,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -6111,14 +6111,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.400188</v>
+        <v>-58.426322</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.583882</v>
+        <v>-34.600097</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6130,27 +6130,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6377</t>
+          <t>-506</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>GUARDIA VIEJA 4377</t>
+          <t>Espinosa 591</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808099347</t>
+          <t>808150511</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6178,7 +6178,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -6187,14 +6187,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.426322</v>
+        <v>-58.449</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.600097</v>
+        <v>-34.616077</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6206,27 +6206,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-506</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Espinosa 591</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808150511</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6254,23 +6254,23 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.449</v>
+        <v>-58.363292</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.616077</v>
+        <v>-34.642869</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6282,17 +6282,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>7030</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>MONTES DE OCA, MANUEL AV. 1809</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -6302,7 +6302,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>ICD30501825</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6317,7 +6317,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6335,14 +6335,14 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.363292</v>
+        <v>-58.372941</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.642869</v>
+        <v>-34.648341</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6358,27 +6358,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7030</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 1809</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>ICD30501825</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6393,7 +6393,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6415,14 +6415,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.372941</v>
+        <v>-58.432805</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.648341</v>
+        <v>-34.574345</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6434,27 +6434,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-517</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Av Dorrego 2721</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808373635</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6469,7 +6469,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6491,14 +6491,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.432805</v>
+        <v>-58.384097</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.574345</v>
+        <v>-34.598913</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6510,27 +6510,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6545,7 +6545,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6567,46 +6567,46 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.384097</v>
+        <v>-58.513643</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.598913</v>
+        <v>-34.594169</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>-531</t>
+          <t>6558</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4632</t>
+          <t>NAZCA 5168</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808530239</t>
+          <t>808703877</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6621,7 +6621,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
+          <t>Aplomar y corregir caja de empalme colgando</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6629,7 +6629,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -6643,10 +6643,10 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.513643</v>
+        <v>-58.505593</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.594169</v>
+        <v>-34.582601</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -6662,27 +6662,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6558</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>NAZCA 5168</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808703877</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6697,7 +6697,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Aplomar y corregir caja de empalme colgando</t>
+          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6705,7 +6705,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -6719,93 +6719,17 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.505593</v>
+        <v>-58.355342</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.582601</v>
+        <v>-34.63565</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>6917</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>8/12/2025</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>BRIN, MINISTRO 1375</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>808918700</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
-        </is>
-      </c>
-      <c r="I84" t="n">
-        <v>1</v>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M84" t="n">
-        <v>-58.355342</v>
-      </c>
-      <c r="N84" t="n">
-        <v>-34.63565</v>
-      </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-11 07:49:47)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P80"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6058,27 +6058,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7030</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 1809</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>ICD30501825</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6093,7 +6093,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Colocar columna donde esta el monoducto para acceso a edifciio</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6115,14 +6115,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.372941</v>
+        <v>-58.432805</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.648341</v>
+        <v>-34.574345</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6134,27 +6134,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-517</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Av Dorrego 2721</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808373635</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6169,7 +6169,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6191,14 +6191,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.432805</v>
+        <v>-58.384097</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.574345</v>
+        <v>-34.598913</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6210,27 +6210,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6245,7 +6245,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6267,46 +6267,46 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.384097</v>
+        <v>-58.513643</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.598913</v>
+        <v>-34.594169</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-531</t>
+          <t>6558</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4632</t>
+          <t>NAZCA 5168</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808530239</t>
+          <t>808703877</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6321,7 +6321,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
+          <t>Aplomar y corregir caja de empalme colgando</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6329,7 +6329,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -6343,10 +6343,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.513643</v>
+        <v>-58.505593</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.594169</v>
+        <v>-34.582601</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6362,27 +6362,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6558</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>NAZCA 5168</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808703877</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6397,7 +6397,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Aplomar y corregir caja de empalme colgando</t>
+          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6405,7 +6405,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -6419,46 +6419,46 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.505593</v>
+        <v>-58.355342</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.582601</v>
+        <v>-34.63565</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6917</t>
+          <t>-593</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>BRIN, MINISTRO 1375</t>
+          <t>Husares 2250</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808918700</t>
+          <t>809642190</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6473,7 +6473,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6495,19 +6495,95 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.355342</v>
+        <v>-58.443269</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.63565</v>
+        <v>-34.552209</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>-594</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>9/10/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Vidal 1861</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>809642175</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.458298</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.566511</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-15 12:07:47)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P80"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4006,27 +4006,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5947</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>CAFAYATE 5007</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807129336</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Columna inclinada Columna con base corroída oxidada</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4049,7 +4049,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4063,14 +4063,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.468182</v>
+        <v>-58.432644</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.685231</v>
+        <v>-34.595434</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4082,27 +4082,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5948</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>MURGUIONDO 3990</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807129347</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,15 +4117,15 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>COLUMNA INCLINADA</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4139,14 +4139,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.477944</v>
+        <v>-58.405749</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.675149</v>
+        <v>-34.58224</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4158,27 +4158,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5954</t>
+          <t>-502</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>YAPEYU 938</t>
+          <t>Tagle 2562</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807129372</t>
+          <t>808036198</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Columna Picada, tambien resolver cables panseados y cortados reclaman ambas cosas</t>
+          <t>Colocar columna para pedir traspaso nodo teco</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4206,7 +4206,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -4215,14 +4215,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.4212</v>
+        <v>-58.400188</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.623575</v>
+        <v>-34.583882</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4234,27 +4234,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5973</t>
+          <t>-506</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>PALOS 432</t>
+          <t>Espinosa 591</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807168105</t>
+          <t>808150511</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4282,7 +4282,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4291,14 +4291,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.362579</v>
+        <v>-58.449</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.635096</v>
+        <v>-34.616077</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4310,27 +4310,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>3715</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>EL SERENO 358</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807168098</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4353,7 +4353,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4363,50 +4363,50 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.487371</v>
+        <v>-58.363292</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.640099</v>
+        <v>-34.642869</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5997</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 256</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807187768</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables con mismo numero de caso</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4443,14 +4443,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.425845</v>
+        <v>-58.432805</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.616562</v>
+        <v>-34.574345</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4462,27 +4462,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6004</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MAZA 181</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807215439</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4497,7 +4497,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4519,14 +4519,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.416477</v>
+        <v>-58.384097</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.61303</v>
+        <v>-34.598913</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4538,27 +4538,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6007</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>HUMAHUACA 4435</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807215448</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada coincide con reclamo de cables</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4595,46 +4595,46 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.427424</v>
+        <v>-58.513643</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.601217</v>
+        <v>-34.594169</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6008</t>
+          <t>-593</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4306</t>
+          <t>Husares 2250</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807215455</t>
+          <t>809642190</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4671,46 +4671,46 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.426665</v>
+        <v>-58.443269</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.598019</v>
+        <v>-34.552209</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6010</t>
+          <t>-594</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>ESTADO DE PALESTINA 771</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807215458</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4725,7 +4725,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada y mal ubicada coincide con reclamo de cables</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4747,1765 +4747,17 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.425478</v>
+        <v>-58.458298</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.601865</v>
+        <v>-34.566511</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>6214</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>6/18/2025</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>GONZALEZ, JOAQUIN V. 2308</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>807605710</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I58" t="n">
-        <v>1</v>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M58" t="n">
-        <v>-58.497698</v>
-      </c>
-      <c r="N58" t="n">
-        <v>-34.612038</v>
-      </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>Devoto</t>
-        </is>
-      </c>
-      <c r="P58" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>6229</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>6/24/2025</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>ALVAREZ THOMAS AV. 309</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>807762987</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Reparar rienda </t>
-        </is>
-      </c>
-      <c r="I59" t="n">
-        <v>1</v>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>Tensor</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M59" t="n">
-        <v>-58.44848</v>
-      </c>
-      <c r="N59" t="n">
-        <v>-34.581338</v>
-      </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P59" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>6228</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>6/24/2025</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>NEWBERY, JORGE AV. 3416</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>807762990</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>Reparar rienda</t>
-        </is>
-      </c>
-      <c r="I60" t="n">
-        <v>1</v>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>Tensor</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M60" t="n">
-        <v>-58.448496</v>
-      </c>
-      <c r="N60" t="n">
-        <v>-34.58182</v>
-      </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P60" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>6076</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>6/24/2025</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>MATHEU 727</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>807763063</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
-        </is>
-      </c>
-      <c r="I61" t="n">
-        <v>1</v>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>Nodo TLC</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M61" t="n">
-        <v>-58.400169</v>
-      </c>
-      <c r="N61" t="n">
-        <v>-34.617784</v>
-      </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P61" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>6249</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>6/25/2025</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>GODOY CRUZ 2696</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>807789682</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>Inclinada posible cambio</t>
-        </is>
-      </c>
-      <c r="I62" t="n">
-        <v>1</v>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M62" t="n">
-        <v>-58.425296</v>
-      </c>
-      <c r="N62" t="n">
-        <v>-34.578706</v>
-      </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P62" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>6271</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>6/26/2025</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>ARGERICH 740</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>807789686</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I63" t="n">
-        <v>1</v>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M63" t="n">
-        <v>-58.474467</v>
-      </c>
-      <c r="N63" t="n">
-        <v>-34.624161</v>
-      </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>Devoto</t>
-        </is>
-      </c>
-      <c r="P63" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>-493</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>6/27/2025</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>JUFRE 424</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>807817955</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
-        </is>
-      </c>
-      <c r="I64" t="n">
-        <v>1</v>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>Desmonte</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M64" t="n">
-        <v>-58.432644</v>
-      </c>
-      <c r="N64" t="n">
-        <v>-34.595434</v>
-      </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P64" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>6284</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>6/30/2025</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>CHILE 2561</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>807851584</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Colocar columna para pedir traspaso</t>
-        </is>
-      </c>
-      <c r="I65" t="n">
-        <v>1</v>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M65" t="n">
-        <v>-58.401827</v>
-      </c>
-      <c r="N65" t="n">
-        <v>-34.617667</v>
-      </c>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P65" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>6298</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>7/1/2025</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>RIVERA INDARTE AV. 1406</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>807877127</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>Columna en plantera Se recomienda el retiro riesgo de caida</t>
-        </is>
-      </c>
-      <c r="I66" t="n">
-        <v>1</v>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L66" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M66" t="n">
-        <v>-58.450359</v>
-      </c>
-      <c r="N66" t="n">
-        <v>-34.643582</v>
-      </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P66" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>6330</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>7/3/2025</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>REPUBLICA DE LA INDIA 3106</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>807965776</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>Picada e inclinada</t>
-        </is>
-      </c>
-      <c r="I67" t="n">
-        <v>1</v>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M67" t="n">
-        <v>-58.413941</v>
-      </c>
-      <c r="N67" t="n">
-        <v>-34.57698</v>
-      </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P67" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>-501</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>7/3/2025</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Cabello 3107</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>807971967</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>Aplomar</t>
-        </is>
-      </c>
-      <c r="I68" t="n">
-        <v>0</v>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M68" t="n">
-        <v>-58.405749</v>
-      </c>
-      <c r="N68" t="n">
-        <v>-34.58224</v>
-      </c>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>Recoleta</t>
-        </is>
-      </c>
-      <c r="P68" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>6357</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>7/7/2025</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>BACACAY 3088</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>808036196</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>Reparar rienda</t>
-        </is>
-      </c>
-      <c r="I69" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>Tensor</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M69" t="n">
-        <v>-58.473179</v>
-      </c>
-      <c r="N69" t="n">
-        <v>-34.629138</v>
-      </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>Devoto</t>
-        </is>
-      </c>
-      <c r="P69" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>-502</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>7/7/2025</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Tagle 2562</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>808036198</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>Colocar columna para pedir traspaso nodo teco</t>
-        </is>
-      </c>
-      <c r="I70" t="n">
-        <v>1</v>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M70" t="n">
-        <v>-58.400188</v>
-      </c>
-      <c r="N70" t="n">
-        <v>-34.583882</v>
-      </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>Recoleta</t>
-        </is>
-      </c>
-      <c r="P70" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>6377</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>7/8/2025</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>GUARDIA VIEJA 4377</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>808099347</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I71" t="n">
-        <v>1</v>
-      </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M71" t="n">
-        <v>-58.426322</v>
-      </c>
-      <c r="N71" t="n">
-        <v>-34.600097</v>
-      </c>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P71" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>-506</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>7/11/2025</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Espinosa 591</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>808150511</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I72" t="n">
-        <v>1</v>
-      </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M72" t="n">
-        <v>-58.449</v>
-      </c>
-      <c r="N72" t="n">
-        <v>-34.616077</v>
-      </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P72" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>-511</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>7/14/2025</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Carlos Melo 491</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>808194932</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I73" t="n">
-        <v>1</v>
-      </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L73" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M73" t="n">
-        <v>-58.363292</v>
-      </c>
-      <c r="N73" t="n">
-        <v>-34.642869</v>
-      </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P73" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>-517</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>7/16/2025</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Av Dorrego 2721</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>808373635</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
-        </is>
-      </c>
-      <c r="I74" t="n">
-        <v>1</v>
-      </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M74" t="n">
-        <v>-58.432805</v>
-      </c>
-      <c r="N74" t="n">
-        <v>-34.574345</v>
-      </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P74" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>-529</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>7/23/2025</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Libertad 820</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>ICD30189941</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
-        </is>
-      </c>
-      <c r="I75" t="n">
-        <v>1</v>
-      </c>
-      <c r="J75" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L75" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M75" t="n">
-        <v>-58.384097</v>
-      </c>
-      <c r="N75" t="n">
-        <v>-34.598913</v>
-      </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>Recoleta</t>
-        </is>
-      </c>
-      <c r="P75" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>-531</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>7/25/2025</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Joaquin V Gonzalez 4632</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>808530239</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
-        </is>
-      </c>
-      <c r="I76" t="n">
-        <v>1</v>
-      </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L76" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M76" t="n">
-        <v>-58.513643</v>
-      </c>
-      <c r="N76" t="n">
-        <v>-34.594169</v>
-      </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P76" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>6558</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>8/4/2025</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>NAZCA 5168</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>808703877</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>Aplomar y corregir caja de empalme colgando</t>
-        </is>
-      </c>
-      <c r="I77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J77" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L77" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M77" t="n">
-        <v>-58.505593</v>
-      </c>
-      <c r="N77" t="n">
-        <v>-34.582601</v>
-      </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P77" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>6917</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>8/12/2025</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>BRIN, MINISTRO 1375</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>808918700</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>Picada tiene tambien una ot de cableado ver en conjunto</t>
-        </is>
-      </c>
-      <c r="I78" t="n">
-        <v>1</v>
-      </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M78" t="n">
-        <v>-58.355342</v>
-      </c>
-      <c r="N78" t="n">
-        <v>-34.63565</v>
-      </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P78" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>-593</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>9/10/2025</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Husares 2250</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>809642190</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M79" t="n">
-        <v>-58.443269</v>
-      </c>
-      <c r="N79" t="n">
-        <v>-34.552209</v>
-      </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P79" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>-594</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>9/10/2025</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Vidal 1861</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>809642175</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I80" t="n">
-        <v>1</v>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M80" t="n">
-        <v>-58.458298</v>
-      </c>
-      <c r="N80" t="n">
-        <v>-34.566511</v>
-      </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P80" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-17 14:57:07)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P57"/>
+  <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4687,82 +4687,6 @@
         </is>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>-594</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>9/10/2025</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Vidal 1861</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>809642175</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I57" t="n">
-        <v>1</v>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M57" t="n">
-        <v>-58.458298</v>
-      </c>
-      <c r="N57" t="n">
-        <v>-34.566511</v>
-      </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>Colegiales</t>
-        </is>
-      </c>
-      <c r="P57" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-19 08:04:47)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P56"/>
+  <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,17 +518,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2463</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7/15/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
+          <t>José Andrés Pacheco de Melo 2084</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>795698153</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -548,12 +548,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
+          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -566,19 +566,15 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>-58.40589</v>
+        <v>-58.395656</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.584156</v>
+        <v>-34.590364</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -594,27 +590,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>6243</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>1/30/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MCAL SOLANO LOPEZ 3110</t>
+          <t>GARCIA, TEODORO 3252</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>792101640</t>
+          <t>779373118</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -629,7 +625,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Retirar columna. TLC ya traspaso nodo</t>
+          <t>Colocar R400 para posterior traspaso</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -642,7 +638,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -651,14 +647,14 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.498448</v>
+        <v>-58.450789</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.595287</v>
+        <v>-34.577949</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -670,27 +666,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3154</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8/27/2024</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>BRAVO, MARIO 853</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>795498456</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -705,7 +701,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Sacar la rienda de la plantera</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -713,7 +709,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -723,18 +719,18 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.41606</v>
+        <v>-58.469148</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.599935</v>
+        <v>-34.687883</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -746,17 +742,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1871</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>9/5/2024</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bulnes 1810</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -766,7 +762,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>796016024</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -781,7 +777,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -794,7 +790,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -803,14 +799,14 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.413803</v>
+        <v>-58.425764</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.590308</v>
+        <v>-34.604359</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -822,27 +818,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3887</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4819</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>798894281</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -857,7 +853,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -865,7 +861,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -875,18 +871,18 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.432085</v>
+        <v>-58.467789</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.60178</v>
+        <v>-34.68463</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -898,27 +894,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3893</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>HERRERA 402</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>798894295</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -933,7 +929,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Inclinado En el form cargaron foto de otro caso</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -941,7 +937,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -951,50 +947,50 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.378613</v>
+        <v>-58.492605</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.6349</v>
+        <v>-34.581454</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>5937</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>José Andrés Pacheco de Melo 2084</t>
+          <t>MONROE 4833</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>807044121</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1004,12 +1000,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1022,51 +1018,55 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M8" t="n">
-        <v>-58.395656</v>
+        <v>-58.483104</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.590364</v>
+        <v>-34.572353</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3938</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11/5/2024</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2604</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>799246642</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Realizar traspasos y retiro de columna vieja</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1103,46 +1103,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.426169</v>
+        <v>-58.483927</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.579697</v>
+        <v>-34.570689</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4025</t>
+          <t>-593</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MEXICO 4249</t>
+          <t>Husares 2250</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>799981143</t>
+          <t>809642190</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Ver foto, colocar columna para traspasar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1179,46 +1179,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.425997</v>
+        <v>-58.443269</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.620454</v>
+        <v>-34.552209</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>4222</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>HUMAHUACA 4500</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>800810078</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Columna con base corroída/oxidada</t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1255,10 +1255,10 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.428283</v>
+        <v>-58.443196</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.601207</v>
+        <v>-34.618534</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1274,27 +1274,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>4426</t>
+          <t>5884</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>12/19/2024</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>LORA, FELIX 27</t>
+          <t>OLLEROS 2952</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>801768138</t>
+          <t>799450967</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
+          <t>Solo retirar columna ya se realizo traspaso</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1331,14 +1331,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.443626</v>
+        <v>-58.447022</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.621032</v>
+        <v>-34.575873</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1350,27 +1350,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>6243</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/30/2024</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>GARCIA, TEODORO 3252</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>779373118</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Colocar R400 para posterior traspaso</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1407,46 +1407,46 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.450789</v>
+        <v>-58.395063</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.577949</v>
+        <v>-34.606257</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-51</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/5/2024</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CHARCAS /ALT/ 4176</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>782773317</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1461,20 +1461,20 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">columna de 114mm de nuestra propiedad que esta quebrada y en mal estado, para remplazar ubicada en CHARCAS 4176 </t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1483,14 +1483,14 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.421741</v>
+        <v>-58.429977</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.584789</v>
+        <v>-34.615514</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1502,27 +1502,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-212</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>FIGUEROA CNEL APOLINARIO /ALT/ 863</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>799485362</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1537,20 +1537,20 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir el traspaso</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1559,46 +1559,46 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.450579</v>
+        <v>-58.421623</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.607673</v>
+        <v>-34.614541</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5884</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>OLLEROS 2952</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>799450967</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1613,11 +1613,11 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1635,14 +1635,14 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.447022</v>
+        <v>-58.400156</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.575873</v>
+        <v>-34.631369</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1654,27 +1654,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1702,7 +1702,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1711,36 +1711,36 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.496935</v>
+        <v>-58.415839</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.599084</v>
+        <v>-34.599291</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1787,10 +1787,10 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.400156</v>
+        <v>-58.375515</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.631369</v>
+        <v>-34.634393</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1806,27 +1806,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1849,12 +1849,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1863,14 +1863,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.402062</v>
+        <v>-58.439751</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.635143</v>
+        <v>-34.609908</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1882,27 +1882,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4696</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2/10/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>YERBAL 489</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>803607520</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1917,11 +1917,11 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron nodo</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1939,14 +1939,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.438053</v>
+        <v>-58.371855</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.617481</v>
+        <v>-34.646958</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1958,27 +1958,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2/14/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CHACO 195</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>803607699</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Desmontar columna personal propio traspaso nodo</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -2015,46 +2015,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.431522</v>
+        <v>-58.513643</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.617523</v>
+        <v>-34.594169</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2069,11 +2069,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2091,14 +2091,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.371855</v>
+        <v>-58.384097</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.646958</v>
+        <v>-34.598913</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2110,27 +2110,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2145,11 +2145,11 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2167,14 +2167,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.403583</v>
+        <v>-58.432805</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.591604</v>
+        <v>-34.574345</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2186,27 +2186,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2216,12 +2216,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2234,23 +2234,23 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.441405</v>
+        <v>-58.363292</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.594348</v>
+        <v>-34.642869</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2262,27 +2262,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>-51</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/5/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>CHARCAS /ALT/ 4176</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>782773317</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2292,12 +2292,16 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">columna de 114mm de nuestra propiedad que esta quebrada y en mal estado, para remplazar ubicada en CHARCAS 4176 </t>
+        </is>
+      </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2315,14 +2319,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.483821</v>
+        <v>-58.421741</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.677698</v>
+        <v>-34.584789</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2334,27 +2338,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>-506</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>Espinosa 591</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>808150511</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2373,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2391,14 +2395,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.445131</v>
+        <v>-58.449</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.572117</v>
+        <v>-34.616077</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2410,17 +2414,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>-502</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>Tagle 2562</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2430,7 +2434,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>808036198</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2449,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
+          <t>Colocar columna para pedir traspaso nodo teco</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2458,7 +2462,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2467,14 +2471,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.425764</v>
+        <v>-58.400188</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.604359</v>
+        <v>-34.583882</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2486,27 +2490,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,11 +2525,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2539,18 +2543,18 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.439751</v>
+        <v>-58.405749</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.609908</v>
+        <v>-34.58224</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2562,27 +2566,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>4938</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>2/14/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>CHACO 195</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>803607699</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2597,7 +2601,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Desmontar columna personal propio traspaso nodo</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2610,7 +2614,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2619,14 +2623,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.375515</v>
+        <v>-58.431522</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.634393</v>
+        <v>-34.617523</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2638,27 +2642,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2677,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2681,7 +2685,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2695,14 +2699,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.415839</v>
+        <v>-58.432644</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.599291</v>
+        <v>-34.595434</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2714,27 +2718,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2749,7 +2753,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2762,7 +2766,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2771,14 +2775,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.469148</v>
+        <v>-58.402062</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.687883</v>
+        <v>-34.635143</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2790,27 +2794,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>4696</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>2/10/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>YERBAL 489</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>803607520</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2829,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Desmonte de columna ya traspasaron nodo</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2847,14 +2851,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.395063</v>
+        <v>-58.438053</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.606257</v>
+        <v>-34.617481</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2866,27 +2870,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2896,12 +2900,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2909,12 +2913,12 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2923,46 +2927,46 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.429977</v>
+        <v>-58.496935</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.615514</v>
+        <v>-34.599084</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>-451</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>Uriarte 2426</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>807044071</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2981,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2985,12 +2989,12 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2999,14 +3003,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.421623</v>
+        <v>-58.423551</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.614541</v>
+        <v>-34.581258</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3018,7 +3022,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-416</t>
+          <t>-445</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3028,17 +3032,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Paraguay 3765</t>
+          <t>Joaquin V Gonzalez 4410</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806926557</t>
+          <t>806945058</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,7 +3057,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3066,55 +3070,55 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.416562</v>
+        <v>-58.51232</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.590589</v>
+        <v>-34.595637</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>4426</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>12/19/2024</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>LORA, FELIX 27</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>801768138</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3129,7 +3133,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3142,7 +3146,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3151,10 +3155,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.429972</v>
+        <v>-58.443626</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.632042</v>
+        <v>-34.621032</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3170,7 +3174,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3180,17 +3184,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3200,16 +3204,16 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3218,7 +3222,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3227,46 +3231,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.47888</v>
+        <v>-58.406585</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.571108</v>
+        <v>-34.592933</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,11 +3285,11 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3303,14 +3307,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.443196</v>
+        <v>-58.403583</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.618534</v>
+        <v>-34.591604</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3398,7 +3402,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-438</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3408,17 +3412,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Juncal 4565</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>806926927</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3433,7 +3437,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3446,7 +3450,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3455,26 +3459,26 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.423148</v>
+        <v>-58.47888</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.576964</v>
+        <v>-34.571108</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3484,17 +3488,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3504,16 +3508,16 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3522,7 +3526,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3531,14 +3535,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.406585</v>
+        <v>-58.429972</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.592933</v>
+        <v>-34.632042</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3550,27 +3554,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-445</t>
+          <t>4222</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>11/28/2024</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4410</t>
+          <t>HUMAHUACA 4500</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>806945058</t>
+          <t>800810078</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,7 +3589,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Columna con base corroída/oxidada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3603,50 +3607,50 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.51232</v>
+        <v>-58.428283</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.595637</v>
+        <v>-34.601207</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5937</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>MONROE 4833</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807044121</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3656,14 +3660,10 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>Columna con base corroída</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr"/>
       <c r="I43" t="n">
         <v>1</v>
       </c>
@@ -3674,7 +3674,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3683,46 +3683,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.483104</v>
+        <v>-58.483821</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.572353</v>
+        <v>-34.677698</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>-416</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>Paraguay 3765</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>806926557</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3745,60 +3745,60 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.483927</v>
+        <v>-58.416562</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.570689</v>
+        <v>-34.590589</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>4025</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>11/12/2024</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>MEXICO 4249</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>799981143</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Ver foto, colocar columna para traspasar</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3826,7 +3826,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3835,46 +3835,46 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.492605</v>
+        <v>-58.425997</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.581454</v>
+        <v>-34.620454</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>3938</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>GODOY CRUZ 2604</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>799246642</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Realizar traspasos y retiro de columna vieja</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3897,7 +3897,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3907,18 +3907,18 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.467789</v>
+        <v>-58.426169</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.68463</v>
+        <v>-34.579697</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3930,27 +3930,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-451</t>
+          <t>3893</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Uriarte 2426</t>
+          <t>HERRERA 402</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807044071</t>
+          <t>798894295</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Inclinado En el form cargaron foto de otro caso</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3973,28 +3973,28 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.423551</v>
+        <v>-58.378613</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.581258</v>
+        <v>-34.6349</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -4006,27 +4006,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>3887</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>ESTADO DE ISRAEL AV. 4819</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>798894281</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4049,7 +4049,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4059,14 +4059,14 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.432644</v>
+        <v>-58.432085</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.595434</v>
+        <v>-34.60178</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4082,27 +4082,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,36 +4117,36 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.405749</v>
+        <v>-58.445131</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.58224</v>
+        <v>-34.572117</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4158,27 +4158,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-502</t>
+          <t>3154</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>8/27/2024</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Tagle 2562</t>
+          <t>BRAVO, MARIO 853</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808036198</t>
+          <t>795498456</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso nodo teco</t>
+          <t>Sacar la rienda de la plantera</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4201,28 +4201,28 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.400188</v>
+        <v>-58.41606</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.583882</v>
+        <v>-34.599935</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4234,27 +4234,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-506</t>
+          <t>2805</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>8/6/2024</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Espinosa 591</t>
+          <t>MCAL SOLANO LOPEZ 3110</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808150511</t>
+          <t>792101640</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna. TLC ya traspaso nodo</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4282,7 +4282,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4291,46 +4291,46 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.449</v>
+        <v>-58.498448</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.616077</v>
+        <v>-34.595287</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>2463</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2024</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>795698153</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4358,23 +4358,23 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.363292</v>
+        <v>-58.40589</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.642869</v>
+        <v>-34.584156</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4386,27 +4386,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-517</t>
+          <t>-212</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Av Dorrego 2721</t>
+          <t>FIGUEROA CNEL APOLINARIO /ALT/ 863</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808373635</t>
+          <t>799485362</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,11 +4421,11 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
+          <t>Colocar columna para pedir el traspaso</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -4434,7 +4434,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4443,46 +4443,46 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.432805</v>
+        <v>-58.450579</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.574345</v>
+        <v>-34.607673</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4492,12 +4492,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4510,7 +4510,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -4519,14 +4519,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.384097</v>
+        <v>-58.441405</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.598913</v>
+        <v>-34.594348</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4538,27 +4538,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-531</t>
+          <t>1871</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>9/5/2024</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4632</t>
+          <t>Bulnes 1810</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808530239</t>
+          <t>796016024</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
+          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4586,7 +4586,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -4595,95 +4595,19 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.513643</v>
+        <v>-58.413803</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.594169</v>
+        <v>-34.590308</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>-593</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>9/10/2025</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Husares 2250</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>809642190</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I56" t="n">
-        <v>1</v>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M56" t="n">
-        <v>-58.443269</v>
-      </c>
-      <c r="N56" t="n">
-        <v>-34.552209</v>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P56" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-23 08:47:50)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -518,17 +518,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>2463</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>7/15/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>José Andrés Pacheco de Melo 2084</t>
+          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>795698153</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -548,12 +548,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
+          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
         </is>
       </c>
       <c r="I2" t="n">
@@ -566,15 +566,19 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr"/>
+          <t>Nodo TLC</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M2" t="n">
-        <v>-58.395656</v>
+        <v>-58.40589</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.590364</v>
+        <v>-34.584156</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -590,27 +594,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>6243</t>
+          <t>2805</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1/30/2024</t>
+          <t>8/6/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>GARCIA, TEODORO 3252</t>
+          <t>MCAL SOLANO LOPEZ 3110</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>779373118</t>
+          <t>792101640</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -625,7 +629,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Colocar R400 para posterior traspaso</t>
+          <t>Retirar columna. TLC ya traspaso nodo</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -638,7 +642,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -647,14 +651,14 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.450789</v>
+        <v>-58.498448</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.577949</v>
+        <v>-34.595287</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -666,27 +670,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>3154</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>8/27/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>BRAVO, MARIO 853</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>795498456</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -701,7 +705,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Sacar la rienda de la plantera</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -709,7 +713,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -719,18 +723,18 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.469148</v>
+        <v>-58.41606</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.687883</v>
+        <v>-34.599935</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -742,17 +746,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>1871</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>9/5/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>Bulnes 1810</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -762,7 +766,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>796016024</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -777,7 +781,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
+          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -790,7 +794,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -799,14 +803,14 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.425764</v>
+        <v>-58.413803</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.604359</v>
+        <v>-34.590308</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -818,27 +822,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>3887</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>ESTADO DE ISRAEL AV. 4819</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>798894281</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -853,7 +857,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -861,7 +865,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -871,18 +875,18 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.467789</v>
+        <v>-58.432085</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.68463</v>
+        <v>-34.60178</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -894,27 +898,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>3893</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>HERRERA 402</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>798894295</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -929,7 +933,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Inclinado En el form cargaron foto de otro caso</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -937,7 +941,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -947,50 +951,50 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-58.492605</v>
+        <v>-58.378613</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.581454</v>
+        <v>-34.6349</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>5937</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MONROE 4833</t>
+          <t>José Andrés Pacheco de Melo 2084</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>807044121</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1000,12 +1004,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1018,55 +1022,51 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
-        <v>-58.483104</v>
+        <v>-58.395656</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.572353</v>
+        <v>-34.590364</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>3938</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>GODOY CRUZ 2604</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>799246642</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Realizar traspasos y retiro de columna vieja</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1103,46 +1103,46 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.483927</v>
+        <v>-58.426169</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.570689</v>
+        <v>-34.579697</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>-593</t>
+          <t>4025</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>11/12/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Husares 2250</t>
+          <t>MEXICO 4249</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>809642190</t>
+          <t>799981143</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1157,7 +1157,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Ver foto, colocar columna para traspasar</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1179,46 +1179,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.443269</v>
+        <v>-58.425997</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.552209</v>
+        <v>-34.620454</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>4222</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>11/28/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>HUMAHUACA 4500</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>800810078</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1233,7 +1233,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Columna con base corroída/oxidada</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1255,10 +1255,10 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.443196</v>
+        <v>-58.428283</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.618534</v>
+        <v>-34.601207</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1274,27 +1274,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5884</t>
+          <t>4426</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>12/19/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>OLLEROS 2952</t>
+          <t>LORA, FELIX 27</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>799450967</t>
+          <t>801768138</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1309,11 +1309,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso</t>
+          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1331,14 +1331,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.447022</v>
+        <v>-58.443626</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.575873</v>
+        <v>-34.621032</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1350,27 +1350,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>6243</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>1/30/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>GARCIA, TEODORO 3252</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>779373118</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Colocar R400 para posterior traspaso</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1407,46 +1407,46 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.395063</v>
+        <v>-58.450789</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.606257</v>
+        <v>-34.577949</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>-51</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>4/5/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>CHARCAS /ALT/ 4176</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>782773317</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1461,20 +1461,20 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t xml:space="preserve">columna de 114mm de nuestra propiedad que esta quebrada y en mal estado, para remplazar ubicada en CHARCAS 4176 </t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1483,14 +1483,14 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.429977</v>
+        <v>-58.421741</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.615514</v>
+        <v>-34.584789</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1502,27 +1502,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>-212</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>FIGUEROA CNEL APOLINARIO /ALT/ 863</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>799485362</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1537,20 +1537,20 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar columna para pedir el traspaso</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1559,46 +1559,46 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.421623</v>
+        <v>-58.450579</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.614541</v>
+        <v>-34.607673</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>5884</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>OLLEROS 2952</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>799450967</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1613,11 +1613,11 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Solo retirar columna ya se realizo traspaso</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1635,14 +1635,14 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.400156</v>
+        <v>-58.447022</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.631369</v>
+        <v>-34.575873</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1654,27 +1654,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1702,7 +1702,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1711,36 +1711,36 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.415839</v>
+        <v>-58.496935</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.599291</v>
+        <v>-34.599084</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1787,10 +1787,10 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.375515</v>
+        <v>-58.400156</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.634393</v>
+        <v>-34.631369</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1806,27 +1806,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1849,12 +1849,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1863,14 +1863,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.439751</v>
+        <v>-58.402062</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.609908</v>
+        <v>-34.635143</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1882,27 +1882,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>4696</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>2/10/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>YERBAL 489</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>803607520</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1917,11 +1917,11 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Desmonte de columna ya traspasaron nodo</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1939,14 +1939,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.371855</v>
+        <v>-58.438053</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.646958</v>
+        <v>-34.617481</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1958,27 +1958,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-531</t>
+          <t>4938</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>2/14/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4632</t>
+          <t>CHACO 195</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>808530239</t>
+          <t>803607699</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
+          <t>Desmontar columna personal propio traspaso nodo</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -2015,46 +2015,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.513643</v>
+        <v>-58.431522</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.594169</v>
+        <v>-34.617523</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2069,11 +2069,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2091,14 +2091,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.384097</v>
+        <v>-58.371855</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.598913</v>
+        <v>-34.646958</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2110,27 +2110,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-517</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Av Dorrego 2721</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>808373635</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2145,11 +2145,11 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2167,14 +2167,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.432805</v>
+        <v>-58.403583</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.574345</v>
+        <v>-34.591604</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2186,27 +2186,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2216,12 +2216,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2234,23 +2234,23 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.363292</v>
+        <v>-58.441405</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.642869</v>
+        <v>-34.594348</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2262,27 +2262,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-51</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/5/2024</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>CHARCAS /ALT/ 4176</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>782773317</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2292,16 +2292,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">columna de 114mm de nuestra propiedad que esta quebrada y en mal estado, para remplazar ubicada en CHARCAS 4176 </t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2319,14 +2315,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.421741</v>
+        <v>-58.483821</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.584789</v>
+        <v>-34.677698</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2338,27 +2334,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-506</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Espinosa 591</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>808150511</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2373,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2395,14 +2391,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.449</v>
+        <v>-58.445131</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.616077</v>
+        <v>-34.572117</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2414,17 +2410,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-502</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Tagle 2562</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -2434,7 +2430,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>808036198</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2449,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso nodo teco</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2462,7 +2458,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2471,14 +2467,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.400188</v>
+        <v>-58.425764</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.583882</v>
+        <v>-34.604359</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2490,27 +2486,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2525,11 +2521,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2543,18 +2539,18 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.405749</v>
+        <v>-58.439751</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.58224</v>
+        <v>-34.609908</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2566,27 +2562,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2/14/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CHACO 195</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>803607699</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2601,7 +2597,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Desmontar columna personal propio traspaso nodo</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2614,7 +2610,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2623,14 +2619,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.431522</v>
+        <v>-58.375515</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.617523</v>
+        <v>-34.634393</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2642,27 +2638,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2677,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2685,7 +2681,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2699,14 +2695,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.432644</v>
+        <v>-58.415839</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.595434</v>
+        <v>-34.599291</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2718,27 +2714,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2753,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2766,7 +2762,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2775,14 +2771,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.402062</v>
+        <v>-58.469148</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.635143</v>
+        <v>-34.687883</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2794,27 +2790,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4696</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2/10/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>YERBAL 489</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>803607520</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2829,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron nodo</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2851,14 +2847,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.438053</v>
+        <v>-58.395063</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.617481</v>
+        <v>-34.606257</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2870,27 +2866,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2900,12 +2896,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2913,12 +2909,12 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2927,46 +2923,46 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.496935</v>
+        <v>-58.429977</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.599084</v>
+        <v>-34.615514</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-451</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Uriarte 2426</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807044071</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2981,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2989,12 +2985,12 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -3003,14 +2999,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.423551</v>
+        <v>-58.421623</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.581258</v>
+        <v>-34.614541</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3022,7 +3018,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-445</t>
+          <t>-416</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3032,17 +3028,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4410</t>
+          <t>Paraguay 3765</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806945058</t>
+          <t>806926557</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3057,7 +3053,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3070,55 +3066,55 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.51232</v>
+        <v>-58.416562</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.595637</v>
+        <v>-34.590589</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>4426</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>12/19/2024</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LORA, FELIX 27</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>801768138</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3133,7 +3129,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3146,7 +3142,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3155,10 +3151,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.443626</v>
+        <v>-58.429972</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.621032</v>
+        <v>-34.632042</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3174,7 +3170,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3184,17 +3180,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3204,16 +3200,16 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3222,7 +3218,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3231,46 +3227,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.406585</v>
+        <v>-58.47888</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.592933</v>
+        <v>-34.571108</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3285,11 +3281,11 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3307,14 +3303,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.403583</v>
+        <v>-58.443196</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.591604</v>
+        <v>-34.618534</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3402,7 +3398,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3412,17 +3408,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3432,16 +3428,16 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3450,7 +3446,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3459,26 +3455,26 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.47888</v>
+        <v>-58.406585</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.571108</v>
+        <v>-34.592933</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-445</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3488,17 +3484,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>Joaquin V Gonzalez 4410</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>806945058</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3513,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3531,50 +3527,50 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.429972</v>
+        <v>-58.51232</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.632042</v>
+        <v>-34.595637</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>4222</t>
+          <t>5937</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>HUMAHUACA 4500</t>
+          <t>MONROE 4833</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>800810078</t>
+          <t>807044121</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3589,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Columna con base corroída/oxidada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3611,46 +3607,46 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.428283</v>
+        <v>-58.483104</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.601207</v>
+        <v>-34.572353</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3660,69 +3656,73 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
       <c r="I43" t="n">
         <v>1</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.483821</v>
+        <v>-58.483927</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.677698</v>
+        <v>-34.570689</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-416</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Paraguay 3765</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>806926557</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3759,46 +3759,46 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.416562</v>
+        <v>-58.492605</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.590589</v>
+        <v>-34.581454</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>4025</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>MEXICO 4249</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>799981143</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Ver foto, colocar columna para traspasar</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3826,7 +3826,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3835,14 +3835,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.425997</v>
+        <v>-58.467789</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.620454</v>
+        <v>-34.68463</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3854,17 +3854,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>3938</t>
+          <t>-451</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>11/5/2024</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2604</t>
+          <t>Uriarte 2426</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>799246642</t>
+          <t>807044071</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Realizar traspasos y retiro de columna vieja</t>
+          <t>Colocar columna para pedir traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3897,24 +3897,24 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.426169</v>
+        <v>-58.423551</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.579697</v>
+        <v>-34.581258</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3930,27 +3930,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>3893</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>HERRERA 402</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>798894295</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Inclinado En el form cargaron foto de otro caso</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3973,7 +3973,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3983,18 +3983,18 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.378613</v>
+        <v>-58.432644</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.6349</v>
+        <v>-34.595434</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -4006,27 +4006,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>3887</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4819</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>798894281</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,11 +4041,11 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4063,14 +4063,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.432085</v>
+        <v>-58.405749</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.60178</v>
+        <v>-34.58224</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4082,27 +4082,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>-502</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>Tagle 2562</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>808036198</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Colocar columna para pedir traspaso nodo teco</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4139,14 +4139,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.445131</v>
+        <v>-58.400188</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.572117</v>
+        <v>-34.583882</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4158,27 +4158,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>3154</t>
+          <t>-506</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>8/27/2024</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>BRAVO, MARIO 853</t>
+          <t>Espinosa 591</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>795498456</t>
+          <t>808150511</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Sacar la rienda de la plantera</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4201,28 +4201,28 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.41606</v>
+        <v>-58.449</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.599935</v>
+        <v>-34.616077</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4234,27 +4234,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>MCAL SOLANO LOPEZ 3110</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>792101640</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Retirar columna. TLC ya traspaso nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4282,55 +4282,55 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.498448</v>
+        <v>-58.363292</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.595287</v>
+        <v>-34.642869</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2463</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/15/2024</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>795698153</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4345,7 +4345,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4367,14 +4367,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.40589</v>
+        <v>-58.432805</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.584156</v>
+        <v>-34.574345</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4386,27 +4386,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-212</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>FIGUEROA CNEL APOLINARIO /ALT/ 863</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>799485362</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4421,11 +4421,11 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir el traspaso</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -4434,7 +4434,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4443,46 +4443,46 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.450579</v>
+        <v>-58.384097</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.607673</v>
+        <v>-34.598913</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4492,12 +4492,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4510,7 +4510,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -4519,46 +4519,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.441405</v>
+        <v>-58.513643</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.594348</v>
+        <v>-34.594169</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>1871</t>
+          <t>-593</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>9/5/2024</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Bulnes 1810</t>
+          <t>Husares 2250</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>796016024</t>
+          <t>809642190</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4573,7 +4573,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4586,7 +4586,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -4595,19 +4595,19 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.413803</v>
+        <v>-58.443269</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.590308</v>
+        <v>-34.552209</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-25 09:19:02)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P55"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1426,27 +1426,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>-51</t>
+          <t>5884</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4/5/2024</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CHARCAS /ALT/ 4176</t>
+          <t>OLLEROS 2952</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>782773317</t>
+          <t>799450967</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t xml:space="preserve">columna de 114mm de nuestra propiedad que esta quebrada y en mal estado, para remplazar ubicada en CHARCAS 4176 </t>
+          <t>Solo retirar columna ya se realizo traspaso</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1483,10 +1483,10 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.421741</v>
+        <v>-58.447022</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.584789</v>
+        <v>-34.575873</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1502,27 +1502,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>-212</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>FIGUEROA CNEL APOLINARIO /ALT/ 863</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>799485362</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1532,16 +1532,16 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir el traspaso</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1559,10 +1559,10 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.450579</v>
+        <v>-58.496935</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.607673</v>
+        <v>-34.599084</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1578,27 +1578,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5884</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>OLLEROS 2952</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>799450967</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1613,11 +1613,11 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1635,14 +1635,14 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.447022</v>
+        <v>-58.400156</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.575873</v>
+        <v>-34.631369</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1654,27 +1654,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1684,12 +1684,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1711,46 +1711,46 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.496935</v>
+        <v>-58.402062</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.599084</v>
+        <v>-34.635143</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>4696</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>2/10/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>YERBAL 489</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>803607520</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Desmonte de columna ya traspasaron nodo</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1787,14 +1787,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.400156</v>
+        <v>-58.438053</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.631369</v>
+        <v>-34.617481</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1806,27 +1806,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>4938</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>2/14/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>CHACO 195</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>803607699</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Desmontar columna personal propio traspaso nodo</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1863,14 +1863,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.402062</v>
+        <v>-58.431522</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.635143</v>
+        <v>-34.617523</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1882,27 +1882,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4696</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2/10/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>YERBAL 489</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>803607520</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1917,11 +1917,11 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron nodo</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1939,14 +1939,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.438053</v>
+        <v>-58.371855</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.617481</v>
+        <v>-34.646958</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1958,27 +1958,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2/14/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>CHACO 195</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>803607699</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1993,11 +1993,11 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Desmontar columna personal propio traspaso nodo</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -2015,14 +2015,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.431522</v>
+        <v>-58.403583</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.617523</v>
+        <v>-34.591604</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2034,27 +2034,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2064,16 +2064,16 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2082,7 +2082,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2091,14 +2091,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.371855</v>
+        <v>-58.441405</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.646958</v>
+        <v>-34.594348</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2110,27 +2110,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2140,16 +2140,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Base picada</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2158,7 +2154,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2167,14 +2163,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.403583</v>
+        <v>-58.483821</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.591604</v>
+        <v>-34.677698</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2186,27 +2182,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2216,12 +2212,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2243,10 +2239,10 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.441405</v>
+        <v>-58.445131</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.594348</v>
+        <v>-34.572117</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2262,27 +2258,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2292,10 +2288,14 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
+        </is>
+      </c>
       <c r="I25" t="n">
         <v>1</v>
       </c>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2315,14 +2315,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.483821</v>
+        <v>-58.425764</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.677698</v>
+        <v>-34.604359</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2334,27 +2334,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2377,12 +2377,12 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2391,14 +2391,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.445131</v>
+        <v>-58.439751</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.572117</v>
+        <v>-34.609908</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2410,27 +2410,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2467,14 +2467,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.425764</v>
+        <v>-58.375515</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.604359</v>
+        <v>-34.634393</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2486,27 +2486,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2543,10 +2543,10 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.439751</v>
+        <v>-58.415839</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.609908</v>
+        <v>-34.599291</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2562,27 +2562,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2597,7 +2597,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2619,14 +2619,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.375515</v>
+        <v>-58.469148</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.634393</v>
+        <v>-34.687883</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2638,27 +2638,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2695,10 +2695,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.415839</v>
+        <v>-58.395063</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.599291</v>
+        <v>-34.606257</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -2714,27 +2714,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2749,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2757,7 +2757,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2771,10 +2771,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.469148</v>
+        <v>-58.429977</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.687883</v>
+        <v>-34.615514</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2790,7 +2790,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2800,17 +2800,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2833,12 +2833,12 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2847,10 +2847,10 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.395063</v>
+        <v>-58.421623</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.606257</v>
+        <v>-34.614541</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2866,27 +2866,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2909,7 +2909,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2923,10 +2923,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.429977</v>
+        <v>-58.429972</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.615514</v>
+        <v>-34.632042</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2942,27 +2942,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2985,7 +2985,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2999,26 +2999,26 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.421623</v>
+        <v>-58.47888</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.614541</v>
+        <v>-34.571108</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-416</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3028,17 +3028,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Paraguay 3765</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806926557</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3075,14 +3075,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.416562</v>
+        <v>-58.443196</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.590589</v>
+        <v>-34.618534</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3094,7 +3094,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3104,17 +3104,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3124,16 +3124,16 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3151,14 +3151,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.429972</v>
+        <v>-58.406585</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.632042</v>
+        <v>-34.592933</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3170,7 +3170,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>-445</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3180,17 +3180,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>Joaquin V Gonzalez 4410</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>806945058</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3205,7 +3205,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3223,18 +3223,18 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.47888</v>
+        <v>-58.51232</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.571108</v>
+        <v>-34.595637</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3246,27 +3246,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>5937</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>MONROE 4833</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>807044121</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3303,46 +3303,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.443196</v>
+        <v>-58.483104</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.618534</v>
+        <v>-34.572353</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-437</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Cochabamba 4090</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>806926861</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3357,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Columna base podrida colocar r400 para pedir traspaso de fuente</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3365,60 +3365,60 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.422268</v>
+        <v>-58.483927</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.627754</v>
+        <v>-34.570689</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3428,16 +3428,16 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3455,46 +3455,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.406585</v>
+        <v>-58.492605</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.592933</v>
+        <v>-34.581454</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-445</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4410</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>806945058</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3509,7 +3509,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3527,50 +3527,50 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.51232</v>
+        <v>-58.467789</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.595637</v>
+        <v>-34.68463</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5937</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>MONROE 4833</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807044121</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3593,7 +3593,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3607,46 +3607,46 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.483104</v>
+        <v>-58.432644</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.572353</v>
+        <v>-34.595434</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3661,11 +3661,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3683,46 +3683,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.483927</v>
+        <v>-58.405749</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.570689</v>
+        <v>-34.58224</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3755,50 +3755,50 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.492605</v>
+        <v>-58.363292</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.581454</v>
+        <v>-34.642869</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3813,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3835,14 +3835,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.467789</v>
+        <v>-58.432805</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.68463</v>
+        <v>-34.574345</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3854,27 +3854,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-451</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Uriarte 2426</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807044071</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo teco</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3902,7 +3902,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3911,14 +3911,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.423551</v>
+        <v>-58.384097</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.581258</v>
+        <v>-34.598913</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3930,27 +3930,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3965,7 +3965,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3973,7 +3973,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3987,46 +3987,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.432644</v>
+        <v>-58.513643</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.595434</v>
+        <v>-34.594169</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>-593</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>Husares 2250</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>809642190</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4041,15 +4041,15 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4059,553 +4059,21 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.405749</v>
+        <v>-58.443269</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.58224</v>
+        <v>-34.552209</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>-502</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>7/7/2025</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Tagle 2562</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>808036198</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Colocar columna para pedir traspaso nodo teco</t>
-        </is>
-      </c>
-      <c r="I49" t="n">
-        <v>1</v>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M49" t="n">
-        <v>-58.400188</v>
-      </c>
-      <c r="N49" t="n">
-        <v>-34.583882</v>
-      </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>Recoleta</t>
-        </is>
-      </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>-506</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>7/11/2025</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Espinosa 591</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>808150511</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I50" t="n">
-        <v>1</v>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M50" t="n">
-        <v>-58.449</v>
-      </c>
-      <c r="N50" t="n">
-        <v>-34.616077</v>
-      </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>Boedo</t>
-        </is>
-      </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>-511</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>7/14/2025</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Carlos Melo 491</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>808194932</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I51" t="n">
-        <v>1</v>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M51" t="n">
-        <v>-58.363292</v>
-      </c>
-      <c r="N51" t="n">
-        <v>-34.642869</v>
-      </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P51" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>-517</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>7/16/2025</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Av Dorrego 2721</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>808373635</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
-        </is>
-      </c>
-      <c r="I52" t="n">
-        <v>1</v>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M52" t="n">
-        <v>-58.432805</v>
-      </c>
-      <c r="N52" t="n">
-        <v>-34.574345</v>
-      </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>-529</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>7/23/2025</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Libertad 820</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>ICD30189941</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
-        </is>
-      </c>
-      <c r="I53" t="n">
-        <v>1</v>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M53" t="n">
-        <v>-58.384097</v>
-      </c>
-      <c r="N53" t="n">
-        <v>-34.598913</v>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>Recoleta</t>
-        </is>
-      </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>-531</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>7/25/2025</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Joaquin V Gonzalez 4632</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>808530239</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
-        </is>
-      </c>
-      <c r="I54" t="n">
-        <v>1</v>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M54" t="n">
-        <v>-58.513643</v>
-      </c>
-      <c r="N54" t="n">
-        <v>-34.594169</v>
-      </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P54" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>-593</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>9/10/2025</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Husares 2250</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>809642190</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I55" t="n">
-        <v>1</v>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M55" t="n">
-        <v>-58.443269</v>
-      </c>
-      <c r="N55" t="n">
-        <v>-34.552209</v>
-      </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P55" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-25 12:08:49)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:R48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,16 @@
           <t>Zona</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>PD</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>N2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -590,6 +600,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>AGU-J</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -666,6 +686,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>PUE-G</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -742,6 +772,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>CLI-G</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -818,6 +858,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>VCR-E</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -894,6 +944,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>CLI-N</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -968,6 +1028,16 @@
       <c r="P7" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>CON-H</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -1042,6 +1112,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>RET-C</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1118,6 +1198,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>VCR-N</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1194,6 +1284,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>ALM-B</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1270,6 +1370,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>CLI-N</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1346,6 +1456,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>PCH-G</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1422,6 +1542,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>ATH-P</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1498,6 +1628,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>ATH-P</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1574,6 +1714,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>PUE-B</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1650,6 +1800,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>PPT-F</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PPT</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1726,6 +1886,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>PPT-K</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1802,6 +1972,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>ALM-G</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1878,6 +2058,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>ALM-F</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1954,6 +2144,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>CON-A</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2030,6 +2230,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>AGU-F</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2104,6 +2314,16 @@
       <c r="P22" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>VCR-H</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -2178,6 +2398,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>PAV-Q</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2254,6 +2484,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>COG-C</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2330,6 +2570,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>ALM-L</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2406,6 +2656,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>ALM-I</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2482,6 +2742,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>CON-B</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2558,6 +2828,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>CLI-L</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2634,6 +2914,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>PAV-T</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2710,6 +3000,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>CLI-B</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2786,6 +3086,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>ALM-J</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2862,6 +3172,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>ALM-C</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2938,6 +3258,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>PPT-S</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3014,6 +3344,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>ATH-J</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3090,6 +3430,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>NRA-A</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3166,6 +3516,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>AGU-B</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3242,6 +3602,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>PUE-O</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PUE</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3318,6 +3688,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>ATH-C</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3394,6 +3774,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>PUE-E</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3470,6 +3860,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>PUE-K</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3546,6 +3946,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>PAV-U</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3622,6 +4032,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>VCR-I</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3698,6 +4118,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>AGU-N</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3774,6 +4204,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>CON-E</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3850,6 +4290,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>BLO-G</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -3926,6 +4376,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>RET-S</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4002,6 +4462,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>PUE-O</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PUE</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4076,6 +4546,16 @@
       <c r="P48" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>BLO-B</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-25 14:24:54)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1298,27 +1298,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>4222</t>
+          <t>4426</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>12/19/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>HUMAHUACA 4500</t>
+          <t>LORA, FELIX 27</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>800810078</t>
+          <t>801768138</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Columna con base corroída/oxidada</t>
+          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1355,14 +1355,14 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.428283</v>
+        <v>-58.443626</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.601207</v>
+        <v>-34.621032</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1372,7 +1372,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>CLI-N</t>
+          <t>PCH-G</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1384,27 +1384,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>4426</t>
+          <t>6243</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>12/19/2024</t>
+          <t>1/30/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>LORA, FELIX 27</t>
+          <t>GARCIA, TEODORO 3252</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>801768138</t>
+          <t>779373118</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
+          <t>Colocar R400 para posterior traspaso</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1441,24 +1441,24 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.443626</v>
+        <v>-58.450789</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.621032</v>
+        <v>-34.577949</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>PCH-G</t>
+          <t>ATH-P</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1470,17 +1470,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>6243</t>
+          <t>5884</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/30/2024</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>GARCIA, TEODORO 3252</t>
+          <t>OLLEROS 2952</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1490,7 +1490,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>779373118</t>
+          <t>799450967</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1505,11 +1505,11 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Colocar R400 para posterior traspaso</t>
+          <t>Solo retirar columna ya se realizo traspaso</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1518,7 +1518,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1527,19 +1527,19 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.450789</v>
+        <v>-58.447022</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.577949</v>
+        <v>-34.575873</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
@@ -1556,27 +1556,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>5884</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>OLLEROS 2952</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>799450967</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1586,16 +1586,16 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1613,24 +1613,24 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.447022</v>
+        <v>-58.496935</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.575873</v>
+        <v>-34.599084</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>ATH-P</t>
+          <t>PUE-B</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
@@ -1642,27 +1642,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1672,12 +1672,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1699,46 +1699,46 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.496935</v>
+        <v>-58.400156</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.599084</v>
+        <v>-34.631369</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PUE-B</t>
+          <t>PPT-F</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PPT</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1776,7 +1776,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1785,10 +1785,10 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.400156</v>
+        <v>-58.402062</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.631369</v>
+        <v>-34.635143</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1802,39 +1802,39 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>PPT-F</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PPT</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>4696</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>2/10/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>YERBAL 489</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>803607520</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1849,7 +1849,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Desmonte de columna ya traspasaron nodo</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1871,14 +1871,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.402062</v>
+        <v>-58.438053</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.635143</v>
+        <v>-34.617481</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>ALM-G</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1900,17 +1900,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>4696</t>
+          <t>4938</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2/10/2025</t>
+          <t>2/14/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>YERBAL 489</t>
+          <t>CHACO 195</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>803607520</t>
+          <t>803607699</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1935,7 +1935,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron nodo</t>
+          <t>Desmontar columna personal propio traspaso nodo</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1957,10 +1957,10 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.438053</v>
+        <v>-58.431522</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.617481</v>
+        <v>-34.617523</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1974,7 +1974,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ALM-G</t>
+          <t>ALM-F</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1986,27 +1986,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2/14/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CHACO 195</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>803607699</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2021,11 +2021,11 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Desmontar columna personal propio traspaso nodo</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -2043,14 +2043,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.431522</v>
+        <v>-58.371855</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.617523</v>
+        <v>-34.646958</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>ALM-F</t>
+          <t>CON-A</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2072,17 +2072,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2092,7 +2092,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2129,14 +2129,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.371855</v>
+        <v>-58.403583</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.646958</v>
+        <v>-34.591604</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>CON-A</t>
+          <t>AGU-F</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2158,27 +2158,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2188,16 +2188,16 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -2215,14 +2215,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.403583</v>
+        <v>-58.441405</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.591604</v>
+        <v>-34.594348</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2232,7 +2232,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>AGU-F</t>
+          <t>VCR-H</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2244,7 +2244,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2254,17 +2254,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2277,11 +2277,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
-        </is>
-      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
         <v>1</v>
       </c>
@@ -2301,14 +2297,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.441405</v>
+        <v>-58.483821</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.594348</v>
+        <v>-34.677698</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2318,7 +2314,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>VCR-H</t>
+          <t>PAV-Q</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2330,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2360,10 +2356,14 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+        </is>
+      </c>
       <c r="I23" t="n">
         <v>1</v>
       </c>
@@ -2383,14 +2383,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.483821</v>
+        <v>-58.445131</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.677698</v>
+        <v>-34.572117</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>PAV-Q</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2460,7 +2460,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -2469,14 +2469,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.445131</v>
+        <v>-58.425764</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.572117</v>
+        <v>-34.604359</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>ALM-L</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2555,10 +2555,10 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.425764</v>
+        <v>-58.439751</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.604359</v>
+        <v>-34.609908</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>ALM-L</t>
+          <t>ALM-I</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,7 +2584,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2594,17 +2594,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2627,7 +2627,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2641,14 +2641,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.439751</v>
+        <v>-58.375515</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.609908</v>
+        <v>-34.634393</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>ALM-I</t>
+          <t>CON-B</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,7 +2705,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2727,14 +2727,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.375515</v>
+        <v>-58.415839</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.634393</v>
+        <v>-34.599291</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2744,7 +2744,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>CON-B</t>
+          <t>CLI-L</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2813,14 +2813,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.415839</v>
+        <v>-58.469148</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.599291</v>
+        <v>-34.687883</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>CLI-L</t>
+          <t>PAV-T</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2890,7 +2890,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2899,14 +2899,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.469148</v>
+        <v>-58.395063</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.687883</v>
+        <v>-34.606257</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2916,7 +2916,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PAV-T</t>
+          <t>CLI-B</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,7 +2928,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2938,17 +2938,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2971,12 +2971,12 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2985,14 +2985,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.395063</v>
+        <v>-58.429977</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.606257</v>
+        <v>-34.615514</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3002,7 +3002,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>CLI-B</t>
+          <t>ALM-J</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,7 +3014,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3071,14 +3071,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.429977</v>
+        <v>-58.421623</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.615514</v>
+        <v>-34.614541</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3088,7 +3088,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>ALM-J</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,27 +3100,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3143,7 +3143,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -3157,14 +3157,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.421623</v>
+        <v>-58.429972</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.614541</v>
+        <v>-34.632042</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -3174,7 +3174,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>PPT-S</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,7 +3186,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3196,17 +3196,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3243,24 +3243,24 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.429972</v>
+        <v>-58.47888</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.632042</v>
+        <v>-34.571108</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>PPT-S</t>
+          <t>ATH-J</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3272,7 +3272,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3282,17 +3282,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3307,7 +3307,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -3329,24 +3329,24 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.47888</v>
+        <v>-58.443196</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.571108</v>
+        <v>-34.618534</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>ATH-J</t>
+          <t>NRA-A</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3358,7 +3358,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3368,17 +3368,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3388,16 +3388,16 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3406,7 +3406,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3415,14 +3415,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.443196</v>
+        <v>-58.406585</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.618534</v>
+        <v>-34.592933</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3432,7 +3432,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>NRA-A</t>
+          <t>AGU-B</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -3444,7 +3444,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>-445</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3454,17 +3454,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>Joaquin V Gonzalez 4410</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>806945058</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3474,16 +3474,16 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3492,65 +3492,65 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.406585</v>
+        <v>-58.51232</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.592933</v>
+        <v>-34.595637</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>AGU-B</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>-445</t>
+          <t>5937</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4410</t>
+          <t>MONROE 4833</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>806945058</t>
+          <t>807044121</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3583,18 +3583,18 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.51232</v>
+        <v>-58.483104</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.595637</v>
+        <v>-34.572353</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3604,39 +3604,39 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>ATH-C</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5937</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>MONROE 4833</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807044121</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3659,7 +3659,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3669,14 +3669,14 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.483104</v>
+        <v>-58.483927</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.572353</v>
+        <v>-34.570689</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3690,7 +3690,7 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>ATH-C</t>
+          <t>PUE-E</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -3702,17 +3702,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3745,7 +3745,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3755,18 +3755,18 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.483927</v>
+        <v>-58.492605</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.570689</v>
+        <v>-34.581454</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3776,7 +3776,7 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>PUE-E</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
@@ -3788,7 +3788,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3798,17 +3798,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3845,24 +3845,24 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.492605</v>
+        <v>-58.467789</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.581454</v>
+        <v>-34.68463</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>PAV-U</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -3874,27 +3874,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3917,7 +3917,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3931,14 +3931,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.467789</v>
+        <v>-58.432644</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.68463</v>
+        <v>-34.595434</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>PAV-U</t>
+          <t>VCR-I</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -3960,27 +3960,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3995,15 +3995,15 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -4013,18 +4013,18 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.432644</v>
+        <v>-58.405749</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.595434</v>
+        <v>-34.58224</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>VCR-I</t>
+          <t>AGU-N</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -4046,27 +4046,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4081,15 +4081,15 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -4103,14 +4103,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.405749</v>
+        <v>-58.363292</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.58224</v>
+        <v>-34.642869</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>AGU-N</t>
+          <t>CON-E</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -4132,27 +4132,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4167,7 +4167,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -4185,18 +4185,18 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.363292</v>
+        <v>-58.432805</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.642869</v>
+        <v>-34.574345</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -4206,7 +4206,7 @@
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>CON-E</t>
+          <t>BLO-G</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -4218,27 +4218,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-517</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Av Dorrego 2721</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808373635</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -4275,14 +4275,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.432805</v>
+        <v>-58.384097</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.574345</v>
+        <v>-34.598913</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -4292,7 +4292,7 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>BLO-G</t>
+          <t>RET-S</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -4304,27 +4304,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -4361,56 +4361,56 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.384097</v>
+        <v>-58.513643</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.598913</v>
+        <v>-34.594169</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>RET-S</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-531</t>
+          <t>-593</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4632</t>
+          <t>Husares 2250</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808530239</t>
+          <t>809642190</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -4425,7 +4425,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -4447,14 +4447,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.513643</v>
+        <v>-58.443269</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.594169</v>
+        <v>-34.552209</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -4464,96 +4464,10 @@
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1PUE</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>-593</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>9/10/2025</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Husares 2250</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>809642190</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I48" t="n">
-        <v>1</v>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M48" t="n">
-        <v>-58.443269</v>
-      </c>
-      <c r="N48" t="n">
-        <v>-34.552209</v>
-      </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>BLO-B</t>
-        </is>
-      </c>
-      <c r="R48" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-29 13:10:55)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,27 +700,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3154</t>
+          <t>1871</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>8/27/2024</t>
+          <t>9/5/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>BRAVO, MARIO 853</t>
+          <t>Bulnes 1810</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>795498456</t>
+          <t>796016024</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -735,7 +735,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Sacar la rienda de la plantera</t>
+          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -743,28 +743,28 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.41606</v>
+        <v>-58.413803</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.599935</v>
+        <v>-34.590308</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -774,7 +774,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>CLI-G</t>
+          <t>VCR-E</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -786,27 +786,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1871</t>
+          <t>3887</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>9/5/2024</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bulnes 1810</t>
+          <t>ESTADO DE ISRAEL AV. 4819</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>796016024</t>
+          <t>798894281</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -829,24 +829,24 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.413803</v>
+        <v>-58.432085</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.590308</v>
+        <v>-34.60178</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -860,7 +860,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>VCR-E</t>
+          <t>CLI-N</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -872,7 +872,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3887</t>
+          <t>3893</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -882,17 +882,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4819</t>
+          <t>HERRERA 402</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>798894281</t>
+          <t>798894295</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -907,7 +907,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Inclinado En el form cargaron foto de otro caso</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -929,14 +929,14 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.432085</v>
+        <v>-58.378613</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.60178</v>
+        <v>-34.6349</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>CLI-N</t>
+          <t>CON-H</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -958,27 +958,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3893</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>HERRERA 402</t>
+          <t>José Andrés Pacheco de Melo 2084</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>798894295</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -988,12 +988,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Inclinado En el form cargaron foto de otro caso</t>
+          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -1001,28 +1001,24 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>-58.378613</v>
+        <v>-58.395656</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.6349</v>
+        <v>-34.590364</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1032,7 +1028,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>CON-H</t>
+          <t>RET-C</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1044,27 +1040,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>3938</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>José Andrés Pacheco de Melo 2084</t>
+          <t>GODOY CRUZ 2604</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>799246642</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1074,12 +1070,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
+          <t>Realizar traspasos y retiro de columna vieja</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1087,24 +1083,28 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
       <c r="M8" t="n">
-        <v>-58.395656</v>
+        <v>-58.426169</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.590364</v>
+        <v>-34.579697</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>RET-C</t>
+          <t>VCR-N</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1126,27 +1126,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3938</t>
+          <t>4025</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11/5/2024</t>
+          <t>11/12/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2604</t>
+          <t>MEXICO 4249</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>799246642</t>
+          <t>799981143</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Realizar traspasos y retiro de columna vieja</t>
+          <t>Ver foto, colocar columna para traspasar</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1169,28 +1169,28 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.426169</v>
+        <v>-58.425997</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.579697</v>
+        <v>-34.620454</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>VCR-N</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1212,27 +1212,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4025</t>
+          <t>4426</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>12/19/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MEXICO 4249</t>
+          <t>LORA, FELIX 27</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>799981143</t>
+          <t>801768138</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Ver foto, colocar columna para traspasar</t>
+          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1269,14 +1269,14 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.425997</v>
+        <v>-58.443626</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.620454</v>
+        <v>-34.621032</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>PCH-G</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1298,27 +1298,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>4426</t>
+          <t>6243</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>12/19/2024</t>
+          <t>1/30/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LORA, FELIX 27</t>
+          <t>GARCIA, TEODORO 3252</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>801768138</t>
+          <t>779373118</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
+          <t>Colocar R400 para posterior traspaso</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1355,24 +1355,24 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.443626</v>
+        <v>-58.450789</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.621032</v>
+        <v>-34.577949</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>PCH-G</t>
+          <t>ATH-P</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1384,17 +1384,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>6243</t>
+          <t>5884</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1/30/2024</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>GARCIA, TEODORO 3252</t>
+          <t>OLLEROS 2952</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>779373118</t>
+          <t>799450967</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1419,11 +1419,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Colocar R400 para posterior traspaso</t>
+          <t>Solo retirar columna ya se realizo traspaso</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1441,19 +1441,19 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.450789</v>
+        <v>-58.447022</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.577949</v>
+        <v>-34.575873</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
@@ -1470,27 +1470,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>5884</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>OLLEROS 2952</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>799450967</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1500,16 +1500,16 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1527,24 +1527,24 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.447022</v>
+        <v>-58.496935</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.575873</v>
+        <v>-34.599084</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>ATH-P</t>
+          <t>PUE-B</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1556,27 +1556,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1586,12 +1586,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1613,46 +1613,46 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.496935</v>
+        <v>-58.400156</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.599084</v>
+        <v>-34.631369</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>PUE-B</t>
+          <t>PPT-F</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PPT</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1662,7 +1662,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1699,10 +1699,10 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.400156</v>
+        <v>-58.402062</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.631369</v>
+        <v>-34.635143</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1716,39 +1716,39 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PPT-F</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PPT</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>4696</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>2/10/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>YERBAL 489</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>803607520</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Desmonte de columna ya traspasaron nodo</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1785,14 +1785,14 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.402062</v>
+        <v>-58.438053</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.635143</v>
+        <v>-34.617481</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1802,7 +1802,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>ALM-G</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1814,17 +1814,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>4696</t>
+          <t>4938</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2/10/2025</t>
+          <t>2/14/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>YERBAL 489</t>
+          <t>CHACO 195</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>803607520</t>
+          <t>803607699</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1849,7 +1849,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron nodo</t>
+          <t>Desmontar columna personal propio traspaso nodo</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1871,10 +1871,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.438053</v>
+        <v>-58.431522</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.617481</v>
+        <v>-34.617523</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>ALM-G</t>
+          <t>ALM-F</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1900,27 +1900,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2/14/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>CHACO 195</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>803607699</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1935,11 +1935,11 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Desmontar columna personal propio traspaso nodo</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1948,7 +1948,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1957,14 +1957,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.431522</v>
+        <v>-58.371855</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.617523</v>
+        <v>-34.646958</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>ALM-F</t>
+          <t>CON-A</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1986,17 +1986,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -2043,14 +2043,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.371855</v>
+        <v>-58.403583</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.646958</v>
+        <v>-34.591604</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>CON-A</t>
+          <t>AGU-F</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2072,27 +2072,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2102,16 +2102,16 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -2129,14 +2129,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.403583</v>
+        <v>-58.441405</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.591604</v>
+        <v>-34.594348</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>AGU-F</t>
+          <t>VCR-H</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2158,7 +2158,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2168,17 +2168,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2191,11 +2191,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
         <v>1</v>
       </c>
@@ -2215,14 +2211,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.441405</v>
+        <v>-58.483821</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.594348</v>
+        <v>-34.677698</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2232,7 +2228,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>VCR-H</t>
+          <t>PAV-Q</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
@@ -2244,27 +2240,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2274,10 +2270,14 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+        </is>
+      </c>
       <c r="I22" t="n">
         <v>1</v>
       </c>
@@ -2297,14 +2297,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.483821</v>
+        <v>-58.445131</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.677698</v>
+        <v>-34.572117</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>PAV-Q</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
@@ -2326,27 +2326,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2374,7 +2374,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2383,14 +2383,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.445131</v>
+        <v>-58.425764</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.572117</v>
+        <v>-34.604359</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>ALM-L</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2455,7 +2455,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2469,10 +2469,10 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.425764</v>
+        <v>-58.439751</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.604359</v>
+        <v>-34.609908</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2486,7 +2486,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>ALM-L</t>
+          <t>ALM-I</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,7 +2498,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2508,17 +2508,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2555,14 +2555,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.439751</v>
+        <v>-58.375515</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.609908</v>
+        <v>-34.634393</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>ALM-I</t>
+          <t>CON-B</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2641,14 +2641,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.375515</v>
+        <v>-58.415839</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.634393</v>
+        <v>-34.599291</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>CON-B</t>
+          <t>CLI-L</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,7 +2705,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2727,14 +2727,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.415839</v>
+        <v>-58.469148</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.599291</v>
+        <v>-34.687883</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2744,7 +2744,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>CLI-L</t>
+          <t>PAV-T</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2813,14 +2813,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.469148</v>
+        <v>-58.395063</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.687883</v>
+        <v>-34.606257</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>PAV-T</t>
+          <t>CLI-B</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,7 +2842,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2852,17 +2852,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2885,12 +2885,12 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2899,14 +2899,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.395063</v>
+        <v>-58.429977</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.606257</v>
+        <v>-34.615514</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2916,7 +2916,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>CLI-B</t>
+          <t>ALM-J</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,7 +2928,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2938,17 +2938,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2985,14 +2985,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.429977</v>
+        <v>-58.421623</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.615514</v>
+        <v>-34.614541</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3002,7 +3002,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>ALM-J</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,27 +3014,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -3071,14 +3071,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.421623</v>
+        <v>-58.429972</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.614541</v>
+        <v>-34.632042</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3088,7 +3088,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>PPT-S</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,7 +3100,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3110,17 +3110,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3157,24 +3157,24 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.429972</v>
+        <v>-58.47888</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.632042</v>
+        <v>-34.571108</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>PPT-S</t>
+          <t>ATH-J</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,7 +3186,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3196,17 +3196,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3243,24 +3243,24 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.47888</v>
+        <v>-58.443196</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.571108</v>
+        <v>-34.618534</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>ATH-J</t>
+          <t>NRA-A</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3272,7 +3272,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3282,17 +3282,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3302,16 +3302,16 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3320,7 +3320,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -3329,14 +3329,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.443196</v>
+        <v>-58.406585</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.618534</v>
+        <v>-34.592933</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3346,7 +3346,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>NRA-A</t>
+          <t>AGU-B</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3358,7 +3358,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>-445</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3368,17 +3368,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>Joaquin V Gonzalez 4410</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>806945058</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3388,16 +3388,16 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3406,65 +3406,65 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.406585</v>
+        <v>-58.51232</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.592933</v>
+        <v>-34.595637</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>AGU-B</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-445</t>
+          <t>5937</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4410</t>
+          <t>MONROE 4833</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>806945058</t>
+          <t>807044121</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3497,18 +3497,18 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.51232</v>
+        <v>-58.483104</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.595637</v>
+        <v>-34.572353</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3518,39 +3518,39 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>ATH-C</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5937</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>MONROE 4833</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807044121</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3573,7 +3573,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3583,14 +3583,14 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.483104</v>
+        <v>-58.483927</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.572353</v>
+        <v>-34.570689</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3604,7 +3604,7 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>ATH-C</t>
+          <t>PUE-E</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -3616,17 +3616,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3636,7 +3636,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3659,7 +3659,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3669,18 +3669,18 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.483927</v>
+        <v>-58.492605</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.570689</v>
+        <v>-34.581454</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>PUE-E</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -3702,7 +3702,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3712,17 +3712,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3759,24 +3759,24 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.492605</v>
+        <v>-58.467789</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.581454</v>
+        <v>-34.68463</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>PAV-U</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
@@ -3788,27 +3788,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3823,7 +3823,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3831,7 +3831,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3845,14 +3845,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.467789</v>
+        <v>-58.432644</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.68463</v>
+        <v>-34.595434</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>PAV-U</t>
+          <t>VCR-I</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -3874,27 +3874,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3909,15 +3909,15 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3927,18 +3927,18 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.432644</v>
+        <v>-58.405749</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.595434</v>
+        <v>-34.58224</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>VCR-I</t>
+          <t>AGU-N</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -3960,27 +3960,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3995,15 +3995,15 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -4017,14 +4017,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.405749</v>
+        <v>-58.363292</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.58224</v>
+        <v>-34.642869</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>AGU-N</t>
+          <t>CON-E</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -4046,27 +4046,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4081,7 +4081,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -4099,18 +4099,18 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.363292</v>
+        <v>-58.432805</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.642869</v>
+        <v>-34.574345</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>CON-E</t>
+          <t>BLO-G</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -4132,27 +4132,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-517</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Av Dorrego 2721</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808373635</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4167,7 +4167,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -4189,14 +4189,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.432805</v>
+        <v>-58.384097</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.574345</v>
+        <v>-34.598913</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -4206,7 +4206,7 @@
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>BLO-G</t>
+          <t>RET-S</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -4218,27 +4218,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -4275,56 +4275,56 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.384097</v>
+        <v>-58.513643</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.598913</v>
+        <v>-34.594169</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>RET-S</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-531</t>
+          <t>-593</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4632</t>
+          <t>Husares 2250</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808530239</t>
+          <t>809642190</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -4361,14 +4361,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.513643</v>
+        <v>-58.443269</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.594169</v>
+        <v>-34.552209</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -4378,96 +4378,10 @@
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1PUE</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>-593</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>9/10/2025</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Husares 2250</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>809642190</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I47" t="n">
-        <v>1</v>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M47" t="n">
-        <v>-58.443269</v>
-      </c>
-      <c r="N47" t="n">
-        <v>-34.552209</v>
-      </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>BLO-B</t>
-        </is>
-      </c>
-      <c r="R47" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-01 08:29:16)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2463</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>7/15/2024</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>795698153</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -558,14 +558,10 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
         <v>1</v>
       </c>
@@ -576,7 +572,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -585,14 +581,14 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.40589</v>
+        <v>-58.483821</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.584156</v>
+        <v>-34.677698</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -602,7 +598,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>AGU-J</t>
+          <t>PAV-Q</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -614,27 +610,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>4696</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>2/10/2025</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>MCAL SOLANO LOPEZ 3110</t>
+          <t>YERBAL 489</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>792101640</t>
+          <t>803607520</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -649,7 +645,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Retirar columna. TLC ya traspaso nodo</t>
+          <t>Desmonte de columna ya traspasaron nodo</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -662,7 +658,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -671,24 +667,24 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.498448</v>
+        <v>-58.438053</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.595287</v>
+        <v>-34.617481</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>PUE-G</t>
+          <t>ALM-G</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -700,27 +696,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1871</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>9/5/2024</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bulnes 1810</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>796016024</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -735,7 +731,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -743,12 +739,12 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -757,14 +753,14 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.413803</v>
+        <v>-58.421623</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.590308</v>
+        <v>-34.614541</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -774,7 +770,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>VCR-E</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -786,17 +782,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3887</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4819</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -806,7 +802,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>798894281</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -821,7 +817,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -829,7 +825,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -839,18 +835,18 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.432085</v>
+        <v>-58.415839</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.60178</v>
+        <v>-34.599291</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -860,7 +856,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>CLI-N</t>
+          <t>CLI-L</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -872,27 +868,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3893</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>HERRERA 402</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>798894295</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -902,12 +898,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Inclinado En el form cargaron foto de otro caso</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -915,28 +911,28 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.378613</v>
+        <v>-58.441405</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.6349</v>
+        <v>-34.594348</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -946,7 +942,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>CON-H</t>
+          <t>VCR-H</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -958,27 +954,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>José Andrés Pacheco de Melo 2084</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -988,12 +984,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -1006,19 +1002,23 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M7" t="n">
-        <v>-58.395656</v>
+        <v>-58.425764</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.590364</v>
+        <v>-34.604359</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>RET-C</t>
+          <t>ALM-L</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1040,27 +1040,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3938</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>11/5/2024</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2604</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>799246642</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Realizar traspasos y retiro de columna vieja</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1083,28 +1083,28 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.426169</v>
+        <v>-58.402062</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.579697</v>
+        <v>-34.635143</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>VCR-N</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1126,27 +1126,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4025</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MEXICO 4249</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>799981143</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Ver foto, colocar columna para traspasar</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1169,12 +1169,12 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1183,14 +1183,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.425997</v>
+        <v>-58.429977</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.620454</v>
+        <v>-34.615514</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>ALM-J</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1212,27 +1212,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4426</t>
+          <t>2463</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>12/19/2024</t>
+          <t>7/15/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>LORA, FELIX 27</t>
+          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>801768138</t>
+          <t>795698153</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
+          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1269,14 +1269,14 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.443626</v>
+        <v>-58.40589</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.621032</v>
+        <v>-34.584156</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>PCH-G</t>
+          <t>AGU-J</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1298,17 +1298,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>6243</t>
+          <t>5884</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1/30/2024</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>GARCIA, TEODORO 3252</t>
+          <t>OLLEROS 2952</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>779373118</t>
+          <t>799450967</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1333,11 +1333,11 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Colocar R400 para posterior traspaso</t>
+          <t>Solo retirar columna ya se realizo traspaso</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1355,19 +1355,19 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.450789</v>
+        <v>-58.447022</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.577949</v>
+        <v>-34.575873</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -1384,27 +1384,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5884</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>OLLEROS 2952</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>799450967</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1419,11 +1419,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1441,14 +1441,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.447022</v>
+        <v>-58.375515</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.575873</v>
+        <v>-34.634393</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1458,7 +1458,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>ATH-P</t>
+          <t>CON-B</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1470,27 +1470,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>5937</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>MONROE 4833</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>807044121</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1500,12 +1500,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1518,7 +1518,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1527,14 +1527,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.496935</v>
+        <v>-58.483104</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.599084</v>
+        <v>-34.572353</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1544,7 +1544,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>PUE-B</t>
+          <t>ATH-C</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1556,27 +1556,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>4025</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>11/12/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>MEXICO 4249</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>799981143</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Ver foto, colocar columna para traspasar</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1613,14 +1613,14 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.400156</v>
+        <v>-58.425997</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.631369</v>
+        <v>-34.620454</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1630,39 +1630,39 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>PPT-F</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PPT</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>2805</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>8/6/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>MCAL SOLANO LOPEZ 3110</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>792101640</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Retirar columna. TLC ya traspaso nodo</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1699,24 +1699,24 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.402062</v>
+        <v>-58.498448</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.635143</v>
+        <v>-34.595287</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>PUE-G</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1728,17 +1728,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4696</t>
+          <t>4426</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2/10/2025</t>
+          <t>12/19/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>YERBAL 489</t>
+          <t>LORA, FELIX 27</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>803607520</t>
+          <t>801768138</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron nodo</t>
+          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1776,7 +1776,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1785,10 +1785,10 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.438053</v>
+        <v>-58.443626</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.617481</v>
+        <v>-34.621032</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>ALM-G</t>
+          <t>PCH-G</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1814,27 +1814,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2/14/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CHACO 195</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>803607699</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1849,7 +1849,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Desmontar columna personal propio traspaso nodo</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1871,14 +1871,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.431522</v>
+        <v>-58.384097</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.617523</v>
+        <v>-34.598913</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>ALM-F</t>
+          <t>RET-S</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1900,27 +1900,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1930,12 +1930,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1957,14 +1957,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.371855</v>
+        <v>-58.406585</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.646958</v>
+        <v>-34.592933</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>CON-A</t>
+          <t>AGU-B</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1986,27 +1986,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2021,15 +2021,15 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2043,14 +2043,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.403583</v>
+        <v>-58.432644</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.591604</v>
+        <v>-34.595434</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>AGU-F</t>
+          <t>VCR-I</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2072,27 +2072,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>José Andrés Pacheco de Melo 2084</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2120,23 +2120,19 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
-        <v>-58.441405</v>
+        <v>-58.395656</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.594348</v>
+        <v>-34.590364</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2146,7 +2142,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>VCR-H</t>
+          <t>RET-C</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2158,27 +2154,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2188,10 +2184,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
+        </is>
+      </c>
       <c r="I21" t="n">
         <v>1</v>
       </c>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -2211,56 +2211,56 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.483821</v>
+        <v>-58.513643</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.677698</v>
+        <v>-34.594169</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>PAV-Q</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>-445</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>Joaquin V Gonzalez 4410</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>806945058</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2288,65 +2288,65 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.445131</v>
+        <v>-58.51232</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.572117</v>
+        <v>-34.595637</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,11 +2361,11 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2383,14 +2383,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.425764</v>
+        <v>-58.371855</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.604359</v>
+        <v>-34.646958</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>ALM-L</t>
+          <t>CON-A</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>-593</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>Husares 2250</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>809642190</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2455,7 +2455,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2469,24 +2469,24 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.439751</v>
+        <v>-58.443269</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.609908</v>
+        <v>-34.552209</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>ALM-I</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,17 +2498,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>3893</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>HERRERA 402</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>798894295</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Inclinado En el form cargaron foto de otro caso</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2551,14 +2551,14 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.375515</v>
+        <v>-58.378613</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.634393</v>
+        <v>-34.6349</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>CON-B</t>
+          <t>CON-H</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>3938</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>GODOY CRUZ 2604</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>799246642</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Realizar traspasos y retiro de columna vieja</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2627,7 +2627,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2637,18 +2637,18 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.415839</v>
+        <v>-58.426169</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.599291</v>
+        <v>-34.579697</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>CLI-L</t>
+          <t>VCR-N</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>6243</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>1/30/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>GARCIA, TEODORO 3252</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>779373118</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,7 +2705,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Colocar R400 para posterior traspaso</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2718,7 +2718,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2727,24 +2727,24 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.469148</v>
+        <v>-58.450789</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.687883</v>
+        <v>-34.577949</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>PAV-T</t>
+          <t>ATH-P</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2813,14 +2813,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.395063</v>
+        <v>-58.467789</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.606257</v>
+        <v>-34.68463</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>CLI-B</t>
+          <t>PAV-U</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>3887</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>ESTADO DE ISRAEL AV. 4819</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>798894281</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2895,18 +2895,18 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.429977</v>
+        <v>-58.432085</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.615514</v>
+        <v>-34.60178</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2916,7 +2916,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>ALM-J</t>
+          <t>CLI-N</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2971,7 +2971,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2985,24 +2985,24 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.421623</v>
+        <v>-58.492605</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.614541</v>
+        <v>-34.581454</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,27 +3014,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3044,12 +3044,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -3071,24 +3071,24 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.429972</v>
+        <v>-58.496935</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.632042</v>
+        <v>-34.599084</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>PPT-S</t>
+          <t>PUE-B</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,27 +3100,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3157,24 +3157,24 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.47888</v>
+        <v>-58.469148</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.571108</v>
+        <v>-34.687883</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>ATH-J</t>
+          <t>PAV-T</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,27 +3186,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3234,7 +3234,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -3243,14 +3243,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.443196</v>
+        <v>-58.445131</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.618534</v>
+        <v>-34.572117</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>NRA-A</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3272,27 +3272,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>4938</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>2/14/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>CHACO 195</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>803607699</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3302,16 +3302,16 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Desmontar columna personal propio traspaso nodo</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3329,14 +3329,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.406585</v>
+        <v>-58.431522</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.592933</v>
+        <v>-34.617523</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3346,7 +3346,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>AGU-B</t>
+          <t>ALM-F</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3358,27 +3358,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-445</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4410</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806945058</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3415,56 +3415,56 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.51232</v>
+        <v>-58.363292</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.595637</v>
+        <v>-34.642869</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>CON-E</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5937</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MONROE 4833</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807044121</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3479,15 +3479,15 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3497,28 +3497,28 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.483104</v>
+        <v>-58.405749</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.572353</v>
+        <v>-34.58224</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>ATH-C</t>
+          <t>AGU-N</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -3530,27 +3530,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>1871</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>9/5/2024</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>Bulnes 1810</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>796016024</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3573,38 +3573,38 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.483927</v>
+        <v>-58.413803</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.570689</v>
+        <v>-34.590308</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>PUE-E</t>
+          <t>VCR-E</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -3616,27 +3616,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3664,7 +3664,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3673,56 +3673,56 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.492605</v>
+        <v>-58.400156</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.581454</v>
+        <v>-34.631369</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>PPT-F</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PPT</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3759,24 +3759,24 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.467789</v>
+        <v>-58.47888</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.68463</v>
+        <v>-34.571108</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>PAV-U</t>
+          <t>ATH-J</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
@@ -3788,27 +3788,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3823,15 +3823,15 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3845,14 +3845,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.432644</v>
+        <v>-58.403583</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.595434</v>
+        <v>-34.591604</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>VCR-I</t>
+          <t>AGU-F</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -3874,27 +3874,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3909,15 +3909,15 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3927,18 +3927,18 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.405749</v>
+        <v>-58.443196</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.58224</v>
+        <v>-34.618534</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>AGU-N</t>
+          <t>NRA-A</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -3960,27 +3960,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3995,7 +3995,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -4008,23 +4008,23 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.363292</v>
+        <v>-58.395063</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.642869</v>
+        <v>-34.606257</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>CON-E</t>
+          <t>CLI-B</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -4132,27 +4132,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4167,7 +4167,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -4189,14 +4189,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.384097</v>
+        <v>-58.429972</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.598913</v>
+        <v>-34.632042</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -4206,7 +4206,7 @@
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>RET-S</t>
+          <t>PPT-S</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -4218,27 +4218,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-531</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4632</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808530239</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -4271,18 +4271,18 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.513643</v>
+        <v>-58.483927</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.594169</v>
+        <v>-34.570689</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -4292,39 +4292,39 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>PUE-E</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-593</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Husares 2250</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>809642190</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -4347,7 +4347,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -4361,24 +4361,24 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.443269</v>
+        <v>-58.439751</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.552209</v>
+        <v>-34.609908</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>ALM-I</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-02 08:57:28)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -528,27 +528,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>2463</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>7/15/2024</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>795698153</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -558,10 +558,14 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
+        </is>
+      </c>
       <c r="I2" t="n">
         <v>1</v>
       </c>
@@ -572,7 +576,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -581,14 +585,14 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-58.483821</v>
+        <v>-58.40589</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.677698</v>
+        <v>-34.584156</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -598,7 +602,7 @@
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>PAV-Q</t>
+          <t>AGU-J</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -610,27 +614,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4696</t>
+          <t>2805</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2/10/2025</t>
+          <t>8/6/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>YERBAL 489</t>
+          <t>MCAL SOLANO LOPEZ 3110</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>803607520</t>
+          <t>792101640</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -645,7 +649,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron nodo</t>
+          <t>Retirar columna. TLC ya traspaso nodo</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -658,7 +662,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -667,24 +671,24 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.438053</v>
+        <v>-58.498448</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.617481</v>
+        <v>-34.595287</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>ALM-G</t>
+          <t>PUE-G</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -696,27 +700,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>1871</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>9/5/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>Bulnes 1810</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>796016024</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -731,7 +735,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -739,12 +743,12 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -753,14 +757,14 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.421623</v>
+        <v>-58.413803</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.614541</v>
+        <v>-34.590308</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -770,7 +774,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>VCR-E</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -782,17 +786,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>3887</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>ESTADO DE ISRAEL AV. 4819</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -802,7 +806,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>798894281</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -817,7 +821,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -825,7 +829,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -835,18 +839,18 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.415839</v>
+        <v>-58.432085</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.599291</v>
+        <v>-34.60178</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -856,7 +860,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>CLI-L</t>
+          <t>CLI-N</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -868,27 +872,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>3893</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>HERRERA 402</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>798894295</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -898,12 +902,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+          <t>Inclinado En el form cargaron foto de otro caso</t>
         </is>
       </c>
       <c r="I6" t="n">
@@ -911,28 +915,28 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.441405</v>
+        <v>-58.378613</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.594348</v>
+        <v>-34.6349</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -942,7 +946,7 @@
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>VCR-H</t>
+          <t>CON-H</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
@@ -954,27 +958,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>José Andrés Pacheco de Melo 2084</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -984,12 +988,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
+          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -1002,23 +1006,19 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>-58.425764</v>
+        <v>-58.395656</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.604359</v>
+        <v>-34.590364</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1028,7 +1028,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>ALM-L</t>
+          <t>RET-C</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1040,27 +1040,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>3938</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>GODOY CRUZ 2604</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>799246642</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Realizar traspasos y retiro de columna vieja</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1083,28 +1083,28 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.402062</v>
+        <v>-58.426169</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.635143</v>
+        <v>-34.579697</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>VCR-N</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -1126,27 +1126,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>4025</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>11/12/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>MEXICO 4249</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>799981143</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Ver foto, colocar columna para traspasar</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1169,12 +1169,12 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1183,14 +1183,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.429977</v>
+        <v>-58.425997</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.615514</v>
+        <v>-34.620454</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>ALM-J</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -1212,27 +1212,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2463</t>
+          <t>4426</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>7/15/2024</t>
+          <t>12/19/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>PACHECO DE MELO, JOSE ANDRES 3066</t>
+          <t>LORA, FELIX 27</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>795698153</t>
+          <t>801768138</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1247,7 +1247,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado solo Retirar Columna</t>
+          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1269,14 +1269,14 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.40589</v>
+        <v>-58.443626</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.584156</v>
+        <v>-34.621032</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>AGU-J</t>
+          <t>PCH-G</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
@@ -1298,17 +1298,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5884</t>
+          <t>6243</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>1/30/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>OLLEROS 2952</t>
+          <t>GARCIA, TEODORO 3252</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>799450967</t>
+          <t>779373118</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1333,11 +1333,11 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso</t>
+          <t>Colocar R400 para posterior traspaso</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1355,19 +1355,19 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.447022</v>
+        <v>-58.450789</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.575873</v>
+        <v>-34.577949</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -1384,27 +1384,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5884</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>OLLEROS 2952</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>799450967</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1419,11 +1419,11 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Solo retirar columna ya se realizo traspaso</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1441,14 +1441,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.375515</v>
+        <v>-58.447022</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.634393</v>
+        <v>-34.575873</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1458,7 +1458,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>CON-B</t>
+          <t>ATH-P</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1470,27 +1470,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>5937</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MONROE 4833</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>807044121</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1500,12 +1500,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1518,7 +1518,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1527,14 +1527,14 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.483104</v>
+        <v>-58.496935</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.572353</v>
+        <v>-34.599084</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1544,7 +1544,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>ATH-C</t>
+          <t>PUE-B</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -1556,27 +1556,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4025</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MEXICO 4249</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>799981143</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Ver foto, colocar columna para traspasar</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1604,7 +1604,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1613,14 +1613,14 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.425997</v>
+        <v>-58.400156</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.620454</v>
+        <v>-34.631369</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1630,39 +1630,39 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>PPT-F</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PPT</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2805</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>MCAL SOLANO LOPEZ 3110</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>792101640</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Retirar columna. TLC ya traspaso nodo</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1699,24 +1699,24 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.498448</v>
+        <v>-58.402062</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.595287</v>
+        <v>-34.635143</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>PUE-G</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R15" t="inlineStr">
@@ -1728,17 +1728,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4426</t>
+          <t>4696</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>12/19/2024</t>
+          <t>2/10/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>LORA, FELIX 27</t>
+          <t>YERBAL 489</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>801768138</t>
+          <t>803607520</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
+          <t>Desmonte de columna ya traspasaron nodo</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1776,7 +1776,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1785,10 +1785,10 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.443626</v>
+        <v>-58.438053</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.621032</v>
+        <v>-34.617481</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>PCH-G</t>
+          <t>ALM-G</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
@@ -1814,27 +1814,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>4938</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>2/14/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>CHACO 195</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>803607699</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1849,7 +1849,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>Desmontar columna personal propio traspaso nodo</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1871,14 +1871,14 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.384097</v>
+        <v>-58.431522</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.598913</v>
+        <v>-34.617523</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>RET-S</t>
+          <t>ALM-F</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1900,27 +1900,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1930,12 +1930,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1957,14 +1957,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.406585</v>
+        <v>-58.371855</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.592933</v>
+        <v>-34.646958</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>AGU-B</t>
+          <t>CON-A</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1986,27 +1986,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2021,15 +2021,15 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2043,14 +2043,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.432644</v>
+        <v>-58.403583</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.595434</v>
+        <v>-34.591604</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>VCR-I</t>
+          <t>AGU-F</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2072,27 +2072,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>José Andrés Pacheco de Melo 2084</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -2120,19 +2120,23 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr"/>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M20" t="n">
-        <v>-58.395656</v>
+        <v>-58.441405</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.590364</v>
+        <v>-34.594348</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2142,7 +2146,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>RET-C</t>
+          <t>VCR-H</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2158,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>-531</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4632</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>808530239</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2184,14 +2188,10 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="n">
         <v>1</v>
       </c>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -2211,56 +2211,56 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.513643</v>
+        <v>-58.483821</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.594169</v>
+        <v>-34.677698</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>PAV-Q</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-445</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4410</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>806945058</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2288,65 +2288,65 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.51232</v>
+        <v>-58.445131</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.595637</v>
+        <v>-34.572117</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,11 +2361,11 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -2383,14 +2383,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.371855</v>
+        <v>-58.425764</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.646958</v>
+        <v>-34.604359</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>CON-A</t>
+          <t>ALM-L</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-593</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Husares 2250</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>809642190</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2455,7 +2455,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2469,24 +2469,24 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.443269</v>
+        <v>-58.439751</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.552209</v>
+        <v>-34.609908</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>BLO-B</t>
+          <t>ALM-I</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,17 +2498,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>3893</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>HERRERA 402</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>798894295</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Inclinado En el form cargaron foto de otro caso</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2551,14 +2551,14 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.378613</v>
+        <v>-58.375515</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.6349</v>
+        <v>-34.634393</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>CON-H</t>
+          <t>CON-B</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>3938</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>11/5/2024</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2604</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>799246642</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Realizar traspasos y retiro de columna vieja</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2627,7 +2627,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2637,18 +2637,18 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.426169</v>
+        <v>-58.415839</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.579697</v>
+        <v>-34.599291</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>VCR-N</t>
+          <t>CLI-L</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,27 +2670,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6243</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1/30/2024</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>GARCIA, TEODORO 3252</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>779373118</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,7 +2705,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Colocar R400 para posterior traspaso</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2718,7 +2718,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2727,24 +2727,24 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.450789</v>
+        <v>-58.469148</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.577949</v>
+        <v>-34.687883</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>ATH-P</t>
+          <t>PAV-T</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2813,14 +2813,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.467789</v>
+        <v>-58.395063</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.68463</v>
+        <v>-34.606257</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>PAV-U</t>
+          <t>CLI-B</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>3887</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4819</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>798894281</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2895,18 +2895,18 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.432085</v>
+        <v>-58.429977</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.60178</v>
+        <v>-34.615514</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2916,7 +2916,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>CLI-N</t>
+          <t>ALM-J</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,27 +2928,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2971,7 +2971,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2985,24 +2985,24 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.492605</v>
+        <v>-58.421623</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.581454</v>
+        <v>-34.614541</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,27 +3014,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3044,12 +3044,12 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -3071,24 +3071,24 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.496935</v>
+        <v>-58.429972</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.599084</v>
+        <v>-34.632042</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>PUE-B</t>
+          <t>PPT-S</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,27 +3100,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3157,24 +3157,24 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.469148</v>
+        <v>-58.47888</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.687883</v>
+        <v>-34.571108</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>PAV-T</t>
+          <t>ATH-J</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,27 +3186,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3234,7 +3234,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -3243,14 +3243,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.445131</v>
+        <v>-58.443196</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.572117</v>
+        <v>-34.618534</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>NRA-A</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3272,27 +3272,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2/14/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>CHACO 195</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>803607699</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3302,16 +3302,16 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Desmontar columna personal propio traspaso nodo</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3329,14 +3329,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.431522</v>
+        <v>-58.406585</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.617523</v>
+        <v>-34.592933</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3346,7 +3346,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>ALM-F</t>
+          <t>AGU-B</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3358,27 +3358,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>-445</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>Joaquin V Gonzalez 4410</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>806945058</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3415,56 +3415,56 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.363292</v>
+        <v>-58.51232</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.642869</v>
+        <v>-34.595637</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>CON-E</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>5937</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>MONROE 4833</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>807044121</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3479,15 +3479,15 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3497,28 +3497,28 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.405749</v>
+        <v>-58.483104</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.58224</v>
+        <v>-34.572353</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>AGU-N</t>
+          <t>ATH-C</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -3530,27 +3530,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1871</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>9/5/2024</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Bulnes 1810</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>796016024</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Equipo de TLC ya traspasado, solo Retirar Columna</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3573,38 +3573,38 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.413803</v>
+        <v>-58.483927</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.590308</v>
+        <v>-34.570689</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>VCR-E</t>
+          <t>PUE-E</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -3616,27 +3616,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3651,7 +3651,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3664,7 +3664,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3673,56 +3673,56 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.400156</v>
+        <v>-58.492605</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.631369</v>
+        <v>-34.581454</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>PPT-F</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PPT</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3737,7 +3737,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3759,24 +3759,24 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.47888</v>
+        <v>-58.467789</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.571108</v>
+        <v>-34.68463</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>ATH-J</t>
+          <t>PAV-U</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
@@ -3788,27 +3788,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3823,15 +3823,15 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3845,14 +3845,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.403583</v>
+        <v>-58.432644</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.591604</v>
+        <v>-34.595434</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>AGU-F</t>
+          <t>VCR-I</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -3874,27 +3874,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3909,15 +3909,15 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3927,18 +3927,18 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.443196</v>
+        <v>-58.405749</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.618534</v>
+        <v>-34.58224</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>NRA-A</t>
+          <t>AGU-N</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -3960,27 +3960,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3995,7 +3995,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -4008,23 +4008,23 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.395063</v>
+        <v>-58.363292</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.606257</v>
+        <v>-34.642869</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>CLI-B</t>
+          <t>CON-E</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -4132,27 +4132,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4167,7 +4167,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -4189,14 +4189,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.429972</v>
+        <v>-58.384097</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.632042</v>
+        <v>-34.598913</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -4206,7 +4206,7 @@
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>PPT-S</t>
+          <t>RET-S</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -4218,27 +4218,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -4271,18 +4271,18 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.483927</v>
+        <v>-58.513643</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.570689</v>
+        <v>-34.594169</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -4292,39 +4292,39 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>PUE-E</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>-593</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>Husares 2250</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>809642190</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4339,7 +4339,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -4347,7 +4347,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -4361,24 +4361,24 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.439751</v>
+        <v>-58.443269</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.609908</v>
+        <v>-34.552209</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>ALM-I</t>
+          <t>BLO-B</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-07 09:02:34)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,16 +514,6 @@
           <t>Zona</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>PD</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>N2</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -600,16 +590,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>AGU-J</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -686,16 +666,6 @@
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>PUE-G</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -772,16 +742,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>VCR-E</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -858,16 +818,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>CLI-N</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -942,16 +892,6 @@
       <c r="P6" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>CON-H</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -1026,16 +966,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>RET-C</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1112,16 +1042,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>VCR-N</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1198,16 +1118,6 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>ALM-B</t>
-        </is>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1284,31 +1194,21 @@
           <t>Capital Sur</t>
         </is>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>PCH-G</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>6243</t>
+          <t>5884</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>1/30/2024</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>GARCIA, TEODORO 3252</t>
+          <t>OLLEROS 2952</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1318,7 +1218,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>779373118</t>
+          <t>799450967</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1333,11 +1233,11 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Colocar R400 para posterior traspaso</t>
+          <t>Solo retirar columna ya se realizo traspaso</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1346,7 +1246,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1355,56 +1255,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.450789</v>
+        <v>-58.447022</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.577949</v>
+        <v>-34.575873</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>ATH-P</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5884</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>OLLEROS 2952</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>799450967</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1414,16 +1304,16 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1441,56 +1331,46 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.447022</v>
+        <v>-58.496935</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.575873</v>
+        <v>-34.599084</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>ATH-P</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1500,12 +1380,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1518,7 +1398,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1527,46 +1407,36 @@
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.496935</v>
+        <v>-58.400156</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.599084</v>
+        <v>-34.631369</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>PUE-B</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1576,7 +1446,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1591,7 +1461,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1604,7 +1474,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1613,10 +1483,10 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.400156</v>
+        <v>-58.402062</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.631369</v>
+        <v>-34.635143</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1626,43 +1496,33 @@
       <c r="P14" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>PPT-F</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1PPT</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>4696</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>2/10/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>YERBAL 489</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>803607520</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1677,7 +1537,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Desmonte de columna ya traspasaron nodo</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1699,46 +1559,36 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.402062</v>
+        <v>-58.438053</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.635143</v>
+        <v>-34.617481</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>PPT-K</t>
-        </is>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4696</t>
+          <t>4938</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2/10/2025</t>
+          <t>2/14/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>YERBAL 489</t>
+          <t>CHACO 195</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1748,7 +1598,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>803607520</t>
+          <t>803607699</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1763,7 +1613,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron nodo</t>
+          <t>Desmontar columna personal propio traspaso nodo</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1785,10 +1635,10 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-58.438053</v>
+        <v>-58.431522</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.617481</v>
+        <v>-34.617523</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1798,43 +1648,33 @@
       <c r="P16" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>ALM-G</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>5496</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2/14/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CHACO 195</t>
+          <t>ISABEL LA CATOLICA 1539</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>803607699</t>
+          <t>803778980</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1849,11 +1689,11 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Desmontar columna personal propio traspaso nodo</t>
+          <t>Picada cambiaron la incorrecta</t>
         </is>
       </c>
       <c r="I17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1862,7 +1702,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1871,46 +1711,36 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-58.431522</v>
+        <v>-58.371855</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.617523</v>
+        <v>-34.646958</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>ALM-F</t>
-        </is>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5496</t>
+          <t>4373</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/12/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>ISABEL LA CATOLICA 1539</t>
+          <t>BERUTI 2716</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1920,7 +1750,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>803778980</t>
+          <t>803969347</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1935,7 +1765,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Picada cambiaron la incorrecta</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1957,56 +1787,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.371855</v>
+        <v>-58.403583</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.646958</v>
+        <v>-34.591604</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>CON-A</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4373</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>3/12/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>BERUTI 2716</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>803969347</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2016,16 +1836,16 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
         </is>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -2034,7 +1854,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -2043,36 +1863,26 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.403583</v>
+        <v>-58.441405</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.591604</v>
+        <v>-34.594348</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>AGU-F</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2082,17 +1892,17 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2105,11 +1915,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
-        </is>
-      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="n">
         <v>1</v>
       </c>
@@ -2129,56 +1935,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.441405</v>
+        <v>-58.483821</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.594348</v>
+        <v>-34.677698</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>VCR-H</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>-317</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/9/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>804569034</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2188,10 +1984,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+        </is>
+      </c>
       <c r="I21" t="n">
         <v>1</v>
       </c>
@@ -2211,56 +2011,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.483821</v>
+        <v>-58.445131</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.677698</v>
+        <v>-34.572117</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>PAV-Q</t>
-        </is>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-317</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/9/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ /ALT/ 612</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804569034</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,7 +2065,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso en las fotos no se ve pero ya esta realizado</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2288,7 +2078,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2297,56 +2087,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.445131</v>
+        <v>-58.425764</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.572117</v>
+        <v>-34.604359</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>COG-C</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,7 +2141,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2369,7 +2149,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2383,10 +2163,10 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.425764</v>
+        <v>-58.439751</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.604359</v>
+        <v>-34.609908</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -2396,23 +2176,13 @@
       <c r="P23" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>ALM-L</t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2422,17 +2192,17 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2217,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2455,7 +2225,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2469,56 +2239,46 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.439751</v>
+        <v>-58.375515</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.609908</v>
+        <v>-34.634393</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>ALM-I</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2533,7 +2293,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2555,56 +2315,46 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.375515</v>
+        <v>-58.415839</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.634393</v>
+        <v>-34.599291</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>CON-B</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>6110</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/6/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>CORRALES 6147</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>805707291</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,7 +2369,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna corroida en su base</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2641,56 +2391,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.415839</v>
+        <v>-58.469148</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.599291</v>
+        <v>-34.687883</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>CLI-L</t>
-        </is>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6110</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5/6/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>CORRALES 6147</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>805707291</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,7 +2445,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Columna corroida en su base</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2718,7 +2458,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2727,36 +2467,26 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.469148</v>
+        <v>-58.395063</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.687883</v>
+        <v>-34.606257</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>PAV-T</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>5836</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2766,17 +2496,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>RIVADAVIA AV. 4548</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>806926405</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,7 +2521,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2799,12 +2529,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2813,36 +2543,26 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.395063</v>
+        <v>-58.429977</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.606257</v>
+        <v>-34.615514</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>CLI-B</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5836</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2852,17 +2572,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 4548</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>806926405</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2899,56 +2619,46 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.429977</v>
+        <v>-58.421623</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.615514</v>
+        <v>-34.614541</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>ALM-J</t>
-        </is>
-      </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>-428</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>Asamblea 301</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>806926697</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,7 +2673,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Chocada en accidente</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2971,7 +2681,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2985,36 +2695,26 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.421623</v>
+        <v>-58.429972</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.614541</v>
+        <v>-34.632042</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>ALM-C</t>
-        </is>
-      </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>-428</t>
+          <t>-429</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3024,17 +2724,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Asamblea 301</t>
+          <t>Blanco encalada 4362</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>806926697</t>
+          <t>806926710</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3049,7 +2749,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Chocada en accidente</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -3071,36 +2771,26 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.429972</v>
+        <v>-58.47888</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.632042</v>
+        <v>-34.571108</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>PPT-S</t>
-        </is>
-      </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>-429</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3110,17 +2800,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Blanco encalada 4362</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>806926710</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,7 +2825,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida dar prioridad </t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3157,36 +2847,26 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.47888</v>
+        <v>-58.443196</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.571108</v>
+        <v>-34.618534</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>ATH-J</t>
-        </is>
-      </c>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>-440</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3196,17 +2876,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>LAPRIDA 1374</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>807005369</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3216,16 +2896,16 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Se coloco columna nueva queda pendiente de traspaso</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -3234,7 +2914,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -3243,36 +2923,26 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.443196</v>
+        <v>-58.406585</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.618534</v>
+        <v>-34.592933</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>NRA-A</t>
-        </is>
-      </c>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>-440</t>
+          <t>-445</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3282,17 +2952,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LAPRIDA 1374</t>
+          <t>Joaquin V Gonzalez 4410</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807005369</t>
+          <t>806945058</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3302,16 +2972,16 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Se coloco columna nueva queda pendiente de traspaso</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -3320,65 +2990,55 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.406585</v>
+        <v>-58.51232</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.592933</v>
+        <v>-34.595637</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>AGU-B</t>
-        </is>
-      </c>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>-445</t>
+          <t>5937</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/28/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4410</t>
+          <t>MONROE 4833</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>806945058</t>
+          <t>807044121</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3393,7 +3053,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3411,60 +3071,50 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.51232</v>
+        <v>-58.483104</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.595637</v>
+        <v>-34.572353</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>PUE-O</t>
-        </is>
-      </c>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5937</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5/28/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MONROE 4833</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807044121</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3479,7 +3129,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3487,7 +3137,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3497,14 +3147,14 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.483104</v>
+        <v>-58.483927</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.572353</v>
+        <v>-34.570689</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3514,33 +3164,23 @@
       <c r="P36" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>ATH-C</t>
-        </is>
-      </c>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3550,7 +3190,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3565,7 +3205,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3573,7 +3213,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3583,40 +3223,30 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.483927</v>
+        <v>-58.492605</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.570689</v>
+        <v>-34.581454</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>PUE-E</t>
-        </is>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3626,17 +3256,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3673,56 +3303,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.492605</v>
+        <v>-58.467789</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.581454</v>
+        <v>-34.68463</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>PUE-K</t>
-        </is>
-      </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>-493</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/27/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>JUFRE 424</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>807817955</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3737,7 +3357,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3745,7 +3365,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3759,56 +3379,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.467789</v>
+        <v>-58.432644</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.68463</v>
+        <v>-34.595434</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>PAV-U</t>
-        </is>
-      </c>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-493</t>
+          <t>-501</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/27/2025</t>
+          <t>7/3/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>JUFRE 424</t>
+          <t>Cabello 3107</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807817955</t>
+          <t>807971967</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3823,15 +3433,15 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Desmontar columna de 168 mm y traspasar redes a columna comunitaria</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3841,60 +3451,50 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.432644</v>
+        <v>-58.405749</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.595434</v>
+        <v>-34.58224</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>VCR-I</t>
-        </is>
-      </c>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-501</t>
+          <t>-511</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7/3/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Cabello 3107</t>
+          <t>Carlos Melo 491</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807971967</t>
+          <t>808194932</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3909,15 +3509,15 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3931,56 +3531,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.405749</v>
+        <v>-58.363292</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.58224</v>
+        <v>-34.642869</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>AGU-N</t>
-        </is>
-      </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>-511</t>
+          <t>-517</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/16/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Carlos Melo 491</t>
+          <t>Av Dorrego 2721</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808194932</t>
+          <t>808373635</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3995,7 +3585,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -4013,60 +3603,50 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.363292</v>
+        <v>-58.432805</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.642869</v>
+        <v>-34.574345</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>CON-E</t>
-        </is>
-      </c>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-517</t>
+          <t>-529</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/16/2025</t>
+          <t>7/23/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Av Dorrego 2721</t>
+          <t>Libertad 820</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808373635</t>
+          <t>ICD30189941</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4081,7 +3661,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Cambiar columna 114 base corroida y cable de fo cortado</t>
+          <t>Colocar columna hablar con Pablo si hay dudas</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -4103,56 +3683,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.432805</v>
+        <v>-58.384097</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.574345</v>
+        <v>-34.598913</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>BLO-G</t>
-        </is>
-      </c>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-529</t>
+          <t>-531</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/23/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Libertad 820</t>
+          <t>Joaquin V Gonzalez 4632</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ICD30189941</t>
+          <t>808530239</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4167,7 +3737,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Colocar columna hablar con Pablo si hay dudas</t>
+          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -4189,56 +3759,46 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.384097</v>
+        <v>-58.513643</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.598913</v>
+        <v>-34.594169</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>RET-S</t>
-        </is>
-      </c>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-531</t>
+          <t>-593</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Joaquin V Gonzalez 4632</t>
+          <t>Husares 2250</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808530239</t>
+          <t>809642190</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4253,7 +3813,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Cambiar por prfv y usar esa 114 en Libertad 820</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -4275,115 +3835,19 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.513643</v>
+        <v>-58.443269</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.594169</v>
+        <v>-34.552209</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
           <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>PUE-O</t>
-        </is>
-      </c>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.1PUE</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>-593</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>9/10/2025</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Husares 2250</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>809642190</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I46" t="n">
-        <v>1</v>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M46" t="n">
-        <v>-58.443269</v>
-      </c>
-      <c r="N46" t="n">
-        <v>-34.552209</v>
-      </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>Saavedra</t>
-        </is>
-      </c>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>BLO-B</t>
-        </is>
-      </c>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-08 08:24:07)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,16 @@
           <t>Zona</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>PD</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>N2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -590,6 +600,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>AGU-J</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -666,6 +686,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>PUE-G</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -742,6 +772,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>VCR-E</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -818,6 +858,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>CLI-N</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -892,6 +942,16 @@
       <c r="P6" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>CON-H</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -966,6 +1026,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>RET-C</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1042,6 +1112,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>VCR-N</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1118,6 +1198,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>ALM-B</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1194,6 +1284,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>PCH-G</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1270,6 +1370,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>ATH-P</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1346,6 +1456,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>PUE-B</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1422,6 +1542,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>PPT-F</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PPT</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1498,6 +1628,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>PPT-K</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1574,6 +1714,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>ALM-G</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1650,6 +1800,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>ALM-F</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1726,6 +1886,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>CON-A</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1802,6 +1972,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>AGU-F</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1876,6 +2056,16 @@
       <c r="P19" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>VCR-H</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
@@ -1950,6 +2140,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>PAV-Q</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2026,6 +2226,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>COG-C</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2102,6 +2312,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>ALM-L</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2178,6 +2398,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>ALM-I</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2254,6 +2484,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>CON-B</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2330,6 +2570,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>CLI-L</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2406,6 +2656,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>PAV-T</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2482,6 +2742,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>CLI-B</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2558,6 +2828,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>ALM-J</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2634,6 +2914,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>ALM-C</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2710,6 +3000,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>PPT-S</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2786,6 +3086,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>ATH-J</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2862,6 +3172,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>NRA-A</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2938,6 +3258,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>AGU-B</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3014,6 +3344,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>PUE-O</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PUE</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3090,6 +3430,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>ATH-C</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3166,6 +3516,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>PUE-E</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3242,6 +3602,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>PUE-K</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3318,6 +3688,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>PAV-U</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3394,6 +3774,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>VCR-I</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3470,6 +3860,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>AGU-N</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3546,6 +3946,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>CON-E</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3622,6 +4032,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>BLO-G</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -3698,6 +4118,16 @@
           <t>Capital Sur</t>
         </is>
       </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>RET-S</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -3774,6 +4204,16 @@
           <t>Capital Norte</t>
         </is>
       </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>PUE-O</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.1PUE</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -3848,6 +4288,16 @@
       <c r="P45" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>BLO-B</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-10-13 07:27:33)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4301,6 +4301,350 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>6475</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>9/17/2025</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Av Amancio Alcorta 3570</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>809800213</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>aplomar</t>
+        </is>
+      </c>
+      <c r="I46" t="n">
+        <v>1</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
+        <v>-58.409278</v>
+      </c>
+      <c r="N46" t="n">
+        <v>-34.653566</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>PPT-H</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>-602</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>9/18/2025</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Agustin de vedia 2110</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>809837501</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I47" t="n">
+        <v>1</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M47" t="n">
+        <v>-58.435679</v>
+      </c>
+      <c r="N47" t="n">
+        <v>-34.643992</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>PPT-O</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>7296</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>9/24/2025</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>VEDIA, AGUSTIN DE 2130</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>809979719</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3 columnas picadas ver en calle cuales son necesarias cambiar con Pablo </t>
+        </is>
+      </c>
+      <c r="I48" t="n">
+        <v>1</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M48" t="n">
+        <v>-58.435634</v>
+      </c>
+      <c r="N48" t="n">
+        <v>-34.64412</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>PPT-O</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>-634</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>10/8/2025</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Curapaligue 1127</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>ICD31464856</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Colocar columna donde se marca en la foto pasante 150 o 200</t>
+        </is>
+      </c>
+      <c r="I49" t="n">
+        <v>1</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M49" t="n">
+        <v>-58.446624</v>
+      </c>
+      <c r="N49" t="n">
+        <v>-34.635851</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>PPT-M</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-16 12:53:49)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R75"/>
+  <dimension ref="A1:R76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6873,6 +6873,92 @@
         </is>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>7516</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>10/15/2025</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>ALVAREZ, CRISOSTOMO 3000</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>810371027</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>-58.458516</v>
+      </c>
+      <c r="N76" t="n">
+        <v>-34.646422</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>PPT-N</t>
+        </is>
+      </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-17 20:17:33)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Optical_Power" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Optical_Power" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-20 07:30:47)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -4812,27 +4812,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5999</t>
+          <t>5894</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 228</t>
+          <t>ALBARELLOS AV. 3100</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808918687</t>
+          <t>ICD30340076</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4842,12 +4842,12 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente de Transito</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Se deriva directamente a traspaso de fuente ya que hay una columna existente</t>
+          <t>QAP fotos del gcba tenia las incorrectas</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4855,38 +4855,38 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.425858</v>
+        <v>-58.512533</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.61629</v>
+        <v>-34.579243</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -4898,7 +4898,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6917</t>
+          <t>5999</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4908,17 +4908,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>BRIN, MINISTRO 1375</t>
+          <t>MARMOL, JOSE 228</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808918700</t>
+          <t>808918687</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4928,16 +4928,16 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Se deriva directamente a traspaso de fuente ya que hay una columna existente</t>
         </is>
       </c>
       <c r="I53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4955,14 +4955,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.355342</v>
+        <v>-58.425858</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.63565</v>
+        <v>-34.61629</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4972,7 +4972,7 @@
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>CON-G</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
@@ -4984,27 +4984,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -5019,7 +5019,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -5041,24 +5041,24 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.472869</v>
+        <v>-58.355342</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.562</v>
+        <v>-34.63565</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>COG-I</t>
+          <t>CON-G</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -5070,27 +5070,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>AGUIRRE 368</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>809268249</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -5127,24 +5127,24 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.434651</v>
+        <v>-58.472869</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.598814</v>
+        <v>-34.562</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>CLI-O</t>
+          <t>COG-I</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -6188,27 +6188,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7359</t>
+          <t>7373</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>9/29/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>VEGA, NICETO, CNEL. 4678</t>
+          <t>SANTIAGO DEL ESTERO 1253</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>810056579</t>
+          <t>810132493</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6223,7 +6223,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -6245,14 +6245,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.430056</v>
+        <v>-58.384406</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.593188</v>
+        <v>-34.622932</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -6262,7 +6262,7 @@
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>VCR-F</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
@@ -6274,7 +6274,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7373</t>
+          <t>7387</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -6284,17 +6284,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SANTIAGO DEL ESTERO 1253</t>
+          <t>PERIBEBUY 6814</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>810132493</t>
+          <t>810132728</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -6309,7 +6309,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -6331,24 +6331,24 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.384406</v>
+        <v>-58.521719</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.622932</v>
+        <v>-34.647467</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PAV-C</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -6360,7 +6360,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7387</t>
+          <t>7394</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -6370,17 +6370,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>PERIBEBUY 6814</t>
+          <t>BONIFACIO, JOSE 2409</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>810132728</t>
+          <t>810132768</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -6395,7 +6395,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -6417,24 +6417,24 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.521719</v>
+        <v>-58.461482</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.647467</v>
+        <v>-34.632432</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>PAV-C</t>
+          <t>PCH-F</t>
         </is>
       </c>
       <c r="R70" t="inlineStr">
@@ -6446,7 +6446,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7394</t>
+          <t>7402</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -6456,17 +6456,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>BONIFACIO, JOSE 2409</t>
+          <t>RIVADAVIA AV. 2479</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>810132768</t>
+          <t>810132836</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -6481,7 +6481,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -6503,14 +6503,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.461482</v>
+        <v>-58.401428</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.632432</v>
+        <v>-34.609797</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -6520,7 +6520,7 @@
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>PCH-F</t>
+          <t>CLI-D</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
@@ -6532,7 +6532,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7402</t>
+          <t>7405</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 2479</t>
+          <t>CHILE 2115</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -6552,7 +6552,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>810132836</t>
+          <t>810132907</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -6567,7 +6567,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -6589,10 +6589,10 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.401428</v>
+        <v>-58.396368</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.609797</v>
+        <v>-34.61718</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -6606,7 +6606,7 @@
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>CLI-D</t>
+          <t>CEN-C</t>
         </is>
       </c>
       <c r="R72" t="inlineStr">
@@ -6618,17 +6618,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7405</t>
+          <t>7410</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>10/1/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>CHILE 2115</t>
+          <t>CHILE 2163</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -6638,7 +6638,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>810132907</t>
+          <t>810132956</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -6675,10 +6675,10 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.396368</v>
+        <v>-58.397024</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.61718</v>
+        <v>-34.617234</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -6704,27 +6704,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7410</t>
+          <t>7498</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>10/1/2025</t>
+          <t>10/13/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>CHILE 2163</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 396</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>810132956</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6739,7 +6739,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cementar vereda y ver si la columna esta a plomo  ademas reclaman cables cortados</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6761,14 +6761,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.397024</v>
+        <v>-58.467049</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.617234</v>
+        <v>-34.626303</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6778,7 +6778,7 @@
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>CEN-C</t>
+          <t>NRA-E</t>
         </is>
       </c>
       <c r="R74" t="inlineStr">
@@ -6790,17 +6790,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7498</t>
+          <t>7516</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>10/13/2025</t>
+          <t>10/15/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 396</t>
+          <t>ALVAREZ, CRISOSTOMO 3000</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -6810,7 +6810,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810371027</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6825,7 +6825,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Cementar vereda y ver si la columna esta a plomo  ademas reclaman cables cortados</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6847,10 +6847,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.467049</v>
+        <v>-58.458516</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.626303</v>
+        <v>-34.646422</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6864,7 +6864,7 @@
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>NRA-E</t>
+          <t>PPT-N</t>
         </is>
       </c>
       <c r="R75" t="inlineStr">
@@ -6876,27 +6876,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7516</t>
+          <t>5783</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>10/15/2025</t>
+          <t>10/17/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ALVAREZ, CRISOSTOMO 3000</t>
+          <t>ALCARAZ 5168</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>810371027</t>
+          <t>810378783</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6933,24 +6933,24 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.458516</v>
+        <v>-58.50875</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.646422</v>
+        <v>-34.623434</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>PPT-N</t>
+          <t>DEV-H</t>
         </is>
       </c>
       <c r="R76" t="inlineStr">

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-22 06:35:36)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R69"/>
+  <dimension ref="A1:R68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -614,17 +614,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3599</t>
+          <t>3765</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>9/26/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BEIRO, FRANCISCO AV. 3360</t>
+          <t>NAZCA AV. 1675</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -634,7 +634,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>797117093</t>
+          <t>01082878</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -649,7 +649,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Chocada</t>
+          <t>ya se traspaso nodo retirar columna</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -662,7 +662,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -671,10 +671,10 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.500297</v>
+        <v>-58.47874</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.598817</v>
+        <v>-34.61462</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -688,7 +688,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>PUE-B</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -4558,27 +4558,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>7169</t>
+          <t>7260</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>9/5/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5045</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>809492980</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4593,7 +4593,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Poste quebrado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4611,18 +4611,18 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.515637</v>
+        <v>-58.458298</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.589993</v>
+        <v>-34.566511</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4632,7 +4632,7 @@
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-F</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -4644,27 +4644,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>7260</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Vidal 1861</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>809642175</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4679,7 +4679,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4697,18 +4697,18 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.458298</v>
+        <v>-58.516218</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.566511</v>
+        <v>-34.589343</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>COG-F</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
@@ -4730,7 +4730,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4740,7 +4740,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>SANABRIA 4817</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4750,7 +4750,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809758873</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4765,7 +4765,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4783,14 +4783,14 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.516218</v>
+        <v>-58.520505</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.589343</v>
+        <v>-34.596045</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4804,39 +4804,39 @@
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>7240</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>SANABRIA 4817</t>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>809758873</t>
+          <t>809784524</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4851,7 +4851,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4873,14 +4873,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.520505</v>
+        <v>-58.481316</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.596045</v>
+        <v>-34.556157</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4890,39 +4890,39 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>7240</t>
+          <t>6475</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>9/16/2025</t>
+          <t>9/17/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+          <t>Av Amancio Alcorta 3570</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>809784524</t>
+          <t>809800213</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4937,7 +4937,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4959,24 +4959,24 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.481316</v>
+        <v>-58.409278</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.556157</v>
+        <v>-34.653566</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
@@ -4988,7 +4988,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>6182</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4998,7 +4998,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Av Amancio Alcorta 3570</t>
+          <t>Los Patos 2702</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -5008,7 +5008,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>809800213</t>
+          <t>809818308</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -5023,7 +5023,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -5031,7 +5031,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -5041,14 +5041,14 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.409278</v>
+        <v>-58.399262</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.653566</v>
+        <v>-34.639685</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -5062,7 +5062,7 @@
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -5074,27 +5074,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6182</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/23/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Los Patos 2702</t>
+          <t>CIUDAD DE LA PAZ 911</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>809818308</t>
+          <t>ICD30958043</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -5109,7 +5109,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
+          <t>Desmonte de columna ya traspasaron un nodo</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -5122,7 +5122,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -5131,24 +5131,24 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.399262</v>
+        <v>-58.447743</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.639685</v>
+        <v>-34.570457</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -5160,27 +5160,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>2528</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>9/23/2025</t>
+          <t>9/24/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 911</t>
+          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>ICD30958043</t>
+          <t>809972754</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -5195,7 +5195,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron un nodo</t>
+          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -5208,7 +5208,7 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -5217,14 +5217,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.447743</v>
+        <v>-58.452532</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.570457</v>
+        <v>-34.609005</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -5234,7 +5234,7 @@
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>NRA-H</t>
         </is>
       </c>
       <c r="R56" t="inlineStr">
@@ -5246,27 +5246,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>7308</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>9/24/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
+          <t>MANZANARES 4186</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>809972754</t>
+          <t>809979726</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5281,7 +5281,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -5303,14 +5303,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.452532</v>
+        <v>-58.485454</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.609005</v>
+        <v>-34.555745</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -5320,7 +5320,7 @@
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>NRA-H</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
@@ -5332,7 +5332,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>7308</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -5342,17 +5342,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MANZANARES 4186</t>
+          <t>BACACAY AV. 5805</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>809979726</t>
+          <t>809979728</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -5367,7 +5367,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar y reparar rienda</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -5385,18 +5385,18 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.485454</v>
+        <v>-58.509324</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.555745</v>
+        <v>-34.635335</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -5406,19 +5406,19 @@
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>DEV-M</t>
         </is>
       </c>
       <c r="R58" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>7314</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -5428,17 +5428,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BACACAY AV. 5805</t>
+          <t>MIRALLA 954</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>809979728</t>
+          <t>809979735</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -5453,7 +5453,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Cambiar y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -5471,14 +5471,14 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.509324</v>
+        <v>-58.501431</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.635335</v>
+        <v>-34.647791</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -5492,39 +5492,39 @@
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>DEV-M</t>
+          <t>PAV-?</t>
         </is>
       </c>
       <c r="R59" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>7314</t>
+          <t>7373</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MIRALLA 954</t>
+          <t>SANTIAGO DEL ESTERO 1253</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>809979735</t>
+          <t>810132493</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -5561,24 +5561,24 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.501431</v>
+        <v>-58.384406</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.647791</v>
+        <v>-34.622932</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>PAV-?</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7373</t>
+          <t>7387</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5600,17 +5600,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>SANTIAGO DEL ESTERO 1253</t>
+          <t>PERIBEBUY 6814</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>810132493</t>
+          <t>810132728</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5647,24 +5647,24 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.384406</v>
+        <v>-58.521719</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.622932</v>
+        <v>-34.647467</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PAV-C</t>
         </is>
       </c>
       <c r="R61" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7387</t>
+          <t>7394</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5686,17 +5686,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>PERIBEBUY 6814</t>
+          <t>BONIFACIO, JOSE 2409</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>810132728</t>
+          <t>810132768</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5733,24 +5733,24 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.521719</v>
+        <v>-58.461482</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.647467</v>
+        <v>-34.632432</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>PAV-C</t>
+          <t>PCH-F</t>
         </is>
       </c>
       <c r="R62" t="inlineStr">
@@ -5762,7 +5762,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7394</t>
+          <t>7402</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5772,17 +5772,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>BONIFACIO, JOSE 2409</t>
+          <t>RIVADAVIA AV. 2479</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>810132768</t>
+          <t>810132836</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5797,7 +5797,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5819,14 +5819,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.461482</v>
+        <v>-58.401428</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.632432</v>
+        <v>-34.609797</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5836,7 +5836,7 @@
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>PCH-F</t>
+          <t>CLI-D</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
@@ -5848,7 +5848,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7402</t>
+          <t>7405</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5858,7 +5858,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 2479</t>
+          <t>CHILE 2115</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5868,7 +5868,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>810132836</t>
+          <t>810132907</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5883,7 +5883,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5905,10 +5905,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.401428</v>
+        <v>-58.396368</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.609797</v>
+        <v>-34.61718</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5922,7 +5922,7 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>CLI-D</t>
+          <t>CEN-C</t>
         </is>
       </c>
       <c r="R64" t="inlineStr">
@@ -5934,17 +5934,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7405</t>
+          <t>7410</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>10/1/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>CHILE 2115</t>
+          <t>CHILE 2163</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5954,7 +5954,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>810132907</t>
+          <t>810132956</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5991,10 +5991,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.396368</v>
+        <v>-58.397024</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.61718</v>
+        <v>-34.617234</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -6020,27 +6020,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7410</t>
+          <t>7498</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>10/1/2025</t>
+          <t>10/13/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CHILE 2163</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 396</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>810132956</t>
+          <t>01071047</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6055,7 +6055,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cementar vereda y ver si la columna esta a plomo  ademas reclaman cables cortados</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -6077,14 +6077,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.397024</v>
+        <v>-58.467049</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.617234</v>
+        <v>-34.626303</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -6094,7 +6094,7 @@
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>CEN-C</t>
+          <t>NRA-E</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
@@ -6106,17 +6106,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7498</t>
+          <t>7516</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>10/13/2025</t>
+          <t>10/15/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 396</t>
+          <t>ALVAREZ, CRISOSTOMO 3000</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -6126,7 +6126,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>01071047</t>
+          <t>810371027</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6141,7 +6141,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Cementar vereda y ver si la columna esta a plomo  ademas reclaman cables cortados</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -6163,10 +6163,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.467049</v>
+        <v>-58.458516</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.626303</v>
+        <v>-34.646422</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -6180,7 +6180,7 @@
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>NRA-E</t>
+          <t>PPT-N</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -6192,27 +6192,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7516</t>
+          <t>5783</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>10/15/2025</t>
+          <t>10/17/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>ALVAREZ, CRISOSTOMO 3000</t>
+          <t>ALCARAZ 5168</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>810371027</t>
+          <t>810378783</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6249,113 +6249,27 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.458516</v>
+        <v>-58.50875</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.646422</v>
+        <v>-34.623434</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>PPT-N</t>
+          <t>DEV-H</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>5783</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>10/17/2025</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>ALCARAZ 5168</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>810378783</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I69" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M69" t="n">
-        <v>-58.50875</v>
-      </c>
-      <c r="N69" t="n">
-        <v>-34.623434</v>
-      </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>Devoto</t>
-        </is>
-      </c>
-      <c r="P69" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>DEV-H</t>
-        </is>
-      </c>
-      <c r="R69" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-27 19:24:43)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R79"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1900,27 +1900,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>7633</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>TREINTA Y TRES ORIENTALES 965</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1930,12 +1930,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1957,14 +1957,14 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.441405</v>
+        <v>-58.423042</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.594348</v>
+        <v>-34.625868</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1974,7 +1974,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>VCR-H</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1986,7 +1986,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1996,17 +1996,17 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2019,7 +2019,11 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+        </is>
+      </c>
       <c r="I19" t="n">
         <v>1</v>
       </c>
@@ -2039,14 +2043,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.483821</v>
+        <v>-58.441405</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.677698</v>
+        <v>-34.594348</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -2056,7 +2060,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>PAV-Q</t>
+          <t>VCR-H</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -2068,27 +2072,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -2098,14 +2102,10 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
       <c r="I20" t="n">
         <v>1</v>
       </c>
@@ -2116,7 +2116,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -2125,14 +2125,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.425764</v>
+        <v>-58.483821</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.604359</v>
+        <v>-34.677698</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>ALM-L</t>
+          <t>PAV-Q</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
@@ -2154,27 +2154,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>LASTRA AV. 4379</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>804663677</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -2189,7 +2189,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2211,56 +2211,56 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.525125</v>
+        <v>-58.425764</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.604668</v>
+        <v>-34.604359</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>DEV-F</t>
+          <t>ALM-L</t>
         </is>
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>5626</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 746</t>
+          <t>LASTRA AV. 4379</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>804876044</t>
+          <t>804663677</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2275,7 +2275,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Aplomador</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2297,36 +2297,36 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.439751</v>
+        <v>-58.525125</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.609908</v>
+        <v>-34.604668</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>ALM-I</t>
+          <t>DEV-F</t>
         </is>
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1DEV</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>5626</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2336,17 +2336,17 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>ACOYTE AV. 746</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>804876044</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Aplomador</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2369,7 +2369,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2383,14 +2383,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.375515</v>
+        <v>-58.439751</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.634393</v>
+        <v>-34.609908</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>CON-B</t>
+          <t>ALM-I</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -2412,27 +2412,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5671</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>TUCUMAN 3589</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>805507284</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2469,14 +2469,14 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.415839</v>
+        <v>-58.375515</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.599291</v>
+        <v>-34.634393</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>CLI-L</t>
+          <t>CON-B</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2498,27 +2498,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>5671</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>TUCUMAN 3589</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>805507284</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2555,14 +2555,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.372751</v>
+        <v>-58.415839</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.631917</v>
+        <v>-34.599291</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>CON-B</t>
+          <t>CLI-L</t>
         </is>
       </c>
       <c r="R25" t="inlineStr">
@@ -2584,27 +2584,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2619,7 +2619,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Picada entro tambien como reclamo 7611</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2632,7 +2632,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2641,14 +2641,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.395063</v>
+        <v>-58.372751</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.606257</v>
+        <v>-34.631917</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>CLI-B</t>
+          <t>CON-B</t>
         </is>
       </c>
       <c r="R26" t="inlineStr">
@@ -2670,7 +2670,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5835</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2680,17 +2680,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>YAPEYU 198</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>806926444</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2705,7 +2705,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2713,12 +2713,12 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2727,10 +2727,10 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.421623</v>
+        <v>-58.395063</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.614541</v>
+        <v>-34.606257</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2744,7 +2744,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>CLI-B</t>
         </is>
       </c>
       <c r="R27" t="inlineStr">
@@ -2756,27 +2756,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5929</t>
+          <t>5835</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>BACACAY 961</t>
+          <t>YAPEYU 198</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>806926757</t>
+          <t>806926444</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Columna inclinada con base corroída</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2799,7 +2799,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2813,10 +2813,10 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.443196</v>
+        <v>-58.421623</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.618534</v>
+        <v>-34.614541</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2830,7 +2830,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>NRA-A</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2842,27 +2842,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>5929</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>BACACAY 961</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>806926757</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Columna inclinada con base corroída</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2895,28 +2895,28 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.483927</v>
+        <v>-58.443196</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.570689</v>
+        <v>-34.618534</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>PUE-E</t>
+          <t>NRA-A</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2928,17 +2928,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5938</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>DE LOS CONSTITUYENTES AV. 4615</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>807044154</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2971,7 +2971,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2981,18 +2981,18 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.492605</v>
+        <v>-58.483927</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.581454</v>
+        <v>-34.570689</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3002,7 +3002,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>PUE-K</t>
+          <t>PUE-E</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3014,7 +3014,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>5938</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -3024,17 +3024,17 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>DE LOS CONSTITUYENTES AV. 4615</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>807044154</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3071,24 +3071,24 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.467789</v>
+        <v>-58.492605</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.68463</v>
+        <v>-34.581454</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>PAV-U</t>
+          <t>PUE-K</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3100,17 +3100,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5948</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>MURGUIONDO 3990</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -3120,7 +3120,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>807129347</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>COLUMNA INCLINADA</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -3153,14 +3153,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.477944</v>
+        <v>-58.467789</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.675149</v>
+        <v>-34.68463</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>PAV-V</t>
+          <t>PAV-U</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3186,27 +3186,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5973</t>
+          <t>5948</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>PALOS 432</t>
+          <t>MURGUIONDO 3990</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>807168105</t>
+          <t>807129347</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>COLUMNA INCLINADA</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -3239,18 +3239,18 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.362579</v>
+        <v>-58.477944</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.635096</v>
+        <v>-34.675149</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>CON-G</t>
+          <t>PAV-V</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3272,7 +3272,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>3715</t>
+          <t>5973</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3282,17 +3282,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>EL SERENO 358</t>
+          <t>PALOS 432</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>807168098</t>
+          <t>807168105</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3307,7 +3307,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -3315,7 +3315,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -3325,60 +3325,60 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.487371</v>
+        <v>-58.362579</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.640099</v>
+        <v>-34.635096</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>PCH-S</t>
+          <t>CON-G</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2PCH</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6004</t>
+          <t>3715</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>MAZA 181</t>
+          <t>EL SERENO 358</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>807215439</t>
+          <t>807168098</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3393,7 +3393,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3401,50 +3401,50 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.416477</v>
+        <v>-58.487371</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.61303</v>
+        <v>-34.640099</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>PCH-S</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2PCH</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>6010</t>
+          <t>6004</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3454,7 +3454,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ESTADO DE PALESTINA 771</t>
+          <t>MAZA 181</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3464,7 +3464,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>807215458</t>
+          <t>807215439</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada y mal ubicada ver con Pedro</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3492,7 +3492,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3501,10 +3501,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.425478</v>
+        <v>-58.416477</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.601865</v>
+        <v>-34.61303</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3518,7 +3518,7 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>CLI-N</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -3530,27 +3530,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>6284</t>
+          <t>6010</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>CHILE 2561</t>
+          <t>ESTADO DE PALESTINA 771</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>807851584</t>
+          <t>807215458</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3560,10 +3560,14 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Picada y mal ubicada ver con Pedro</t>
+        </is>
+      </c>
       <c r="I37" t="n">
         <v>1</v>
       </c>
@@ -3574,7 +3578,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3583,10 +3587,10 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.401827</v>
+        <v>-58.425478</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.617667</v>
+        <v>-34.601865</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3600,7 +3604,7 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>CEN-M</t>
+          <t>CLI-N</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -3612,27 +3616,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3642,83 +3646,79 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>Reparar rienda</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr"/>
       <c r="I38" t="n">
         <v>1</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.473179</v>
+        <v>-58.401827</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.629138</v>
+        <v>-34.617667</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>NRA-R</t>
+          <t>CEN-M</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2NRA</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3733,7 +3733,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3741,7 +3741,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3751,60 +3751,60 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.422229</v>
+        <v>-58.473179</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.573148</v>
+        <v>-34.629138</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>VCR-M</t>
+          <t>NRA-R</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2NRA</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>7336</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CRAMER AV. 2141</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3827,7 +3827,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3841,24 +3841,24 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.461582</v>
+        <v>-58.422229</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.564296</v>
+        <v>-34.573148</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>COG-H</t>
+          <t>VCR-M</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -3870,27 +3870,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>7336</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>CRAMER AV. 2141</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3905,7 +3905,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3923,28 +3923,28 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.494864</v>
+        <v>-58.461582</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.678826</v>
+        <v>-34.564296</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>PAV-M</t>
+          <t>COG-H</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -3956,27 +3956,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3999,7 +3999,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -4009,18 +4009,18 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.375684</v>
+        <v>-58.494864</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.656092</v>
+        <v>-34.678826</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -4030,7 +4030,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>CON-I</t>
+          <t>PAV-M</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -4042,27 +4042,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4077,7 +4077,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Poste inclinado ingreso tambien como 7201</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -4095,28 +4095,28 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.461024</v>
+        <v>-58.375684</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.539409</v>
+        <v>-34.656092</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>BLO-F</t>
+          <t>CON-I</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -4128,27 +4128,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5999</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 228</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808918687</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4158,51 +4158,51 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Se deriva directamente a traspaso de fuente ya que hay una columna existente</t>
+          <t>Poste inclinado ingreso tambien como 7201</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.425858</v>
+        <v>-58.461024</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.61629</v>
+        <v>-34.539409</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>BLO-F</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -4214,7 +4214,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6917</t>
+          <t>5999</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -4224,17 +4224,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>BRIN, MINISTRO 1375</t>
+          <t>MARMOL, JOSE 228</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808918700</t>
+          <t>808918687</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4244,16 +4244,16 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Se deriva directamente a traspaso de fuente ya que hay una columna existente</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
@@ -4262,7 +4262,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -4271,14 +4271,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.355342</v>
+        <v>-58.425858</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.63565</v>
+        <v>-34.61629</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>CON-G</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -4300,27 +4300,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -4357,24 +4357,24 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.472869</v>
+        <v>-58.355342</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.562</v>
+        <v>-34.63565</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>COG-I</t>
+          <t>CON-G</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
@@ -4386,27 +4386,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>7260</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Vidal 1861</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>809642175</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -4443,10 +4443,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.458298</v>
+        <v>-58.472869</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.566511</v>
+        <v>-34.562</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -4460,7 +4460,7 @@
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>COG-F</t>
+          <t>COG-I</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
@@ -4472,27 +4472,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>7260</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4507,7 +4507,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4525,18 +4525,18 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.516218</v>
+        <v>-58.458298</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.589343</v>
+        <v>-34.566511</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-F</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
@@ -4558,7 +4558,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4568,7 +4568,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>SANABRIA 4817</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4578,7 +4578,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>809758873</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4593,7 +4593,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4611,14 +4611,14 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.520505</v>
+        <v>-58.516218</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.596045</v>
+        <v>-34.589343</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4632,39 +4632,39 @@
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>7240</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>9/16/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+          <t>SANABRIA 4817</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>809784524</t>
+          <t>809758873</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4679,7 +4679,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4701,14 +4701,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.481316</v>
+        <v>-58.520505</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.556157</v>
+        <v>-34.596045</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4718,39 +4718,39 @@
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>7240</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Av Amancio Alcorta 3570</t>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>809800213</t>
+          <t>809784524</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4765,7 +4765,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4773,7 +4773,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4787,24 +4787,24 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.409278</v>
+        <v>-58.481316</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.653566</v>
+        <v>-34.556157</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
@@ -4816,7 +4816,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6182</t>
+          <t>6475</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4826,7 +4826,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Los Patos 2702</t>
+          <t>Av Amancio Alcorta 3570</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4836,7 +4836,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>809818308</t>
+          <t>809800213</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4851,7 +4851,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4859,7 +4859,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4869,14 +4869,14 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.399262</v>
+        <v>-58.409278</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.639685</v>
+        <v>-34.653566</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -4902,27 +4902,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>6182</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>9/23/2025</t>
+          <t>9/17/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 911</t>
+          <t>Los Patos 2702</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>ICD30958043</t>
+          <t>809818308</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4937,7 +4937,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron un nodo</t>
+          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4950,7 +4950,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4959,24 +4959,24 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.447743</v>
+        <v>-58.399262</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.570457</v>
+        <v>-34.639685</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
@@ -4988,27 +4988,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>9/24/2025</t>
+          <t>9/23/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
+          <t>CIUDAD DE LA PAZ 911</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>809972754</t>
+          <t>ICD30958043</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -5023,7 +5023,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
+          <t>Desmonte de columna ya traspasaron un nodo</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -5036,7 +5036,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -5045,14 +5045,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.452532</v>
+        <v>-58.447743</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.609005</v>
+        <v>-34.570457</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -5062,7 +5062,7 @@
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>NRA-H</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -5074,27 +5074,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>7308</t>
+          <t>2528</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>9/24/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>MANZANARES 4186</t>
+          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>809979726</t>
+          <t>809972754</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -5109,7 +5109,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -5131,14 +5131,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.485454</v>
+        <v>-58.452532</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.555745</v>
+        <v>-34.609005</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -5148,7 +5148,7 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>NRA-H</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -5160,7 +5160,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>7308</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -5170,17 +5170,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>BACACAY AV. 5805</t>
+          <t>MANZANARES 4186</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>809979728</t>
+          <t>809979726</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -5195,7 +5195,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Cambiar y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -5213,18 +5213,18 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.509324</v>
+        <v>-58.485454</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.635335</v>
+        <v>-34.555745</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -5234,19 +5234,19 @@
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>DEV-M</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R56" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>7314</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -5256,17 +5256,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>MIRALLA 954</t>
+          <t>BACACAY AV. 5805</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>809979735</t>
+          <t>809979728</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5281,7 +5281,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar y reparar rienda</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -5299,14 +5299,14 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.501431</v>
+        <v>-58.509324</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.647791</v>
+        <v>-34.635335</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -5320,39 +5320,39 @@
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>PAV-?</t>
+          <t>DEV-M</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>7373</t>
+          <t>7314</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SANTIAGO DEL ESTERO 1253</t>
+          <t>MIRALLA 954</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>810132493</t>
+          <t>809979735</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -5389,24 +5389,24 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.384406</v>
+        <v>-58.501431</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.622932</v>
+        <v>-34.647791</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PAV-?</t>
         </is>
       </c>
       <c r="R58" t="inlineStr">
@@ -5418,7 +5418,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>7387</t>
+          <t>7373</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -5428,17 +5428,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>PERIBEBUY 6814</t>
+          <t>SANTIAGO DEL ESTERO 1253</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>810132728</t>
+          <t>810132493</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -5453,7 +5453,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -5475,24 +5475,24 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.521719</v>
+        <v>-58.384406</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.647467</v>
+        <v>-34.622932</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>PAV-C</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R59" t="inlineStr">
@@ -5504,7 +5504,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>7394</t>
+          <t>7387</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -5514,17 +5514,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>BONIFACIO, JOSE 2409</t>
+          <t>PERIBEBUY 6814</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>810132768</t>
+          <t>810132728</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -5539,7 +5539,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -5561,24 +5561,24 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.461482</v>
+        <v>-58.521719</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.632432</v>
+        <v>-34.647467</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>PCH-F</t>
+          <t>PAV-C</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7402</t>
+          <t>7394</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5600,17 +5600,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 2479</t>
+          <t>BONIFACIO, JOSE 2409</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>810132836</t>
+          <t>810132768</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5647,14 +5647,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.401428</v>
+        <v>-58.461482</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.609797</v>
+        <v>-34.632432</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5664,7 +5664,7 @@
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>CLI-D</t>
+          <t>PCH-F</t>
         </is>
       </c>
       <c r="R61" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7405</t>
+          <t>7402</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5686,7 +5686,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>CHILE 2115</t>
+          <t>RIVADAVIA AV. 2479</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5696,7 +5696,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>810132907</t>
+          <t>810132836</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5733,10 +5733,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.396368</v>
+        <v>-58.401428</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.61718</v>
+        <v>-34.609797</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5750,7 +5750,7 @@
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>CEN-C</t>
+          <t>CLI-D</t>
         </is>
       </c>
       <c r="R62" t="inlineStr">
@@ -5762,17 +5762,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7410</t>
+          <t>7405</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>10/1/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>CHILE 2163</t>
+          <t>CHILE 2115</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5782,7 +5782,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>810132956</t>
+          <t>810132907</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5819,10 +5819,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.397024</v>
+        <v>-58.396368</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.617234</v>
+        <v>-34.61718</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5848,27 +5848,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7481</t>
+          <t>7410</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>10/8/2025</t>
+          <t>10/1/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>BACACAY 2455</t>
+          <t>CHILE 2163</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>810259148</t>
+          <t>810132956</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5905,14 +5905,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.464662</v>
+        <v>-58.397024</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.626638</v>
+        <v>-34.617234</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5922,7 +5922,7 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>NRA-E</t>
+          <t>CEN-C</t>
         </is>
       </c>
       <c r="R64" t="inlineStr">
@@ -5934,17 +5934,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7496</t>
+          <t>7481</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>10/13/2025</t>
+          <t>10/8/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BOGOTA 2594</t>
+          <t>BACACAY 2455</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5954,7 +5954,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>810333058</t>
+          <t>810259148</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5991,10 +5991,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.466896</v>
+        <v>-58.464662</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.626136</v>
+        <v>-34.626638</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -6020,7 +6020,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7497</t>
+          <t>7496</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -6030,7 +6030,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>BOGOTA 2684</t>
+          <t>BOGOTA 2594</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -6040,7 +6040,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>810333044</t>
+          <t>810333058</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6077,10 +6077,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.468091</v>
+        <v>-58.466896</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.626512</v>
+        <v>-34.626136</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -6106,7 +6106,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7498</t>
+          <t>7499</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -6116,7 +6116,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 396</t>
+          <t>BOGOTA 2626</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -6126,7 +6126,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>01071047</t>
+          <t>810333049</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6141,7 +6141,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Cementar vereda y ver si la columna esta a plomo  ademas reclaman cables cortados</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -6163,10 +6163,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.467049</v>
+        <v>-58.467473</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.626303</v>
+        <v>-34.626316</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -6192,7 +6192,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7499</t>
+          <t>7595</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -6202,7 +6202,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BOGOTA 2626</t>
+          <t>FALCON, RAMON L.,CNEL. 2353</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -6212,7 +6212,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>810333049</t>
+          <t>810333018</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6249,10 +6249,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.467473</v>
+        <v>-58.46138</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.626316</v>
+        <v>-34.629774</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -6266,7 +6266,7 @@
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>NRA-E</t>
+          <t>PCH-J</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
@@ -6278,17 +6278,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7595</t>
+          <t>7512</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>10/13/2025</t>
+          <t>10/16/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 2353</t>
+          <t>FALCON, RAMON L.,CNEL. 1930</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -6298,7 +6298,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>810333018</t>
+          <t>810371025</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -6335,10 +6335,10 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.46138</v>
+        <v>-58.456399</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.629774</v>
+        <v>-34.62829</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -6364,17 +6364,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7512</t>
+          <t>7516</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>10/16/2025</t>
+          <t>10/15/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1930</t>
+          <t>ALVAREZ, CRISOSTOMO 3000</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -6384,7 +6384,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>810371025</t>
+          <t>810371027</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -6421,10 +6421,10 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.456399</v>
+        <v>-58.458516</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.62829</v>
+        <v>-34.646422</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -6438,7 +6438,7 @@
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>PCH-J</t>
+          <t>PPT-N</t>
         </is>
       </c>
       <c r="R70" t="inlineStr">
@@ -6450,27 +6450,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7516</t>
+          <t>5783</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>10/15/2025</t>
+          <t>10/17/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>ALVAREZ, CRISOSTOMO 3000</t>
+          <t>ALCARAZ 5168</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>810371027</t>
+          <t>810378783</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -6507,24 +6507,24 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.458516</v>
+        <v>-58.50875</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.646422</v>
+        <v>-34.623434</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>PPT-N</t>
+          <t>DEV-H</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
@@ -6536,27 +6536,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>5783</t>
+          <t>7621</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>10/17/2025</t>
+          <t>10/20/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ALCARAZ 5168</t>
+          <t>Quito 3832</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>810378783</t>
+          <t>810404273</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -6593,24 +6593,24 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.50875</v>
+        <v>-58.420412</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.623434</v>
+        <v>-34.616726</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>DEV-H</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R72" t="inlineStr">
@@ -7216,6 +7216,522 @@
         </is>
       </c>
       <c r="R79" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>7620</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>10/24/2025</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>QUITO 3954</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>810447247</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>-58.422216</v>
+      </c>
+      <c r="N80" t="n">
+        <v>-34.616828</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>ALM-C</t>
+        </is>
+      </c>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>-654</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>10/24/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Calfucura 2750</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>810447248</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Columna Metalica podrida en base</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.480709</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.608973</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>NRA-O</t>
+        </is>
+      </c>
+      <c r="R81" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>5749</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>10/27/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1754</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Pendiente de Carga</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Traspaso de nodo propio</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>-58.4018</v>
+      </c>
+      <c r="N82" t="n">
+        <v>-34.590471</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Recoleta</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>AGU-F</t>
+        </is>
+      </c>
+      <c r="R82" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>7631</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>10/27/2025</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>CALVO, CARLOS 3762</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>810451584</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
+        <v>-58.418542</v>
+      </c>
+      <c r="N83" t="n">
+        <v>-34.624609</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>ALM-A</t>
+        </is>
+      </c>
+      <c r="R83" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>7630</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>10/27/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>INDEPENDENCIA AV. 3690</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>810451588</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.417821</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.621158</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>ALM-A</t>
+        </is>
+      </c>
+      <c r="R84" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>7624</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>10/27/2025</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>DIAZ VELEZ AV. 4516</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>810454541</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>-58.430613</v>
+      </c>
+      <c r="N85" t="n">
+        <v>-34.608805</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>ALM-J</t>
+        </is>
+      </c>
+      <c r="R85" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-28 11:18:34)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R85"/>
+  <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3616,17 +3616,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6284</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>CHILE 2561</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3636,7 +3636,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807851584</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3646,10 +3646,14 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Hay que colocar nuevamente la R400 porque la chocaron</t>
+        </is>
+      </c>
       <c r="I38" t="n">
         <v>1</v>
       </c>
@@ -3660,7 +3664,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3669,10 +3673,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.401827</v>
+        <v>-58.401624</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.617667</v>
+        <v>-34.612001</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -3686,7 +3690,7 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>CEN-M</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -3698,27 +3702,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3728,83 +3732,79 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Reparar rienda</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="n">
         <v>1</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.473179</v>
+        <v>-58.401827</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.629138</v>
+        <v>-34.617667</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>NRA-R</t>
+          <t>CEN-M</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2NRA</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3827,7 +3827,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3837,60 +3837,60 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.422229</v>
+        <v>-58.473179</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.573148</v>
+        <v>-34.629138</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>VCR-M</t>
+          <t>NRA-R</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2NRA</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>7336</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>CRAMER AV. 2141</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3905,7 +3905,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3913,7 +3913,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3927,24 +3927,24 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.461582</v>
+        <v>-58.422229</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.564296</v>
+        <v>-34.573148</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>COG-H</t>
+          <t>VCR-M</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -3956,27 +3956,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>7336</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>CRAMER AV. 2141</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3999,7 +3999,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -4009,28 +4009,28 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.494864</v>
+        <v>-58.461582</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.678826</v>
+        <v>-34.564296</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>PAV-M</t>
+          <t>COG-H</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -4042,27 +4042,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4077,7 +4077,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -4085,7 +4085,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -4095,18 +4095,18 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.375684</v>
+        <v>-58.494864</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.656092</v>
+        <v>-34.678826</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -4116,7 +4116,7 @@
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>CON-I</t>
+          <t>PAV-M</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -4128,27 +4128,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Poste inclinado ingreso tambien como 7201</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -4181,28 +4181,28 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.461024</v>
+        <v>-58.375684</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.539409</v>
+        <v>-34.656092</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>BLO-F</t>
+          <t>CON-I</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -4214,27 +4214,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5999</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 228</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808918687</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4244,51 +4244,51 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Se deriva directamente a traspaso de fuente ya que hay una columna existente</t>
+          <t>Poste inclinado ingreso tambien como 7201</t>
         </is>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.425858</v>
+        <v>-58.461024</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.61629</v>
+        <v>-34.539409</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>BLO-F</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -4300,7 +4300,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6917</t>
+          <t>5999</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -4310,17 +4310,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>BRIN, MINISTRO 1375</t>
+          <t>MARMOL, JOSE 228</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808918700</t>
+          <t>808918687</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4330,16 +4330,16 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Se deriva directamente a traspaso de fuente ya que hay una columna existente</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -4348,7 +4348,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -4357,14 +4357,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.355342</v>
+        <v>-58.425858</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.63565</v>
+        <v>-34.61629</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -4374,7 +4374,7 @@
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>CON-G</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
@@ -4386,27 +4386,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -4443,24 +4443,24 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.472869</v>
+        <v>-58.355342</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.562</v>
+        <v>-34.63565</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>COG-I</t>
+          <t>CON-G</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
@@ -4472,27 +4472,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>7260</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Vidal 1861</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>809642175</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4529,10 +4529,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.458298</v>
+        <v>-58.472869</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.566511</v>
+        <v>-34.562</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4546,7 +4546,7 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>COG-F</t>
+          <t>COG-I</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
@@ -4558,27 +4558,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>7260</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4593,7 +4593,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4611,18 +4611,18 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.516218</v>
+        <v>-58.458298</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.589343</v>
+        <v>-34.566511</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4632,7 +4632,7 @@
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-F</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4654,7 +4654,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>SANABRIA 4817</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4664,7 +4664,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>809758873</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4679,7 +4679,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4697,14 +4697,14 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.520505</v>
+        <v>-58.516218</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.596045</v>
+        <v>-34.589343</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4718,39 +4718,39 @@
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>7240</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>9/16/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+          <t>SANABRIA 4817</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>809784524</t>
+          <t>809758873</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4765,7 +4765,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4787,14 +4787,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.481316</v>
+        <v>-58.520505</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.556157</v>
+        <v>-34.596045</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4804,39 +4804,39 @@
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>7240</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Av Amancio Alcorta 3570</t>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>809800213</t>
+          <t>809784524</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4851,7 +4851,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4859,7 +4859,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4873,24 +4873,24 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.409278</v>
+        <v>-58.481316</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.653566</v>
+        <v>-34.556157</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -4902,7 +4902,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6182</t>
+          <t>6475</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4912,7 +4912,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Los Patos 2702</t>
+          <t>Av Amancio Alcorta 3570</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4922,7 +4922,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>809818308</t>
+          <t>809800213</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4937,7 +4937,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4955,14 +4955,14 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.399262</v>
+        <v>-58.409278</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.639685</v>
+        <v>-34.653566</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4976,7 +4976,7 @@
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
@@ -4988,27 +4988,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>6182</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>9/23/2025</t>
+          <t>9/17/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 911</t>
+          <t>Los Patos 2702</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>ICD30958043</t>
+          <t>809818308</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -5023,7 +5023,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron un nodo</t>
+          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -5036,7 +5036,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -5045,24 +5045,24 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.447743</v>
+        <v>-58.399262</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.570457</v>
+        <v>-34.639685</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -5074,27 +5074,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>9/24/2025</t>
+          <t>9/23/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
+          <t>CIUDAD DE LA PAZ 911</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>809972754</t>
+          <t>ICD30958043</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -5109,7 +5109,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
+          <t>Desmonte de columna ya traspasaron un nodo</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -5122,7 +5122,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -5131,14 +5131,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.452532</v>
+        <v>-58.447743</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.609005</v>
+        <v>-34.570457</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -5148,7 +5148,7 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>NRA-H</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -5160,27 +5160,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>7308</t>
+          <t>2528</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>9/24/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>MANZANARES 4186</t>
+          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>809979726</t>
+          <t>809972754</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -5195,7 +5195,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -5217,14 +5217,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.485454</v>
+        <v>-58.452532</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.555745</v>
+        <v>-34.609005</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -5234,7 +5234,7 @@
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>NRA-H</t>
         </is>
       </c>
       <c r="R56" t="inlineStr">
@@ -5246,7 +5246,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>7308</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -5256,17 +5256,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>BACACAY AV. 5805</t>
+          <t>MANZANARES 4186</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>809979728</t>
+          <t>809979726</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5281,7 +5281,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Cambiar y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -5299,18 +5299,18 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.509324</v>
+        <v>-58.485454</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.635335</v>
+        <v>-34.555745</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -5320,19 +5320,19 @@
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>DEV-M</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>7314</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -5342,17 +5342,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MIRALLA 954</t>
+          <t>BACACAY AV. 5805</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>809979735</t>
+          <t>809979728</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -5367,7 +5367,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar y reparar rienda</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -5385,14 +5385,14 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.501431</v>
+        <v>-58.509324</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.647791</v>
+        <v>-34.635335</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -5406,39 +5406,39 @@
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>PAV-?</t>
+          <t>DEV-M</t>
         </is>
       </c>
       <c r="R58" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>7373</t>
+          <t>7314</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SANTIAGO DEL ESTERO 1253</t>
+          <t>MIRALLA 954</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>810132493</t>
+          <t>809979735</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -5475,24 +5475,24 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.384406</v>
+        <v>-58.501431</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.622932</v>
+        <v>-34.647791</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PAV-?</t>
         </is>
       </c>
       <c r="R59" t="inlineStr">
@@ -5504,7 +5504,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>7387</t>
+          <t>7373</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -5514,17 +5514,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>PERIBEBUY 6814</t>
+          <t>SANTIAGO DEL ESTERO 1253</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>810132728</t>
+          <t>810132493</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -5539,7 +5539,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -5561,24 +5561,24 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.521719</v>
+        <v>-58.384406</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.647467</v>
+        <v>-34.622932</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>PAV-C</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
@@ -5590,7 +5590,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7394</t>
+          <t>7387</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -5600,17 +5600,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>BONIFACIO, JOSE 2409</t>
+          <t>PERIBEBUY 6814</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>810132768</t>
+          <t>810132728</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5647,24 +5647,24 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.461482</v>
+        <v>-58.521719</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.632432</v>
+        <v>-34.647467</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>PCH-F</t>
+          <t>PAV-C</t>
         </is>
       </c>
       <c r="R61" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7402</t>
+          <t>7394</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5686,17 +5686,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 2479</t>
+          <t>BONIFACIO, JOSE 2409</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>810132836</t>
+          <t>810132768</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5711,7 +5711,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5733,14 +5733,14 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.401428</v>
+        <v>-58.461482</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.609797</v>
+        <v>-34.632432</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5750,7 +5750,7 @@
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>CLI-D</t>
+          <t>PCH-F</t>
         </is>
       </c>
       <c r="R62" t="inlineStr">
@@ -5762,7 +5762,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7405</t>
+          <t>7402</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5772,7 +5772,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>CHILE 2115</t>
+          <t>RIVADAVIA AV. 2479</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5782,7 +5782,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>810132907</t>
+          <t>810132836</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5797,7 +5797,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5819,10 +5819,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.396368</v>
+        <v>-58.401428</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.61718</v>
+        <v>-34.609797</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5836,7 +5836,7 @@
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>CEN-C</t>
+          <t>CLI-D</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
@@ -5848,17 +5848,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7410</t>
+          <t>7405</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>10/1/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CHILE 2163</t>
+          <t>CHILE 2115</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5868,7 +5868,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>810132956</t>
+          <t>810132907</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5905,10 +5905,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.397024</v>
+        <v>-58.396368</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.617234</v>
+        <v>-34.61718</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5934,27 +5934,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7481</t>
+          <t>7410</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>10/8/2025</t>
+          <t>10/1/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BACACAY 2455</t>
+          <t>CHILE 2163</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>810259148</t>
+          <t>810132956</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5991,14 +5991,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.464662</v>
+        <v>-58.397024</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.626638</v>
+        <v>-34.617234</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -6008,7 +6008,7 @@
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>NRA-E</t>
+          <t>CEN-C</t>
         </is>
       </c>
       <c r="R65" t="inlineStr">
@@ -6020,17 +6020,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7496</t>
+          <t>7481</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>10/13/2025</t>
+          <t>10/8/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>BOGOTA 2594</t>
+          <t>BACACAY 2455</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -6040,7 +6040,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>810333058</t>
+          <t>810259148</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6077,10 +6077,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.466896</v>
+        <v>-58.464662</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.626136</v>
+        <v>-34.626638</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -6106,7 +6106,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7499</t>
+          <t>7496</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -6116,7 +6116,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>BOGOTA 2626</t>
+          <t>BOGOTA 2594</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -6126,7 +6126,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>810333049</t>
+          <t>810333058</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6163,10 +6163,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.467473</v>
+        <v>-58.466896</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.626316</v>
+        <v>-34.626136</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -7732,6 +7732,92 @@
         </is>
       </c>
       <c r="R85" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>7643</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>10/28/2025</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>ACEVEDO 524</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>810458896</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>1</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M86" t="n">
+        <v>-58.439164</v>
+      </c>
+      <c r="N86" t="n">
+        <v>-34.597069</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>VCR-J</t>
+        </is>
+      </c>
+      <c r="R86" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-29 11:16:32)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R86"/>
+  <dimension ref="A1:R88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7823,6 +7823,178 @@
         </is>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>7665</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>10/28/2025</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>ARAOZ 2313</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>810461115</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Picada y cable cortado</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M87" t="n">
+        <v>-58.417634</v>
+      </c>
+      <c r="N87" t="n">
+        <v>-34.587439</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>VCR-G</t>
+        </is>
+      </c>
+      <c r="R87" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>7619</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>10/29/2025</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>QUITO 4180</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>810471618</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I88" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M88" t="n">
+        <v>-58.425596</v>
+      </c>
+      <c r="N88" t="n">
+        <v>-34.617038</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>ALM-C</t>
+        </is>
+      </c>
+      <c r="R88" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-30 07:13:44)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R89"/>
+  <dimension ref="A1:R88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,7 +571,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>No corresponde</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -579,7 +579,11 @@
           <t>Fuente Teco</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M2" t="n">
         <v>-58.408259</v>
       </c>
@@ -3784,27 +3788,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6284</t>
+          <t>6141</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>6/11/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>CHILE 2561</t>
+          <t>EL PAMPERO 2618</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807851584</t>
+          <t>807458310</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3814,7 +3818,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H40" t="inlineStr"/>
@@ -3828,7 +3832,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3837,24 +3841,24 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.401827</v>
+        <v>-58.481942</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.617667</v>
+        <v>-34.602989</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>CEN-M</t>
+          <t>NRA-P</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -3866,27 +3870,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6357</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7/7/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>BACACAY 3088</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808036196</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3896,83 +3900,79 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Reparar rienda</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr"/>
       <c r="I41" t="n">
         <v>1</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.473179</v>
+        <v>-58.401827</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.629138</v>
+        <v>-34.617667</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>NRA-R</t>
+          <t>CEN-M</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2NRA</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6497</t>
+          <t>6357</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/7/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4691</t>
+          <t>BACACAY 3088</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808533127</t>
+          <t>808036196</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3987,7 +3987,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3995,7 +3995,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -4005,60 +4005,60 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.422229</v>
+        <v>-58.473179</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.573148</v>
+        <v>-34.629138</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>VCR-M</t>
+          <t>NRA-R</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2NRA</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>7336</t>
+          <t>6497</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CRAMER AV. 2141</t>
+          <t>SEGUI, JUAN FRANCISCO 4691</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>808533127</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4073,7 +4073,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -4081,7 +4081,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -4095,24 +4095,24 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.461582</v>
+        <v>-58.422229</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.564296</v>
+        <v>-34.573148</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>COG-H</t>
+          <t>VCR-M</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -4124,27 +4124,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>7336</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>CRAMER AV. 2141</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808663881</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4159,7 +4159,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -4167,7 +4167,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -4177,28 +4177,28 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.494864</v>
+        <v>-58.461582</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.678826</v>
+        <v>-34.564296</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>PAV-M</t>
+          <t>COG-H</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -4210,27 +4210,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4245,7 +4245,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -4263,18 +4263,18 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.375684</v>
+        <v>-58.494864</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.656092</v>
+        <v>-34.678826</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -4284,7 +4284,7 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>CON-I</t>
+          <t>PAV-M</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -4296,27 +4296,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4331,7 +4331,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Poste inclinado ingreso tambien como 7201</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -4349,28 +4349,28 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.461024</v>
+        <v>-58.375684</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.539409</v>
+        <v>-34.656092</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>BLO-F</t>
+          <t>CON-I</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
@@ -4382,27 +4382,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5999</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 228</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808918687</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -4412,51 +4412,51 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Se deriva directamente a traspaso de fuente ya que hay una columna existente</t>
+          <t>Poste inclinado ingreso tambien como 7201</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.425858</v>
+        <v>-58.461024</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.61629</v>
+        <v>-34.539409</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>BLO-F</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
@@ -4468,7 +4468,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6917</t>
+          <t>5999</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4478,17 +4478,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>BRIN, MINISTRO 1375</t>
+          <t>MARMOL, JOSE 228</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808918700</t>
+          <t>808918687</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4498,16 +4498,16 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Se deriva directamente a traspaso de fuente ya que hay una columna existente</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4516,7 +4516,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -4525,14 +4525,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.355342</v>
+        <v>-58.425858</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.63565</v>
+        <v>-34.61629</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4542,7 +4542,7 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>CON-G</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
@@ -4554,27 +4554,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>6917</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>BRIN, MINISTRO 1375</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>808918700</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4589,7 +4589,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4611,24 +4611,24 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.472869</v>
+        <v>-58.355342</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.562</v>
+        <v>-34.63565</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>COG-I</t>
+          <t>CON-G</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -4640,27 +4640,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>7260</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Vidal 1861</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>809642175</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4697,10 +4697,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.458298</v>
+        <v>-58.472869</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.566511</v>
+        <v>-34.562</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4714,7 +4714,7 @@
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>COG-F</t>
+          <t>COG-I</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
@@ -4726,27 +4726,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>7260</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4761,7 +4761,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4779,18 +4779,18 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.516218</v>
+        <v>-58.458298</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.589343</v>
+        <v>-34.566511</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4800,7 +4800,7 @@
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-F</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
@@ -4812,7 +4812,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4822,7 +4822,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>SANABRIA 4817</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4832,7 +4832,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>809758873</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4847,7 +4847,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4865,14 +4865,14 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.520505</v>
+        <v>-58.516218</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.596045</v>
+        <v>-34.589343</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4886,39 +4886,39 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>7240</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>9/16/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+          <t>SANABRIA 4817</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>809784524</t>
+          <t>809758873</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4933,7 +4933,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4955,14 +4955,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.481316</v>
+        <v>-58.520505</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.556157</v>
+        <v>-34.596045</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4972,39 +4972,39 @@
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>PUE-O</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PUE</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>7240</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Av Amancio Alcorta 3570</t>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>809800213</t>
+          <t>809784524</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -5019,7 +5019,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -5027,7 +5027,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -5041,24 +5041,24 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.409278</v>
+        <v>-58.481316</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.653566</v>
+        <v>-34.556157</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -5070,7 +5070,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6182</t>
+          <t>6475</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -5080,7 +5080,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Los Patos 2702</t>
+          <t>Av Amancio Alcorta 3570</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -5090,7 +5090,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>809818308</t>
+          <t>809800213</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -5113,7 +5113,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -5123,14 +5123,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.399262</v>
+        <v>-58.409278</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.639685</v>
+        <v>-34.653566</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -5144,7 +5144,7 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -5156,27 +5156,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>6182</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>9/23/2025</t>
+          <t>9/17/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 911</t>
+          <t>Los Patos 2702</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>ICD30958043</t>
+          <t>809818308</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -5191,7 +5191,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron un nodo</t>
+          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -5204,7 +5204,7 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -5213,24 +5213,24 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.447743</v>
+        <v>-58.399262</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.570457</v>
+        <v>-34.639685</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R56" t="inlineStr">
@@ -5242,27 +5242,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>9/24/2025</t>
+          <t>9/23/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
+          <t>CIUDAD DE LA PAZ 911</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>809972754</t>
+          <t>ICD30958043</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5277,7 +5277,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
+          <t>Desmonte de columna ya traspasaron un nodo</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -5290,7 +5290,7 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L57" t="inlineStr">
@@ -5299,14 +5299,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.452532</v>
+        <v>-58.447743</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.609005</v>
+        <v>-34.570457</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -5316,7 +5316,7 @@
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>NRA-H</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
@@ -5328,27 +5328,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>7308</t>
+          <t>2528</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>9/24/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MANZANARES 4186</t>
+          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>809979726</t>
+          <t>809972754</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -5363,7 +5363,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -5385,14 +5385,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.485454</v>
+        <v>-58.452532</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.555745</v>
+        <v>-34.609005</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -5402,7 +5402,7 @@
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>NRA-H</t>
         </is>
       </c>
       <c r="R58" t="inlineStr">
@@ -5414,7 +5414,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>7308</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -5424,17 +5424,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BACACAY AV. 5805</t>
+          <t>MANZANARES 4186</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>809979728</t>
+          <t>809979726</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -5449,7 +5449,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Cambiar y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -5467,18 +5467,18 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.509324</v>
+        <v>-58.485454</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.635335</v>
+        <v>-34.555745</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -5488,19 +5488,19 @@
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>DEV-M</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R59" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>7314</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -5510,17 +5510,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MIRALLA 954</t>
+          <t>BACACAY AV. 5805</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>809979735</t>
+          <t>809979728</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -5535,7 +5535,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar y reparar rienda</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -5553,14 +5553,14 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.501431</v>
+        <v>-58.509324</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.647791</v>
+        <v>-34.635335</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -5574,39 +5574,39 @@
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>PAV-?</t>
+          <t>DEV-M</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7373</t>
+          <t>7314</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>SANTIAGO DEL ESTERO 1253</t>
+          <t>MIRALLA 954</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>810132493</t>
+          <t>809979735</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5643,24 +5643,24 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.384406</v>
+        <v>-58.501431</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.622932</v>
+        <v>-34.647791</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PAV-?</t>
         </is>
       </c>
       <c r="R61" t="inlineStr">
@@ -5672,7 +5672,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7387</t>
+          <t>7373</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5682,17 +5682,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>PERIBEBUY 6814</t>
+          <t>SANTIAGO DEL ESTERO 1253</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>810132728</t>
+          <t>810132493</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5707,7 +5707,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5729,24 +5729,24 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.521719</v>
+        <v>-58.384406</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.647467</v>
+        <v>-34.622932</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>PAV-C</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R62" t="inlineStr">
@@ -5758,7 +5758,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7394</t>
+          <t>7387</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5768,17 +5768,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>BONIFACIO, JOSE 2409</t>
+          <t>PERIBEBUY 6814</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>810132768</t>
+          <t>810132728</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5793,7 +5793,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5815,24 +5815,24 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.461482</v>
+        <v>-58.521719</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.632432</v>
+        <v>-34.647467</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>PCH-F</t>
+          <t>PAV-C</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
@@ -5844,7 +5844,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7402</t>
+          <t>7394</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5854,17 +5854,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>RIVADAVIA AV. 2479</t>
+          <t>BONIFACIO, JOSE 2409</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>810132836</t>
+          <t>810132768</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5879,7 +5879,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5901,14 +5901,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.401428</v>
+        <v>-58.461482</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.609797</v>
+        <v>-34.632432</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5918,7 +5918,7 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>CLI-D</t>
+          <t>PCH-F</t>
         </is>
       </c>
       <c r="R64" t="inlineStr">
@@ -5930,27 +5930,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7405</t>
+          <t>7481</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>10/8/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>CHILE 2115</t>
+          <t>BACACAY 2455</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>810132907</t>
+          <t>810259148</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5987,14 +5987,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.396368</v>
+        <v>-58.464662</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.61718</v>
+        <v>-34.626638</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -6004,7 +6004,7 @@
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>CEN-C</t>
+          <t>NRA-E</t>
         </is>
       </c>
       <c r="R65" t="inlineStr">
@@ -6016,27 +6016,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7410</t>
+          <t>7496</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>10/1/2025</t>
+          <t>10/13/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CHILE 2163</t>
+          <t>BOGOTA 2594</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>810132956</t>
+          <t>810333058</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6073,14 +6073,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.397024</v>
+        <v>-58.466896</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.617234</v>
+        <v>-34.626136</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -6090,7 +6090,7 @@
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>CEN-C</t>
+          <t>NRA-E</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
@@ -6102,17 +6102,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7481</t>
+          <t>7595</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>10/8/2025</t>
+          <t>10/13/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>BACACAY 2455</t>
+          <t>FALCON, RAMON L.,CNEL. 2353</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -6122,7 +6122,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>810259148</t>
+          <t>810333018</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6159,10 +6159,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.464662</v>
+        <v>-58.46138</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.626638</v>
+        <v>-34.629774</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -6176,7 +6176,7 @@
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>NRA-E</t>
+          <t>PCH-J</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -6188,17 +6188,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7496</t>
+          <t>7512</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>10/13/2025</t>
+          <t>10/16/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BOGOTA 2594</t>
+          <t>FALCON, RAMON L.,CNEL. 1930</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -6208,7 +6208,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>810333058</t>
+          <t>810371025</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6245,10 +6245,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.466896</v>
+        <v>-58.456399</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.626136</v>
+        <v>-34.62829</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -6262,7 +6262,7 @@
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>NRA-E</t>
+          <t>PCH-J</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
@@ -6274,17 +6274,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7595</t>
+          <t>7516</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>10/13/2025</t>
+          <t>10/15/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 2353</t>
+          <t>ALVAREZ, CRISOSTOMO 3000</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -6294,7 +6294,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>810333018</t>
+          <t>810371027</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -6331,10 +6331,10 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.46138</v>
+        <v>-58.458516</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.629774</v>
+        <v>-34.646422</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -6348,7 +6348,7 @@
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>PCH-J</t>
+          <t>PPT-N</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -6360,27 +6360,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7512</t>
+          <t>5783</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>10/16/2025</t>
+          <t>10/17/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1930</t>
+          <t>ALCARAZ 5168</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>810371025</t>
+          <t>810378783</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -6417,24 +6417,24 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.456399</v>
+        <v>-58.50875</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.62829</v>
+        <v>-34.623434</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>PCH-J</t>
+          <t>DEV-H</t>
         </is>
       </c>
       <c r="R70" t="inlineStr">
@@ -6446,27 +6446,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7516</t>
+          <t>7621</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>10/15/2025</t>
+          <t>10/20/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>ALVAREZ, CRISOSTOMO 3000</t>
+          <t>Quito 3832</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>810371027</t>
+          <t>810404273</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -6503,14 +6503,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.458516</v>
+        <v>-58.420412</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.646422</v>
+        <v>-34.616726</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -6520,7 +6520,7 @@
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>PPT-N</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
@@ -6532,27 +6532,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>5783</t>
+          <t>-648</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>10/17/2025</t>
+          <t>10/21/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ALCARAZ 5168</t>
+          <t>Azcuenaga 1619</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>810378783</t>
+          <t>810093631</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -6589,56 +6589,56 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.50875</v>
+        <v>-58.397296</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.623434</v>
+        <v>-34.590444</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>DEV-H</t>
+          <t>RET-D</t>
         </is>
       </c>
       <c r="R72" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7621</t>
+          <t>7571</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>10/20/2025</t>
+          <t>10/22/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Quito 3832</t>
+          <t>SAENZ AV. 1204</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>810404273</t>
+          <t>810416653</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -6675,14 +6675,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.420412</v>
+        <v>-58.416237</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.616726</v>
+        <v>-34.65477</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -6692,7 +6692,7 @@
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R73" t="inlineStr">
@@ -6704,7 +6704,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-648</t>
+          <t>7556</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -6714,17 +6714,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Azcuenaga 1619</t>
+          <t>SANCHEZ DE LORIA 1923</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>810093631</t>
+          <t>810416656</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6739,7 +6739,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>cambiar</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6761,14 +6761,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.397296</v>
+        <v>-58.411426</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.590444</v>
+        <v>-34.633266</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6778,19 +6778,19 @@
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>RET-D</t>
+          <t>PPT-Q</t>
         </is>
       </c>
       <c r="R74" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7571</t>
+          <t>7579</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6800,17 +6800,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>SAENZ AV. 1204</t>
+          <t>AGUIRRE 508</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>810416653</t>
+          <t>810421912</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6843,18 +6843,18 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.416237</v>
+        <v>-58.435731</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.65477</v>
+        <v>-34.597659</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6864,7 +6864,7 @@
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>VCR-H</t>
         </is>
       </c>
       <c r="R75" t="inlineStr">
@@ -6876,27 +6876,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7556</t>
+          <t>7592</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>10/21/2025</t>
+          <t>10/22/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1923</t>
+          <t>LAPRIDA 1612</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>810416656</t>
+          <t>810421919</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6911,7 +6911,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6933,14 +6933,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.411426</v>
+        <v>-58.404086</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.633266</v>
+        <v>-34.590935</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6950,7 +6950,7 @@
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>PPT-Q</t>
+          <t>AGU-E</t>
         </is>
       </c>
       <c r="R76" t="inlineStr">
@@ -6962,7 +6962,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7579</t>
+          <t>7594</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6972,17 +6972,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>AGUIRRE 508</t>
+          <t>NEWBERY, JORGE 2696</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>810421912</t>
+          <t>810421921</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -7019,10 +7019,10 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.435731</v>
+        <v>-58.44293</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.597659</v>
+        <v>-34.574483</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -7036,7 +7036,7 @@
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>VCR-H</t>
+          <t>COG-B</t>
         </is>
       </c>
       <c r="R77" t="inlineStr">
@@ -7048,7 +7048,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7592</t>
+          <t>7601</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -7058,7 +7058,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>LAPRIDA 1612</t>
+          <t>AYACUCHO 1997</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -7068,7 +7068,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>810421919</t>
+          <t>810421922</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -7105,10 +7105,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.404086</v>
+        <v>-58.38923</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.590935</v>
+        <v>-34.587666</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -7122,7 +7122,7 @@
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>AGU-E</t>
+          <t>RET-A</t>
         </is>
       </c>
       <c r="R78" t="inlineStr">
@@ -7134,27 +7134,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7594</t>
+          <t>7620</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>10/22/2025</t>
+          <t>10/24/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 2696</t>
+          <t>QUITO 3954</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>810421921</t>
+          <t>810447247</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -7187,18 +7187,18 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.44293</v>
+        <v>-58.422216</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.574483</v>
+        <v>-34.616828</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -7208,7 +7208,7 @@
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>COG-B</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R79" t="inlineStr">
@@ -7220,27 +7220,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7601</t>
+          <t>-654</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>10/22/2025</t>
+          <t>10/24/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>AYACUCHO 1997</t>
+          <t>Calfucura 2750</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>810421922</t>
+          <t>810447248</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -7255,7 +7255,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna Metalica podrida en base</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -7277,24 +7277,24 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.38923</v>
+        <v>-58.480709</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.587666</v>
+        <v>-34.608973</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>RET-A</t>
+          <t>NRA-O</t>
         </is>
       </c>
       <c r="R80" t="inlineStr">
@@ -7306,27 +7306,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7620</t>
+          <t>5749</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>10/24/2025</t>
+          <t>10/27/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>QUITO 3954</t>
+          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1754</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>810447247</t>
+          <t>Pendiente de Carga</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -7336,16 +7336,16 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de nodo propio</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -7354,7 +7354,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
@@ -7363,14 +7363,14 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.422216</v>
+        <v>-58.4018</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.616828</v>
+        <v>-34.590471</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -7380,7 +7380,7 @@
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>AGU-F</t>
         </is>
       </c>
       <c r="R81" t="inlineStr">
@@ -7392,27 +7392,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>-654</t>
+          <t>7631</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>10/24/2025</t>
+          <t>10/27/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Calfucura 2750</t>
+          <t>CALVO, CARLOS 3762</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>810447248</t>
+          <t>810451584</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -7427,7 +7427,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Columna Metalica podrida en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -7449,24 +7449,24 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.480709</v>
+        <v>-58.418542</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.608973</v>
+        <v>-34.624609</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>NRA-O</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R82" t="inlineStr">
@@ -7478,7 +7478,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>5749</t>
+          <t>7630</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -7488,17 +7488,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1754</t>
+          <t>INDEPENDENCIA AV. 3690</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Pendiente de Carga</t>
+          <t>810451588</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -7508,16 +7508,16 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Traspaso de nodo propio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
@@ -7526,7 +7526,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -7535,14 +7535,14 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.4018</v>
+        <v>-58.417821</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.590471</v>
+        <v>-34.621158</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -7552,7 +7552,7 @@
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>AGU-F</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R83" t="inlineStr">
@@ -7564,7 +7564,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7631</t>
+          <t>7624</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -7574,17 +7574,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 3762</t>
+          <t>DIAZ VELEZ AV. 4516</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>810451584</t>
+          <t>810454541</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -7599,7 +7599,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -7621,14 +7621,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.418542</v>
+        <v>-58.430613</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.624609</v>
+        <v>-34.608805</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>ALM-J</t>
         </is>
       </c>
       <c r="R84" t="inlineStr">
@@ -7650,27 +7650,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7630</t>
+          <t>7643</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>10/27/2025</t>
+          <t>10/28/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>INDEPENDENCIA AV. 3690</t>
+          <t>ACEVEDO 524</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>810451588</t>
+          <t>810458896</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -7707,14 +7707,14 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.417821</v>
+        <v>-58.439164</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.621158</v>
+        <v>-34.597069</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -7724,7 +7724,7 @@
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>VCR-J</t>
         </is>
       </c>
       <c r="R85" t="inlineStr">
@@ -7736,27 +7736,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>7624</t>
+          <t>7665</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>10/27/2025</t>
+          <t>10/28/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>DIAZ VELEZ AV. 4516</t>
+          <t>ARAOZ 2313</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>810454541</t>
+          <t>810461115</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -7771,7 +7771,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada y cable cortado</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -7793,14 +7793,14 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.430613</v>
+        <v>-58.417634</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.608805</v>
+        <v>-34.587439</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -7810,7 +7810,7 @@
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>ALM-J</t>
+          <t>VCR-G</t>
         </is>
       </c>
       <c r="R86" t="inlineStr">
@@ -7822,27 +7822,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>7643</t>
+          <t>7619</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>10/28/2025</t>
+          <t>10/29/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>ACEVEDO 524</t>
+          <t>QUITO 4180</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>810458896</t>
+          <t>810471618</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -7879,14 +7879,14 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.439164</v>
+        <v>-58.425596</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.597069</v>
+        <v>-34.617038</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
@@ -7896,7 +7896,7 @@
       </c>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>VCR-J</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R87" t="inlineStr">
@@ -7908,27 +7908,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>7665</t>
+          <t>7689</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>10/28/2025</t>
+          <t>10/29/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>ARAOZ 2313</t>
+          <t>VIALE, LUIS 2026</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>810461115</t>
+          <t>810481197</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7943,7 +7943,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Picada y cable cortado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7965,113 +7965,27 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.417634</v>
+        <v>-58.464531</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.587439</v>
+        <v>-34.613946</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>VCR-G</t>
+          <t>NRA-J</t>
         </is>
       </c>
       <c r="R88" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>7619</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>10/29/2025</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>QUITO 4180</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>810471618</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I89" t="n">
-        <v>1</v>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M89" t="n">
-        <v>-58.425596</v>
-      </c>
-      <c r="N89" t="n">
-        <v>-34.617038</v>
-      </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P89" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-      <c r="Q89" t="inlineStr">
-        <is>
-          <t>ALM-C</t>
-        </is>
-      </c>
-      <c r="R89" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-30 11:51:58)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R88"/>
+  <dimension ref="A1:R89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7478,7 +7478,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7624</t>
+          <t>-657</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -7488,17 +7488,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>DIAZ VELEZ AV. 4516</t>
+          <t>Conde 1632</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>810454541</t>
+          <t>810454540</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -7513,7 +7513,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Poste inclinado cambiar o desmontar</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -7531,28 +7531,28 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.430613</v>
+        <v>-58.461492</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.608805</v>
+        <v>-34.57199</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>ALM-J</t>
+          <t>ATH-R</t>
         </is>
       </c>
       <c r="R83" t="inlineStr">
@@ -7564,27 +7564,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7643</t>
+          <t>7624</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>10/28/2025</t>
+          <t>10/27/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>ACEVEDO 524</t>
+          <t>DIAZ VELEZ AV. 4516</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>810458896</t>
+          <t>810454541</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -7599,7 +7599,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -7621,14 +7621,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.439164</v>
+        <v>-58.430613</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.597069</v>
+        <v>-34.608805</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>VCR-J</t>
+          <t>ALM-J</t>
         </is>
       </c>
       <c r="R84" t="inlineStr">
@@ -7650,7 +7650,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7665</t>
+          <t>7643</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -7660,17 +7660,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>ARAOZ 2313</t>
+          <t>ACEVEDO 524</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>810461115</t>
+          <t>810458896</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -7685,7 +7685,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Picada y cable cortado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -7707,10 +7707,10 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.417634</v>
+        <v>-58.439164</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.587439</v>
+        <v>-34.597069</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -7724,7 +7724,7 @@
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>VCR-G</t>
+          <t>VCR-J</t>
         </is>
       </c>
       <c r="R85" t="inlineStr">
@@ -7736,27 +7736,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>7619</t>
+          <t>7665</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>10/29/2025</t>
+          <t>10/28/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>QUITO 4180</t>
+          <t>ARAOZ 2313</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>810471618</t>
+          <t>810461115</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -7771,7 +7771,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada y cable cortado</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -7793,14 +7793,14 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.425596</v>
+        <v>-58.417634</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.617038</v>
+        <v>-34.587439</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
@@ -7810,7 +7810,7 @@
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>VCR-G</t>
         </is>
       </c>
       <c r="R86" t="inlineStr">
@@ -7822,7 +7822,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>7689</t>
+          <t>7619</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -7832,17 +7832,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>VIALE, LUIS 2026</t>
+          <t>QUITO 4180</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>810481197</t>
+          <t>810471618</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -7879,24 +7879,24 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.464531</v>
+        <v>-58.425596</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.613946</v>
+        <v>-34.617038</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>NRA-J</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R87" t="inlineStr">
@@ -7908,7 +7908,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>-660</t>
+          <t>7689</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -7918,17 +7918,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>CABILDO AV. 4351</t>
+          <t>VIALE, LUIS 2026</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>810481362</t>
+          <t>810481197</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7943,7 +7943,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Chocada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7965,14 +7965,14 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.471817</v>
+        <v>-58.464531</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.543967</v>
+        <v>-34.613946</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
@@ -7982,12 +7982,94 @@
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>BLO-S</t>
+          <t>NRA-J</t>
         </is>
       </c>
       <c r="R88" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>-661</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>10/30/2025</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>FLORES, VENANCIO, GRAL. 3715</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>-58.47989</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.631709</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Devoto</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>DEV-L</t>
+        </is>
+      </c>
+      <c r="R89" t="inlineStr">
+        <is>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-10-30 14:58:59)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R89"/>
+  <dimension ref="A1:R96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6102,27 +6102,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7512</t>
+          <t>7703</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>10/16/2025</t>
+          <t>10/15/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 1930</t>
+          <t>ROSARIO DE LA FRONTERA 4996</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>810371025</t>
+          <t>810355303</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6159,24 +6159,24 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.456399</v>
+        <v>-58.514176</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.62829</v>
+        <v>-34.589877</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>PCH-J</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -6188,17 +6188,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7516</t>
+          <t>7512</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>10/15/2025</t>
+          <t>10/16/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>ALVAREZ, CRISOSTOMO 3000</t>
+          <t>FALCON, RAMON L.,CNEL. 1930</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -6208,7 +6208,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>810371027</t>
+          <t>810371025</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6245,10 +6245,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.458516</v>
+        <v>-58.456399</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.646422</v>
+        <v>-34.62829</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -6262,7 +6262,7 @@
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>PPT-N</t>
+          <t>PCH-J</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
@@ -6274,27 +6274,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>5783</t>
+          <t>7516</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>10/17/2025</t>
+          <t>10/15/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ALCARAZ 5168</t>
+          <t>ALVAREZ, CRISOSTOMO 3000</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>810378783</t>
+          <t>810371027</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -6331,24 +6331,24 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.50875</v>
+        <v>-58.458516</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.623434</v>
+        <v>-34.646422</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>DEV-H</t>
+          <t>PPT-N</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -6360,27 +6360,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7621</t>
+          <t>7735</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>10/20/2025</t>
+          <t>10/15/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Quito 3832</t>
+          <t>GARCIA, MARTIN AV. 772</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>810404273</t>
+          <t>810371042</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -6417,14 +6417,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.420412</v>
+        <v>-58.374086</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.616726</v>
+        <v>-34.633168</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -6434,7 +6434,7 @@
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>CON-B</t>
         </is>
       </c>
       <c r="R70" t="inlineStr">
@@ -6446,27 +6446,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-648</t>
+          <t>5783</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>10/21/2025</t>
+          <t>10/17/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Azcuenaga 1619</t>
+          <t>ALCARAZ 5168</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>810093631</t>
+          <t>810378783</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -6503,56 +6503,56 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.397296</v>
+        <v>-58.50875</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.590444</v>
+        <v>-34.623434</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>RET-D</t>
+          <t>DEV-H</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1RET</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7571</t>
+          <t>7621</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>10/22/2025</t>
+          <t>10/20/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>SAENZ AV. 1204</t>
+          <t>Quito 3832</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>810416653</t>
+          <t>810404273</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -6589,14 +6589,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.416237</v>
+        <v>-58.420412</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.65477</v>
+        <v>-34.616726</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -6606,7 +6606,7 @@
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R72" t="inlineStr">
@@ -6618,7 +6618,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7556</t>
+          <t>-648</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -6628,17 +6628,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1923</t>
+          <t>Azcuenaga 1619</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>810416656</t>
+          <t>810093631</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -6653,7 +6653,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -6675,14 +6675,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.411426</v>
+        <v>-58.397296</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.633266</v>
+        <v>-34.590444</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -6692,19 +6692,19 @@
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>PPT-Q</t>
+          <t>RET-D</t>
         </is>
       </c>
       <c r="R73" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1RET</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7579</t>
+          <t>7571</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -6714,17 +6714,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>AGUIRRE 508</t>
+          <t>SAENZ AV. 1204</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>810421912</t>
+          <t>810416653</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6757,18 +6757,18 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.435731</v>
+        <v>-58.416237</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.597659</v>
+        <v>-34.65477</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6778,7 +6778,7 @@
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>VCR-H</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R74" t="inlineStr">
@@ -6790,27 +6790,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7592</t>
+          <t>7556</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>10/22/2025</t>
+          <t>10/21/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>LAPRIDA 1612</t>
+          <t>SANCHEZ DE LORIA 1923</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>810421919</t>
+          <t>810416656</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6825,7 +6825,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>cambiar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6847,14 +6847,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.404086</v>
+        <v>-58.411426</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.590935</v>
+        <v>-34.633266</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6864,7 +6864,7 @@
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>AGU-E</t>
+          <t>PPT-Q</t>
         </is>
       </c>
       <c r="R75" t="inlineStr">
@@ -6876,7 +6876,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7594</t>
+          <t>7579</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6886,17 +6886,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 2696</t>
+          <t>AGUIRRE 508</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>810421921</t>
+          <t>810421912</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6933,10 +6933,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.44293</v>
+        <v>-58.435731</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.574483</v>
+        <v>-34.597659</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6950,7 +6950,7 @@
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>COG-B</t>
+          <t>VCR-H</t>
         </is>
       </c>
       <c r="R76" t="inlineStr">
@@ -6962,7 +6962,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7601</t>
+          <t>7592</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6972,7 +6972,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>AYACUCHO 1997</t>
+          <t>LAPRIDA 1612</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -6982,7 +6982,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>810421922</t>
+          <t>810421919</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -7019,10 +7019,10 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.38923</v>
+        <v>-58.404086</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.587666</v>
+        <v>-34.590935</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -7036,7 +7036,7 @@
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>RET-A</t>
+          <t>AGU-E</t>
         </is>
       </c>
       <c r="R77" t="inlineStr">
@@ -7048,27 +7048,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7620</t>
+          <t>7594</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>10/24/2025</t>
+          <t>10/22/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>QUITO 3954</t>
+          <t>NEWBERY, JORGE 2696</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>810447247</t>
+          <t>810421921</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -7101,18 +7101,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.422216</v>
+        <v>-58.44293</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.616828</v>
+        <v>-34.574483</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -7122,7 +7122,7 @@
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>COG-B</t>
         </is>
       </c>
       <c r="R78" t="inlineStr">
@@ -7134,27 +7134,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-654</t>
+          <t>7601</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>10/24/2025</t>
+          <t>10/22/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Calfucura 2750</t>
+          <t>AYACUCHO 1997</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>810447248</t>
+          <t>810421922</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -7169,7 +7169,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Columna Metalica podrida en base</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -7191,24 +7191,24 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.480709</v>
+        <v>-58.38923</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.608973</v>
+        <v>-34.587666</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>NRA-O</t>
+          <t>RET-A</t>
         </is>
       </c>
       <c r="R79" t="inlineStr">
@@ -7220,27 +7220,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>5749</t>
+          <t>7620</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>10/27/2025</t>
+          <t>10/24/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1754</t>
+          <t>QUITO 3954</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Pendiente de Carga</t>
+          <t>810447247</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -7250,16 +7250,16 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Traspaso de nodo propio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
@@ -7268,7 +7268,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
@@ -7277,14 +7277,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.4018</v>
+        <v>-58.422216</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.590471</v>
+        <v>-34.616828</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -7294,7 +7294,7 @@
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>AGU-F</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R80" t="inlineStr">
@@ -7306,27 +7306,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7631</t>
+          <t>-654</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>10/27/2025</t>
+          <t>10/24/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 3762</t>
+          <t>Calfucura 2750</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>810451584</t>
+          <t>810447248</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -7341,7 +7341,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna Metalica podrida en base</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -7363,24 +7363,24 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.418542</v>
+        <v>-58.480709</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.624609</v>
+        <v>-34.608973</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>NRA-O</t>
         </is>
       </c>
       <c r="R81" t="inlineStr">
@@ -7392,7 +7392,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7630</t>
+          <t>5749</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -7402,17 +7402,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>INDEPENDENCIA AV. 3690</t>
+          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1754</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>810451588</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -7422,16 +7422,16 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de nodo propio</t>
         </is>
       </c>
       <c r="I82" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
@@ -7440,7 +7440,7 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
@@ -7449,14 +7449,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.417821</v>
+        <v>-58.4018</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.621158</v>
+        <v>-34.590471</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -7466,7 +7466,7 @@
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>AGU-F</t>
         </is>
       </c>
       <c r="R82" t="inlineStr">
@@ -7478,7 +7478,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-657</t>
+          <t>7631</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -7488,17 +7488,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Conde 1632</t>
+          <t>CALVO, CARLOS 3762</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>810454540</t>
+          <t>810451584</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -7513,7 +7513,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Poste inclinado cambiar o desmontar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -7531,28 +7531,28 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.461492</v>
+        <v>-58.418542</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.57199</v>
+        <v>-34.624609</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>ATH-R</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R83" t="inlineStr">
@@ -7564,7 +7564,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7624</t>
+          <t>7630</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -7574,17 +7574,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>DIAZ VELEZ AV. 4516</t>
+          <t>INDEPENDENCIA AV. 3690</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>810454541</t>
+          <t>810451588</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -7599,7 +7599,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -7621,14 +7621,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.430613</v>
+        <v>-58.417821</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.608805</v>
+        <v>-34.621158</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -7638,7 +7638,7 @@
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>ALM-J</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R84" t="inlineStr">
@@ -7650,27 +7650,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7643</t>
+          <t>7624</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>10/28/2025</t>
+          <t>10/27/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>ACEVEDO 524</t>
+          <t>DIAZ VELEZ AV. 4516</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>810458896</t>
+          <t>810454541</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -7685,7 +7685,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -7707,14 +7707,14 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.439164</v>
+        <v>-58.430613</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.597069</v>
+        <v>-34.608805</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -7724,7 +7724,7 @@
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>VCR-J</t>
+          <t>ALM-J</t>
         </is>
       </c>
       <c r="R85" t="inlineStr">
@@ -7736,27 +7736,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>7665</t>
+          <t>7622</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>10/28/2025</t>
+          <t>10/27/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>ARAOZ 2313</t>
+          <t>MIRALLA 950</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>810461115</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -7771,7 +7771,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Picada y cable cortado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -7784,7 +7784,7 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L86" t="inlineStr">
@@ -7793,24 +7793,24 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.417634</v>
+        <v>-58.50161</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.587439</v>
+        <v>-34.647648</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>VCR-G</t>
+          <t>PAV-?</t>
         </is>
       </c>
       <c r="R86" t="inlineStr">
@@ -7822,27 +7822,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>7619</t>
+          <t>7643</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>10/29/2025</t>
+          <t>10/28/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>QUITO 4180</t>
+          <t>ACEVEDO 524</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>810471618</t>
+          <t>810458896</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -7879,14 +7879,14 @@
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.425596</v>
+        <v>-58.439164</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.617038</v>
+        <v>-34.597069</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
@@ -7896,7 +7896,7 @@
       </c>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>VCR-J</t>
         </is>
       </c>
       <c r="R87" t="inlineStr">
@@ -7908,27 +7908,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>7689</t>
+          <t>7665</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>10/29/2025</t>
+          <t>10/28/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>VIALE, LUIS 2026</t>
+          <t>ARAOZ 2313</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>810481197</t>
+          <t>810461115</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7943,7 +7943,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada y cable cortado</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7965,24 +7965,24 @@
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.464531</v>
+        <v>-58.417634</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.613946</v>
+        <v>-34.587439</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>NRA-J</t>
+          <t>VCR-G</t>
         </is>
       </c>
       <c r="R88" t="inlineStr">
@@ -7994,82 +7994,688 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
+          <t>7683</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>10/28/2025</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1684</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>colocar columna para pedir traspaso de nodo</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>-58.402647</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.591114</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Recoleta</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>AGU-F</t>
+        </is>
+      </c>
+      <c r="R89" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>7619</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>10/29/2025</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>QUITO 4180</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>810471618</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
+        <v>-58.425596</v>
+      </c>
+      <c r="N90" t="n">
+        <v>-34.617038</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>ALM-C</t>
+        </is>
+      </c>
+      <c r="R90" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>-658</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>10/29/2025</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Vera 311</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Traspasar Fuente</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>1</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M91" t="n">
+        <v>-58.436262</v>
+      </c>
+      <c r="N91" t="n">
+        <v>-34.600478</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>CLI-O</t>
+        </is>
+      </c>
+      <c r="R91" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>7689</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>10/29/2025</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>VIALE, LUIS 2026</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>810481197</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>1</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M92" t="n">
+        <v>-58.464531</v>
+      </c>
+      <c r="N92" t="n">
+        <v>-34.613946</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>NRA-J</t>
+        </is>
+      </c>
+      <c r="R92" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
           <t>-661</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="B93" t="inlineStr">
         <is>
           <t>10/30/2025</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
+      <c r="C93" t="inlineStr">
         <is>
           <t>FLORES, VENANCIO, GRAL. 3715</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr">
+      <c r="D93" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr"/>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>810487013</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H89" t="inlineStr">
+      <c r="H93" t="inlineStr">
         <is>
           <t>Picada</t>
         </is>
       </c>
-      <c r="I89" t="n">
-        <v>1</v>
-      </c>
-      <c r="J89" t="inlineStr">
+      <c r="I93" t="n">
+        <v>1</v>
+      </c>
+      <c r="J93" t="inlineStr">
         <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K89" t="inlineStr">
+      <c r="K93" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L89" t="inlineStr">
+      <c r="L93" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M89" t="n">
+      <c r="M93" t="n">
         <v>-58.47989</v>
       </c>
-      <c r="N89" t="n">
+      <c r="N93" t="n">
         <v>-34.631709</v>
       </c>
-      <c r="O89" t="inlineStr">
+      <c r="O93" t="inlineStr">
         <is>
           <t>Devoto</t>
         </is>
       </c>
-      <c r="P89" t="inlineStr">
+      <c r="P93" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q89" t="inlineStr">
+      <c r="Q93" t="inlineStr">
         <is>
           <t>DEV-L</t>
         </is>
       </c>
-      <c r="R89" t="inlineStr">
+      <c r="R93" t="inlineStr">
         <is>
           <t>ARATO-25058.PO.2DEV</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>7709</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>10/30/2025</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>SAN BLAS 2891</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>810487021</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
+        <v>1</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M94" t="n">
+        <v>-58.48121</v>
+      </c>
+      <c r="N94" t="n">
+        <v>-34.61126</v>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P94" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>NRA-Q</t>
+        </is>
+      </c>
+      <c r="R94" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>7719</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>10/30/2025</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>CIUDAD DE LA PAZ 180</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Colocar R400 para traspaso</t>
+        </is>
+      </c>
+      <c r="I95" t="n">
+        <v>1</v>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>Nodo/Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M95" t="n">
+        <v>-58.440031</v>
+      </c>
+      <c r="N95" t="n">
+        <v>-34.575409</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P95" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>COG-B</t>
+        </is>
+      </c>
+      <c r="R95" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>7732</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>10/30/2025</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>LINIERS VIRREY 1142</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>810487035</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I96" t="n">
+        <v>1</v>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M96" t="n">
+        <v>-58.413563</v>
+      </c>
+      <c r="N96" t="n">
+        <v>-34.624645</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P96" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>CEN-P</t>
+        </is>
+      </c>
+      <c r="R96" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-03 07:26:37)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R96"/>
+  <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8593,92 +8593,6 @@
         </is>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>-664</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>10/31/2025</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>Mercedes 346</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>810493536</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>Estaba chocada pasada por Juli</t>
-        </is>
-      </c>
-      <c r="I96" t="n">
-        <v>0</v>
-      </c>
-      <c r="J96" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M96" t="n">
-        <v>-58.484683</v>
-      </c>
-      <c r="N96" t="n">
-        <v>-34.630456</v>
-      </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>Devoto</t>
-        </is>
-      </c>
-      <c r="P96" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q96" t="inlineStr">
-        <is>
-          <t>DEV-L</t>
-        </is>
-      </c>
-      <c r="R96" t="inlineStr">
-        <is>
-          <t>ARATO-25058.PO.2DEV</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-06 10:01:59)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Optical_Power" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Optical_Power" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-12 12:51:11)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R88"/>
+  <dimension ref="A1:R90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7758,7 +7758,11 @@
           <t>5</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr"/>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>810712796</t>
+        </is>
+      </c>
       <c r="F86" t="inlineStr">
         <is>
           <t>Optical Power</t>
@@ -7926,7 +7930,11 @@
           <t>6</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr"/>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>810712875</t>
+        </is>
+      </c>
       <c r="F88" t="inlineStr">
         <is>
           <t>Optical Power</t>
@@ -7982,6 +7990,178 @@
         </is>
       </c>
       <c r="R88" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>7746</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>11/11/2025</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>CAMPICHUELO 229</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>810712887</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>1</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>-58.433855</v>
+      </c>
+      <c r="N89" t="n">
+        <v>-34.614487</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>ALM-J</t>
+        </is>
+      </c>
+      <c r="R89" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>7842</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>11/12/2025</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>FERRARI 410</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>810713039</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
+        <v>-58.441198</v>
+      </c>
+      <c r="N90" t="n">
+        <v>-34.605341</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>ALM-O</t>
+        </is>
+      </c>
+      <c r="R90" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-13 12:03:39)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R91"/>
+  <dimension ref="A1:R90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7138,17 +7138,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7689</t>
+          <t>7709</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>10/29/2025</t>
+          <t>10/30/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>VIALE, LUIS 2026</t>
+          <t>SAN BLAS 2891</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -7158,7 +7158,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>810481197</t>
+          <t>810487021</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -7195,10 +7195,10 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.464531</v>
+        <v>-58.48121</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.613946</v>
+        <v>-34.61126</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -7212,7 +7212,7 @@
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>NRA-J</t>
+          <t>NRA-Q</t>
         </is>
       </c>
       <c r="R79" t="inlineStr">
@@ -7224,7 +7224,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7709</t>
+          <t>7719</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -7234,17 +7234,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>SAN BLAS 2891</t>
+          <t>CIUDAD DE LA PAZ 180</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>810487021</t>
+          <t>01229656</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -7259,7 +7259,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para traspaso</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -7272,7 +7272,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
@@ -7281,24 +7281,24 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.48121</v>
+        <v>-58.440031</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.61126</v>
+        <v>-34.575409</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>NRA-Q</t>
+          <t>COG-B</t>
         </is>
       </c>
       <c r="R80" t="inlineStr">
@@ -7310,7 +7310,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7719</t>
+          <t>7732</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -7320,17 +7320,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 180</t>
+          <t>LINIERS VIRREY 1142</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>01229656</t>
+          <t>810487035</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -7345,7 +7345,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspaso</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
@@ -7367,14 +7367,14 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.440031</v>
+        <v>-58.413563</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.575409</v>
+        <v>-34.624645</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -7384,7 +7384,7 @@
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>COG-B</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R81" t="inlineStr">
@@ -7396,27 +7396,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7732</t>
+          <t>7744</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>10/30/2025</t>
+          <t>10/31/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>LINIERS VIRREY 1142</t>
+          <t>NECOCHEA 369</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>810487035</t>
+          <t>01233359</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -7431,7 +7431,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R200 para rtaspaso de nodo</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -7444,7 +7444,7 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
@@ -7453,14 +7453,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.413563</v>
+        <v>-58.364132</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.624645</v>
+        <v>-34.628423</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -7470,7 +7470,7 @@
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>CON-F</t>
         </is>
       </c>
       <c r="R82" t="inlineStr">
@@ -7482,27 +7482,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7744</t>
+          <t>7780</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>10/31/2025</t>
+          <t>11/4/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>NECOCHEA 369</t>
+          <t>INDEPENDENCIA AV. 1654</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>01233359</t>
+          <t>810573618</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -7517,7 +7517,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Colocar R200 para rtaspaso de nodo</t>
+          <t>Columna picada e inclinada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -7530,7 +7530,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -7539,10 +7539,10 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.364132</v>
+        <v>-58.389676</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.628423</v>
+        <v>-34.618127</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -7556,7 +7556,7 @@
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>CON-F</t>
+          <t>CEN-?</t>
         </is>
       </c>
       <c r="R83" t="inlineStr">
@@ -7568,27 +7568,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7780</t>
+          <t>7810</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>11/4/2025</t>
+          <t>11/10/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>INDEPENDENCIA AV. 1654</t>
+          <t>GUTENBERG 3212</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>810573618</t>
+          <t>810651343</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -7603,7 +7603,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Columna picada e inclinada</t>
+          <t>Cambiar columna y ver que el vano quede separado del balcon esta inclinada hacia la casa</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -7625,36 +7625,36 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.389676</v>
+        <v>-58.501325</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.618127</v>
+        <v>-34.594325</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>CEN-?</t>
+          <t>PUE-Q</t>
         </is>
       </c>
       <c r="R84" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2PUE</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7810</t>
+          <t>-670</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -7664,17 +7664,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>GUTENBERG 3212</t>
+          <t>Timoteo Gordillo 1666</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>810651343</t>
+          <t>810651269</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -7689,7 +7689,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Cambiar columna y ver que el vano quede separado del balcon esta inclinada hacia la casa</t>
+          <t>Cambiar columna de lugar la actual es un poste ex Cablevision correrla ya que el vecino reclama obstruccion de la cochera</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -7711,14 +7711,14 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.501325</v>
+        <v>-58.510994</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.594325</v>
+        <v>-34.655027</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -7728,39 +7728,39 @@
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>PUE-Q</t>
+          <t>PAV-J</t>
         </is>
       </c>
       <c r="R85" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>-670</t>
+          <t>7604</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>11/10/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Timoteo Gordillo 1666</t>
+          <t>SAN JUAN AV. 3741</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>810651269</t>
+          <t>810712796</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -7775,7 +7775,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Cambiar columna de lugar la actual es un poste ex Cablevision correrla ya que el vecino reclama obstruccion de la cochera</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -7797,24 +7797,24 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.510994</v>
+        <v>-58.418108</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.655027</v>
+        <v>-34.62564</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>PAV-J</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R86" t="inlineStr">
@@ -7826,7 +7826,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>7604</t>
+          <t>7764</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -7836,17 +7836,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>SAN JUAN AV. 3741</t>
+          <t>2 DE ABRIL DE 1982 6510</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>810712796</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -7861,7 +7861,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmontar poste en desuso</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7869,7 +7869,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -7879,14 +7879,14 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.418108</v>
+        <v>-58.490261</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.62564</v>
+        <v>-34.677337</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -7900,7 +7900,7 @@
       </c>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>PAV-M</t>
         </is>
       </c>
       <c r="R87" t="inlineStr">
@@ -7912,7 +7912,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>7764</t>
+          <t>6415</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -7922,17 +7922,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6510</t>
+          <t>CAMPICHUELO 215</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810712875</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7947,7 +7947,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Desmontar poste en desuso</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7955,7 +7955,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -7965,18 +7965,18 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.490261</v>
+        <v>-58.433771</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.677337</v>
+        <v>-34.614668</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
@@ -7986,7 +7986,7 @@
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>PAV-M</t>
+          <t>ALM-J</t>
         </is>
       </c>
       <c r="R88" t="inlineStr">
@@ -7998,7 +7998,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>6415</t>
+          <t>7746</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -8008,7 +8008,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>CAMPICHUELO 215</t>
+          <t>CAMPICHUELO 229</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -8018,7 +8018,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>810712875</t>
+          <t>810712887</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -8033,7 +8033,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -8055,10 +8055,10 @@
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.433771</v>
+        <v>-58.433855</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.614668</v>
+        <v>-34.614487</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
@@ -8084,27 +8084,27 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>7746</t>
+          <t>7842</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>11/11/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>CAMPICHUELO 229</t>
+          <t>FERRARI 410</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>810712887</t>
+          <t>810713039</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -8119,7 +8119,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -8141,113 +8141,27 @@
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.433855</v>
+        <v>-58.441198</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.614487</v>
+        <v>-34.605341</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>ALM-J</t>
+          <t>ALM-O</t>
         </is>
       </c>
       <c r="R90" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>7842</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>11/12/2025</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>FERRARI 410</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>810713039</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I91" t="n">
-        <v>1</v>
-      </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M91" t="n">
-        <v>-58.441198</v>
-      </c>
-      <c r="N91" t="n">
-        <v>-34.605341</v>
-      </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P91" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q91" t="inlineStr">
-        <is>
-          <t>ALM-O</t>
-        </is>
-      </c>
-      <c r="R91" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-17 15:43:55)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R91"/>
+  <dimension ref="A1:R90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3612,27 +3612,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>7336</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>CRAMER AV. 2141</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>808663881</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3647,7 +3647,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna 114 base corroida </t>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3655,7 +3655,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3665,28 +3665,28 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.461582</v>
+        <v>-58.494864</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.564296</v>
+        <v>-34.678826</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>COG-H</t>
+          <t>PAV-M</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -3698,27 +3698,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3733,7 +3733,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3741,7 +3741,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3751,18 +3751,18 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.494864</v>
+        <v>-58.375684</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.678826</v>
+        <v>-34.656092</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3772,7 +3772,7 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>PAV-M</t>
+          <t>CON-I</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
@@ -3784,27 +3784,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Poste inclinado ingreso tambien como 7201</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3837,28 +3837,28 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.375684</v>
+        <v>-58.461024</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.656092</v>
+        <v>-34.539409</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>CON-I</t>
+          <t>BLO-F</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -3870,27 +3870,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>5999</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>MARMOL, JOSE 228</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808918687</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3900,51 +3900,51 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Poste inclinado ingreso tambien como 7201</t>
+          <t>Se deriva directamente a traspaso de fuente ya que hay una columna existente</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.461024</v>
+        <v>-58.425858</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.539409</v>
+        <v>-34.61629</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>BLO-F</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -3956,27 +3956,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5999</t>
+          <t>7098</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 228</t>
+          <t>UGARTE, MANUEL 3484</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>808918687</t>
+          <t>809126236</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3986,16 +3986,16 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Se deriva directamente a traspaso de fuente ya que hay una columna existente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -4013,24 +4013,24 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.425858</v>
+        <v>-58.472869</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.61629</v>
+        <v>-34.562</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>COG-I</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -4042,27 +4042,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>7098</t>
+          <t>7260</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>UGARTE, MANUEL 3484</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>809126236</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4099,10 +4099,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.472869</v>
+        <v>-58.458298</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.562</v>
+        <v>-34.566511</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -4116,7 +4116,7 @@
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>COG-I</t>
+          <t>COG-F</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -4128,27 +4128,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>7260</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Vidal 1861</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>809642175</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -4181,18 +4181,18 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.458298</v>
+        <v>-58.516218</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.566511</v>
+        <v>-34.589343</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -4202,7 +4202,7 @@
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>COG-F</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -4214,27 +4214,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>7240</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809784524</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4249,7 +4249,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -4267,18 +4267,18 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.516218</v>
+        <v>-58.481316</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.589343</v>
+        <v>-34.556157</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -4288,7 +4288,7 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -4300,27 +4300,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>6475</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/17/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SANABRIA 4817</t>
+          <t>Av Amancio Alcorta 3570</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>809758873</t>
+          <t>809800213</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Aplomar poste y reparar rienda ver con Pablo si se pude desmontar</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -4343,7 +4343,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -4357,56 +4357,56 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.520505</v>
+        <v>-58.409278</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.596045</v>
+        <v>-34.653566</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>PUE-O</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>7240</t>
+          <t>6182</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>9/16/2025</t>
+          <t>9/17/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+          <t>Los Patos 2702</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>809784524</t>
+          <t>809818308</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -4439,28 +4439,28 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.481316</v>
+        <v>-58.399262</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.556157</v>
+        <v>-34.639685</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
@@ -4472,27 +4472,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/23/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Av Amancio Alcorta 3570</t>
+          <t>CIUDAD DE LA PAZ 911</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>809800213</t>
+          <t>ICD30958043</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4507,7 +4507,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Desmonte de columna ya traspasaron un nodo</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4515,38 +4515,38 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.409278</v>
+        <v>-58.447743</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.653566</v>
+        <v>-34.570457</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
@@ -4558,27 +4558,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6182</t>
+          <t>2528</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/24/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Los Patos 2702</t>
+          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>809818308</t>
+          <t>809972754</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4593,7 +4593,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
+          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4615,24 +4615,24 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.399262</v>
+        <v>-58.452532</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.639685</v>
+        <v>-34.609005</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>NRA-H</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -4644,27 +4644,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>7308</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>9/23/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 911</t>
+          <t>MANZANARES 4186</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>ICD30958043</t>
+          <t>809979726</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4679,7 +4679,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron un nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4692,7 +4692,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -4701,14 +4701,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.447743</v>
+        <v>-58.485454</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.570457</v>
+        <v>-34.555745</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
@@ -4730,27 +4730,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>9/24/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>FIGUEROA, D. APOLINARIO, CORONEL 1047</t>
+          <t>BACACAY AV. 5805</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>809972754</t>
+          <t>809979728</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4765,7 +4765,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Cambiar columna ver si es necesario rienda con Pablo</t>
+          <t>Cambiar y reparar rienda</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4783,18 +4783,18 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.452532</v>
+        <v>-58.509324</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.609005</v>
+        <v>-34.635335</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4804,19 +4804,19 @@
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>NRA-H</t>
+          <t>DEV-M</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>7308</t>
+          <t>7314</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4826,17 +4826,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>MANZANARES 4186</t>
+          <t>MIRALLA 954</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>809979726</t>
+          <t>809979735</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4873,14 +4873,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.485454</v>
+        <v>-58.501431</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.555745</v>
+        <v>-34.647791</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4890,7 +4890,7 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>PAV-?</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -4902,27 +4902,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>7373</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>BACACAY AV. 5805</t>
+          <t>SANTIAGO DEL ESTERO 1253</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>809979728</t>
+          <t>810132493</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4937,7 +4937,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Cambiar y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4955,50 +4955,50 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.509324</v>
+        <v>-58.384406</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.635335</v>
+        <v>-34.622932</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>DEV-M</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>7314</t>
+          <t>7387</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MIRALLA 954</t>
+          <t>PERIBEBUY 6814</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -5008,7 +5008,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>809979735</t>
+          <t>810132728</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -5023,7 +5023,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -5045,10 +5045,10 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.501431</v>
+        <v>-58.521719</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.647791</v>
+        <v>-34.647467</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -5062,7 +5062,7 @@
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>PAV-?</t>
+          <t>PAV-C</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -5074,7 +5074,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>7373</t>
+          <t>7394</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -5084,17 +5084,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>SANTIAGO DEL ESTERO 1253</t>
+          <t>BONIFACIO, JOSE 2409</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>810132493</t>
+          <t>810132768</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -5109,7 +5109,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada volvio a ingresar mail con caso 7597</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -5131,14 +5131,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.384406</v>
+        <v>-58.461482</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.622932</v>
+        <v>-34.632432</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -5148,7 +5148,7 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PCH-F</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -5160,27 +5160,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>7387</t>
+          <t>7570</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>10/6/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>PERIBEBUY 6814</t>
+          <t>VILLEGAS, CONRADO, GRAL. 5402</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>810132728</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -5195,7 +5195,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Colocar R150 o R200</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -5208,7 +5208,7 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -5217,24 +5217,24 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.521719</v>
+        <v>-58.465176</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.647467</v>
+        <v>-34.680979</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>PAV-C</t>
+          <t>PAV-U</t>
         </is>
       </c>
       <c r="R56" t="inlineStr">
@@ -5246,17 +5246,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>7394</t>
+          <t>7595</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>10/13/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>BONIFACIO, JOSE 2409</t>
+          <t>FALCON, RAMON L.,CNEL. 2353</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -5266,7 +5266,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>810132768</t>
+          <t>810333018</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5281,7 +5281,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada volvio a ingresar mail con caso 7597</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -5303,10 +5303,10 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.461482</v>
+        <v>-58.46138</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.632432</v>
+        <v>-34.629774</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>PCH-F</t>
+          <t>PCH-J</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
@@ -5332,27 +5332,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>7595</t>
+          <t>7703</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>10/13/2025</t>
+          <t>10/15/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 2353</t>
+          <t>ROSARIO DE LA FRONTERA 4996</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>810333018</t>
+          <t>810355303</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -5389,24 +5389,24 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.46138</v>
+        <v>-58.514176</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.629774</v>
+        <v>-34.589877</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>PCH-J</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R58" t="inlineStr">
@@ -5418,7 +5418,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>7703</t>
+          <t>7516</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -5428,17 +5428,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>ROSARIO DE LA FRONTERA 4996</t>
+          <t>ALVAREZ, CRISOSTOMO 3000</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>810355303</t>
+          <t>810371027</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -5475,24 +5475,24 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.514176</v>
+        <v>-58.458516</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.589877</v>
+        <v>-34.646422</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>PPT-N</t>
         </is>
       </c>
       <c r="R59" t="inlineStr">
@@ -5504,7 +5504,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>7516</t>
+          <t>7735</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -5514,17 +5514,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>ALVAREZ, CRISOSTOMO 3000</t>
+          <t>GARCIA, MARTIN AV. 772</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>810371027</t>
+          <t>810371042</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -5561,14 +5561,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.458516</v>
+        <v>-58.374086</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.646422</v>
+        <v>-34.633168</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -5578,7 +5578,7 @@
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>PPT-N</t>
+          <t>CON-B</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
@@ -5590,27 +5590,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7735</t>
+          <t>5783</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>10/15/2025</t>
+          <t>10/17/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>GARCIA, MARTIN AV. 772</t>
+          <t>ALCARAZ 5168</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>810371042</t>
+          <t>810378783</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5647,24 +5647,24 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.374086</v>
+        <v>-58.50875</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.633168</v>
+        <v>-34.623434</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>CON-B</t>
+          <t>DEV-H</t>
         </is>
       </c>
       <c r="R61" t="inlineStr">
@@ -5676,27 +5676,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>5783</t>
+          <t>7621</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>10/17/2025</t>
+          <t>10/20/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ALCARAZ 5168</t>
+          <t>Quito 3832</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>810378783</t>
+          <t>810404273</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5733,24 +5733,24 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.50875</v>
+        <v>-58.420412</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.623434</v>
+        <v>-34.616726</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>DEV-H</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R62" t="inlineStr">
@@ -5762,27 +5762,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7621</t>
+          <t>7571</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>10/20/2025</t>
+          <t>10/22/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Quito 3832</t>
+          <t>SAENZ AV. 1204</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>810404273</t>
+          <t>810416653</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5819,14 +5819,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.420412</v>
+        <v>-58.416237</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.616726</v>
+        <v>-34.65477</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5836,7 +5836,7 @@
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
@@ -5848,27 +5848,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7571</t>
+          <t>7556</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>10/22/2025</t>
+          <t>10/21/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>SAENZ AV. 1204</t>
+          <t>SANCHEZ DE LORIA 1923</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>810416653</t>
+          <t>810416656</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5883,7 +5883,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>cambiar</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5905,10 +5905,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.416237</v>
+        <v>-58.411426</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.65477</v>
+        <v>-34.633266</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5922,7 +5922,7 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>PPT-Q</t>
         </is>
       </c>
       <c r="R64" t="inlineStr">
@@ -5934,27 +5934,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7556</t>
+          <t>7579</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>10/21/2025</t>
+          <t>10/22/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1923</t>
+          <t>AGUIRRE 508</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>810416656</t>
+          <t>810421912</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5969,7 +5969,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5987,18 +5987,18 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.411426</v>
+        <v>-58.435731</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.633266</v>
+        <v>-34.597659</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -6008,7 +6008,7 @@
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>PPT-Q</t>
+          <t>VCR-H</t>
         </is>
       </c>
       <c r="R65" t="inlineStr">
@@ -6020,7 +6020,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7579</t>
+          <t>7594</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -6030,17 +6030,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>AGUIRRE 508</t>
+          <t>NEWBERY, JORGE 2696</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>810421912</t>
+          <t>810421921</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6077,10 +6077,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.435731</v>
+        <v>-58.44293</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.597659</v>
+        <v>-34.574483</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -6094,7 +6094,7 @@
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>VCR-H</t>
+          <t>COG-B</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
@@ -6106,27 +6106,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7594</t>
+          <t>7620</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>10/22/2025</t>
+          <t>10/24/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 2696</t>
+          <t>QUITO 3954</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>810421921</t>
+          <t>810447247</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6159,18 +6159,18 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.44293</v>
+        <v>-58.422216</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.574483</v>
+        <v>-34.616828</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -6180,7 +6180,7 @@
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>COG-B</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -6192,27 +6192,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7620</t>
+          <t>5749</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>10/24/2025</t>
+          <t>10/27/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>QUITO 3954</t>
+          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1754</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>810447247</t>
+          <t>01230434</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6222,16 +6222,16 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de nodo propio</t>
         </is>
       </c>
       <c r="I68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
@@ -6240,7 +6240,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
@@ -6249,14 +6249,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.422216</v>
+        <v>-58.4018</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.616828</v>
+        <v>-34.590471</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -6266,7 +6266,7 @@
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>AGU-F</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
@@ -6278,7 +6278,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>5749</t>
+          <t>7631</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -6288,17 +6288,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1754</t>
+          <t>CALVO, CARLOS 3762</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>01230434</t>
+          <t>810451584</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -6308,16 +6308,16 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Traspaso de nodo propio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
@@ -6326,7 +6326,7 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -6335,14 +6335,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.4018</v>
+        <v>-58.418542</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.590471</v>
+        <v>-34.624609</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -6352,7 +6352,7 @@
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>AGU-F</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -6364,7 +6364,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7631</t>
+          <t>7630</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -6374,7 +6374,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 3762</t>
+          <t>INDEPENDENCIA AV. 3690</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -6384,7 +6384,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>810451584</t>
+          <t>810451588</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -6421,10 +6421,10 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.418542</v>
+        <v>-58.417821</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.624609</v>
+        <v>-34.621158</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -6450,7 +6450,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7630</t>
+          <t>7800</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -6460,17 +6460,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>INDEPENDENCIA AV. 3690</t>
+          <t>CONDE 1638</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>810451588</t>
+          <t>810454540</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -6485,7 +6485,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>El poste quedo inclinado</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -6503,28 +6503,28 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.417821</v>
+        <v>-58.461646</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.621158</v>
+        <v>-34.571812</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>ATH-R</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
@@ -6536,7 +6536,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7800</t>
+          <t>7624</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -6546,17 +6546,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>CONDE 1638</t>
+          <t>DIAZ VELEZ AV. 4516</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>810454540</t>
+          <t>810454541</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -6571,7 +6571,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>El poste quedo inclinado</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -6589,28 +6589,28 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.461646</v>
+        <v>-58.430613</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.571812</v>
+        <v>-34.608805</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>ATH-R</t>
+          <t>ALM-J</t>
         </is>
       </c>
       <c r="R72" t="inlineStr">
@@ -6622,7 +6622,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7624</t>
+          <t>7622</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -6632,17 +6632,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>DIAZ VELEZ AV. 4516</t>
+          <t>MIRALLA 950</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>810454541</t>
+          <t>01233440</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -6657,7 +6657,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -6670,7 +6670,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -6679,24 +6679,24 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.430613</v>
+        <v>-58.50161</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.608805</v>
+        <v>-34.647648</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>ALM-J</t>
+          <t>PAV-?</t>
         </is>
       </c>
       <c r="R73" t="inlineStr">
@@ -6708,27 +6708,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7622</t>
+          <t>7643</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>10/27/2025</t>
+          <t>10/28/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>MIRALLA 950</t>
+          <t>ACEVEDO 524</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>01233440</t>
+          <t>810458896</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6756,7 +6756,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -6765,24 +6765,24 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.50161</v>
+        <v>-58.439164</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.647648</v>
+        <v>-34.597069</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>PAV-?</t>
+          <t>VCR-J</t>
         </is>
       </c>
       <c r="R74" t="inlineStr">
@@ -6794,7 +6794,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7643</t>
+          <t>7665</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6804,17 +6804,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>ACEVEDO 524</t>
+          <t>ARAOZ 2313</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>810458896</t>
+          <t>01450977</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6829,7 +6829,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada y cable cortado</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6851,10 +6851,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.439164</v>
+        <v>-58.417634</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.597069</v>
+        <v>-34.587439</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6868,7 +6868,7 @@
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>VCR-J</t>
+          <t>VCR-G</t>
         </is>
       </c>
       <c r="R75" t="inlineStr">
@@ -6880,7 +6880,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7665</t>
+          <t>7683</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6890,17 +6890,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ARAOZ 2313</t>
+          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1684</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>810461115</t>
+          <t>01230516</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6915,7 +6915,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada y cable cortado</t>
+          <t>colocar columna para pedir traspaso de nodo</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6928,7 +6928,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -6937,14 +6937,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.417634</v>
+        <v>-58.402647</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.587439</v>
+        <v>-34.591114</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6954,7 +6954,7 @@
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>VCR-G</t>
+          <t>AGU-F</t>
         </is>
       </c>
       <c r="R76" t="inlineStr">
@@ -6966,27 +6966,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7683</t>
+          <t>7619</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>10/28/2025</t>
+          <t>10/29/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1684</t>
+          <t>QUITO 4180</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>01230516</t>
+          <t>810471618</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -7001,7 +7001,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>colocar columna para pedir traspaso de nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -7014,7 +7014,7 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
@@ -7023,14 +7023,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.402647</v>
+        <v>-58.425596</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.591114</v>
+        <v>-34.617038</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -7040,7 +7040,7 @@
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>AGU-F</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R77" t="inlineStr">
@@ -7052,7 +7052,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7619</t>
+          <t>-658</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -7062,17 +7062,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>QUITO 4180</t>
+          <t>Vera 311</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>810471618</t>
+          <t>01230602</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -7082,12 +7082,12 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspasar Fuente</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -7100,23 +7100,23 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.425596</v>
+        <v>-58.436262</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.617038</v>
+        <v>-34.600478</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -7126,7 +7126,7 @@
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>CLI-O</t>
         </is>
       </c>
       <c r="R78" t="inlineStr">
@@ -7138,27 +7138,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-658</t>
+          <t>7709</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>10/29/2025</t>
+          <t>10/30/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Vera 311</t>
+          <t>SAN BLAS 2891</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>01230602</t>
+          <t>810487021</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -7168,12 +7168,12 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Traspasar Fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -7186,33 +7186,33 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.436262</v>
+        <v>-58.48121</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.600478</v>
+        <v>-34.61126</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>CLI-O</t>
+          <t>NRA-Q</t>
         </is>
       </c>
       <c r="R79" t="inlineStr">
@@ -7224,7 +7224,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7709</t>
+          <t>7719</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -7234,17 +7234,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>SAN BLAS 2891</t>
+          <t>CIUDAD DE LA PAZ 180</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>810487021</t>
+          <t>01229656</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -7259,7 +7259,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para traspaso</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -7272,7 +7272,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
@@ -7281,24 +7281,24 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.48121</v>
+        <v>-58.440031</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.61126</v>
+        <v>-34.575409</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>NRA-Q</t>
+          <t>COG-B</t>
         </is>
       </c>
       <c r="R80" t="inlineStr">
@@ -7310,7 +7310,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7719</t>
+          <t>7732</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -7320,17 +7320,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 180</t>
+          <t>LINIERS VIRREY 1142</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>01229656</t>
+          <t>810487035</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -7345,7 +7345,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspaso</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
@@ -7367,14 +7367,14 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.440031</v>
+        <v>-58.413563</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.575409</v>
+        <v>-34.624645</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -7384,7 +7384,7 @@
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>COG-B</t>
+          <t>CEN-P</t>
         </is>
       </c>
       <c r="R81" t="inlineStr">
@@ -7396,27 +7396,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7732</t>
+          <t>7744</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>10/30/2025</t>
+          <t>10/31/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>LINIERS VIRREY 1142</t>
+          <t>NECOCHEA 369</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>810487035</t>
+          <t>01233359</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -7431,7 +7431,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R200 para rtaspaso de nodo</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -7444,7 +7444,7 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
@@ -7453,14 +7453,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.413563</v>
+        <v>-58.364132</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.624645</v>
+        <v>-34.628423</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -7470,7 +7470,7 @@
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>CEN-P</t>
+          <t>CON-F</t>
         </is>
       </c>
       <c r="R82" t="inlineStr">
@@ -7482,27 +7482,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7744</t>
+          <t>7780</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>10/31/2025</t>
+          <t>11/4/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>NECOCHEA 369</t>
+          <t>INDEPENDENCIA AV. 1654</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>01233359</t>
+          <t>810573618</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -7517,7 +7517,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Colocar R200 para rtaspaso de nodo</t>
+          <t>Columna picada e inclinada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -7530,7 +7530,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -7539,10 +7539,10 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.364132</v>
+        <v>-58.389676</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.628423</v>
+        <v>-34.618127</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -7556,7 +7556,7 @@
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>CON-F</t>
+          <t>CEN-?</t>
         </is>
       </c>
       <c r="R83" t="inlineStr">
@@ -7568,27 +7568,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7780</t>
+          <t>7810</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>11/4/2025</t>
+          <t>11/10/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>INDEPENDENCIA AV. 1654</t>
+          <t>GUTENBERG 3212</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>810573618</t>
+          <t>810651343</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -7603,7 +7603,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Columna picada e inclinada</t>
+          <t>Cambiar columna y ver que el vano quede separado del balcon esta inclinada hacia la casa</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -7625,36 +7625,36 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.389676</v>
+        <v>-58.501325</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.618127</v>
+        <v>-34.594325</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>CEN-?</t>
+          <t>PUE-Q</t>
         </is>
       </c>
       <c r="R84" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2PUE</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7810</t>
+          <t>-670</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -7664,17 +7664,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>GUTENBERG 3212</t>
+          <t>Timoteo Gordillo 1666</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>810651343</t>
+          <t>810651269</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -7689,7 +7689,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Cambiar columna y ver que el vano quede separado del balcon esta inclinada hacia la casa</t>
+          <t>Cambiar columna de lugar la actual es un poste ex Cablevision correrla ya que el vecino reclama obstruccion de la cochera</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -7711,14 +7711,14 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.501325</v>
+        <v>-58.510994</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.594325</v>
+        <v>-34.655027</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -7728,39 +7728,39 @@
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>PUE-Q</t>
+          <t>PAV-J</t>
         </is>
       </c>
       <c r="R85" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2PUE</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>-670</t>
+          <t>7604</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>11/10/2025</t>
+          <t>11/11/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Timoteo Gordillo 1666</t>
+          <t>SAN JUAN AV. 3741</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>810651269</t>
+          <t>810712796</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -7775,7 +7775,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Cambiar columna de lugar la actual es un poste ex Cablevision correrla ya que el vecino reclama obstruccion de la cochera</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -7797,24 +7797,24 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.510994</v>
+        <v>-58.418108</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.655027</v>
+        <v>-34.62564</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P86" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>PAV-J</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R86" t="inlineStr">
@@ -7826,7 +7826,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>7604</t>
+          <t>7764</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -7836,17 +7836,17 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>SAN JUAN AV. 3741</t>
+          <t>2 DE ABRIL DE 1982 6510</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>810712796</t>
+          <t>01411184</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -7861,7 +7861,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmontar poste en desuso</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -7869,7 +7869,7 @@
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -7879,14 +7879,14 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.418108</v>
+        <v>-58.490261</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.62564</v>
+        <v>-34.677337</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -7900,7 +7900,7 @@
       </c>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>PAV-M</t>
         </is>
       </c>
       <c r="R87" t="inlineStr">
@@ -7912,7 +7912,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>7764</t>
+          <t>6415</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -7922,17 +7922,17 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6510</t>
+          <t>CAMPICHUELO 215</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810712875</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7947,7 +7947,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Desmontar poste en desuso</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7955,7 +7955,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -7965,18 +7965,18 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.490261</v>
+        <v>-58.433771</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.677337</v>
+        <v>-34.614668</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
@@ -7986,7 +7986,7 @@
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>PAV-M</t>
+          <t>ALM-J</t>
         </is>
       </c>
       <c r="R88" t="inlineStr">
@@ -7998,7 +7998,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>6415</t>
+          <t>7746</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -8008,7 +8008,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>CAMPICHUELO 215</t>
+          <t>CAMPICHUELO 229</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -8018,7 +8018,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>810712875</t>
+          <t>810712887</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -8033,7 +8033,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -8055,10 +8055,10 @@
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.433771</v>
+        <v>-58.433855</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.614668</v>
+        <v>-34.614487</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
@@ -8084,27 +8084,27 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>7746</t>
+          <t>7842</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>11/11/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>CAMPICHUELO 229</t>
+          <t>FERRARI 410</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>810712887</t>
+          <t>810713039</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -8119,7 +8119,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -8141,113 +8141,27 @@
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.433855</v>
+        <v>-58.441198</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.614487</v>
+        <v>-34.605341</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q90" t="inlineStr">
         <is>
-          <t>ALM-J</t>
+          <t>ALM-O</t>
         </is>
       </c>
       <c r="R90" t="inlineStr">
-        <is>
-          <t>Fuera de Poligono OVL</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>7842</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>11/12/2025</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>FERRARI 410</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>810713039</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I91" t="n">
-        <v>1</v>
-      </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M91" t="n">
-        <v>-58.441198</v>
-      </c>
-      <c r="N91" t="n">
-        <v>-34.605341</v>
-      </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P91" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-      <c r="Q91" t="inlineStr">
-        <is>
-          <t>ALM-O</t>
-        </is>
-      </c>
-      <c r="R91" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-20 09:28:22)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R86"/>
+  <dimension ref="A1:R87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,7 +548,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810804380</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -634,7 +634,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810804375</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2764,27 +2764,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>7571</t>
+          <t>7755</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>10/22/2025</t>
+          <t>10/24/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>SAENZ AV. 1204</t>
+          <t>Munich 1715</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>810416653</t>
+          <t>810447258</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2821,24 +2821,24 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.416237</v>
+        <v>-58.453119</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.65477</v>
+        <v>-34.55489</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>BLO-C</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2850,7 +2850,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>7579</t>
+          <t>7571</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2860,17 +2860,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>AGUIRRE 508</t>
+          <t>SAENZ AV. 1204</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>810421912</t>
+          <t>810416653</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2903,18 +2903,18 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.435731</v>
+        <v>-58.416237</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.597659</v>
+        <v>-34.65477</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2924,7 +2924,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>VCR-H</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
@@ -2936,27 +2936,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>7556</t>
+          <t>7579</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>10/21/2025</t>
+          <t>10/22/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1923</t>
+          <t>AGUIRRE 508</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>810416656</t>
+          <t>810421912</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2971,7 +2971,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2989,18 +2989,18 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.411426</v>
+        <v>-58.435731</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.633266</v>
+        <v>-34.597659</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -3010,7 +3010,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>PPT-Q</t>
+          <t>VCR-H</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
@@ -3022,17 +3022,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>7621</t>
+          <t>7556</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>10/20/2025</t>
+          <t>10/21/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Quito 3832</t>
+          <t>SANCHEZ DE LORIA 1923</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -3042,7 +3042,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>810404273</t>
+          <t>810416656</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>cambiar</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -3079,14 +3079,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.420412</v>
+        <v>-58.411426</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.616726</v>
+        <v>-34.633266</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -3096,7 +3096,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>PPT-Q</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3108,27 +3108,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5783</t>
+          <t>7621</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>10/17/2025</t>
+          <t>10/20/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ALCARAZ 5168</t>
+          <t>Quito 3832</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>810378783</t>
+          <t>810404273</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3165,24 +3165,24 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.50875</v>
+        <v>-58.420412</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.623434</v>
+        <v>-34.616726</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>DEV-H</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3194,27 +3194,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>7516</t>
+          <t>5783</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>10/15/2025</t>
+          <t>10/17/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ALVAREZ, CRISOSTOMO 3000</t>
+          <t>ALCARAZ 5168</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>810371027</t>
+          <t>810378783</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3251,24 +3251,24 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.458516</v>
+        <v>-58.50875</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.646422</v>
+        <v>-34.623434</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>PPT-N</t>
+          <t>DEV-H</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -3280,7 +3280,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>7735</t>
+          <t>7516</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3290,17 +3290,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>GARCIA, MARTIN AV. 772</t>
+          <t>ALVAREZ, CRISOSTOMO 3000</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>810371042</t>
+          <t>810371027</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -3337,14 +3337,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.374086</v>
+        <v>-58.458516</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.633168</v>
+        <v>-34.646422</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -3354,7 +3354,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>CON-B</t>
+          <t>PPT-N</t>
         </is>
       </c>
       <c r="R34" t="inlineStr">
@@ -3366,27 +3366,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>7595</t>
+          <t>7735</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>10/13/2025</t>
+          <t>10/15/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 2353</t>
+          <t>GARCIA, MARTIN AV. 772</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>810333018</t>
+          <t>810371042</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3423,14 +3423,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.46138</v>
+        <v>-58.374086</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.629774</v>
+        <v>-34.633168</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3440,7 +3440,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>PCH-J</t>
+          <t>CON-B</t>
         </is>
       </c>
       <c r="R35" t="inlineStr">
@@ -3452,27 +3452,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>7570</t>
+          <t>7595</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>10/6/2025</t>
+          <t>10/13/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>VILLEGAS, CONRADO, GRAL. 5402</t>
+          <t>FALCON, RAMON L.,CNEL. 2353</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810333018</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3482,12 +3482,12 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Colocar R150 o R200</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3500,7 +3500,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3509,10 +3509,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.465176</v>
+        <v>-58.46138</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.680979</v>
+        <v>-34.629774</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>PAV-U</t>
+          <t>PCH-J</t>
         </is>
       </c>
       <c r="R36" t="inlineStr">
@@ -3538,27 +3538,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>7373</t>
+          <t>7570</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>10/6/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>SANTIAGO DEL ESTERO 1253</t>
+          <t>VILLEGAS, CONRADO, GRAL. 5402</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>810132493</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3568,12 +3568,12 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R150 o R200</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3586,7 +3586,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3595,14 +3595,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.384406</v>
+        <v>-58.465176</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.622932</v>
+        <v>-34.680979</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3612,7 +3612,7 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PAV-U</t>
         </is>
       </c>
       <c r="R37" t="inlineStr">
@@ -3624,7 +3624,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>7387</t>
+          <t>7373</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3634,17 +3634,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>PERIBEBUY 6814</t>
+          <t>SANTIAGO DEL ESTERO 1253</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>810132728</t>
+          <t>810132493</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3659,7 +3659,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3681,24 +3681,24 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.521719</v>
+        <v>-58.384406</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.647467</v>
+        <v>-34.622932</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>PAV-C</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
@@ -3710,7 +3710,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>7394</t>
+          <t>7387</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3720,17 +3720,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>BONIFACIO, JOSE 2409</t>
+          <t>PERIBEBUY 6814</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>810132768</t>
+          <t>810132728</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3745,7 +3745,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada volvio a ingresar mail con caso 7597</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3767,24 +3767,24 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.461482</v>
+        <v>-58.521719</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.632432</v>
+        <v>-34.647467</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>PCH-F</t>
+          <t>PAV-C</t>
         </is>
       </c>
       <c r="R39" t="inlineStr">
@@ -3796,27 +3796,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>7308</t>
+          <t>7394</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>MANZANARES 4186</t>
+          <t>BONIFACIO, JOSE 2409</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>809979726</t>
+          <t>810132768</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3831,7 +3831,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada volvio a ingresar mail con caso 7597</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3853,24 +3853,24 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.485454</v>
+        <v>-58.461482</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.555745</v>
+        <v>-34.632432</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>PCH-F</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -3882,7 +3882,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>7308</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3892,17 +3892,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>BACACAY AV. 5805</t>
+          <t>MANZANARES 4186</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>809979728</t>
+          <t>809979726</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3917,7 +3917,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Cambiar y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3935,18 +3935,18 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.509324</v>
+        <v>-58.485454</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.635335</v>
+        <v>-34.555745</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3956,19 +3956,19 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>DEV-M</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>7314</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3978,17 +3978,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>MIRALLA 954</t>
+          <t>BACACAY AV. 5805</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>809979735</t>
+          <t>809979728</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4003,7 +4003,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar y reparar rienda</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -4021,14 +4021,14 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.501431</v>
+        <v>-58.509324</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.647791</v>
+        <v>-34.635335</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -4042,39 +4042,39 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>PAV-?</t>
+          <t>DEV-M</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>7314</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>9/23/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 911</t>
+          <t>MIRALLA 954</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>ICD30958043</t>
+          <t>809979735</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron un nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -4102,7 +4102,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -4111,14 +4111,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.447743</v>
+        <v>-58.501431</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.570457</v>
+        <v>-34.647791</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -4128,7 +4128,7 @@
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>PAV-?</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -4140,27 +4140,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/23/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Av Amancio Alcorta 3570</t>
+          <t>CIUDAD DE LA PAZ 911</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>809800213</t>
+          <t>ICD30958043</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4175,7 +4175,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Desmonte de columna ya traspasaron un nodo</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -4183,38 +4183,38 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.409278</v>
+        <v>-58.447743</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.653566</v>
+        <v>-34.570457</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -4226,7 +4226,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6182</t>
+          <t>6475</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -4236,7 +4236,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Los Patos 2702</t>
+          <t>Av Amancio Alcorta 3570</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -4246,7 +4246,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>809818308</t>
+          <t>809800213</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -4269,7 +4269,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -4279,14 +4279,14 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.399262</v>
+        <v>-58.409278</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.639685</v>
+        <v>-34.653566</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -4300,7 +4300,7 @@
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -4312,27 +4312,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>7240</t>
+          <t>6182</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>9/16/2025</t>
+          <t>9/17/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+          <t>Los Patos 2702</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>809784524</t>
+          <t>809818308</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4347,7 +4347,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -4365,28 +4365,28 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.481316</v>
+        <v>-58.399262</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.556157</v>
+        <v>-34.639685</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
@@ -4398,27 +4398,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>7240</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809784524</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -4433,7 +4433,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -4451,18 +4451,18 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.516218</v>
+        <v>-58.481316</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.589343</v>
+        <v>-34.556157</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -4472,7 +4472,7 @@
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
@@ -4484,27 +4484,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>7260</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Vidal 1861</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>809642175</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4519,7 +4519,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4537,18 +4537,18 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.458298</v>
+        <v>-58.516218</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.566511</v>
+        <v>-34.589343</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4558,7 +4558,7 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>COG-F</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
@@ -4570,27 +4570,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5999</t>
+          <t>7260</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 228</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808918687</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4600,16 +4600,16 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Se deriva directamente a traspaso de fuente ya que hay una columna existente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -4618,7 +4618,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4627,24 +4627,24 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.425858</v>
+        <v>-58.458298</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.61629</v>
+        <v>-34.566511</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>ALM-D</t>
+          <t>COG-F</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -4656,27 +4656,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6579</t>
+          <t>5999</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>8/7/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
+          <t>MARMOL, JOSE 228</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808749184</t>
+          <t>808918687</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4686,51 +4686,51 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Poste inclinado ingreso tambien como 7201</t>
+          <t>Se deriva directamente a traspaso de fuente ya que hay una columna existente</t>
         </is>
       </c>
       <c r="I50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.461024</v>
+        <v>-58.425858</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.539409</v>
+        <v>-34.61629</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>BLO-F</t>
+          <t>ALM-D</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
@@ -4742,27 +4742,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6567</t>
+          <t>6579</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/7/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SAN ANTONIO 1221</t>
+          <t>RIVADAVIA MARTIN, COMODORO 1350</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808733914</t>
+          <t>808749184</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4777,7 +4777,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Poste inclinado ingreso tambien como 7201</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4795,28 +4795,28 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.375684</v>
+        <v>-58.461024</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.656092</v>
+        <v>-34.539409</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>CON-I</t>
+          <t>BLO-F</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
@@ -4828,27 +4828,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6556</t>
+          <t>6567</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2 DE ABRIL DE 1982 6982</t>
+          <t>SAN ANTONIO 1221</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>ICD30334420</t>
+          <t>808733914</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4863,7 +4863,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4871,7 +4871,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4881,18 +4881,18 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.494864</v>
+        <v>-58.375684</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.678826</v>
+        <v>-34.656092</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4902,7 +4902,7 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>PAV-M</t>
+          <t>CON-I</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -4914,27 +4914,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6284</t>
+          <t>6556</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6/30/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>CHILE 2561</t>
+          <t>2 DE ABRIL DE 1982 6982</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807851584</t>
+          <t>ICD30334420</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4944,37 +4944,41 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Traspasar a columna o cortar redes en punta y desmontar poste</t>
+        </is>
+      </c>
       <c r="I53" t="n">
         <v>1</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.401827</v>
+        <v>-58.494864</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.617667</v>
+        <v>-34.678826</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4984,7 +4988,7 @@
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>CEN-M</t>
+          <t>PAV-M</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
@@ -4996,17 +5000,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>6284</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/30/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>CHILE 2561</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -5016,7 +5020,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>810533286</t>
+          <t>807851584</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -5026,14 +5030,10 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Desmontar PRFV 400</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr"/>
       <c r="I54" t="n">
         <v>1</v>
       </c>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -5053,10 +5053,10 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.401624</v>
+        <v>-58.401827</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.612001</v>
+        <v>-34.617667</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -5070,7 +5070,7 @@
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>CEN-G</t>
+          <t>CEN-M</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -5082,27 +5082,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6004</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>MAZA 181</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807215439</t>
+          <t>810533286</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -5112,12 +5112,12 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmontar PRFV 400</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -5130,7 +5130,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -5139,10 +5139,10 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.416477</v>
+        <v>-58.401624</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.61303</v>
+        <v>-34.612001</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -5156,7 +5156,7 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>CLI-I</t>
+          <t>CEN-G</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -5168,7 +5168,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6010</t>
+          <t>6004</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -5178,7 +5178,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ESTADO DE PALESTINA 771</t>
+          <t>MAZA 181</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -5188,7 +5188,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807215458</t>
+          <t>807215439</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -5198,12 +5198,12 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada y mal ubicada ver con Pedro</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -5216,7 +5216,7 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -5225,10 +5225,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.425478</v>
+        <v>-58.416477</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.601865</v>
+        <v>-34.61303</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -5242,7 +5242,7 @@
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>CLI-N</t>
+          <t>CLI-I</t>
         </is>
       </c>
       <c r="R56" t="inlineStr">
@@ -5254,27 +5254,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>3715</t>
+          <t>6010</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>EL SERENO 358</t>
+          <t>ESTADO DE PALESTINA 771</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807168098</t>
+          <t>807215458</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5289,7 +5289,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Poste inclinado</t>
+          <t>Picada y mal ubicada ver con Pedro</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -5297,7 +5297,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -5307,60 +5307,60 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.487371</v>
+        <v>-58.425478</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.640099</v>
+        <v>-34.601865</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>PCH-S</t>
+          <t>CLI-N</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2PCH</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5948</t>
+          <t>3715</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/2/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MURGUIONDO 3990</t>
+          <t>EL SERENO 358</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807129347</t>
+          <t>807168098</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -5375,7 +5375,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>COLUMNA INCLINADA</t>
+          <t>Poste inclinado</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -5383,7 +5383,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -5393,50 +5393,50 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.477944</v>
+        <v>-58.487371</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.675149</v>
+        <v>-34.640099</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>PAV-V</t>
+          <t>PCH-S</t>
         </is>
       </c>
       <c r="R58" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2PCH</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>5948</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/2/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
+          <t>MURGUIONDO 3990</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -5446,7 +5446,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807044186</t>
+          <t>807129347</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>COLUMNA INCLINADA</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -5479,14 +5479,14 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.467789</v>
+        <v>-58.477944</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.68463</v>
+        <v>-34.675149</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -5500,7 +5500,7 @@
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>PAV-U</t>
+          <t>PAV-V</t>
         </is>
       </c>
       <c r="R59" t="inlineStr">
@@ -5512,27 +5512,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>5935</t>
+          <t>5944</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>5/27/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 3305</t>
+          <t>GARCIA, PEDRO A.,CNEL. 5887</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807044131</t>
+          <t>807044186</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -5547,7 +5547,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -5555,7 +5555,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -5565,28 +5565,28 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.483927</v>
+        <v>-58.467789</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.570689</v>
+        <v>-34.68463</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>PUE-E</t>
+          <t>PAV-U</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
@@ -5598,27 +5598,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>5839</t>
+          <t>5935</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/27/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>AYACUCHO 267</t>
+          <t>ALVAREZ THOMAS AV. 3305</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>806926385</t>
+          <t>807044131</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5641,38 +5641,38 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.395063</v>
+        <v>-58.483927</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.606257</v>
+        <v>-34.570689</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>CLI-B</t>
+          <t>PUE-E</t>
         </is>
       </c>
       <c r="R61" t="inlineStr">
@@ -5684,27 +5684,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6180</t>
+          <t>5839</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>5/4/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>AZARA 15</t>
+          <t>AYACUCHO 267</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>805655333</t>
+          <t>806926385</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5719,7 +5719,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada entro tambien como reclamo 7611</t>
+          <t>Colocar columna y dar aviso para traspaso de nodo teco</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5732,7 +5732,7 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
@@ -5741,14 +5741,14 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.372751</v>
+        <v>-58.395063</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.631917</v>
+        <v>-34.606257</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5758,7 +5758,7 @@
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>CON-B</t>
+          <t>CLI-B</t>
         </is>
       </c>
       <c r="R62" t="inlineStr">
@@ -5770,17 +5770,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>5651</t>
+          <t>6180</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>5/4/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MONTES DE OCA, MANUEL AV. 511</t>
+          <t>AZARA 15</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5790,7 +5790,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>804876051</t>
+          <t>805655333</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5805,7 +5805,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Pegar los ductos al prfv</t>
+          <t>Picada entro tambien como reclamo 7611</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5827,10 +5827,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.375515</v>
+        <v>-58.372751</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.634393</v>
+        <v>-34.631917</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5856,27 +5856,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>5573</t>
+          <t>5651</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>4/14/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>LASTRA AV. 4379</t>
+          <t>MONTES DE OCA, MANUEL AV. 511</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>804663677</t>
+          <t>804876051</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5891,7 +5891,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Pegar los ductos al prfv</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5899,7 +5899,7 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -5913,56 +5913,56 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.525125</v>
+        <v>-58.375515</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.604668</v>
+        <v>-34.634393</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>DEV-F</t>
+          <t>CON-B</t>
         </is>
       </c>
       <c r="R64" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6009</t>
+          <t>5573</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>4/8/2025</t>
+          <t>4/14/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SARMIENTO 4290</t>
+          <t>LASTRA AV. 4379</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>804569065</t>
+          <t>804663677</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5977,7 +5977,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Columna corroída en su base entro tambien como caso 7049</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5985,7 +5985,7 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -5999,56 +5999,56 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.425764</v>
+        <v>-58.525125</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.604359</v>
+        <v>-34.604668</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>ALM-L</t>
+          <t>DEV-F</t>
         </is>
       </c>
       <c r="R65" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1DEV</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2114</t>
+          <t>6009</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/8/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>THAMES 649</t>
+          <t>SARMIENTO 4290</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>804309655</t>
+          <t>804569065</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6058,12 +6058,12 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+          <t>Columna corroída en su base entro tambien como caso 7049</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -6076,7 +6076,7 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L66" t="inlineStr">
@@ -6085,14 +6085,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.441405</v>
+        <v>-58.425764</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.594348</v>
+        <v>-34.604359</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -6102,7 +6102,7 @@
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>VCR-H</t>
+          <t>ALM-L</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
@@ -6114,7 +6114,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>4179</t>
+          <t>2114</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -6124,17 +6124,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>ZELARRAYAN 6147</t>
+          <t>THAMES 649</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>804309801</t>
+          <t>804309655</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6147,7 +6147,11 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H67" t="inlineStr"/>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>QAP traspaso fuente propia para posterior pasar a TLC</t>
+        </is>
+      </c>
       <c r="I67" t="n">
         <v>1</v>
       </c>
@@ -6167,14 +6171,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.483821</v>
+        <v>-58.441405</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.677698</v>
+        <v>-34.594348</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -6184,7 +6188,7 @@
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>PAV-Q</t>
+          <t>VCR-H</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -6196,27 +6200,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7633</t>
+          <t>4179</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>3/18/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>TREINTA Y TRES ORIENTALES 965</t>
+          <t>ZELARRAYAN 6147</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>804161231</t>
+          <t>804309801</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6226,14 +6230,10 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr"/>
       <c r="I68" t="n">
         <v>1</v>
       </c>
@@ -6244,7 +6244,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
@@ -6253,10 +6253,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.423042</v>
+        <v>-58.483821</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.625868</v>
+        <v>-34.677698</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -6270,7 +6270,7 @@
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>PAV-Q</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
@@ -6282,27 +6282,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>4974</t>
+          <t>7633</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2/17/2025</t>
+          <t>3/18/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SAN PEDRITO AV. 96</t>
+          <t>TREINTA Y TRES ORIENTALES 965</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>803607768</t>
+          <t>804161231</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -6317,7 +6317,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -6325,7 +6325,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -6335,14 +6335,14 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.468938</v>
+        <v>-58.423042</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.632015</v>
+        <v>-34.625868</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -6356,7 +6356,7 @@
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>PCH-H</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -6368,27 +6368,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>4938</t>
+          <t>4974</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2/14/2025</t>
+          <t>2/17/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>CHACO 195</t>
+          <t>SAN PEDRITO AV. 96</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>803607699</t>
+          <t>803607768</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -6403,7 +6403,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Desmontar columna personal propio traspaso nodo</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -6411,24 +6411,24 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.431522</v>
+        <v>-58.468938</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.617523</v>
+        <v>-34.632015</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -6442,7 +6442,7 @@
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>ALM-F</t>
+          <t>PCH-H</t>
         </is>
       </c>
       <c r="R70" t="inlineStr">
@@ -6454,17 +6454,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>4696</t>
+          <t>4938</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2/10/2025</t>
+          <t>2/14/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>YERBAL 489</t>
+          <t>CHACO 195</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -6474,7 +6474,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>803607520</t>
+          <t>803607699</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -6489,7 +6489,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron nodo</t>
+          <t>Desmontar columna personal propio traspaso nodo</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -6511,10 +6511,10 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.438053</v>
+        <v>-58.431522</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.617481</v>
+        <v>-34.617523</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -6528,7 +6528,7 @@
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>ALM-G</t>
+          <t>ALM-F</t>
         </is>
       </c>
       <c r="R71" t="inlineStr">
@@ -6540,27 +6540,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>4791</t>
+          <t>4696</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>2/10/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>RONDEAU 2775</t>
+          <t>YERBAL 489</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>802988219</t>
+          <t>803607520</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -6575,7 +6575,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Relevar</t>
+          <t>Desmonte de columna ya traspasaron nodo</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -6597,14 +6597,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.402062</v>
+        <v>-58.438053</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.635143</v>
+        <v>-34.617481</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -6614,7 +6614,7 @@
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>ALM-G</t>
         </is>
       </c>
       <c r="R72" t="inlineStr">
@@ -6626,17 +6626,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>5750</t>
+          <t>4791</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>1/24/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>BRASIL 2561</t>
+          <t>RONDEAU 2775</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -6646,7 +6646,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>802871857</t>
+          <t>802988219</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -6661,7 +6661,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Colocar columna R400 - Fuente Teco</t>
+          <t>Relevar</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -6674,7 +6674,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -6683,10 +6683,10 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.400156</v>
+        <v>-58.402062</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.631369</v>
+        <v>-34.635143</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -6700,39 +6700,39 @@
       </c>
       <c r="Q73" t="inlineStr">
         <is>
-          <t>PPT-F</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R73" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.1PPT</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>5750</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>1/22/2025</t>
+          <t>1/24/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>CUENCA 3345</t>
+          <t>BRASIL 2561</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>802843289</t>
+          <t>802871857</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6742,12 +6742,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna R400 - Fuente Teco</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6760,7 +6760,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -6769,56 +6769,56 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.496935</v>
+        <v>-58.400156</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.599084</v>
+        <v>-34.631369</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q74" t="inlineStr">
         <is>
-          <t>PUE-B</t>
+          <t>PPT-F</t>
         </is>
       </c>
       <c r="R74" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.1PPT</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>4622</t>
+          <t>4680</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>1/14/2025</t>
+          <t>1/22/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Campana	534</t>
+          <t>CUENCA 3345</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>802657454</t>
+          <t>802843289</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6828,7 +6828,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -6846,7 +6846,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -6855,14 +6855,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.477376</v>
+        <v>-58.496935</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.626126</v>
+        <v>-34.599084</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6872,29 +6872,29 @@
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>NRA-R</t>
+          <t>PUE-B</t>
         </is>
       </c>
       <c r="R75" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2NRA</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>4082</t>
+          <t>4622</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>12/21/2024</t>
+          <t>1/14/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>MERCEDES 254</t>
+          <t>Campana	534</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -6904,7 +6904,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>801901755</t>
+          <t>802657454</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6914,12 +6914,12 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Colocar R200 para pedir traspaso de equipo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6932,7 +6932,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -6941,10 +6941,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.484232</v>
+        <v>-58.477376</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.631431</v>
+        <v>-34.626126</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6958,39 +6958,39 @@
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>DEV-L</t>
+          <t>NRA-R</t>
         </is>
       </c>
       <c r="R76" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2DEV</t>
+          <t>ARATO-25058.PO.2NRA</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>4426</t>
+          <t>4082</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>12/19/2024</t>
+          <t>12/21/2024</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>LORA, FELIX 27</t>
+          <t>MERCEDES 254</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>801768138</t>
+          <t>801901755</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -7000,12 +7000,12 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
+          <t>Colocar R200 para pedir traspaso de equipo</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -7018,7 +7018,7 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
@@ -7027,56 +7027,56 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.443626</v>
+        <v>-58.484232</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.621032</v>
+        <v>-34.631431</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>PCH-G</t>
+          <t>DEV-L</t>
         </is>
       </c>
       <c r="R77" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>4025</t>
+          <t>4426</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>12/19/2024</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>MEXICO 4249</t>
+          <t>LORA, FELIX 27</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>799981143</t>
+          <t>801768138</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -7091,7 +7091,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Ver foto, colocar columna para traspasar</t>
+          <t>Traspaso de redes y retiro de columna TLC ya traspaso el nodo</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -7104,7 +7104,7 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
@@ -7113,14 +7113,14 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.425997</v>
+        <v>-58.443626</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.620454</v>
+        <v>-34.621032</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -7130,7 +7130,7 @@
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>ALM-B</t>
+          <t>PCH-G</t>
         </is>
       </c>
       <c r="R78" t="inlineStr">
@@ -7142,27 +7142,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>5884</t>
+          <t>4025</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>11/12/2024</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>OLLEROS 2952</t>
+          <t>MEXICO 4249</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>799450967</t>
+          <t>799981143</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -7177,11 +7177,11 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Solo retirar columna ya se realizo traspaso</t>
+          <t>Ver foto, colocar columna para traspasar</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -7199,14 +7199,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.447022</v>
+        <v>-58.425997</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.575873</v>
+        <v>-34.620454</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -7216,7 +7216,7 @@
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>ATH-P</t>
+          <t>ALM-B</t>
         </is>
       </c>
       <c r="R79" t="inlineStr">
@@ -7228,27 +7228,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>3938</t>
+          <t>5884</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>11/5/2024</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>GODOY CRUZ 2604</t>
+          <t>OLLEROS 2952</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>799246642</t>
+          <t>799450967</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -7263,32 +7263,32 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Realizar traspasos y retiro de columna vieja</t>
+          <t>Solo retirar columna ya se realizo traspaso</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.426169</v>
+        <v>-58.447022</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.579697</v>
+        <v>-34.575873</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -7302,7 +7302,7 @@
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>VCR-N</t>
+          <t>ATH-P</t>
         </is>
       </c>
       <c r="R80" t="inlineStr">
@@ -7314,27 +7314,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>3887</t>
+          <t>3938</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>10/29/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>ESTADO DE ISRAEL AV. 4819</t>
+          <t>GODOY CRUZ 2604</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>798894281</t>
+          <t>799246642</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -7349,7 +7349,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Realizar traspasos y retiro de columna vieja</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -7371,10 +7371,10 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.432085</v>
+        <v>-58.426169</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.60178</v>
+        <v>-34.579697</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -7388,7 +7388,7 @@
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>CLI-N</t>
+          <t>VCR-N</t>
         </is>
       </c>
       <c r="R81" t="inlineStr">
@@ -7400,7 +7400,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>3893</t>
+          <t>3887</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -7410,17 +7410,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>HERRERA 402</t>
+          <t>ESTADO DE ISRAEL AV. 4819</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>798894295</t>
+          <t>798894281</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -7435,7 +7435,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Inclinado En el form cargaron foto de otro caso</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -7457,14 +7457,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.378613</v>
+        <v>-58.432085</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.6349</v>
+        <v>-34.60178</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -7474,7 +7474,7 @@
       </c>
       <c r="Q82" t="inlineStr">
         <is>
-          <t>CON-H</t>
+          <t>CLI-N</t>
         </is>
       </c>
       <c r="R82" t="inlineStr">
@@ -7486,27 +7486,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>3765</t>
+          <t>3893</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>10/29/2024</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>NAZCA AV. 1675</t>
+          <t>HERRERA 402</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>01082878</t>
+          <t>798894295</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -7521,7 +7521,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>ya se traspaso nodo retirar columna</t>
+          <t>Inclinado En el form cargaron foto de otro caso</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -7529,38 +7529,38 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.47874</v>
+        <v>-58.378613</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.61462</v>
+        <v>-34.6349</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>NRA-M</t>
+          <t>CON-H</t>
         </is>
       </c>
       <c r="R83" t="inlineStr">
@@ -7572,7 +7572,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>3765</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -7582,17 +7582,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>José Andrés Pacheco de Melo 2084</t>
+          <t>NAZCA AV. 1675</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>798897149</t>
+          <t>01082878</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -7602,12 +7602,12 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
+          <t>ya se traspaso nodo retirar columna</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -7623,26 +7623,30 @@
           <t>Fuente Teco</t>
         </is>
       </c>
-      <c r="L84" t="inlineStr"/>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M84" t="n">
-        <v>-58.395656</v>
+        <v>-58.47874</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.590364</v>
+        <v>-34.61462</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>RET-C</t>
+          <t>NRA-M</t>
         </is>
       </c>
       <c r="R84" t="inlineStr">
@@ -7654,27 +7658,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>-111</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>7/12/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>CATAMARCA /ALT/ 1127</t>
+          <t>José Andrés Pacheco de Melo 2084</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>790298182</t>
+          <t>798897149</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -7684,16 +7688,16 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Cambio de columna.-</t>
+          <t>Pendiente de traspaso Fuente TECO y retiro de columna</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
@@ -7702,23 +7706,19 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr"/>
       <c r="M85" t="n">
-        <v>-58.404265</v>
+        <v>-58.395656</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.623154</v>
+        <v>-34.590364</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -7728,7 +7728,7 @@
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>CEN-K</t>
+          <t>RET-C</t>
         </is>
       </c>
       <c r="R85" t="inlineStr">
@@ -7740,84 +7740,170 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
+          <t>-111</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>7/12/2024</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>CATAMARCA /ALT/ 1127</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>790298182</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Cambio de columna.-</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M86" t="n">
+        <v>-58.404265</v>
+      </c>
+      <c r="N86" t="n">
+        <v>-34.623154</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>CEN-K</t>
+        </is>
+      </c>
+      <c r="R86" t="inlineStr">
+        <is>
+          <t>Fuera de Poligono OVL</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
           <t>7758</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
+      <c r="B87" t="inlineStr">
         <is>
           <t>2/20/2024</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="C87" t="inlineStr">
         <is>
           <t>ZABALA 2844</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
+      <c r="D87" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr">
+      <c r="E87" t="inlineStr">
         <is>
           <t>780340125</t>
         </is>
       </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>Optical Power</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Optical Power</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H86" t="inlineStr">
+      <c r="H87" t="inlineStr">
         <is>
           <t>cambiar columna y emprolijar cables y cajas de empalme que se ven en las fotos</t>
         </is>
       </c>
-      <c r="I86" t="n">
-        <v>1</v>
-      </c>
-      <c r="J86" t="inlineStr">
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="inlineStr">
         <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K86" t="inlineStr">
+      <c r="K87" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L86" t="inlineStr">
+      <c r="L87" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M86" t="n">
+      <c r="M87" t="n">
         <v>-58.452328</v>
       </c>
-      <c r="N86" t="n">
+      <c r="N87" t="n">
         <v>-34.572196</v>
       </c>
-      <c r="O86" t="inlineStr">
+      <c r="O87" t="inlineStr">
         <is>
           <t>Colegiales</t>
         </is>
       </c>
-      <c r="P86" t="inlineStr">
+      <c r="P87" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>
       </c>
-      <c r="Q86" t="inlineStr">
+      <c r="Q87" t="inlineStr">
         <is>
           <t>ATH-Q</t>
         </is>
       </c>
-      <c r="R86" t="inlineStr">
+      <c r="R87" t="inlineStr">
         <is>
           <t>Fuera de Poligono OVL</t>
         </is>

</xml_diff>

<commit_message>
Actualizacion automatica del mapa (2025-11-28 15:53:00)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_Optical_Power.xlsx
+++ b/mapa_interactivo_Optical_Power.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R90"/>
+  <dimension ref="A1:R92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3784,17 +3784,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>7260</t>
+          <t>-579</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>9/10/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Vidal 1861</t>
+          <t>Pedro Rivera 2546</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3804,7 +3804,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>809642175</t>
+          <t>ICD30612785</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R200 para pedir traspaso de equipos</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3832,7 +3832,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3841,14 +3841,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.458298</v>
+        <v>-58.462479</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.566511</v>
+        <v>-34.55765</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>COG-F</t>
+          <t>COG-K</t>
         </is>
       </c>
       <c r="R40" t="inlineStr">
@@ -3870,27 +3870,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>7218</t>
+          <t>7260</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>9/15/2025</t>
+          <t>9/10/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SAN NICOLAS 5123</t>
+          <t>Vidal 1861</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>809758863</t>
+          <t>809642175</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3905,7 +3905,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3923,18 +3923,18 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.516218</v>
+        <v>-58.458298</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.589343</v>
+        <v>-34.566511</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3944,7 +3944,7 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>PUE-J</t>
+          <t>COG-F</t>
         </is>
       </c>
       <c r="R41" t="inlineStr">
@@ -3956,27 +3956,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>7240</t>
+          <t>7218</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>9/16/2025</t>
+          <t>9/15/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>LARRALDE, CRISOLOGO AV. 3875</t>
+          <t>SAN NICOLAS 5123</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>809784524</t>
+          <t>809758863</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -4009,18 +4009,18 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.481316</v>
+        <v>-58.516218</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.556157</v>
+        <v>-34.589343</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -4030,7 +4030,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>PUE-J</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -4042,27 +4042,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>7240</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>9/17/2025</t>
+          <t>9/16/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Av Amancio Alcorta 3570</t>
+          <t>LARRALDE, CRISOLOGO AV. 3875</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>809800213</t>
+          <t>809784524</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4077,7 +4077,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -4085,7 +4085,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -4099,24 +4099,24 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.409278</v>
+        <v>-58.481316</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.653566</v>
+        <v>-34.556157</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R43" t="inlineStr">
@@ -4128,7 +4128,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6182</t>
+          <t>6475</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -4138,7 +4138,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Los Patos 2702</t>
+          <t>Av Amancio Alcorta 3570</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -4148,7 +4148,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>809818308</t>
+          <t>809800213</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
+          <t>aplomar</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -4171,7 +4171,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -4181,14 +4181,14 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.399262</v>
+        <v>-58.409278</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.639685</v>
+        <v>-34.653566</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -4202,7 +4202,7 @@
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>PPT-K</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
@@ -4214,27 +4214,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>6182</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>9/23/2025</t>
+          <t>9/17/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>CIUDAD DE LA PAZ 911</t>
+          <t>Los Patos 2702</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ICD30958043</t>
+          <t>809818308</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -4249,7 +4249,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Desmonte de columna ya traspasaron un nodo</t>
+          <t>Sacar PRFV del cantero, colocar en vereda y aplomar</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -4262,7 +4262,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -4271,24 +4271,24 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.447743</v>
+        <v>-58.399262</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.570457</v>
+        <v>-34.639685</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>COG-C</t>
+          <t>PPT-K</t>
         </is>
       </c>
       <c r="R45" t="inlineStr">
@@ -4300,27 +4300,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>7308</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>9/25/2025</t>
+          <t>9/23/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>MANZANARES 4186</t>
+          <t>CIUDAD DE LA PAZ 911</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>809979726</t>
+          <t>ICD30958043</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4335,7 +4335,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmonte de columna ya traspasaron un nodo</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -4348,7 +4348,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -4357,14 +4357,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.485454</v>
+        <v>-58.447743</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.555745</v>
+        <v>-34.570457</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -4374,7 +4374,7 @@
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>COG-O</t>
+          <t>COG-C</t>
         </is>
       </c>
       <c r="R46" t="inlineStr">
@@ -4386,7 +4386,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>7310</t>
+          <t>7308</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -4396,17 +4396,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>BACACAY AV. 5805</t>
+          <t>MANZANARES 4186</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>809979728</t>
+          <t>809979726</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Cambiar y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -4439,18 +4439,18 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.509324</v>
+        <v>-58.485454</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.635335</v>
+        <v>-34.555745</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -4460,19 +4460,19 @@
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>DEV-M</t>
+          <t>COG-O</t>
         </is>
       </c>
       <c r="R47" t="inlineStr">
         <is>
-          <t>ARATO-25058.PO.2DEV</t>
+          <t>Fuera de Poligono OVL</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>7314</t>
+          <t>7310</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4482,17 +4482,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MIRALLA 954</t>
+          <t>BACACAY AV. 5805</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>809979735</t>
+          <t>809979728</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4507,7 +4507,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar y reparar rienda</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4525,14 +4525,14 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.501431</v>
+        <v>-58.509324</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.647791</v>
+        <v>-34.635335</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4546,39 +4546,39 @@
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>PAV-?</t>
+          <t>DEV-M</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
         <is>
-          <t>Fuera de Poligono OVL</t>
+          <t>ARATO-25058.PO.2DEV</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>7373</t>
+          <t>7314</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>10/2/2025</t>
+          <t>9/25/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>SANTIAGO DEL ESTERO 1253</t>
+          <t>MIRALLA 954</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>810132493</t>
+          <t>809979735</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4615,24 +4615,24 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.384406</v>
+        <v>-58.501431</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.622932</v>
+        <v>-34.647791</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>CON-M</t>
+          <t>PAV-?</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -4644,7 +4644,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>7387</t>
+          <t>7373</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4654,17 +4654,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>PERIBEBUY 6814</t>
+          <t>SANTIAGO DEL ESTERO 1253</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>810132728</t>
+          <t>810132493</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4679,7 +4679,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4701,24 +4701,24 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.521719</v>
+        <v>-58.384406</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.647467</v>
+        <v>-34.622932</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>PAV-C</t>
+          <t>CON-M</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
@@ -4730,7 +4730,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>7394</t>
+          <t>7387</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4740,17 +4740,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>BONIFACIO, JOSE 2409</t>
+          <t>PERIBEBUY 6814</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>810132768</t>
+          <t>810132728</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4765,7 +4765,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada volvio a ingresar mail con caso 7597</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4787,24 +4787,24 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.461482</v>
+        <v>-58.521719</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.632432</v>
+        <v>-34.647467</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>PCH-F</t>
+          <t>PAV-C</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
@@ -4816,27 +4816,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>7570</t>
+          <t>7394</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>10/6/2025</t>
+          <t>10/2/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>VILLEGAS, CONRADO, GRAL. 5402</t>
+          <t>BONIFACIO, JOSE 2409</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>810132768</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4846,12 +4846,12 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Colocar R150 o R200</t>
+          <t>Picada volvio a ingresar mail con caso 7597</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4864,7 +4864,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4873,10 +4873,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.465176</v>
+        <v>-58.461482</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.680979</v>
+        <v>-34.632432</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>PAV-U</t>
+          <t>PCH-F</t>
         </is>
       </c>
       <c r="R52" t="inlineStr">
@@ -4902,27 +4902,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>7595</t>
+          <t>7570</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>10/13/2025</t>
+          <t>10/6/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>FALCON, RAMON L.,CNEL. 2353</t>
+          <t>VILLEGAS, CONRADO, GRAL. 5402</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>810333018</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4932,12 +4932,12 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R150 o R200</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4950,7 +4950,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4959,10 +4959,10 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.46138</v>
+        <v>-58.465176</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.629774</v>
+        <v>-34.680979</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4976,7 +4976,7 @@
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>PCH-J</t>
+          <t>PAV-U</t>
         </is>
       </c>
       <c r="R53" t="inlineStr">
@@ -4988,17 +4988,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>7516</t>
+          <t>7595</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>10/15/2025</t>
+          <t>10/13/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>ALVAREZ, CRISOSTOMO 3000</t>
+          <t>FALCON, RAMON L.,CNEL. 2353</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -5008,7 +5008,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>810371027</t>
+          <t>810333018</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -5045,10 +5045,10 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.458516</v>
+        <v>-58.46138</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.646422</v>
+        <v>-34.629774</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -5062,7 +5062,7 @@
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>PPT-N</t>
+          <t>PCH-J</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
@@ -5074,7 +5074,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>7735</t>
+          <t>7516</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -5084,17 +5084,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>GARCIA, MARTIN AV. 772</t>
+          <t>ALVAREZ, CRISOSTOMO 3000</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>810371042</t>
+          <t>810371027</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -5131,14 +5131,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.374086</v>
+        <v>-58.458516</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.633168</v>
+        <v>-34.646422</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -5148,7 +5148,7 @@
       </c>
       <c r="Q55" t="inlineStr">
         <is>
-          <t>CON-B</t>
+          <t>PPT-N</t>
         </is>
       </c>
       <c r="R55" t="inlineStr">
@@ -5160,27 +5160,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5783</t>
+          <t>7735</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>10/17/2025</t>
+          <t>10/15/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ALCARAZ 5168</t>
+          <t>GARCIA, MARTIN AV. 772</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>810378783</t>
+          <t>810371042</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -5217,24 +5217,24 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.50875</v>
+        <v>-58.374086</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.623434</v>
+        <v>-34.633168</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q56" t="inlineStr">
         <is>
-          <t>DEV-H</t>
+          <t>CON-B</t>
         </is>
       </c>
       <c r="R56" t="inlineStr">
@@ -5246,27 +5246,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>7621</t>
+          <t>5783</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>10/20/2025</t>
+          <t>10/17/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Quito 3832</t>
+          <t>ALCARAZ 5168</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>810404273</t>
+          <t>810378783</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5303,24 +5303,24 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.420412</v>
+        <v>-58.50875</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.616726</v>
+        <v>-34.623434</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q57" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>DEV-H</t>
         </is>
       </c>
       <c r="R57" t="inlineStr">
@@ -5332,27 +5332,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>7571</t>
+          <t>7621</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>10/22/2025</t>
+          <t>10/20/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SAENZ AV. 1204</t>
+          <t>Quito 3832</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>810416653</t>
+          <t>810404273</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -5389,14 +5389,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.416237</v>
+        <v>-58.420412</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.65477</v>
+        <v>-34.616726</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -5406,7 +5406,7 @@
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>PPT-H</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R58" t="inlineStr">
@@ -5418,27 +5418,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>7556</t>
+          <t>7571</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>10/21/2025</t>
+          <t>10/22/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1923</t>
+          <t>SAENZ AV. 1204</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>810416656</t>
+          <t>810416653</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -5453,7 +5453,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -5475,10 +5475,10 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.411426</v>
+        <v>-58.416237</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.633266</v>
+        <v>-34.65477</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -5492,7 +5492,7 @@
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>PPT-Q</t>
+          <t>PPT-H</t>
         </is>
       </c>
       <c r="R59" t="inlineStr">
@@ -5504,27 +5504,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>7579</t>
+          <t>7556</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>10/22/2025</t>
+          <t>10/21/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>AGUIRRE 508</t>
+          <t>SANCHEZ DE LORIA 1923</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>810421912</t>
+          <t>810416656</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -5539,7 +5539,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>cambiar</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -5557,18 +5557,18 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.435731</v>
+        <v>-58.411426</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.597659</v>
+        <v>-34.633266</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -5578,7 +5578,7 @@
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>VCR-H</t>
+          <t>PPT-Q</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
@@ -5590,27 +5590,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7620</t>
+          <t>7579</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>10/24/2025</t>
+          <t>10/22/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>QUITO 3954</t>
+          <t>AGUIRRE 508</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>810447247</t>
+          <t>810421912</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5643,18 +5643,18 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.422216</v>
+        <v>-58.435731</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.616828</v>
+        <v>-34.597659</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5664,7 +5664,7 @@
       </c>
       <c r="Q61" t="inlineStr">
         <is>
-          <t>ALM-C</t>
+          <t>VCR-H</t>
         </is>
       </c>
       <c r="R61" t="inlineStr">
@@ -5676,7 +5676,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7755</t>
+          <t>7620</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5686,17 +5686,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Munich 1715</t>
+          <t>QUITO 3954</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>810447258</t>
+          <t>810447247</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5733,24 +5733,24 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.453119</v>
+        <v>-58.422216</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.55489</v>
+        <v>-34.616828</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>BLO-C</t>
+          <t>ALM-C</t>
         </is>
       </c>
       <c r="R62" t="inlineStr">
@@ -5762,27 +5762,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>5749</t>
+          <t>7755</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>10/27/2025</t>
+          <t>10/24/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1754</t>
+          <t>Munich 1715</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>01230434</t>
+          <t>810447258</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5792,16 +5792,16 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Traspaso de nodo propio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -5810,7 +5810,7 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
@@ -5819,24 +5819,24 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.4018</v>
+        <v>-58.453119</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.590471</v>
+        <v>-34.55489</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>AGU-F</t>
+          <t>BLO-C</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
@@ -5848,7 +5848,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7631</t>
+          <t>5749</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5858,17 +5858,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 3762</t>
+          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1754</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>810451584</t>
+          <t>01230434</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5878,16 +5878,16 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de nodo propio</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
@@ -5896,7 +5896,7 @@
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L64" t="inlineStr">
@@ -5905,14 +5905,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.418542</v>
+        <v>-58.4018</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.624609</v>
+        <v>-34.590471</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5922,7 +5922,7 @@
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>ALM-A</t>
+          <t>AGU-F</t>
         </is>
       </c>
       <c r="R64" t="inlineStr">
@@ -5934,7 +5934,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7630</t>
+          <t>7631</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5944,7 +5944,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>INDEPENDENCIA AV. 3690</t>
+          <t>CALVO, CARLOS 3762</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5954,7 +5954,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>810451588</t>
+          <t>810451584</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5991,10 +5991,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.417821</v>
+        <v>-58.418542</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.621158</v>
+        <v>-34.624609</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -6020,7 +6020,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7624</t>
+          <t>7630</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -6030,17 +6030,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>DIAZ VELEZ AV. 4516</t>
+          <t>INDEPENDENCIA AV. 3690</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>810454541</t>
+          <t>810451588</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -6055,7 +6055,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -6077,14 +6077,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.430613</v>
+        <v>-58.417821</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.608805</v>
+        <v>-34.621158</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -6094,7 +6094,7 @@
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>ALM-J</t>
+          <t>ALM-A</t>
         </is>
       </c>
       <c r="R66" t="inlineStr">
@@ -6106,7 +6106,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7622</t>
+          <t>7624</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -6116,17 +6116,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>MIRALLA 950</t>
+          <t>DIAZ VELEZ AV. 4516</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>01233440</t>
+          <t>810454541</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6141,7 +6141,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -6154,7 +6154,7 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
@@ -6163,24 +6163,24 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.50161</v>
+        <v>-58.430613</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.647648</v>
+        <v>-34.608805</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>PAV-?</t>
+          <t>ALM-J</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -6192,27 +6192,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7643</t>
+          <t>7622</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>10/28/2025</t>
+          <t>10/27/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>ACEVEDO 524</t>
+          <t>MIRALLA 950</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>810458896</t>
+          <t>01233440</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6240,7 +6240,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L68" t="inlineStr">
@@ -6249,24 +6249,24 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.439164</v>
+        <v>-58.50161</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.597069</v>
+        <v>-34.647648</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>VCR-J</t>
+          <t>PAV-?</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
@@ -6278,7 +6278,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7665</t>
+          <t>7643</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -6288,17 +6288,